<commit_message>
feat: 06072135 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\my-carbon-site\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,21 +17,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="childishgambino2" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="childishgambino2" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="bloodorange4" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
+    <definedName name="bloodorange4_1" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -34,15 +32,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="接続" type="4" refreshedVersion="4" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/childishgambino2.htm" htmlTables="1">
+  <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/bloodorange4.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
-  <connection id="2" name="接続1" type="4" refreshedVersion="4" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/childishgambino2.htm" htmlTables="1">
+  <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/bloodorange4.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -52,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="40">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,62 +70,119 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Composer </t>
-  </si>
-  <si>
-    <t>Donald Glover / James Francies, Jr. / Denise Renee</t>
-  </si>
-  <si>
-    <t>Childish Gambino</t>
-  </si>
-  <si>
-    <t>Algorhythm</t>
-  </si>
-  <si>
-    <t>Donald Glover / Dacoury Natche / Eyobed Getachew / Riley Mackin / Kurtis McKenzie / Ely Rise / Keir Gist / Reneé Neufville / Abdullah Bahr / Leon Ware / Zane Grey</t>
-  </si>
-  <si>
-    <t>Donald Glover / Dacoury Natche / Ludwig Göransson / Chukwudi Hodge / Sarah Aarons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donald Glover / Dacoury Natche / Shéyaa Bin Abraham-Joseph / Atia "Ink" Boggs / Kadhja Bonet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Donald Glover / Dacoury Natche / Ludwig Göransson / Chukwudi / Hodge / Kurtis McKenzie / James Francies, Jr. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Donald Glover / Dacoury Natche / Carlos "Loshendrix" Munoz</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Donald Glover / Dacoury Natche / Ludwig Göransson / Chukwudi Hodge / Kurtis McKenzie / James Francies, Jr.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Donald Glover / Dacoury Natche / Erwin Henderson, Jr. / Curtis Kirk / Peaches Monroee / Sam Sugarman</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Donald Glover / James Francies, Jr. / Riley Mackin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Donald Glover / Ludwig Göransson</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Donald Glover / Dacoury Natche / Ludwig Göransson / Chukwudi Hodge / Legend Glover</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Donald Glover / Dacoury Natche / James Francies, Jr.</t>
+    <t>Title/Composer</t>
+  </si>
+  <si>
+    <t>I Wanna C U</t>
+  </si>
+  <si>
+    <t>Devonte Hynes / Aaron Maine</t>
+  </si>
+  <si>
+    <t>Blood Orange</t>
+  </si>
+  <si>
+    <t>Something to Do</t>
+  </si>
+  <si>
+    <t>Devonte Hynes</t>
+  </si>
+  <si>
+    <t>Dark &amp; Handsome</t>
+  </si>
+  <si>
+    <t>Chaz Bear / Devonte Hynes</t>
+  </si>
+  <si>
+    <t>Blood Orange feat. Toro Y Moi</t>
+  </si>
+  <si>
+    <t>Benzo</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Bryndon Cook / Devonte Hynes / Ian Isiah / Dudley Randall</t>
+  </si>
+  <si>
+    <t>Blood Orange feat. Kelsey Lu, Ian Isiah</t>
+  </si>
+  <si>
+    <t>Good for You</t>
+  </si>
+  <si>
+    <t>Devonte Hynes / Justine Skye</t>
+  </si>
+  <si>
+    <t>Blood Orange feat. Justin Skye</t>
+  </si>
+  <si>
+    <t>Baby Florence (Figure)</t>
+  </si>
+  <si>
+    <t>Devonte Hynes / Arthur Russell</t>
+  </si>
+  <si>
+    <t>Gold Teeth</t>
+  </si>
+  <si>
+    <t>Paul Beauregard / Gangsta Boo / Jordan Houston / Patrick Houston / Devonte Hynes / Lola Mitchell / Project Pat</t>
+  </si>
+  <si>
+    <t>Blood Orange feat. Project Pat, Gangsta Boo, Tinashe</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Devonte Hynes / Ian Isiah / Aaron Maine</t>
+  </si>
+  <si>
+    <t>Blood Orange feat. Porches, Ian Isiah</t>
+  </si>
+  <si>
+    <t>Tuesday Feeling (Choose to Stay)</t>
+  </si>
+  <si>
+    <t>Devonte Hynes / Tinashe Kachingwe</t>
+  </si>
+  <si>
+    <t>Blood Orange feat. TInashe</t>
+  </si>
+  <si>
+    <t>Seven Hours, Pt. 1</t>
+  </si>
+  <si>
+    <t>Devonte Hynes / Benny Revival</t>
+  </si>
+  <si>
+    <t>Blood Orange deat. Benny Revival</t>
+  </si>
+  <si>
+    <t>Take It Back</t>
+  </si>
+  <si>
+    <t>Arca / Russell Boring / Alejandro Ghersi / Devonte Hynes / Joba</t>
+  </si>
+  <si>
+    <t>Blood Orange feat. Arca, Joba, Justine Skye</t>
+  </si>
+  <si>
+    <t>Happiness</t>
+  </si>
+  <si>
+    <t>Today</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,11 +267,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="childishgambino2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bloodorange4_1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="childishgambino2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bloodorange4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -508,7 +563,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -519,25 +574,22 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCellId="1" sqref="A1:XFD1048576 A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" customWidth="1"/>
-    <col min="3" max="3" width="80.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="49.77734375" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
@@ -545,12 +597,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -559,10 +611,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.12430555555555556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+        <v>5.1388888888888894E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -576,222 +628,250 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.14722222222222223</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+        <v>3.5416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0.25486111111111109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.10625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>12.38</v>
+      <c r="B5" t="s">
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.2722222222222222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>19.100000000000001</v>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2">
-        <v>0.21388888888888891</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+        <v>6.458333333333334E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>24.19</v>
+      <c r="B7" t="s">
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
-        <v>0.33263888888888887</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+        <v>9.8611111111111108E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>32.22</v>
+      <c r="B8" t="s">
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13333333333333333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.12291666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>35.31</v>
+      <c r="B9" t="s">
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16388888888888889</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.12569444444444444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>39.28</v>
+      <c r="B10" t="s">
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12430555555555556</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+        <v>8.1944444444444445E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>42.26</v>
+      <c r="B11" t="s">
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
-        <v>0.22291666666666665</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.12291666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>47.48</v>
+      <c r="B12" t="s">
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
-        <v>53.49</v>
+      <c r="B13" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.18194444444444444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="2">
-        <v>0.16319444444444445</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E14" s="2">
+        <v>8.9583333333333334E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5.486111111111111E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:5">
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:5">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:5">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:5">
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:5">
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:5">
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:5">
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:5">
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:5">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:5">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:5">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:5">
       <c r="E28" s="2"/>
     </row>
   </sheetData>
@@ -805,42 +885,42 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="A3:K16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" customWidth="1"/>
-    <col min="3" max="3" width="3.90625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.08984375" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="3" max="3" width="3.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="4" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" customWidth="1"/>
-    <col min="7" max="7" width="4.453125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" customWidth="1"/>
-    <col min="9" max="9" width="4.36328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1"/>
-    <col min="11" max="11" width="3.453125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.21875" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" customWidth="1"/>
+    <col min="11" max="11" width="3.44140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>162</v>
+        <v>110</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -853,21 +933,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title     </v>
+        <v xml:space="preserve"> Title                           </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                        </v>
+        <v xml:space="preserve"> Composers                                                                                                    </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer       </v>
+        <v xml:space="preserve"> Performer                                           </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -880,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -892,21 +972,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">---------- </v>
+        <v xml:space="preserve">-------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> -------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -918,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -931,34 +1011,34 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">0         </v>
+        <v xml:space="preserve">I Wanna C U                     </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Donald Glover / James Francies, Jr. / Denise Renee                                                                                                                </v>
+        <v xml:space="preserve"> Devonte Hynes / Aaron Maine                                                                                   </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange                                        </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:59 </v>
+        <v xml:space="preserve">01:14 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -971,34 +1051,34 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Algorhythm</v>
+        <v xml:space="preserve">Something to Do                 </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Donald Glover / Dacoury Natche / Eyobed Getachew / Riley Mackin / Kurtis McKenzie / Ely Rise / Keir Gist / Reneé Neufville / Abdullah Bahr / Leon Ware / Zane Gre</v>
+        <v xml:space="preserve"> Devonte Hynes                                                                                                 </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange                                        </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:32 </v>
+        <v xml:space="preserve">00:51 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1011,34 +1091,34 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Time      </v>
+        <v xml:space="preserve">Dark &amp; Handsome                 </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Donald Glover / Dacoury Natche / Ludwig Göransson / Chukwudi Hodge / Sarah Aarons                                                                                </v>
+        <v xml:space="preserve"> Chaz Bear / Devonte Hynes                                                                                     </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange feat. Toro Y Moi                       </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:07 </v>
+        <v xml:space="preserve">02:33 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1051,34 +1131,34 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">12.38     </v>
+        <v xml:space="preserve">Benzo                           </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Donald Glover / Dacoury Natche / Shéyaa Bin Abraham-Joseph / Atia "Ink" Boggs / Kadhja Bonet                                                                     </v>
+        <v xml:space="preserve"> Devonte Hynes                                                                                                 </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange                                        </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:32 </v>
+        <v xml:space="preserve">02:30 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1091,34 +1171,34 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">19.1      </v>
+        <v xml:space="preserve">Birmingham                      </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Donald Glover / Dacoury Natche / Ludwig Göransson / Chukwudi / Hodge / Kurtis McKenzie / James Francies, Jr.                                                     </v>
+        <v xml:space="preserve"> Bryndon Cook / Devonte Hynes / Ian Isiah / Dudley Randall                                                     </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange feat. Kelsey Lu, Ian Isiah             </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:08 </v>
+        <v xml:space="preserve">01:33 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1131,34 +1211,34 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">24.19     </v>
+        <v xml:space="preserve">Good for You                    </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">  Donald Glover / Dacoury Natche / Carlos "Loshendrix" Munoz                                                                                                       </v>
+        <v xml:space="preserve"> Devonte Hynes / Justine Skye                                                                                  </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange feat. Justin Skye                      </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">07:59 </v>
+        <v xml:space="preserve">02:22 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1171,34 +1251,34 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">32.22     </v>
+        <v xml:space="preserve">Baby Florence (Figure)          </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">  Donald Glover / Dacoury Natche / Ludwig Göransson / Chukwudi Hodge / Kurtis McKenzie / James Francies, Jr.                                                      </v>
+        <v xml:space="preserve"> Devonte Hynes / Arthur Russell                                                                                </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange                                        </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:12 </v>
+        <v xml:space="preserve">02:57 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1211,34 +1291,34 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">35.31     </v>
+        <v xml:space="preserve">Gold Teeth                      </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">  Donald Glover / Dacoury Natche / Erwin Henderson, Jr. / Curtis Kirk / Peaches Monroee / Sam Sugarman                                                             </v>
+        <v xml:space="preserve"> Paul Beauregard / Gangsta Boo / Jordan Houston / Patrick Houston / Devonte Hynes / Lola Mitchell / Project Pat</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v>Blood Orange feat. Project Pat, Gangsta Boo, Tinashe</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:56 </v>
+        <v xml:space="preserve">03:01 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1251,34 +1331,34 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">39.28     </v>
+        <v xml:space="preserve">Berlin                          </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">  Donald Glover / James Francies, Jr. / Riley Mackin                                                                                                               </v>
+        <v xml:space="preserve"> Devonte Hynes / Ian Isiah / Aaron Maine                                                                       </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange feat. Porches, Ian Isiah               </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:59 </v>
+        <v xml:space="preserve">01:58 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1291,34 +1371,34 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">42.26     </v>
+        <v>Tuesday Feeling (Choose to Stay)</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">  Donald Glover / Ludwig Göransson                                                                                                                                </v>
+        <v xml:space="preserve"> Devonte Hynes / Tinashe Kachingwe                                                                             </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange feat. TInashe                          </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:21 </v>
+        <v xml:space="preserve">02:57 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1331,34 +1411,34 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">47.48     </v>
+        <v xml:space="preserve">Seven Hours, Pt. 1              </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">  Donald Glover / Dacoury Natche / Ludwig Göransson / Chukwudi Hodge / Legend Glover                                                                              </v>
+        <v xml:space="preserve"> Devonte Hynes / Benny Revival                                                                                 </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange deat. Benny Revival                    </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:00 </v>
+        <v xml:space="preserve">02:40 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1371,114 +1451,114 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">53.49     </v>
+        <v xml:space="preserve">Take It Back                    </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">  Donald Glover / Dacoury Natche / James Francies, Jr.                                                                                                             </v>
+        <v xml:space="preserve"> Arca / Russell Boring / Alejandro Ghersi / Devonte Hynes / Joba                                               </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Childish Gambino</v>
+        <v xml:space="preserve">Blood Orange feat. Arca, Joba, Justine Skye         </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:55 </v>
+        <v xml:space="preserve">04:22 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">Happiness                       </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve"> Devonte Hynes                                                                                                 </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">Blood Orange                                        </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:09 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">Today                           </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve"> Devonte Hynes                                                                                                 </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">Blood Orange                                        </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">01:19 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1491,21 +1571,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                                                    </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1518,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1531,21 +1611,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                                                    </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1558,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1571,21 +1651,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                                                    </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1598,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1611,21 +1691,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                                                    </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1638,7 +1718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1651,21 +1731,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                                                    </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1678,7 +1758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1691,21 +1771,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                                                    </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1718,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1731,21 +1811,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                                </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                                                    </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1773,22 +1853,19 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" customWidth="1"/>
-    <col min="3" max="3" width="80.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="49.77734375" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
@@ -1796,12 +1873,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1810,10 +1887,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.12430555555555556</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+        <v>5.1388888888888894E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1827,222 +1904,250 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.14722222222222223</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+        <v>3.5416666666666666E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0.25486111111111109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.10625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>12.38</v>
+      <c r="B5" t="s">
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.2722222222222222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>19.100000000000001</v>
+      <c r="B6" t="s">
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2">
-        <v>0.21388888888888891</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+        <v>6.458333333333334E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>24.19</v>
+      <c r="B7" t="s">
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
-        <v>0.33263888888888887</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+        <v>9.8611111111111108E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>32.22</v>
+      <c r="B8" t="s">
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13333333333333333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.12291666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>35.31</v>
+      <c r="B9" t="s">
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16388888888888889</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.12569444444444444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>39.28</v>
+      <c r="B10" t="s">
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12430555555555556</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+        <v>8.1944444444444445E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>42.26</v>
+      <c r="B11" t="s">
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
-        <v>0.22291666666666665</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.12291666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>47.48</v>
+      <c r="B12" t="s">
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="5">
-        <v>53.49</v>
+      <c r="B13" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.18194444444444444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="2">
-        <v>0.16319444444444445</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="E14" s="2">
+        <v>8.9583333333333334E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>5.486111111111111E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:5">
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:5">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:5">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:5">
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:5">
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:5">
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:5">
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:5">
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:5">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:5">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:5">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:5">
       <c r="E28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat:06082240   2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="bloodorange4" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
-    <definedName name="bloodorange4_1" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="chancetherapper3" localSheetId="0">Sheet1!$A$1:$E$23</definedName>
+    <definedName name="chancetherapper3" localSheetId="2">Sheet3!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/bloodorange4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/chancetherapper3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/bloodorange4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/chancetherapper3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="64">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,106 +73,178 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>I Wanna C U</t>
-  </si>
-  <si>
-    <t>Devonte Hynes / Aaron Maine</t>
-  </si>
-  <si>
-    <t>Blood Orange</t>
-  </si>
-  <si>
-    <t>Something to Do</t>
-  </si>
-  <si>
-    <t>Devonte Hynes</t>
-  </si>
-  <si>
-    <t>Dark &amp; Handsome</t>
-  </si>
-  <si>
-    <t>Chaz Bear / Devonte Hynes</t>
-  </si>
-  <si>
-    <t>Blood Orange feat. Toro Y Moi</t>
-  </si>
-  <si>
-    <t>Benzo</t>
-  </si>
-  <si>
-    <t>Birmingham</t>
-  </si>
-  <si>
-    <t>Bryndon Cook / Devonte Hynes / Ian Isiah / Dudley Randall</t>
-  </si>
-  <si>
-    <t>Blood Orange feat. Kelsey Lu, Ian Isiah</t>
-  </si>
-  <si>
-    <t>Good for You</t>
-  </si>
-  <si>
-    <t>Devonte Hynes / Justine Skye</t>
-  </si>
-  <si>
-    <t>Blood Orange feat. Justin Skye</t>
-  </si>
-  <si>
-    <t>Baby Florence (Figure)</t>
-  </si>
-  <si>
-    <t>Devonte Hynes / Arthur Russell</t>
-  </si>
-  <si>
-    <t>Gold Teeth</t>
-  </si>
-  <si>
-    <t>Paul Beauregard / Gangsta Boo / Jordan Houston / Patrick Houston / Devonte Hynes / Lola Mitchell / Project Pat</t>
-  </si>
-  <si>
-    <t>Blood Orange feat. Project Pat, Gangsta Boo, Tinashe</t>
-  </si>
-  <si>
-    <t>Berlin</t>
-  </si>
-  <si>
-    <t>Devonte Hynes / Ian Isiah / Aaron Maine</t>
-  </si>
-  <si>
-    <t>Blood Orange feat. Porches, Ian Isiah</t>
-  </si>
-  <si>
-    <t>Tuesday Feeling (Choose to Stay)</t>
-  </si>
-  <si>
-    <t>Devonte Hynes / Tinashe Kachingwe</t>
-  </si>
-  <si>
-    <t>Blood Orange feat. TInashe</t>
-  </si>
-  <si>
-    <t>Seven Hours, Pt. 1</t>
-  </si>
-  <si>
-    <t>Devonte Hynes / Benny Revival</t>
-  </si>
-  <si>
-    <t>Blood Orange deat. Benny Revival</t>
-  </si>
-  <si>
-    <t>Take It Back</t>
-  </si>
-  <si>
-    <t>Arca / Russell Boring / Alejandro Ghersi / Devonte Hynes / Joba</t>
-  </si>
-  <si>
-    <t>Blood Orange feat. Arca, Joba, Justine Skye</t>
-  </si>
-  <si>
-    <t>Happiness</t>
-  </si>
-  <si>
-    <t>Today</t>
+    <t>All Day Long</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Darius Scott, Dwayne Verner, Jr., Greg Landfair, Nate Fox, Nico Segal, Peter Wilkins</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. John Legend</t>
+  </si>
+  <si>
+    <t>Do You Remember</t>
+  </si>
+  <si>
+    <t>Benjamin Gibbard, Chancelor, J. Bennett, Dwayne Verner, Eric Butler, Francis Starlite, Garren Langford, Justin Vernon, Nate Fox, Nico Segal, Peter Wilkins</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Death Cab for Cutie</t>
+  </si>
+  <si>
+    <t>Eternal</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Christopher Smith, Jr, .Darian Garcia, Darius Scott, Garren Langford, Greg Landfair, Ken Bennett</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Smino</t>
+  </si>
+  <si>
+    <t>Hot Shower</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Darian Garcia, Jonathan L. Kirk, Malcolm Jamaal Davis</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Madein TYO, DaBaby</t>
+  </si>
+  <si>
+    <t>We Go High</t>
+  </si>
+  <si>
+    <t>Ben Lusher, Chancelor J. Bennett, Darius Scott, Mike Servin, Nate Fox, Nico Segal, Peter Wilkins</t>
+  </si>
+  <si>
+    <t>Chance the Rapper</t>
+  </si>
+  <si>
+    <t>I Got You (Always and Forever)</t>
+  </si>
+  <si>
+    <t>Carter Lang, Chancelor J. Bennett, Courtney Shanade Salter, Dwayne Verner, En Vogue, Eric Butler, Garren Langford, Kierra Sheard, Nate Fox, Peter Wilkins</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. En Vogue, Ari Lennox, Kierra Sheard</t>
+  </si>
+  <si>
+    <t>Photo Ops (Skit)</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Colleen Mares</t>
+  </si>
+  <si>
+    <t>Roo</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, CocoRosie, Taylor Bennett</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Taylor Bennett, CocoRosie</t>
+  </si>
+  <si>
+    <t>The Big Day</t>
+  </si>
+  <si>
+    <t>Carter Lang, Chancelor J. Bennett, Darius Scott, Francis Starlite, James Cleveland, Joe Rainey Sr., John Stephens, Justin Vernon, Nico Segal, Peter Wilkins</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Francis and the Lights</t>
+  </si>
+  <si>
+    <t>Let's Go on the Run</t>
+  </si>
+  <si>
+    <t>Ben Lusher, Carter Lang, Chancelor J. Bennett, Darius Scott, Dwayne Verner, Kevin K. Rhomberg, Nate Fox, Nico Segal</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Knox Fortune</t>
+  </si>
+  <si>
+    <t>Handsome</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Darian Garcia, Dex Coleman, Megan Pete, Peter Wilkins, Pink Sweats, TrapMoneyBenny</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Megan Thee Stallion</t>
+  </si>
+  <si>
+    <t>Big Fish</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Radric Davis, Tim Mosley</t>
+  </si>
+  <si>
+    <t>Ballin Flossin</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett,Darius Scott, Greg Landfair, Keith Edward Crouch, Kevin James, Nate Fox, Peter Wilkins, Darius Scott Harris, Shawn Mendes</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Gucci Mane</t>
+  </si>
+  <si>
+    <t>4 Quarters in the Black (Skit)</t>
+  </si>
+  <si>
+    <t>5 Year Plan</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Darius Scott, Francis Starlite, Gabe Jaskowiak, Jordan Ware, Macie Stewart, Nate Fox, Peter Wilkins, Randy Newman</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Randy Newman</t>
+  </si>
+  <si>
+    <t>Get a Bag</t>
+  </si>
+  <si>
+    <t>Calvin Woods, Chancelor J. Bennett, James Taylor, Nate Fox, Peter Losnegard, Peter Wilkins</t>
+  </si>
+  <si>
+    <t>Chance the Rapper deat. Calboy</t>
+  </si>
+  <si>
+    <t>Slide Around</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Durk Banks, Nate Fox, Onika Maraj, Pi'erre Bourne</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Lil Durk, Nicki Minaj</t>
+  </si>
+  <si>
+    <t>Sun Come Down</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Darian Garcia, Darius Scott, Dwayne Verner, Eric Butler, Gabe Jaskowiak, Nate Fox, Nico Segal, Peter Wilkins, Ryan Vojtesak</t>
+  </si>
+  <si>
+    <t>Found a Good One (Single No More)</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Darius Sjascott, Dwayne Verner, Greg Landfair, Lisa Mishra, Nate Fox, Nico Segal, Peter Wilkins, SWV, Shane Lee Lindstrom</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. SWV, Pretty Vee</t>
+  </si>
+  <si>
+    <t>Town on the Hill</t>
+  </si>
+  <si>
+    <t>Chancelor J. Bennett, Francis Starlite, Justin Vernon, Peter Wilkins</t>
+  </si>
+  <si>
+    <t>Our House (Skit)</t>
+  </si>
+  <si>
+    <t>Zanies and Fools</t>
+  </si>
+  <si>
+    <t>Carter Lang, Chancelor J. Bennett, Darius Scott, Dwayne Verner, Greg Landfair, Nate Fox, Nico Segal, Onika Maraj, Oscar Hammerstein, Peter Wilkins, Richard Rodgers</t>
+  </si>
+  <si>
+    <t>Chance the Rapper feat. Scott, Nicki Mina</t>
   </si>
 </sst>
 </file>
@@ -267,11 +339,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bloodorange4_1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="chancetherapper3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="bloodorange4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="chancetherapper3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,15 +646,15 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="A1:XFD1048576 A1:XFD1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="49.77734375" customWidth="1"/>
+    <col min="4" max="4" width="56.21875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -611,7 +683,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>5.1388888888888894E-2</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -625,10 +697,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>3.5416666666666666E-2</v>
+        <v>0.16388888888888889</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -636,16 +708,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.10625</v>
+        <v>0.16874999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -653,16 +725,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
-        <v>0.10416666666666667</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -670,16 +742,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
-        <v>6.458333333333334E-2</v>
+        <v>0.2076388888888889</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -687,16 +759,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2">
-        <v>9.8611111111111108E-2</v>
+        <v>0.19513888888888889</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -704,16 +776,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2">
-        <v>0.12291666666666667</v>
+        <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -721,16 +793,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.11875000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -738,16 +810,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2">
-        <v>8.1944444444444445E-2</v>
+        <v>0.16805555555555554</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -755,16 +827,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
-        <v>0.12291666666666667</v>
+        <v>0.15347222222222223</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -772,16 +844,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1111111111111111</v>
+        <v>0.12013888888888889</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -789,16 +861,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2">
-        <v>0.18194444444444444</v>
+        <v>0.12916666666666668</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -806,16 +878,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2">
-        <v>8.9583333333333334E-2</v>
+        <v>0.1173611111111111</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -823,55 +895,167 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2">
-        <v>5.486111111111111E-2</v>
+        <v>9.2361111111111116E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="5:5">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="5:5">
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="5:5">
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="5:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.17847222222222223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.13958333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14930555555555555</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.17916666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.12430555555555556</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.22430555555555556</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="5:5">
+    <row r="25" spans="1:5">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="5:5">
+    <row r="26" spans="1:5">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="5:5">
+    <row r="27" spans="1:5">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="5:5">
+    <row r="28" spans="1:5">
       <c r="E28" s="2"/>
     </row>
   </sheetData>
@@ -885,7 +1069,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -905,15 +1089,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>110</v>
+        <v>163</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -933,21 +1117,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                           </v>
+        <v xml:space="preserve"> Title                            </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                    </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                         </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                           </v>
+        <v xml:space="preserve"> Performer                                                  </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -972,21 +1156,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">-------------------------------- </v>
+        <v xml:space="preserve">--------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1011,28 +1195,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I Wanna C U                     </v>
+        <v xml:space="preserve">All Day Long                     </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes / Aaron Maine                                                                                   </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Darius Scott, Dwayne Verner, Jr., Greg Landfair, Nate Fox, Nico Segal, Peter Wilkins                                                         </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange                                        </v>
+        <v xml:space="preserve">Chance the Rapper feat. John Legend                        </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:14 </v>
+        <v xml:space="preserve">03:28 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1051,28 +1235,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Something to Do                 </v>
+        <v xml:space="preserve">Do You Remember                  </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes                                                                                                 </v>
+        <v xml:space="preserve"> Benjamin Gibbard, Chancelor, J. Bennett, Dwayne Verner, Eric Butler, Francis Starlite, Garren Langford, Justin Vernon, Nate Fox, Nico Segal, Peter Wilkins         </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange                                        </v>
+        <v xml:space="preserve">Chance the Rapper feat. Death Cab for Cutie                </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:51 </v>
+        <v xml:space="preserve">03:56 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1091,28 +1275,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dark &amp; Handsome                 </v>
+        <v xml:space="preserve">Eternal                          </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chaz Bear / Devonte Hynes                                                                                     </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Christopher Smith, Jr, .Darian Garcia, Darius Scott, Garren Langford, Greg Landfair, Ken Bennett                                             </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange feat. Toro Y Moi                       </v>
+        <v xml:space="preserve">Chance the Rapper feat. Smino                              </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:33 </v>
+        <v xml:space="preserve">04:03 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1131,28 +1315,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Benzo                           </v>
+        <v xml:space="preserve">Hot Shower                       </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes                                                                                                 </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Darian Garcia, Jonathan L. Kirk, Malcolm Jamaal Davis                                                                                        </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange                                        </v>
+        <v xml:space="preserve">Chance the Rapper feat. Madein TYO, DaBaby                 </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:30 </v>
+        <v xml:space="preserve">03:45 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1171,28 +1355,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Birmingham                      </v>
+        <v xml:space="preserve">We Go High                       </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bryndon Cook / Devonte Hynes / Ian Isiah / Dudley Randall                                                     </v>
+        <v xml:space="preserve"> Ben Lusher, Chancelor J. Bennett, Darius Scott, Mike Servin, Nate Fox, Nico Segal, Peter Wilkins                                                                   </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange feat. Kelsey Lu, Ian Isiah             </v>
+        <v xml:space="preserve">Chance the Rapper                                          </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:33 </v>
+        <v xml:space="preserve">04:59 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1211,28 +1395,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Good for You                    </v>
+        <v xml:space="preserve">I Got You (Always and Forever)   </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes / Justine Skye                                                                                  </v>
+        <v xml:space="preserve"> Carter Lang, Chancelor J. Bennett, Courtney Shanade Salter, Dwayne Verner, En Vogue, Eric Butler, Garren Langford, Kierra Sheard, Nate Fox, Peter Wilkins          </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange feat. Justin Skye                      </v>
+        <v>Chance the Rapper feat. En Vogue, Ari Lennox, Kierra Sheard</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:22 </v>
+        <v xml:space="preserve">04:41 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1251,28 +1435,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Baby Florence (Figure)          </v>
+        <v xml:space="preserve">Photo Ops (Skit)                 </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes / Arthur Russell                                                                                </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Colleen Mares                                                                                                                                </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange                                        </v>
+        <v xml:space="preserve">Chance the Rapper                                          </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:57 </v>
+        <v xml:space="preserve">01:15 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1291,28 +1475,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Gold Teeth                      </v>
+        <v xml:space="preserve">Roo                              </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Paul Beauregard / Gangsta Boo / Jordan Houston / Patrick Houston / Devonte Hynes / Lola Mitchell / Project Pat</v>
+        <v xml:space="preserve"> Chancelor J. Bennett, CocoRosie, Taylor Bennett                                                                                                                    </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Blood Orange feat. Project Pat, Gangsta Boo, Tinashe</v>
+        <v xml:space="preserve">Chance the Rapper feat. Taylor Bennett, CocoRosie          </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:01 </v>
+        <v xml:space="preserve">02:51 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1331,28 +1515,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Berlin                          </v>
+        <v xml:space="preserve">The Big Day                      </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes / Ian Isiah / Aaron Maine                                                                       </v>
+        <v xml:space="preserve"> Carter Lang, Chancelor J. Bennett, Darius Scott, Francis Starlite, James Cleveland, Joe Rainey Sr., John Stephens, Justin Vernon, Nico Segal, Peter Wilkins        </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange feat. Porches, Ian Isiah               </v>
+        <v xml:space="preserve">Chance the Rapper feat. Francis and the Lights             </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:58 </v>
+        <v xml:space="preserve">04:02 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1371,28 +1555,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Tuesday Feeling (Choose to Stay)</v>
+        <v xml:space="preserve">Let's Go on the Run              </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes / Tinashe Kachingwe                                                                             </v>
+        <v xml:space="preserve"> Ben Lusher, Carter Lang, Chancelor J. Bennett, Darius Scott, Dwayne Verner, Kevin K. Rhomberg, Nate Fox, Nico Segal                                                </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange feat. TInashe                          </v>
+        <v xml:space="preserve">Chance the Rapper feat. Knox Fortune                       </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:57 </v>
+        <v xml:space="preserve">03:41 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1411,28 +1595,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Seven Hours, Pt. 1              </v>
+        <v xml:space="preserve">Handsome                         </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes / Benny Revival                                                                                 </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Darian Garcia, Dex Coleman, Megan Pete, Peter Wilkins, Pink Sweats, TrapMoneyBenny                                                           </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange deat. Benny Revival                    </v>
+        <v xml:space="preserve">Chance the Rapper feat. Megan Thee Stallion                </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:40 </v>
+        <v xml:space="preserve">02:53 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1451,28 +1635,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Take It Back                    </v>
+        <v xml:space="preserve">Big Fish                         </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Arca / Russell Boring / Alejandro Ghersi / Devonte Hynes / Joba                                               </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Radric Davis, Tim Mosley                                                                                                                     </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange feat. Arca, Joba, Justine Skye         </v>
+        <v xml:space="preserve">Chance the Rapper                                          </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:22 </v>
+        <v xml:space="preserve">03:06 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1491,28 +1675,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Happiness                       </v>
+        <v xml:space="preserve">Ballin Flossin                   </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes                                                                                                 </v>
+        <v xml:space="preserve"> Chancelor J. Bennett,Darius Scott, Greg Landfair, Keith Edward Crouch, Kevin James, Nate Fox, Peter Wilkins, Darius Scott Harris, Shawn Mendes                     </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange                                        </v>
+        <v xml:space="preserve">Chance the Rapper feat. Gucci Mane                         </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:09 </v>
+        <v xml:space="preserve">02:49 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1531,28 +1715,28 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Today                           </v>
+        <v xml:space="preserve">4 Quarters in the Black (Skit)   </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Devonte Hynes                                                                                                 </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Colleen Mares                                                                                                                                </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Blood Orange                                        </v>
+        <v xml:space="preserve">Chance the Rapper                                          </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:19 </v>
+        <v xml:space="preserve">02:13 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1564,35 +1748,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">5 Year Plan                      </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                               </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Darius Scott, Francis Starlite, Gabe Jaskowiak, Jordan Ware, Macie Stewart, Nate Fox, Peter Wilkins, Randy Newman                            </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                    </v>
+        <v xml:space="preserve">Chance the Rapper feat. Randy Newman                       </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:17 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1604,35 +1788,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">Get a Bag                        </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                               </v>
+        <v xml:space="preserve"> Calvin Woods, Chancelor J. Bennett, James Taylor, Nate Fox, Peter Losnegard, Peter Wilkins                                                                         </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                    </v>
+        <v xml:space="preserve">Chance the Rapper deat. Calboy                             </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:21 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1644,35 +1828,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">Slide Around                     </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                               </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Durk Banks, Nate Fox, Onika Maraj, Pi'erre Bourne                                                                                            </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                    </v>
+        <v xml:space="preserve">Chance the Rapper feat. Lil Durk, Nicki Minaj              </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:30 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1684,35 +1868,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">Sun Come Down                    </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                               </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Darian Garcia, Darius Scott, Dwayne Verner, Eric Butler, Gabe Jaskowiak, Nate Fox, Nico Segal, Peter Wilkins, Ryan Vojtesak                  </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                    </v>
+        <v xml:space="preserve">Chance the Rapper                                          </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:35 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1724,35 +1908,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v>Found a Good One (Single No More)</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                               </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Darius Sjascott, Dwayne Verner, Greg Landfair, Lisa Mishra, Nate Fox, Nico Segal, Peter Wilkins, SWV, Shane Lee Lindstrom                    </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                    </v>
+        <v xml:space="preserve">Chance the Rapper feat. SWV, Pretty Vee                    </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:18 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -1764,35 +1948,35 @@
       </c>
       <c r="B24">
         <f>Sheet1!A21</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">Town on the Hill                 </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                               </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Francis Starlite, Justin Vernon, Peter Wilkins                                                                                               </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                    </v>
+        <v xml:space="preserve">Chance the Rapper                                          </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="3" t="str">
         <f>TEXT(Sheet1!E21,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:59 </v>
       </c>
       <c r="K24" s="4" t="s">
         <v>0</v>
@@ -1804,35 +1988,35 @@
       </c>
       <c r="B25">
         <f>Sheet1!A22</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                </v>
+        <v xml:space="preserve">Our House (Skit)                 </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                               </v>
+        <v xml:space="preserve"> Chancelor J. Bennett, Colleen Mares                                                                                                                                </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                    </v>
+        <v xml:space="preserve">Chance the Rapper                                          </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J25" s="3" t="str">
         <f>TEXT(Sheet1!E22,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">01:05 </v>
       </c>
       <c r="K25" s="4" t="s">
         <v>0</v>
@@ -1856,9 +2040,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="49.77734375" customWidth="1"/>
+    <col min="4" max="4" width="56.21875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1887,7 +2071,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>5.1388888888888894E-2</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1901,10 +2085,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>3.5416666666666666E-2</v>
+        <v>0.16388888888888889</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1912,16 +2096,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.10625</v>
+        <v>0.16874999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1929,16 +2113,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
-        <v>0.10416666666666667</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1946,16 +2130,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
-        <v>6.458333333333334E-2</v>
+        <v>0.2076388888888889</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1963,16 +2147,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2">
-        <v>9.8611111111111108E-2</v>
+        <v>0.19513888888888889</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1980,16 +2164,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2">
-        <v>0.12291666666666667</v>
+        <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1997,16 +2181,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.11875000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2014,16 +2198,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2">
-        <v>8.1944444444444445E-2</v>
+        <v>0.16805555555555554</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2031,16 +2215,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
-        <v>0.12291666666666667</v>
+        <v>0.15347222222222223</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2048,16 +2232,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1111111111111111</v>
+        <v>0.12013888888888889</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2065,16 +2249,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2">
-        <v>0.18194444444444444</v>
+        <v>0.12916666666666668</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2082,16 +2266,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="E14" s="2">
-        <v>8.9583333333333334E-2</v>
+        <v>0.1173611111111111</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2099,55 +2283,167 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E15" s="2">
-        <v>5.486111111111111E-2</v>
+        <v>9.2361111111111116E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="5:5">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="5:5">
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="5:5">
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="5:5">
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="5:5">
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="5:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.17847222222222223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.13958333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.1875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14930555555555555</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.17916666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.12430555555555556</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.22430555555555556</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="5:5">
+    <row r="25" spans="1:5">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="5:5">
+    <row r="26" spans="1:5">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="5:5">
+    <row r="27" spans="1:5">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="5:5">
+    <row r="28" spans="1:5">
       <c r="E28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 06092220 added 2 old revies
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,11 +17,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="chancetherapper3" localSheetId="0">Sheet1!$A$1:$E$23</definedName>
-    <definedName name="chancetherapper3" localSheetId="2">Sheet3!$A$1:$E$23</definedName>
+    <definedName name="espalding3" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
+    <definedName name="espalding3" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/chancetherapper3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/espalding3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/chancetherapper3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/espalding3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="26">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,178 +72,64 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>All Day Long</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Darius Scott, Dwayne Verner, Jr., Greg Landfair, Nate Fox, Nico Segal, Peter Wilkins</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. John Legend</t>
-  </si>
-  <si>
-    <t>Do You Remember</t>
-  </si>
-  <si>
-    <t>Benjamin Gibbard, Chancelor, J. Bennett, Dwayne Verner, Eric Butler, Francis Starlite, Garren Langford, Justin Vernon, Nate Fox, Nico Segal, Peter Wilkins</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Death Cab for Cutie</t>
-  </si>
-  <si>
-    <t>Eternal</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Christopher Smith, Jr, .Darian Garcia, Darius Scott, Garren Langford, Greg Landfair, Ken Bennett</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Smino</t>
-  </si>
-  <si>
-    <t>Hot Shower</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Darian Garcia, Jonathan L. Kirk, Malcolm Jamaal Davis</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Madein TYO, DaBaby</t>
-  </si>
-  <si>
-    <t>We Go High</t>
-  </si>
-  <si>
-    <t>Ben Lusher, Chancelor J. Bennett, Darius Scott, Mike Servin, Nate Fox, Nico Segal, Peter Wilkins</t>
-  </si>
-  <si>
-    <t>Chance the Rapper</t>
-  </si>
-  <si>
-    <t>I Got You (Always and Forever)</t>
-  </si>
-  <si>
-    <t>Carter Lang, Chancelor J. Bennett, Courtney Shanade Salter, Dwayne Verner, En Vogue, Eric Butler, Garren Langford, Kierra Sheard, Nate Fox, Peter Wilkins</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. En Vogue, Ari Lennox, Kierra Sheard</t>
-  </si>
-  <si>
-    <t>Photo Ops (Skit)</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Colleen Mares</t>
-  </si>
-  <si>
-    <t>Roo</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, CocoRosie, Taylor Bennett</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Taylor Bennett, CocoRosie</t>
-  </si>
-  <si>
-    <t>The Big Day</t>
-  </si>
-  <si>
-    <t>Carter Lang, Chancelor J. Bennett, Darius Scott, Francis Starlite, James Cleveland, Joe Rainey Sr., John Stephens, Justin Vernon, Nico Segal, Peter Wilkins</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Francis and the Lights</t>
-  </si>
-  <si>
-    <t>Let's Go on the Run</t>
-  </si>
-  <si>
-    <t>Ben Lusher, Carter Lang, Chancelor J. Bennett, Darius Scott, Dwayne Verner, Kevin K. Rhomberg, Nate Fox, Nico Segal</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Knox Fortune</t>
-  </si>
-  <si>
-    <t>Handsome</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Darian Garcia, Dex Coleman, Megan Pete, Peter Wilkins, Pink Sweats, TrapMoneyBenny</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Megan Thee Stallion</t>
-  </si>
-  <si>
-    <t>Big Fish</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Radric Davis, Tim Mosley</t>
-  </si>
-  <si>
-    <t>Ballin Flossin</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett,Darius Scott, Greg Landfair, Keith Edward Crouch, Kevin James, Nate Fox, Peter Wilkins, Darius Scott Harris, Shawn Mendes</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Gucci Mane</t>
-  </si>
-  <si>
-    <t>4 Quarters in the Black (Skit)</t>
-  </si>
-  <si>
-    <t>5 Year Plan</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Darius Scott, Francis Starlite, Gabe Jaskowiak, Jordan Ware, Macie Stewart, Nate Fox, Peter Wilkins, Randy Newman</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Randy Newman</t>
-  </si>
-  <si>
-    <t>Get a Bag</t>
-  </si>
-  <si>
-    <t>Calvin Woods, Chancelor J. Bennett, James Taylor, Nate Fox, Peter Losnegard, Peter Wilkins</t>
-  </si>
-  <si>
-    <t>Chance the Rapper deat. Calboy</t>
-  </si>
-  <si>
-    <t>Slide Around</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Durk Banks, Nate Fox, Onika Maraj, Pi'erre Bourne</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Lil Durk, Nicki Minaj</t>
-  </si>
-  <si>
-    <t>Sun Come Down</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Darian Garcia, Darius Scott, Dwayne Verner, Eric Butler, Gabe Jaskowiak, Nate Fox, Nico Segal, Peter Wilkins, Ryan Vojtesak</t>
-  </si>
-  <si>
-    <t>Found a Good One (Single No More)</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Darius Sjascott, Dwayne Verner, Greg Landfair, Lisa Mishra, Nate Fox, Nico Segal, Peter Wilkins, SWV, Shane Lee Lindstrom</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. SWV, Pretty Vee</t>
-  </si>
-  <si>
-    <t>Town on the Hill</t>
-  </si>
-  <si>
-    <t>Chancelor J. Bennett, Francis Starlite, Justin Vernon, Peter Wilkins</t>
-  </si>
-  <si>
-    <t>Our House (Skit)</t>
-  </si>
-  <si>
-    <t>Zanies and Fools</t>
-  </si>
-  <si>
-    <t>Carter Lang, Chancelor J. Bennett, Darius Scott, Dwayne Verner, Greg Landfair, Nate Fox, Nico Segal, Onika Maraj, Oscar Hammerstein, Peter Wilkins, Richard Rodgers</t>
-  </si>
-  <si>
-    <t>Chance the Rapper feat. Scott, Nicki Mina</t>
+    <t>12 Little Spells</t>
+  </si>
+  <si>
+    <t>Esperanza Spalding</t>
+  </si>
+  <si>
+    <t>To Tide Us over</t>
+  </si>
+  <si>
+    <t>Esperanza Spalding / Justin Tyson</t>
+  </si>
+  <si>
+    <t>Til the Next</t>
+  </si>
+  <si>
+    <t>Thang</t>
+  </si>
+  <si>
+    <t>Touch in Mine</t>
+  </si>
+  <si>
+    <t>The Longing Deep Down</t>
+  </si>
+  <si>
+    <t>You Have to Dance</t>
+  </si>
+  <si>
+    <t>Now Know</t>
+  </si>
+  <si>
+    <t>All Limbs Are</t>
+  </si>
+  <si>
+    <t>Readying to Rise</t>
+  </si>
+  <si>
+    <t>Dancing the Animal</t>
+  </si>
+  <si>
+    <t>With Others</t>
+  </si>
+  <si>
+    <t>Lest We Forget</t>
+  </si>
+  <si>
+    <t>How to</t>
+  </si>
+  <si>
+    <t>Morgan Guerin / Esperanza Spalding</t>
+  </si>
+  <si>
+    <t>Move Many</t>
+  </si>
+  <si>
+    <t>Esperanza Spalding / Matthew Stevens</t>
+  </si>
+  <si>
+    <t>Ways Together</t>
   </si>
 </sst>
 </file>
@@ -339,11 +224,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="chancetherapper3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="espalding3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="chancetherapper3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="espalding3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -652,9 +537,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="56.21875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -680,10 +565,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14444444444444446</v>
+        <v>0.20347222222222219</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -691,16 +576,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16388888888888889</v>
+        <v>0.20347222222222219</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -708,16 +593,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.17847222222222223</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -725,16 +610,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>0.15625</v>
+        <v>0.19097222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -742,16 +627,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
-        <v>0.2076388888888889</v>
+        <v>0.20347222222222219</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -759,16 +644,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19513888888888889</v>
+        <v>0.19097222222222221</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -776,16 +661,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>5.2083333333333336E-2</v>
+        <v>0.14375000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -793,16 +678,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2">
-        <v>0.11875000000000001</v>
+        <v>0.18472222222222223</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -810,16 +695,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
-        <v>0.16805555555555554</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -827,16 +712,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.21319444444444444</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -844,16 +729,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12013888888888889</v>
+        <v>0.21319444444444444</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -861,16 +746,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E13" s="2">
-        <v>0.12916666666666668</v>
+        <v>0.24444444444444446</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -878,16 +763,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2">
-        <v>0.1173611111111111</v>
+        <v>0.21944444444444444</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -895,16 +780,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E15" s="2">
-        <v>9.2361111111111116E-2</v>
+        <v>0.16250000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -912,16 +797,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="E16" s="2">
-        <v>0.17847222222222223</v>
+        <v>0.12152777777777778</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -929,119 +814,35 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E17" s="2">
-        <v>0.13958333333333334</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.1875</v>
-      </c>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14930555555555555</v>
-      </c>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.17916666666666667</v>
-      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.12430555555555556</v>
-      </c>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2">
-        <v>4.5138888888888888E-2</v>
-      </c>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.22430555555555556</v>
-      </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="E24" s="2"/>
@@ -1069,7 +870,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="K20" sqref="A3:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -1089,15 +890,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -1117,21 +918,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                            </v>
+        <v xml:space="preserve"> Title                </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                         </v>
+        <v xml:space="preserve"> Composers                          </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                                  </v>
+        <v xml:space="preserve"> Performer         </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1156,21 +957,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------------------- </v>
+        <v xml:space="preserve">--------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------ </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1195,28 +996,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">All Day Long                     </v>
+        <v xml:space="preserve">12 Little Spells     </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Darius Scott, Dwayne Verner, Jr., Greg Landfair, Nate Fox, Nico Segal, Peter Wilkins                                                         </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. John Legend                        </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:28 </v>
+        <v xml:space="preserve">04:53 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1235,28 +1036,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Do You Remember                  </v>
+        <v xml:space="preserve">To Tide Us over      </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Benjamin Gibbard, Chancelor, J. Bennett, Dwayne Verner, Eric Butler, Francis Starlite, Garren Langford, Justin Vernon, Nate Fox, Nico Segal, Peter Wilkins         </v>
+        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Death Cab for Cutie                </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:56 </v>
+        <v xml:space="preserve">04:53 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1275,28 +1076,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Eternal                          </v>
+        <v xml:space="preserve">Til the Next         </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Christopher Smith, Jr, .Darian Garcia, Darius Scott, Garren Langford, Greg Landfair, Ken Bennett                                             </v>
+        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Smino                              </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:03 </v>
+        <v xml:space="preserve">04:17 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1315,28 +1116,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hot Shower                       </v>
+        <v xml:space="preserve">Thang                </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Darian Garcia, Jonathan L. Kirk, Malcolm Jamaal Davis                                                                                        </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Madein TYO, DaBaby                 </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:45 </v>
+        <v xml:space="preserve">04:35 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1355,28 +1156,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">We Go High                       </v>
+        <v xml:space="preserve">Touch in Mine        </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Lusher, Chancelor J. Bennett, Darius Scott, Mike Servin, Nate Fox, Nico Segal, Peter Wilkins                                                                   </v>
+        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper                                          </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:59 </v>
+        <v xml:space="preserve">04:53 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1395,28 +1196,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I Got You (Always and Forever)   </v>
+        <v>The Longing Deep Down</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Carter Lang, Chancelor J. Bennett, Courtney Shanade Salter, Dwayne Verner, En Vogue, Eric Butler, Garren Langford, Kierra Sheard, Nate Fox, Peter Wilkins          </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Chance the Rapper feat. En Vogue, Ari Lennox, Kierra Sheard</v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:41 </v>
+        <v xml:space="preserve">04:35 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1435,28 +1236,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Photo Ops (Skit)                 </v>
+        <v xml:space="preserve">You Have to Dance    </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Colleen Mares                                                                                                                                </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper                                          </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:15 </v>
+        <v xml:space="preserve">03:27 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1475,28 +1276,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Roo                              </v>
+        <v xml:space="preserve">Now Know             </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, CocoRosie, Taylor Bennett                                                                                                                    </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Taylor Bennett, CocoRosie          </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:51 </v>
+        <v xml:space="preserve">04:26 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1515,28 +1316,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Big Day                      </v>
+        <v xml:space="preserve">All Limbs Are        </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Carter Lang, Chancelor J. Bennett, Darius Scott, Francis Starlite, James Cleveland, Joe Rainey Sr., John Stephens, Justin Vernon, Nico Segal, Peter Wilkins        </v>
+        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Francis and the Lights             </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:02 </v>
+        <v xml:space="preserve">03:36 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1555,28 +1356,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Let's Go on the Run              </v>
+        <v xml:space="preserve">Readying to Rise     </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Lusher, Carter Lang, Chancelor J. Bennett, Darius Scott, Dwayne Verner, Kevin K. Rhomberg, Nate Fox, Nico Segal                                                </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Knox Fortune                       </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:41 </v>
+        <v xml:space="preserve">05:07 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1595,28 +1396,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Handsome                         </v>
+        <v xml:space="preserve">Dancing the Animal   </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Darian Garcia, Dex Coleman, Megan Pete, Peter Wilkins, Pink Sweats, TrapMoneyBenny                                                           </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Megan Thee Stallion                </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:53 </v>
+        <v xml:space="preserve">05:07 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1635,28 +1436,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Big Fish                         </v>
+        <v xml:space="preserve">With Others          </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Radric Davis, Tim Mosley                                                                                                                     </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper                                          </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:06 </v>
+        <v xml:space="preserve">05:52 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1675,28 +1476,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ballin Flossin                   </v>
+        <v xml:space="preserve">Lest We Forget       </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett,Darius Scott, Greg Landfair, Keith Edward Crouch, Kevin James, Nate Fox, Peter Wilkins, Darius Scott Harris, Shawn Mendes                     </v>
+        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Gucci Mane                         </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:49 </v>
+        <v xml:space="preserve">05:16 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1715,28 +1516,28 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">4 Quarters in the Black (Skit)   </v>
+        <v xml:space="preserve">How to               </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Colleen Mares                                                                                                                                </v>
+        <v xml:space="preserve"> Morgan Guerin / Esperanza Spalding  </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper                                          </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:13 </v>
+        <v xml:space="preserve">03:54 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1755,28 +1556,28 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">5 Year Plan                      </v>
+        <v xml:space="preserve">Move Many            </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Darius Scott, Francis Starlite, Gabe Jaskowiak, Jordan Ware, Macie Stewart, Nate Fox, Peter Wilkins, Randy Newman                            </v>
+        <v xml:space="preserve"> Esperanza Spalding / Matthew Stevens</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Randy Newman                       </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:17 </v>
+        <v xml:space="preserve">02:55 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1795,28 +1596,28 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Get a Bag                        </v>
+        <v xml:space="preserve">Ways Together        </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Calvin Woods, Chancelor J. Bennett, James Taylor, Nate Fox, Peter Losnegard, Peter Wilkins                                                                         </v>
+        <v xml:space="preserve"> Esperanza Spalding                  </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper deat. Calboy                             </v>
+        <v>Esperanza Spalding</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:21 </v>
+        <v xml:space="preserve">03:45 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1828,35 +1629,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Slide Around                     </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Durk Banks, Nate Fox, Onika Maraj, Pi'erre Bourne                                                                                            </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. Lil Durk, Nicki Minaj              </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:30 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1868,35 +1669,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sun Come Down                    </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Darian Garcia, Darius Scott, Dwayne Verner, Eric Butler, Gabe Jaskowiak, Nate Fox, Nico Segal, Peter Wilkins, Ryan Vojtesak                  </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper                                          </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:35 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1908,35 +1709,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Found a Good One (Single No More)</v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Darius Sjascott, Dwayne Verner, Greg Landfair, Lisa Mishra, Nate Fox, Nico Segal, Peter Wilkins, SWV, Shane Lee Lindstrom                    </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper feat. SWV, Pretty Vee                    </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:18 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -1948,35 +1749,35 @@
       </c>
       <c r="B24">
         <f>Sheet1!A21</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Town on the Hill                 </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Francis Starlite, Justin Vernon, Peter Wilkins                                                                                               </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper                                          </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="3" t="str">
         <f>TEXT(Sheet1!E21,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:59 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K24" s="4" t="s">
         <v>0</v>
@@ -1988,35 +1789,35 @@
       </c>
       <c r="B25">
         <f>Sheet1!A22</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Our House (Skit)                 </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chancelor J. Bennett, Colleen Mares                                                                                                                                </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chance the Rapper                                          </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J25" s="3" t="str">
         <f>TEXT(Sheet1!E22,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:05 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K25" s="4" t="s">
         <v>0</v>
@@ -2040,9 +1841,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="33.77734375" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="56.21875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2068,10 +1869,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14444444444444446</v>
+        <v>0.20347222222222219</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2079,16 +1880,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16388888888888889</v>
+        <v>0.20347222222222219</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2096,16 +1897,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.17847222222222223</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2113,16 +1914,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>0.15625</v>
+        <v>0.19097222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2130,16 +1931,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
-        <v>0.2076388888888889</v>
+        <v>0.20347222222222219</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2147,16 +1948,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19513888888888889</v>
+        <v>0.19097222222222221</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2164,16 +1965,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>5.2083333333333336E-2</v>
+        <v>0.14375000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2181,16 +1982,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2">
-        <v>0.11875000000000001</v>
+        <v>0.18472222222222223</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2198,16 +1999,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
-        <v>0.16805555555555554</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2215,16 +2016,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.21319444444444444</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2232,16 +2033,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12013888888888889</v>
+        <v>0.21319444444444444</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2249,16 +2050,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E13" s="2">
-        <v>0.12916666666666668</v>
+        <v>0.24444444444444446</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2266,16 +2067,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2">
-        <v>0.1173611111111111</v>
+        <v>0.21944444444444444</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2283,16 +2084,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E15" s="2">
-        <v>9.2361111111111116E-2</v>
+        <v>0.16250000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2300,16 +2101,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="E16" s="2">
-        <v>0.17847222222222223</v>
+        <v>0.12152777777777778</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2317,119 +2118,35 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E17" s="2">
-        <v>0.13958333333333334</v>
+        <v>0.15625</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.1875</v>
-      </c>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14930555555555555</v>
-      </c>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.17916666666666667</v>
-      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.12430555555555556</v>
-      </c>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2">
-        <v>4.5138888888888888E-2</v>
-      </c>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.22430555555555556</v>
-      </c>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="E24" s="2"/>

</xml_diff>

<commit_message>
feat; added 2 old reviews 06120000
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="espalding3" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
-    <definedName name="espalding3" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
+    <definedName name="common9" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="common9" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/espalding3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/common9.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/espalding3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/common9.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="40">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -69,67 +69,109 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Title/Composer</t>
-  </si>
-  <si>
-    <t>12 Little Spells</t>
-  </si>
-  <si>
-    <t>Esperanza Spalding</t>
-  </si>
-  <si>
-    <t>To Tide Us over</t>
-  </si>
-  <si>
-    <t>Esperanza Spalding / Justin Tyson</t>
-  </si>
-  <si>
-    <t>Til the Next</t>
-  </si>
-  <si>
-    <t>Thang</t>
-  </si>
-  <si>
-    <t>Touch in Mine</t>
-  </si>
-  <si>
-    <t>The Longing Deep Down</t>
-  </si>
-  <si>
-    <t>You Have to Dance</t>
-  </si>
-  <si>
-    <t>Now Know</t>
-  </si>
-  <si>
-    <t>All Limbs Are</t>
-  </si>
-  <si>
-    <t>Readying to Rise</t>
-  </si>
-  <si>
-    <t>Dancing the Animal</t>
-  </si>
-  <si>
-    <t>With Others</t>
-  </si>
-  <si>
-    <t>Lest We Forget</t>
-  </si>
-  <si>
-    <t>How to</t>
-  </si>
-  <si>
-    <t>Morgan Guerin / Esperanza Spalding</t>
-  </si>
-  <si>
-    <t>Move Many</t>
-  </si>
-  <si>
-    <t>Esperanza Spalding / Matthew Stevens</t>
-  </si>
-  <si>
-    <t>Ways Together</t>
+    <t xml:space="preserve"> No.</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Composer</t>
+  </si>
+  <si>
+    <t>Good Morning Love</t>
+  </si>
+  <si>
+    <t>Lonnie Lynn / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common feat. Samora Pinderhughes</t>
+  </si>
+  <si>
+    <t>Her Love</t>
+  </si>
+  <si>
+    <t>Andwele Gardner / Lonnie Lynn / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis / Lauren Wood</t>
+  </si>
+  <si>
+    <t>Common feat. Daniel Caesar</t>
+  </si>
+  <si>
+    <t>Dwele's Interlude</t>
+  </si>
+  <si>
+    <t>Andwele Gardner / Samora Pinderhughes / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Hercules</t>
+  </si>
+  <si>
+    <t>Kasseem Dean / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common feat. Swizz Beatz</t>
+  </si>
+  <si>
+    <t>Fifth Story</t>
+  </si>
+  <si>
+    <t>Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common feat. Leikeli47</t>
+  </si>
+  <si>
+    <t>Forever Your Love</t>
+  </si>
+  <si>
+    <t>BJ the Chicago Kid / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Isaiah Sharkey / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common feat. BJ The Chiago Kid</t>
+  </si>
+  <si>
+    <t>Leaders (Crib Love)</t>
+  </si>
+  <si>
+    <t>Lonnie Lynn / Alain Macklovitch / Samora Pinderhughes / Karriem Riggins / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common feat. A-Tank</t>
+  </si>
+  <si>
+    <t>Memories of Home</t>
+  </si>
+  <si>
+    <t>BJ the Chicago Kid / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common feat. BJ The Chiago Kid, Samora Pinderhughes</t>
+  </si>
+  <si>
+    <t>Show Me That You Love</t>
+  </si>
+  <si>
+    <t>Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Jill Scott / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common feat. Jill Scott, Samora Pinderhughes</t>
+  </si>
+  <si>
+    <t>My Fancy Free Future Love</t>
+  </si>
+  <si>
+    <t>Ron Brown / Lonnie Lynn / Nicholas Payton / Karriem Riggins / Isaiah Sharkey</t>
+  </si>
+  <si>
+    <t>God Is Love</t>
+  </si>
+  <si>
+    <t>Leon Bridges / Lonnie Lynn / Jonathan McReynolds / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis</t>
+  </si>
+  <si>
+    <t>Common feat. Leon Bridges, Jonathan McReynolds</t>
   </si>
 </sst>
 </file>
@@ -224,11 +266,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="espalding3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="common9" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="espalding3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="common9" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,16 +578,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="51.5546875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -559,16 +607,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>0.20347222222222219</v>
+        <v>0.2298611111111111</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -576,16 +624,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>0.20347222222222219</v>
+        <v>0.18680555555555556</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -593,16 +641,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17847222222222223</v>
+        <v>4.7916666666666663E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -610,16 +658,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
-        <v>0.19097222222222221</v>
+        <v>0.12083333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -627,16 +675,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2">
-        <v>0.20347222222222219</v>
+        <v>0.22083333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -644,16 +692,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19097222222222221</v>
+        <v>0.15208333333333332</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -661,16 +709,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2">
-        <v>0.14375000000000002</v>
+        <v>0.15347222222222223</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -678,16 +726,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2">
-        <v>0.18472222222222223</v>
+        <v>0.17222222222222225</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -695,16 +743,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2">
-        <v>0.15</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -712,16 +760,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2">
-        <v>0.21319444444444444</v>
+        <v>0.18124999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -729,134 +777,65 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2">
-        <v>0.21319444444444444</v>
+        <v>0.16458333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.24444444444444446</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.21944444444444444</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.16250000000000001</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.12152777777777778</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.15625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="5:5">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="5:5">
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="5:5">
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="5:5">
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="5:5">
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="5:5">
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="5:5">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="5:5">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="5:5">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="5:5">
       <c r="E28" s="2"/>
     </row>
   </sheetData>
@@ -870,7 +849,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="A3:K20"/>
+      <selection activeCell="K15" sqref="A3:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -890,15 +869,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -918,21 +897,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                </v>
+        <v xml:space="preserve"> Title                    </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                          </v>
+        <v xml:space="preserve"> Composers                                                                                                              </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer         </v>
+        <v xml:space="preserve"> Performer                                          </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -957,21 +936,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------- </v>
+        <v xml:space="preserve">------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------ </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------ </v>
+        <v xml:space="preserve"> --------------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -996,28 +975,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">12 Little Spells     </v>
+        <v xml:space="preserve">Good Morning Love        </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve"> Lonnie Lynn / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis                                     </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common feat. Samora Pinderhughes                   </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:53 </v>
+        <v xml:space="preserve">05:31 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1036,28 +1015,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">To Tide Us over      </v>
+        <v xml:space="preserve">Her Love                 </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
+        <v xml:space="preserve"> Andwele Gardner / Lonnie Lynn / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis / Lauren Wood     </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common feat. Daniel Caesar                         </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:53 </v>
+        <v xml:space="preserve">04:29 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1076,28 +1055,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Til the Next         </v>
+        <v xml:space="preserve">Dwele's Interlude        </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
+        <v xml:space="preserve"> Andwele Gardner / Samora Pinderhughes / Burniss Travis                                                                  </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common                                             </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:17 </v>
+        <v xml:space="preserve">01:09 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1116,28 +1095,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Thang                </v>
+        <v xml:space="preserve">Hercules                 </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve"> Kasseem Dean / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis                                     </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common feat. Swizz Beatz                           </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:35 </v>
+        <v xml:space="preserve">02:54 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1156,28 +1135,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Touch in Mine        </v>
+        <v xml:space="preserve">Fifth Story              </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
+        <v xml:space="preserve"> Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis                                                    </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common feat. Leikeli47                             </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:53 </v>
+        <v xml:space="preserve">05:18 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1196,28 +1175,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>The Longing Deep Down</v>
+        <v xml:space="preserve">Forever Your Love        </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve"> BJ the Chicago Kid / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Isaiah Sharkey / Burniss Travis              </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common feat. BJ The Chiago Kid                     </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:35 </v>
+        <v xml:space="preserve">03:39 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1236,28 +1215,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">You Have to Dance    </v>
+        <v xml:space="preserve">Leaders (Crib Love)      </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve"> Lonnie Lynn / Alain Macklovitch / Samora Pinderhughes / Karriem Riggins / Burniss Travis                                </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common feat. A-Tank                                </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:27 </v>
+        <v xml:space="preserve">03:41 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1276,28 +1255,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Now Know             </v>
+        <v xml:space="preserve">Memories of Home         </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve"> BJ the Chicago Kid / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis                               </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v>Common feat. BJ The Chiago Kid, Samora Pinderhughes</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:26 </v>
+        <v xml:space="preserve">04:08 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1316,28 +1295,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">All Limbs Are        </v>
+        <v xml:space="preserve">Show Me That You Love    </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
+        <v xml:space="preserve"> Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Jill Scott / Burniss Travis                                       </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common feat. Jill Scott, Samora Pinderhughes       </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:36 </v>
+        <v xml:space="preserve">07:30 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1356,28 +1335,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Readying to Rise     </v>
+        <v>My Fancy Free Future Love</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve"> Ron Brown / Lonnie Lynn / Nicholas Payton / Karriem Riggins / Isaiah Sharkey                                            </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common                                             </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:07 </v>
+        <v xml:space="preserve">04:21 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1396,28 +1375,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dancing the Animal   </v>
+        <v xml:space="preserve">God Is Love              </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve"> Leon Bridges / Lonnie Lynn / Jonathan McReynolds / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">Common feat. Leon Bridges, Jonathan McReynolds     </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:07 </v>
+        <v xml:space="preserve">03:57 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1429,35 +1408,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">With Others          </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:52 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1469,35 +1448,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lest We Forget       </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding / Justin Tyson   </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:16 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1509,35 +1488,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">How to               </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Morgan Guerin / Esperanza Spalding  </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:54 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1549,35 +1528,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Move Many            </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding / Matthew Stevens</v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:55 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1589,35 +1568,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ways Together        </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Esperanza Spalding                  </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Esperanza Spalding</v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:45 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1636,21 +1615,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1676,21 +1655,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1716,21 +1695,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1756,21 +1735,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1796,21 +1775,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                                                                                                         </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                                   </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1840,16 +1819,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="51.5546875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1863,16 +1848,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>0.20347222222222219</v>
+        <v>0.2298611111111111</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1880,16 +1865,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>0.20347222222222219</v>
+        <v>0.18680555555555556</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1897,16 +1882,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17847222222222223</v>
+        <v>4.7916666666666663E-2</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1914,16 +1899,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
-        <v>0.19097222222222221</v>
+        <v>0.12083333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1931,16 +1916,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2">
-        <v>0.20347222222222219</v>
+        <v>0.22083333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1948,16 +1933,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19097222222222221</v>
+        <v>0.15208333333333332</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1965,16 +1950,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E8" s="2">
-        <v>0.14375000000000002</v>
+        <v>0.15347222222222223</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1982,16 +1967,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2">
-        <v>0.18472222222222223</v>
+        <v>0.17222222222222225</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1999,16 +1984,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="E10" s="2">
-        <v>0.15</v>
+        <v>0.3125</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2016,16 +2001,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2">
-        <v>0.21319444444444444</v>
+        <v>0.18124999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2033,134 +2018,65 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2">
-        <v>0.21319444444444444</v>
+        <v>0.16458333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.24444444444444446</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.21944444444444444</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.16250000000000001</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.12152777777777778</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.15625</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="5:5">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="5:5">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="5:5">
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="5:5">
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="5:5">
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="5:5">
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="5:5">
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="5:5">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="5:5">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="5:5">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="5:5">
       <c r="E28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="common9" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
-    <definedName name="common9" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
+    <definedName name="ellevarner2" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="ellevarner2" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/common9.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/ellevarner2.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/common9.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/ellevarner2.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="24">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -69,109 +69,61 @@
     <t>Time</t>
   </si>
   <si>
-    <t xml:space="preserve"> No.</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Composer</t>
-  </si>
-  <si>
-    <t>Good Morning Love</t>
-  </si>
-  <si>
-    <t>Lonnie Lynn / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common feat. Samora Pinderhughes</t>
-  </si>
-  <si>
-    <t>Her Love</t>
-  </si>
-  <si>
-    <t>Andwele Gardner / Lonnie Lynn / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis / Lauren Wood</t>
-  </si>
-  <si>
-    <t>Common feat. Daniel Caesar</t>
-  </si>
-  <si>
-    <t>Dwele's Interlude</t>
-  </si>
-  <si>
-    <t>Andwele Gardner / Samora Pinderhughes / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common</t>
-  </si>
-  <si>
-    <t>Hercules</t>
-  </si>
-  <si>
-    <t>Kasseem Dean / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common feat. Swizz Beatz</t>
-  </si>
-  <si>
-    <t>Fifth Story</t>
-  </si>
-  <si>
-    <t>Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common feat. Leikeli47</t>
-  </si>
-  <si>
-    <t>Forever Your Love</t>
-  </si>
-  <si>
-    <t>BJ the Chicago Kid / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Isaiah Sharkey / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common feat. BJ The Chiago Kid</t>
-  </si>
-  <si>
-    <t>Leaders (Crib Love)</t>
-  </si>
-  <si>
-    <t>Lonnie Lynn / Alain Macklovitch / Samora Pinderhughes / Karriem Riggins / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common feat. A-Tank</t>
-  </si>
-  <si>
-    <t>Memories of Home</t>
-  </si>
-  <si>
-    <t>BJ the Chicago Kid / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common feat. BJ The Chiago Kid, Samora Pinderhughes</t>
-  </si>
-  <si>
-    <t>Show Me That You Love</t>
-  </si>
-  <si>
-    <t>Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Jill Scott / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common feat. Jill Scott, Samora Pinderhughes</t>
-  </si>
-  <si>
-    <t>My Fancy Free Future Love</t>
-  </si>
-  <si>
-    <t>Ron Brown / Lonnie Lynn / Nicholas Payton / Karriem Riggins / Isaiah Sharkey</t>
-  </si>
-  <si>
-    <t>God Is Love</t>
-  </si>
-  <si>
-    <t>Leon Bridges / Lonnie Lynn / Jonathan McReynolds / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis</t>
-  </si>
-  <si>
-    <t>Common feat. Leon Bridges, Jonathan McReynolds</t>
+    <t>Title/Composer</t>
+  </si>
+  <si>
+    <t>Coffee on the Roof</t>
+  </si>
+  <si>
+    <t>Elle Varner / Jimmy Varner</t>
+  </si>
+  <si>
+    <t>Elle Varner</t>
+  </si>
+  <si>
+    <t>Pour Me</t>
+  </si>
+  <si>
+    <t>Olubowale Akintimehin / Elle Varner / Jimmy Varner</t>
+  </si>
+  <si>
+    <t>Elle Varner feat. Wale</t>
+  </si>
+  <si>
+    <t>1 to 10</t>
+  </si>
+  <si>
+    <t>Elle Varner / Jordan Ware</t>
+  </si>
+  <si>
+    <t>Wishing Well</t>
+  </si>
+  <si>
+    <t>Marlanna Evans / Elle Varner / Jimmy Varner</t>
+  </si>
+  <si>
+    <t>Elle Varner feat. Rapsody</t>
+  </si>
+  <si>
+    <t>Number One Song</t>
+  </si>
+  <si>
+    <t>Loving U Blind</t>
+  </si>
+  <si>
+    <t>Kinda Love</t>
+  </si>
+  <si>
+    <t>Stacy Barthe / Los Hendrix / L3gion / Elle Varner / Jordan Ware</t>
+  </si>
+  <si>
+    <t>Casanova</t>
+  </si>
+  <si>
+    <t>Be Encouraged</t>
+  </si>
+  <si>
+    <t>Nascent / Elle Varner / Jimmy Varner</t>
   </si>
 </sst>
 </file>
@@ -266,11 +218,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="common9" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ellevarner2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="common9" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ellevarner2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -578,22 +530,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="51.5546875" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="59.21875" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -607,16 +553,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.2298611111111111</v>
+        <v>0.18611111111111112</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -624,16 +570,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.18680555555555556</v>
+        <v>0.17083333333333331</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -641,16 +587,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>4.7916666666666663E-2</v>
+        <v>0.15694444444444444</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -658,16 +604,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>0.12083333333333333</v>
+        <v>0.18055555555555555</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -675,16 +621,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.22083333333333333</v>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -692,16 +638,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -709,16 +655,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.13472222222222222</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -726,16 +672,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17222222222222225</v>
+        <v>0.17430555555555557</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -743,51 +689,23 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.3125</v>
+        <v>0.13125000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.18124999999999999</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.16458333333333333</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="5"/>
@@ -849,7 +767,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="A3:K15"/>
+      <selection activeCell="A3" sqref="A3:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -869,15 +787,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -897,21 +815,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                    </v>
+        <v xml:space="preserve"> Title             </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                              </v>
+        <v xml:space="preserve"> Composers                                                     </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                          </v>
+        <v xml:space="preserve"> Performer                </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -936,21 +854,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------------- </v>
+        <v xml:space="preserve">------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> --------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> --------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -975,28 +893,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Good Morning Love        </v>
+        <v>Coffee on the Roof</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Lonnie Lynn / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis                                     </v>
+        <v xml:space="preserve"> Elle Varner / Jimmy Varner                                     </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common feat. Samora Pinderhughes                   </v>
+        <v xml:space="preserve">Elle Varner              </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:31 </v>
+        <v xml:space="preserve">04:28 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1015,28 +933,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Her Love                 </v>
+        <v xml:space="preserve">Pour Me           </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Andwele Gardner / Lonnie Lynn / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis / Lauren Wood     </v>
+        <v xml:space="preserve"> Olubowale Akintimehin / Elle Varner / Jimmy Varner             </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common feat. Daniel Caesar                         </v>
+        <v xml:space="preserve">Elle Varner feat. Wale   </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:29 </v>
+        <v xml:space="preserve">04:06 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1055,28 +973,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dwele's Interlude        </v>
+        <v xml:space="preserve">1 to 10           </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Andwele Gardner / Samora Pinderhughes / Burniss Travis                                                                  </v>
+        <v xml:space="preserve"> Elle Varner / Jordan Ware                                      </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common                                             </v>
+        <v xml:space="preserve">Elle Varner              </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:09 </v>
+        <v xml:space="preserve">03:46 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1095,28 +1013,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hercules                 </v>
+        <v xml:space="preserve">Wishing Well      </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kasseem Dean / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis                                     </v>
+        <v xml:space="preserve"> Marlanna Evans / Elle Varner / Jimmy Varner                    </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common feat. Swizz Beatz                           </v>
+        <v>Elle Varner feat. Rapsody</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:54 </v>
+        <v xml:space="preserve">04:20 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1135,28 +1053,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fifth Story              </v>
+        <v xml:space="preserve">Number One Song   </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis                                                    </v>
+        <v xml:space="preserve"> Elle Varner / Jimmy Varner                                     </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common feat. Leikeli47                             </v>
+        <v xml:space="preserve">Elle Varner              </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:18 </v>
+        <v xml:space="preserve">05:06 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1175,28 +1093,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Forever Your Love        </v>
+        <v xml:space="preserve">Loving U Blind    </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> BJ the Chicago Kid / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Isaiah Sharkey / Burniss Travis              </v>
+        <v xml:space="preserve"> Elle Varner / Jimmy Varner                                     </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common feat. BJ The Chiago Kid                     </v>
+        <v xml:space="preserve">Elle Varner              </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:39 </v>
+        <v xml:space="preserve">03:28 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1215,28 +1133,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Leaders (Crib Love)      </v>
+        <v xml:space="preserve">Kinda Love        </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Lonnie Lynn / Alain Macklovitch / Samora Pinderhughes / Karriem Riggins / Burniss Travis                                </v>
+        <v xml:space="preserve"> Stacy Barthe / Los Hendrix / L3gion / Elle Varner / Jordan Ware</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common feat. A-Tank                                </v>
+        <v xml:space="preserve">Elle Varner              </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:41 </v>
+        <v xml:space="preserve">03:14 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1255,28 +1173,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Memories of Home         </v>
+        <v xml:space="preserve">Casanova          </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> BJ the Chicago Kid / Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Burniss Travis                               </v>
+        <v xml:space="preserve"> Elle Varner                                                    </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Common feat. BJ The Chiago Kid, Samora Pinderhughes</v>
+        <v xml:space="preserve">Elle Varner              </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:08 </v>
+        <v xml:space="preserve">04:11 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1295,28 +1213,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Show Me That You Love    </v>
+        <v xml:space="preserve">Be Encouraged     </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Lonnie Lynn / Samora Pinderhughes / Karriem Riggins / Jill Scott / Burniss Travis                                       </v>
+        <v xml:space="preserve"> Nascent / Elle Varner / Jimmy Varner                           </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common feat. Jill Scott, Samora Pinderhughes       </v>
+        <v xml:space="preserve">Elle Varner              </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">07:30 </v>
+        <v xml:space="preserve">03:09 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1328,35 +1246,35 @@
       </c>
       <c r="B14">
         <f>Sheet1!A11</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>My Fancy Free Future Love</v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ron Brown / Lonnie Lynn / Nicholas Payton / Karriem Riggins / Isaiah Sharkey                                            </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common                                             </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:21 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1368,35 +1286,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">God Is Love              </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Leon Bridges / Lonnie Lynn / Jonathan McReynolds / Samora Pinderhughes / James Poyser / Karriem Riggins / Burniss Travis</v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Common feat. Leon Bridges, Jonathan McReynolds     </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:57 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1415,21 +1333,21 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
@@ -1455,21 +1373,21 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
@@ -1495,21 +1413,21 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
@@ -1535,21 +1453,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1575,21 +1493,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1615,21 +1533,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1655,21 +1573,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1695,21 +1613,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1735,21 +1653,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1775,21 +1693,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                         </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1819,22 +1737,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="51.5546875" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="59.21875" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1848,16 +1760,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.2298611111111111</v>
+        <v>0.18611111111111112</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1865,16 +1777,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.18680555555555556</v>
+        <v>0.17083333333333331</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1882,16 +1794,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>4.7916666666666663E-2</v>
+        <v>0.15694444444444444</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1899,16 +1811,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>0.12083333333333333</v>
+        <v>0.18055555555555555</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1916,16 +1828,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.22083333333333333</v>
+        <v>0.21249999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1933,16 +1845,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.14444444444444446</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1950,16 +1862,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.13472222222222222</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1967,16 +1879,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17222222222222225</v>
+        <v>0.17430555555555557</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1984,51 +1896,23 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.3125</v>
+        <v>0.13125000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.18124999999999999</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.16458333333333333</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" s="5"/>

</xml_diff>

<commit_message>
feat: 06132310 added best2018 , 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ellevarner2" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
-    <definedName name="ellevarner2" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
+    <definedName name="janellemonae3" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="janellemonae3" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/ellevarner2.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/janellemonae3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/ellevarner2.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/janellemonae3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="39">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,58 +72,103 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>Coffee on the Roof</t>
-  </si>
-  <si>
-    <t>Elle Varner / Jimmy Varner</t>
-  </si>
-  <si>
-    <t>Elle Varner</t>
-  </si>
-  <si>
-    <t>Pour Me</t>
-  </si>
-  <si>
-    <t>Olubowale Akintimehin / Elle Varner / Jimmy Varner</t>
-  </si>
-  <si>
-    <t>Elle Varner feat. Wale</t>
-  </si>
-  <si>
-    <t>1 to 10</t>
-  </si>
-  <si>
-    <t>Elle Varner / Jordan Ware</t>
-  </si>
-  <si>
-    <t>Wishing Well</t>
-  </si>
-  <si>
-    <t>Marlanna Evans / Elle Varner / Jimmy Varner</t>
-  </si>
-  <si>
-    <t>Elle Varner feat. Rapsody</t>
-  </si>
-  <si>
-    <t>Number One Song</t>
-  </si>
-  <si>
-    <t>Loving U Blind</t>
-  </si>
-  <si>
-    <t>Kinda Love</t>
-  </si>
-  <si>
-    <t>Stacy Barthe / Los Hendrix / L3gion / Elle Varner / Jordan Ware</t>
-  </si>
-  <si>
-    <t>Casanova</t>
-  </si>
-  <si>
-    <t>Be Encouraged</t>
-  </si>
-  <si>
-    <t>Nascent / Elle Varner / Jimmy Varner</t>
+    <t>Dirty Computer</t>
+  </si>
+  <si>
+    <t>Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nate "Rocket" Wonder</t>
+  </si>
+  <si>
+    <t>Janelle Monae feat, Brian Wilson</t>
+  </si>
+  <si>
+    <t>Crazy, Classic, Life</t>
+  </si>
+  <si>
+    <t>Charles Joseph II / Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nate "Rocket" Wonder</t>
+  </si>
+  <si>
+    <t>Janelle Monae</t>
+  </si>
+  <si>
+    <t>Take a Byte</t>
+  </si>
+  <si>
+    <t>Dr. Nathaniel Irvin III / John Webb Jr. / Janelle Monae Robinson / Nana Kwabena Tuffuor / Nate "Rocket" Wonder</t>
+  </si>
+  <si>
+    <t>Jane's Dream</t>
+  </si>
+  <si>
+    <t>Jon Brion</t>
+  </si>
+  <si>
+    <t>Screwed</t>
+  </si>
+  <si>
+    <t>Roman GianArthur / Charles Joseph II / Dr. Nathaniel Irvin III / Benjamin Hudson McIldowie / Janelle Monae Robinson</t>
+  </si>
+  <si>
+    <t>Janelle Monae feat. Zoe Kravitz</t>
+  </si>
+  <si>
+    <t>Django Jane</t>
+  </si>
+  <si>
+    <t>Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nana Kwabena Tuffuor</t>
+  </si>
+  <si>
+    <t>PYNK</t>
+  </si>
+  <si>
+    <t>Wynne Bennett / Charles Joseph II / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson</t>
+  </si>
+  <si>
+    <t>Janelle Monae feat. Grimes</t>
+  </si>
+  <si>
+    <t>Make Me Feel</t>
+  </si>
+  <si>
+    <t>Robin Fredriksson / Matt Friedman / Julia Michaels / Janelle Monae Robinson / Justin Tranter</t>
+  </si>
+  <si>
+    <t>I Got the Juice</t>
+  </si>
+  <si>
+    <t>Joshua Dean / Roman GianArthur / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson / Nana Kwabena Tuffuor / Pharrell Williams</t>
+  </si>
+  <si>
+    <t>Janelle Monae feat, Pharrell Williams</t>
+  </si>
+  <si>
+    <t>I Like That</t>
+  </si>
+  <si>
+    <t>Patrick Brown / Dr. Nathaniel Irvin III / Ray Murray / Taylor Parks / Janelle Monae Robinson / Rico Wade</t>
+  </si>
+  <si>
+    <t>Stevie's Dream</t>
+  </si>
+  <si>
+    <t>Roman GianArthur / Dr. Nathaniel Irvin III</t>
+  </si>
+  <si>
+    <t>Don't Judge Me</t>
+  </si>
+  <si>
+    <t>Joshua Dean / Roman GianArthur / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson</t>
+  </si>
+  <si>
+    <t>So Afraid</t>
+  </si>
+  <si>
+    <t>Dr. Nathaniel Irvin III / Janelle Monae Robinson</t>
+  </si>
+  <si>
+    <t>Americans</t>
+  </si>
+  <si>
+    <t>Charles Joseph II / Dr. Nathaniel Irvin III / John Webb Jr. / Janelle Monae Robinson</t>
   </si>
 </sst>
 </file>
@@ -218,11 +263,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ellevarner2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="janellemonae3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ellevarner2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="janellemonae3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,10 +575,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="59.21875" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -562,7 +607,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.18611111111111112</v>
+        <v>8.2638888888888887E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -579,7 +624,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.17083333333333331</v>
+        <v>0.1986111111111111</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -593,10 +638,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.17152777777777775</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -610,10 +655,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2">
-        <v>0.18055555555555555</v>
+        <v>1.2499999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -621,16 +666,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>0.21249999999999999</v>
+        <v>0.20972222222222223</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -638,16 +683,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
-        <v>0.14444444444444446</v>
+        <v>0.13194444444444445</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -655,16 +700,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -672,16 +717,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17430555555555557</v>
+        <v>0.13472222222222222</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -689,33 +734,102 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13125000000000001</v>
+        <v>0.15694444444444444</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="E11" s="2"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.1388888888888889</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.25208333333333333</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="B13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3.1944444444444449E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.16944444444444443</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.17083333333333331</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="E16" s="2"/>
@@ -767,7 +881,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K13"/>
+      <selection activeCell="K18" sqref="A3:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -787,15 +901,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>63</v>
+        <v>139</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -815,21 +929,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title             </v>
+        <v xml:space="preserve"> Title               </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                     </v>
+        <v xml:space="preserve"> Composers                                                                                                                                 </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                </v>
+        <v xml:space="preserve"> Performer                            </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -854,21 +968,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------ </v>
+        <v xml:space="preserve">-------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> --------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -893,28 +1007,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Coffee on the Roof</v>
+        <v xml:space="preserve">Dirty Computer      </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Elle Varner / Jimmy Varner                                     </v>
+        <v xml:space="preserve"> Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nate "Rocket" Wonder                                                                    </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Elle Varner              </v>
+        <v xml:space="preserve">Janelle Monae feat, Brian Wilson     </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:28 </v>
+        <v xml:space="preserve">01:59 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -933,28 +1047,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pour Me           </v>
+        <v>Crazy, Classic, Life</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Olubowale Akintimehin / Elle Varner / Jimmy Varner             </v>
+        <v xml:space="preserve"> Charles Joseph II / Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nate "Rocket" Wonder                                                </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Elle Varner feat. Wale   </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:06 </v>
+        <v xml:space="preserve">04:46 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -973,28 +1087,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">1 to 10           </v>
+        <v xml:space="preserve">Take a Byte         </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Elle Varner / Jordan Ware                                      </v>
+        <v xml:space="preserve"> Dr. Nathaniel Irvin III / John Webb Jr. / Janelle Monae Robinson / Nana Kwabena Tuffuor / Nate "Rocket" Wonder                             </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Elle Varner              </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:46 </v>
+        <v xml:space="preserve">04:07 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1013,28 +1127,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Wishing Well      </v>
+        <v xml:space="preserve">Jane's Dream        </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Marlanna Evans / Elle Varner / Jimmy Varner                    </v>
+        <v xml:space="preserve"> Jon Brion                                                                                                                                  </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Elle Varner feat. Rapsody</v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:20 </v>
+        <v xml:space="preserve">00:18 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1053,28 +1167,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Number One Song   </v>
+        <v xml:space="preserve">Screwed             </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Elle Varner / Jimmy Varner                                     </v>
+        <v xml:space="preserve"> Roman GianArthur / Charles Joseph II / Dr. Nathaniel Irvin III / Benjamin Hudson McIldowie / Janelle Monae Robinson                        </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Elle Varner              </v>
+        <v xml:space="preserve">Janelle Monae feat. Zoe Kravitz      </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:06 </v>
+        <v xml:space="preserve">05:02 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1093,28 +1207,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Loving U Blind    </v>
+        <v xml:space="preserve">Django Jane         </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Elle Varner / Jimmy Varner                                     </v>
+        <v xml:space="preserve"> Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nana Kwabena Tuffuor                                                                    </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Elle Varner              </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:28 </v>
+        <v xml:space="preserve">03:10 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1133,28 +1247,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Kinda Love        </v>
+        <v xml:space="preserve">PYNK                </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Stacy Barthe / Los Hendrix / L3gion / Elle Varner / Jordan Ware</v>
+        <v xml:space="preserve"> Wynne Bennett / Charles Joseph II / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson                                        </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Elle Varner              </v>
+        <v xml:space="preserve">Janelle Monae feat. Grimes           </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:14 </v>
+        <v xml:space="preserve">04:00 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1173,28 +1287,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Casanova          </v>
+        <v xml:space="preserve">Make Me Feel        </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Elle Varner                                                    </v>
+        <v xml:space="preserve"> Robin Fredriksson / Matt Friedman / Julia Michaels / Janelle Monae Robinson / Justin Tranter                                               </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Elle Varner              </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:11 </v>
+        <v xml:space="preserve">03:14 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1213,28 +1327,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Be Encouraged     </v>
+        <v xml:space="preserve">I Got the Juice     </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nascent / Elle Varner / Jimmy Varner                           </v>
+        <v xml:space="preserve"> Joshua Dean / Roman GianArthur / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson / Nana Kwabena Tuffuor / Pharrell Williams</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Elle Varner              </v>
+        <v>Janelle Monae feat, Pharrell Williams</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:09 </v>
+        <v xml:space="preserve">03:46 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1246,35 +1360,35 @@
       </c>
       <c r="B14">
         <f>Sheet1!A11</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">I Like That         </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve"> Patrick Brown / Dr. Nathaniel Irvin III / Ray Murray / Taylor Parks / Janelle Monae Robinson / Rico Wade                                   </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:20 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1286,35 +1400,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Stevie's Dream      </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve"> Roman GianArthur / Dr. Nathaniel Irvin III                                                                                                 </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">06:03 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1326,35 +1440,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Don't Judge Me      </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve"> Joshua Dean / Roman GianArthur / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson                                           </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">00:46 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1366,35 +1480,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">So Afraid           </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve"> Dr. Nathaniel Irvin III / Janelle Monae Robinson                                                                                           </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:04 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1406,35 +1520,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Americans           </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve"> Charles Joseph II / Dr. Nathaniel Irvin III / John Webb Jr. / Janelle Monae Robinson                                                       </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">Janelle Monae                        </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:06 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1453,21 +1567,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve">                                                                                                                                            </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1493,21 +1607,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve">                                                                                                                                            </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1533,21 +1647,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve">                                                                                                                                            </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1573,21 +1687,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve">                                                                                                                                            </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1613,21 +1727,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve">                                                                                                                                            </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1653,21 +1767,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve">                                                                                                                                            </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1693,21 +1807,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                </v>
+        <v xml:space="preserve">                                                                                                                                            </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1737,10 +1851,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="59.21875" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1769,7 +1883,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.18611111111111112</v>
+        <v>8.2638888888888887E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1786,7 +1900,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.17083333333333331</v>
+        <v>0.1986111111111111</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1800,10 +1914,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.17152777777777775</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1817,10 +1931,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2">
-        <v>0.18055555555555555</v>
+        <v>1.2499999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1828,16 +1942,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>0.21249999999999999</v>
+        <v>0.20972222222222223</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1845,16 +1959,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
-        <v>0.14444444444444446</v>
+        <v>0.13194444444444445</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1862,16 +1976,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1879,16 +1993,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17430555555555557</v>
+        <v>0.13472222222222222</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1896,33 +2010,102 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13125000000000001</v>
+        <v>0.15694444444444444</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="E11" s="2"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.1388888888888889</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.25208333333333333</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="B13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3.1944444444444449E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.16944444444444443</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.17083333333333331</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="E16" s="2"/>

</xml_diff>

<commit_message>
feat: 06142135 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="janellemonae3" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
-    <definedName name="janellemonae3" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
+    <definedName name="cardib1" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
+    <definedName name="cardib1" localSheetId="2">Sheet3!$A$1:$E$14</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/janellemonae3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/cardib1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/janellemonae3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/cardib1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="40">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,103 +72,106 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>Dirty Computer</t>
-  </si>
-  <si>
-    <t>Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nate "Rocket" Wonder</t>
-  </si>
-  <si>
-    <t>Janelle Monae feat, Brian Wilson</t>
-  </si>
-  <si>
-    <t>Crazy, Classic, Life</t>
-  </si>
-  <si>
-    <t>Charles Joseph II / Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nate "Rocket" Wonder</t>
-  </si>
-  <si>
-    <t>Janelle Monae</t>
-  </si>
-  <si>
-    <t>Take a Byte</t>
-  </si>
-  <si>
-    <t>Dr. Nathaniel Irvin III / John Webb Jr. / Janelle Monae Robinson / Nana Kwabena Tuffuor / Nate "Rocket" Wonder</t>
-  </si>
-  <si>
-    <t>Jane's Dream</t>
-  </si>
-  <si>
-    <t>Jon Brion</t>
-  </si>
-  <si>
-    <t>Screwed</t>
-  </si>
-  <si>
-    <t>Roman GianArthur / Charles Joseph II / Dr. Nathaniel Irvin III / Benjamin Hudson McIldowie / Janelle Monae Robinson</t>
-  </si>
-  <si>
-    <t>Janelle Monae feat. Zoe Kravitz</t>
-  </si>
-  <si>
-    <t>Django Jane</t>
-  </si>
-  <si>
-    <t>Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nana Kwabena Tuffuor</t>
-  </si>
-  <si>
-    <t>PYNK</t>
-  </si>
-  <si>
-    <t>Wynne Bennett / Charles Joseph II / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson</t>
-  </si>
-  <si>
-    <t>Janelle Monae feat. Grimes</t>
-  </si>
-  <si>
-    <t>Make Me Feel</t>
-  </si>
-  <si>
-    <t>Robin Fredriksson / Matt Friedman / Julia Michaels / Janelle Monae Robinson / Justin Tranter</t>
-  </si>
-  <si>
-    <t>I Got the Juice</t>
-  </si>
-  <si>
-    <t>Joshua Dean / Roman GianArthur / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson / Nana Kwabena Tuffuor / Pharrell Williams</t>
-  </si>
-  <si>
-    <t>Janelle Monae feat, Pharrell Williams</t>
-  </si>
-  <si>
-    <t>I Like That</t>
-  </si>
-  <si>
-    <t>Patrick Brown / Dr. Nathaniel Irvin III / Ray Murray / Taylor Parks / Janelle Monae Robinson / Rico Wade</t>
-  </si>
-  <si>
-    <t>Stevie's Dream</t>
-  </si>
-  <si>
-    <t>Roman GianArthur / Dr. Nathaniel Irvin III</t>
-  </si>
-  <si>
-    <t>Don't Judge Me</t>
-  </si>
-  <si>
-    <t>Joshua Dean / Roman GianArthur / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson</t>
-  </si>
-  <si>
-    <t>So Afraid</t>
-  </si>
-  <si>
-    <t>Dr. Nathaniel Irvin III / Janelle Monae Robinson</t>
-  </si>
-  <si>
-    <t>Americans</t>
-  </si>
-  <si>
-    <t>Charles Joseph II / Dr. Nathaniel Irvin III / John Webb Jr. / Janelle Monae Robinson</t>
+    <t>Get Up 10</t>
+  </si>
+  <si>
+    <t>Sean Allen / Belcalis Almanzar / Maurice Jordan / Jermaine Preyan / James SwanQo / Anthony Tucker / Robert Williams</t>
+  </si>
+  <si>
+    <t>Cardi B feat. Migos</t>
+  </si>
+  <si>
+    <t>Drip</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Kirsnick Ball / Kiari Cephus / Joshua Cross / Quavious Marshall</t>
+  </si>
+  <si>
+    <t>Cardi B</t>
+  </si>
+  <si>
+    <t>Bickenhead</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / James Foye III / Philip Coleman, Jr. / Austin Owens / Jordan Thorpe</t>
+  </si>
+  <si>
+    <t>Bodak Yellow</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Laquan Green / J. White Did It / Dieuson Octave / Klenord Raphael / Jordan Thorpe / Jermaine White</t>
+  </si>
+  <si>
+    <t>Be Careful</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Alan Bergman / Marilyn Bergman / Dennis Coles / Robert Diggs / Adam Feeney / Gary Grice / Marvin Hamlisch / Lamont Hawkins / Anderson Hernandez / Lauryn Hill / Jason Hunter / Russell Jones / Matthew Samuels / Clifford Smith / Jordan Thorpe / U-God / Corey Woods</t>
+  </si>
+  <si>
+    <t>Best Life</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Chancelor Bennett / Allen Ritter / Matthew Samuels</t>
+  </si>
+  <si>
+    <t>Cardi B feat. Chacne The Rapper</t>
+  </si>
+  <si>
+    <t>I Like It</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Jos? ?lvaro Osorio Balvin / Benito Antonio Martinez Ocasio / Tony Pabon / Manny Rodriguez</t>
+  </si>
+  <si>
+    <t>Cardi B feat. Bad Bunny, J. Balvin</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Khari Cain / Nija Charles / Kehlani Parrish / Mike Riley</t>
+  </si>
+  <si>
+    <t>Cardi B feat. Kehlani</t>
+  </si>
+  <si>
+    <t>Money Bag</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Jordan Thorpe / Jermaine White</t>
+  </si>
+  <si>
+    <t>Bartier Cardi</t>
+  </si>
+  <si>
+    <t>Shayaa Bin Abraham-Joseph / Belcalis Almanzar / Samuel Gloade / Darryl McCorkell</t>
+  </si>
+  <si>
+    <t>Cardi B feat, 21 Savage</t>
+  </si>
+  <si>
+    <t>She Bad</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Keenon Jackson / Leslie Andre Wakefield Jr. / Dijon McFarlane</t>
+  </si>
+  <si>
+    <t>Cardi B feat, YG</t>
+  </si>
+  <si>
+    <t>Thru Your Phone</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Benjamin Levin / Alexandra Tamposi / Justin Tranter / Andrew Wotman</t>
+  </si>
+  <si>
+    <t>I Do</t>
+  </si>
+  <si>
+    <t>Belcalis Almanzar / Nija Charles / Kevin Gomringer / Tim Gomringer / Shane Lindstrom / Solana Rowe</t>
+  </si>
+  <si>
+    <t>Cardi B feat. SZA</t>
   </si>
 </sst>
 </file>
@@ -263,11 +266,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="janellemonae3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cardib1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="janellemonae3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cardib1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -576,9 +579,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -607,7 +610,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>8.2638888888888887E-2</v>
+        <v>0.16041666666666668</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -624,7 +627,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1986111111111111</v>
+        <v>0.18263888888888891</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -641,7 +644,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17152777777777775</v>
+        <v>0.12569444444444444</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -658,7 +661,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="2">
-        <v>1.2499999999999999E-2</v>
+        <v>0.15486111111111112</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -672,10 +675,10 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2">
-        <v>0.20972222222222223</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -683,16 +686,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
       <c r="E7" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.19722222222222222</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -709,7 +712,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.17569444444444446</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -723,10 +726,10 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.12291666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -734,16 +737,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.15902777777777777</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -757,10 +760,10 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.15555555555555556</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -768,16 +771,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2">
-        <v>0.25208333333333333</v>
+        <v>0.15972222222222224</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -785,16 +788,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2">
-        <v>3.1944444444444449E-2</v>
+        <v>0.13055555555555556</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -802,34 +805,20 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2">
-        <v>0.16944444444444443</v>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.17083333333333331</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="E16" s="2"/>
@@ -881,7 +870,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="A3:K18"/>
+      <selection activeCell="K3" sqref="A3:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -901,15 +890,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>139</v>
+        <v>281</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -929,21 +918,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title               </v>
+        <v xml:space="preserve"> Title          </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                 </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                                                                                                                                               </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                            </v>
+        <v xml:space="preserve"> Performer                         </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -968,21 +957,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">-------------------- </v>
+        <v xml:space="preserve">--------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1007,28 +996,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dirty Computer      </v>
+        <v xml:space="preserve">Get Up 10      </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nate "Rocket" Wonder                                                                    </v>
+        <v xml:space="preserve"> Sean Allen / Belcalis Almanzar / Maurice Jordan / Jermaine Preyan / James SwanQo / Anthony Tucker / Robert Williams                                                                                                                                                                      </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae feat, Brian Wilson     </v>
+        <v xml:space="preserve">Cardi B feat. Migos               </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:59 </v>
+        <v xml:space="preserve">03:51 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1047,28 +1036,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Crazy, Classic, Life</v>
+        <v xml:space="preserve">Drip           </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Charles Joseph II / Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nate "Rocket" Wonder                                                </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Kirsnick Ball / Kiari Cephus / Joshua Cross / Quavious Marshall                                                                                                                                                                                                      </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B                           </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:46 </v>
+        <v xml:space="preserve">04:23 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1087,28 +1076,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Take a Byte         </v>
+        <v xml:space="preserve">Bickenhead     </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dr. Nathaniel Irvin III / John Webb Jr. / Janelle Monae Robinson / Nana Kwabena Tuffuor / Nate "Rocket" Wonder                             </v>
+        <v xml:space="preserve"> Belcalis Almanzar / James Foye III / Philip Coleman, Jr. / Austin Owens / Jordan Thorpe                                                                                                                                                                                                  </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B                           </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:07 </v>
+        <v xml:space="preserve">03:01 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1127,28 +1116,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Jane's Dream        </v>
+        <v xml:space="preserve">Bodak Yellow   </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jon Brion                                                                                                                                  </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Laquan Green / J. White Did It / Dieuson Octave / Klenord Raphael / Jordan Thorpe / Jermaine White                                                                                                                                                                   </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B                           </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:18 </v>
+        <v xml:space="preserve">03:43 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1167,28 +1156,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Screwed             </v>
+        <v xml:space="preserve">Be Careful     </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Roman GianArthur / Charles Joseph II / Dr. Nathaniel Irvin III / Benjamin Hudson McIldowie / Janelle Monae Robinson                        </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Alan Bergman / Marilyn Bergman / Dennis Coles / Robert Diggs / Adam Feeney / Gary Grice / Marvin Hamlisch / Lamont Hawkins / Anderson Hernandez / Lauryn Hill / Jason Hunter / Russell Jones / Matthew Samuels / Clifford Smith / Jordan Thorpe / U-God / Corey Woods</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae feat. Zoe Kravitz      </v>
+        <v xml:space="preserve">Cardi B                           </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:02 </v>
+        <v xml:space="preserve">03:30 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1207,28 +1196,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Django Jane         </v>
+        <v xml:space="preserve">Best Life      </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dr. Nathaniel Irvin III / Janelle Monae Robinson / Nana Kwabena Tuffuor                                                                    </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Chancelor Bennett / Allen Ritter / Matthew Samuels                                                                                                                                                                                                                   </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B feat. Chacne The Rapper   </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:10 </v>
+        <v xml:space="preserve">04:44 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1247,28 +1236,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">PYNK                </v>
+        <v xml:space="preserve">I Like It      </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Wynne Bennett / Charles Joseph II / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson                                        </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Jos? ?lvaro Osorio Balvin / Benito Antonio Martinez Ocasio / Tony Pabon / Manny Rodriguez                                                                                                                                                                            </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae feat. Grimes           </v>
+        <v>Cardi B feat. Bad Bunny, J. Balvin</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:00 </v>
+        <v xml:space="preserve">04:13 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1287,28 +1276,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Make Me Feel        </v>
+        <v xml:space="preserve">Ring           </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robin Fredriksson / Matt Friedman / Julia Michaels / Janelle Monae Robinson / Justin Tranter                                               </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Khari Cain / Nija Charles / Kehlani Parrish / Mike Riley                                                                                                                                                                                                             </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B feat. Kehlani             </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:14 </v>
+        <v xml:space="preserve">02:57 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1327,28 +1316,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I Got the Juice     </v>
+        <v xml:space="preserve">Money Bag      </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Joshua Dean / Roman GianArthur / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson / Nana Kwabena Tuffuor / Pharrell Williams</v>
+        <v xml:space="preserve"> Belcalis Almanzar / Jordan Thorpe / Jermaine White                                                                                                                                                                                                                                       </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Janelle Monae feat, Pharrell Williams</v>
+        <v xml:space="preserve">Cardi B                           </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:46 </v>
+        <v xml:space="preserve">03:49 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1367,28 +1356,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I Like That         </v>
+        <v xml:space="preserve">Bartier Cardi  </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Patrick Brown / Dr. Nathaniel Irvin III / Ray Murray / Taylor Parks / Janelle Monae Robinson / Rico Wade                                   </v>
+        <v xml:space="preserve"> Shayaa Bin Abraham-Joseph / Belcalis Almanzar / Samuel Gloade / Darryl McCorkell                                                                                                                                                                                                         </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B feat, 21 Savage           </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:20 </v>
+        <v xml:space="preserve">03:44 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1407,28 +1396,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Stevie's Dream      </v>
+        <v xml:space="preserve">She Bad        </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Roman GianArthur / Dr. Nathaniel Irvin III                                                                                                 </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Keenon Jackson / Leslie Andre Wakefield Jr. / Dijon McFarlane                                                                                                                                                                                                        </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B feat, YG                  </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:03 </v>
+        <v xml:space="preserve">03:50 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1447,28 +1436,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Don't Judge Me      </v>
+        <v>Thru Your Phone</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Joshua Dean / Roman GianArthur / Dr. Nathaniel Irvin III / Taylor Parks / Janelle Monae Robinson                                           </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Benjamin Levin / Alexandra Tamposi / Justin Tranter / Andrew Wotman                                                                                                                                                                                                  </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B                           </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:46 </v>
+        <v xml:space="preserve">03:08 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1487,28 +1476,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">So Afraid           </v>
+        <v xml:space="preserve">I Do           </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dr. Nathaniel Irvin III / Janelle Monae Robinson                                                                                           </v>
+        <v xml:space="preserve"> Belcalis Almanzar / Nija Charles / Kevin Gomringer / Tim Gomringer / Shane Lindstrom / Solana Rowe                                                                                                                                                                                       </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">Cardi B feat. SZA                 </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:04 </v>
+        <v xml:space="preserve">03:20 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1520,35 +1509,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Americans           </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Charles Joseph II / Dr. Nathaniel Irvin III / John Webb Jr. / Janelle Monae Robinson                                                       </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Janelle Monae                        </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:06 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1567,21 +1556,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1607,21 +1596,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1647,21 +1636,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1687,21 +1676,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1727,21 +1716,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1767,21 +1756,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1807,21 +1796,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1852,9 +1841,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="34.21875" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1883,7 +1872,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>8.2638888888888887E-2</v>
+        <v>0.16041666666666668</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1900,7 +1889,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1986111111111111</v>
+        <v>0.18263888888888891</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1917,7 +1906,7 @@
         <v>11</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17152777777777775</v>
+        <v>0.12569444444444444</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1934,7 +1923,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="2">
-        <v>1.2499999999999999E-2</v>
+        <v>0.15486111111111112</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1948,10 +1937,10 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2">
-        <v>0.20972222222222223</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1959,16 +1948,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
       <c r="E7" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.19722222222222222</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1985,7 +1974,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.17569444444444446</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1999,10 +1988,10 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.12291666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2010,16 +1999,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.15902777777777777</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2033,10 +2022,10 @@
         <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.15555555555555556</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2044,16 +2033,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2">
-        <v>0.25208333333333333</v>
+        <v>0.15972222222222224</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2061,16 +2050,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="2">
-        <v>3.1944444444444449E-2</v>
+        <v>0.13055555555555556</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2078,34 +2067,20 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2">
-        <v>0.16944444444444443</v>
+        <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.17083333333333331</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="E16" s="2"/>

</xml_diff>

<commit_message>
feat:06152125 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="cardib1" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
-    <definedName name="cardib1" localSheetId="2">Sheet3!$A$1:$E$14</definedName>
+    <definedName name="travisscott3" localSheetId="0">Sheet1!$A$1:$E$18</definedName>
+    <definedName name="travisscott3" localSheetId="2">Sheet3!$A$1:$E$18</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/cardib1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/travisscott3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/cardib1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/travisscott3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="41">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,106 +72,109 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>Get Up 10</t>
-  </si>
-  <si>
-    <t>Sean Allen / Belcalis Almanzar / Maurice Jordan / Jermaine Preyan / James SwanQo / Anthony Tucker / Robert Williams</t>
-  </si>
-  <si>
-    <t>Cardi B feat. Migos</t>
-  </si>
-  <si>
-    <t>Drip</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Kirsnick Ball / Kiari Cephus / Joshua Cross / Quavious Marshall</t>
-  </si>
-  <si>
-    <t>Cardi B</t>
-  </si>
-  <si>
-    <t>Bickenhead</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / James Foye III / Philip Coleman, Jr. / Austin Owens / Jordan Thorpe</t>
-  </si>
-  <si>
-    <t>Bodak Yellow</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Laquan Green / J. White Did It / Dieuson Octave / Klenord Raphael / Jordan Thorpe / Jermaine White</t>
-  </si>
-  <si>
-    <t>Be Careful</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Alan Bergman / Marilyn Bergman / Dennis Coles / Robert Diggs / Adam Feeney / Gary Grice / Marvin Hamlisch / Lamont Hawkins / Anderson Hernandez / Lauryn Hill / Jason Hunter / Russell Jones / Matthew Samuels / Clifford Smith / Jordan Thorpe / U-God / Corey Woods</t>
-  </si>
-  <si>
-    <t>Best Life</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Chancelor Bennett / Allen Ritter / Matthew Samuels</t>
-  </si>
-  <si>
-    <t>Cardi B feat. Chacne The Rapper</t>
-  </si>
-  <si>
-    <t>I Like It</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Jos? ?lvaro Osorio Balvin / Benito Antonio Martinez Ocasio / Tony Pabon / Manny Rodriguez</t>
-  </si>
-  <si>
-    <t>Cardi B feat. Bad Bunny, J. Balvin</t>
-  </si>
-  <si>
-    <t>Ring</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Khari Cain / Nija Charles / Kehlani Parrish / Mike Riley</t>
-  </si>
-  <si>
-    <t>Cardi B feat. Kehlani</t>
-  </si>
-  <si>
-    <t>Money Bag</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Jordan Thorpe / Jermaine White</t>
-  </si>
-  <si>
-    <t>Bartier Cardi</t>
-  </si>
-  <si>
-    <t>Shayaa Bin Abraham-Joseph / Belcalis Almanzar / Samuel Gloade / Darryl McCorkell</t>
-  </si>
-  <si>
-    <t>Cardi B feat, 21 Savage</t>
-  </si>
-  <si>
-    <t>She Bad</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Keenon Jackson / Leslie Andre Wakefield Jr. / Dijon McFarlane</t>
-  </si>
-  <si>
-    <t>Cardi B feat, YG</t>
-  </si>
-  <si>
-    <t>Thru Your Phone</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Benjamin Levin / Alexandra Tamposi / Justin Tranter / Andrew Wotman</t>
-  </si>
-  <si>
-    <t>I Do</t>
-  </si>
-  <si>
-    <t>Belcalis Almanzar / Nija Charles / Kevin Gomringer / Tim Gomringer / Shane Lindstrom / Solana Rowe</t>
-  </si>
-  <si>
-    <t>Cardi B feat. SZA</t>
+    <t>Stargazing</t>
+  </si>
+  <si>
+    <t>Mike Dean / Samuel Gloade / Brandon Korn / Jamie Lepe / Lamont Porter / Sonny Corey Uwaezuoke / Jacques Webster / Brandon Whitfield / Cydel Young</t>
+  </si>
+  <si>
+    <t>Travis Scott</t>
+  </si>
+  <si>
+    <t>Carousel</t>
+  </si>
+  <si>
+    <t>Christopher Breaux / Roget Chahayed / Michael Diamond / Mike Diamond / Chauncey Hollis / Adam Horovitz / Rick Rubin / Jacques Webster / Adam Yauch</t>
+  </si>
+  <si>
+    <t>Sicko Mode</t>
+  </si>
+  <si>
+    <t>Khalif Brown / Luther Campbell / Harry Casey / Harry Wayne "K.C." Casey / Brytavious Chambers / Mike Dean / Mirsad Dervic / Keith Elam / Kamaal Fareed / Richard Finch / Kevin Gomringer / Tim Gomringer / Aubrey Graham / Osten Harvey / John Edward Hawkins / Bryan Higgins / Chauncey Hollis / James Jackson / Kirk Jones / Chris Martin / Christopher Martin / Ali Shaheed Muhammad / Chylow Parker / Fred Scruggs / Trevor Smith / Malik Taylor / Tyrone Taylor / Christopher Wallace / Jacques Webster / Ozan Yildirim / Cydel Young</t>
+  </si>
+  <si>
+    <t>R.I.P Screw</t>
+  </si>
+  <si>
+    <t>Khalif Brown / Mike Dean / Trocon Roberts / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Stop Trying to Be God</t>
+  </si>
+  <si>
+    <t>Joshua Adams / James Blake / Mike Dean / Kevin Gomringer / Tim Gomringer / James Litherland / Jacques Webster</t>
+  </si>
+  <si>
+    <t>No Bystanders</t>
+  </si>
+  <si>
+    <t>Paul Beauregard / Darnell Carlton / Mike Dean / Ricky Dunigan / Khadimou Fall / Khadimoul Fall / Bj?rk Gudmundsdottir / Bj?rk Gu?mundsd?ttir / Jarad Higgins / Jordan Houston / Lola Mitchell / Ebony Oshunrinde / Robert Phillips / Sigurjon Sigurdsson / Bryan Simmons / Jacques Webster / Cydel Young</t>
+  </si>
+  <si>
+    <t>Skeletons</t>
+  </si>
+  <si>
+    <t>Mike Dean / Reine Fiske / Kevin Parker / Abel Tesfaye / Jacques Webster / Kanye West / Pharrell Williams</t>
+  </si>
+  <si>
+    <t>Wake Up</t>
+  </si>
+  <si>
+    <t>Mike Dean / Adam Feeney / Kaan Gunesberk / Nima Jahanbin / Paimon Jahanbin / Abel Tesfaye / Rupert Thomas / Jacques Webster</t>
+  </si>
+  <si>
+    <t>5% Tint</t>
+  </si>
+  <si>
+    <t>Robert Barnett / Patrick Brown / Mike Dean / Cameron Gipp / Willie Knighton / Ray Murray / Trocon Roberts / Rico Wade / Jacques Webster</t>
+  </si>
+  <si>
+    <t>NC-17</t>
+  </si>
+  <si>
+    <t>Mike Dean / Kevin Gomringer / Tim Gomringer / Tom Gomringer / Shayaa Joseph / Allen Ritter / Matthew Samuels / Johnny Stefene / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Astrothunder</t>
+  </si>
+  <si>
+    <t>Stephen Bruner / Adam Feeney / John Mayer / Thomas Paxton-Beesley / Matthew Tavares / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Yosemite</t>
+  </si>
+  <si>
+    <t>Chandler Durham / Navraj Goraya / June James / Sergio Kitchens / Ramiro Morales / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Can't Say</t>
+  </si>
+  <si>
+    <t>James Austin Cyr / Ebony Oshunrinde / Don Toliver / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Who? What!</t>
+  </si>
+  <si>
+    <t>Kirshnik Ball / Adam Feeney / Samuel Gloade / Brock Korsan / Ronald LaTour / Quavious Marshall / Lamont Porter / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Butterfly Effect</t>
+  </si>
+  <si>
+    <t>Shane Lindstrom / Donald Paton / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Houstonfornication</t>
+  </si>
+  <si>
+    <t>Nima Jahanbin / Paimon Jahanbin / Matthew Samuels / Rupert Thomas / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Coffee Bean</t>
+  </si>
+  <si>
+    <t>Mike Dean / Paul Jefferies / Tim Suby / Jacques Webster / Cydel Young</t>
   </si>
 </sst>
 </file>
@@ -266,11 +269,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cardib1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="travisscott3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cardib1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="travisscott3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,9 +582,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -610,7 +613,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -624,10 +627,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.18263888888888891</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -635,16 +638,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.21666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -652,16 +655,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.15486111111111112</v>
+        <v>0.12847222222222224</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -669,16 +672,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.14583333333333334</v>
+        <v>0.23472222222222219</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -686,16 +689,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19722222222222222</v>
+        <v>0.15138888888888888</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -703,16 +706,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17569444444444446</v>
+        <v>0.10069444444444443</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -720,16 +723,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12291666666666667</v>
+        <v>0.16041666666666668</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -737,16 +740,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.15902777777777777</v>
+        <v>0.1361111111111111</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -754,16 +757,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15555555555555556</v>
+        <v>0.10833333333333334</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -771,16 +774,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.15972222222222224</v>
+        <v>9.8611111111111108E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -788,16 +791,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.10347222222222223</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -805,58 +808,114 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.13749999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.12222222222222223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.13194444444444445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.15069444444444444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="5:5">
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.1451388888888889</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="5:5">
+    <row r="20" spans="1:5">
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="5:5">
+    <row r="21" spans="1:5">
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="5:5">
+    <row r="22" spans="1:5">
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="5:5">
+    <row r="23" spans="1:5">
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="5:5">
+    <row r="24" spans="1:5">
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="5:5">
+    <row r="25" spans="1:5">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="5:5">
+    <row r="26" spans="1:5">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="5:5">
+    <row r="27" spans="1:5">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="5:5">
+    <row r="28" spans="1:5">
       <c r="E28" s="2"/>
     </row>
   </sheetData>
@@ -870,7 +929,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="A3:K3"/>
+      <selection activeCell="K21" sqref="A3:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -890,15 +949,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>281</v>
+        <v>522</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -918,21 +977,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title          </v>
+        <v xml:space="preserve"> Title                </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                                                                                                                                               </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                         </v>
+        <v xml:space="preserve"> Performer   </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -957,21 +1016,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------- </v>
+        <v xml:space="preserve">--------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------- </v>
+        <v xml:space="preserve"> ------------ </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -996,28 +1055,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Get Up 10      </v>
+        <v xml:space="preserve">Stargazing           </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Sean Allen / Belcalis Almanzar / Maurice Jordan / Jermaine Preyan / James SwanQo / Anthony Tucker / Robert Williams                                                                                                                                                                      </v>
+        <v xml:space="preserve"> Mike Dean / Samuel Gloade / Brandon Korn / Jamie Lepe / Lamont Porter / Sonny Corey Uwaezuoke / Jacques Webster / Brandon Whitfield / Cydel Young                                                                                                                                                                                                                                                                                                                                                                                         </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B feat. Migos               </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:51 </v>
+        <v xml:space="preserve">04:30 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1036,28 +1095,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Drip           </v>
+        <v xml:space="preserve">Carousel             </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Kirsnick Ball / Kiari Cephus / Joshua Cross / Quavious Marshall                                                                                                                                                                                                      </v>
+        <v xml:space="preserve"> Christopher Breaux / Roget Chahayed / Michael Diamond / Mike Diamond / Chauncey Hollis / Adam Horovitz / Rick Rubin / Jacques Webster / Adam Yauch                                                                                                                                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B                           </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:23 </v>
+        <v xml:space="preserve">03:00 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1076,28 +1135,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bickenhead     </v>
+        <v xml:space="preserve">Sicko Mode           </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / James Foye III / Philip Coleman, Jr. / Austin Owens / Jordan Thorpe                                                                                                                                                                                                  </v>
+        <v xml:space="preserve"> Khalif Brown / Luther Campbell / Harry Casey / Harry Wayne "K.C." Casey / Brytavious Chambers / Mike Dean / Mirsad Dervic / Keith Elam / Kamaal Fareed / Richard Finch / Kevin Gomringer / Tim Gomringer / Aubrey Graham / Osten Harvey / John Edward Hawkins / Bryan Higgins / Chauncey Hollis / James Jackson / Kirk Jones / Chris Martin / Christopher Martin / Ali Shaheed Muhammad / Chylow Parker / Fred Scruggs / Trevor Smith / Malik Taylor / Tyrone Taylor / Christopher Wallace / Jacques Webster / Ozan Yildirim / Cydel Young</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B                           </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:01 </v>
+        <v xml:space="preserve">05:12 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1116,28 +1175,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bodak Yellow   </v>
+        <v xml:space="preserve">R.I.P Screw          </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Laquan Green / J. White Did It / Dieuson Octave / Klenord Raphael / Jordan Thorpe / Jermaine White                                                                                                                                                                   </v>
+        <v xml:space="preserve"> Khalif Brown / Mike Dean / Trocon Roberts / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                                                               </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B                           </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:43 </v>
+        <v xml:space="preserve">03:05 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1156,28 +1215,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Be Careful     </v>
+        <v>Stop Trying to Be God</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Alan Bergman / Marilyn Bergman / Dennis Coles / Robert Diggs / Adam Feeney / Gary Grice / Marvin Hamlisch / Lamont Hawkins / Anderson Hernandez / Lauryn Hill / Jason Hunter / Russell Jones / Matthew Samuels / Clifford Smith / Jordan Thorpe / U-God / Corey Woods</v>
+        <v xml:space="preserve"> Joshua Adams / James Blake / Mike Dean / Kevin Gomringer / Tim Gomringer / James Litherland / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                             </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B                           </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:30 </v>
+        <v xml:space="preserve">05:38 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1196,28 +1255,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Best Life      </v>
+        <v xml:space="preserve">No Bystanders        </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Chancelor Bennett / Allen Ritter / Matthew Samuels                                                                                                                                                                                                                   </v>
+        <v xml:space="preserve"> Paul Beauregard / Darnell Carlton / Mike Dean / Ricky Dunigan / Khadimou Fall / Khadimoul Fall / Bj?rk Gudmundsdottir / Bj?rk Gu?mundsd?ttir / Jarad Higgins / Jordan Houston / Lola Mitchell / Ebony Oshunrinde / Robert Phillips / Sigurjon Sigurdsson / Bryan Simmons / Jacques Webster / Cydel Young                                                                                                                                                                                                                                  </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B feat. Chacne The Rapper   </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:44 </v>
+        <v xml:space="preserve">03:38 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1236,28 +1295,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I Like It      </v>
+        <v xml:space="preserve">Skeletons            </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Jos? ?lvaro Osorio Balvin / Benito Antonio Martinez Ocasio / Tony Pabon / Manny Rodriguez                                                                                                                                                                            </v>
+        <v xml:space="preserve"> Mike Dean / Reine Fiske / Kevin Parker / Abel Tesfaye / Jacques Webster / Kanye West / Pharrell Williams                                                                                                                                                                                                                                                                                                                                                                                                                                  </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Cardi B feat. Bad Bunny, J. Balvin</v>
+        <v>Travis Scott</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:13 </v>
+        <v xml:space="preserve">02:25 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1276,28 +1335,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ring           </v>
+        <v xml:space="preserve">Wake Up              </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Khari Cain / Nija Charles / Kehlani Parrish / Mike Riley                                                                                                                                                                                                             </v>
+        <v xml:space="preserve"> Mike Dean / Adam Feeney / Kaan Gunesberk / Nima Jahanbin / Paimon Jahanbin / Abel Tesfaye / Rupert Thomas / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                               </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B feat. Kehlani             </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:57 </v>
+        <v xml:space="preserve">03:51 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1316,28 +1375,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Money Bag      </v>
+        <v xml:space="preserve">5% Tint              </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Jordan Thorpe / Jermaine White                                                                                                                                                                                                                                       </v>
+        <v xml:space="preserve"> Robert Barnett / Patrick Brown / Mike Dean / Cameron Gipp / Willie Knighton / Ray Murray / Trocon Roberts / Rico Wade / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                   </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B                           </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:49 </v>
+        <v xml:space="preserve">03:16 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1356,28 +1415,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bartier Cardi  </v>
+        <v xml:space="preserve">NC-17                </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Shayaa Bin Abraham-Joseph / Belcalis Almanzar / Samuel Gloade / Darryl McCorkell                                                                                                                                                                                                         </v>
+        <v xml:space="preserve"> Mike Dean / Kevin Gomringer / Tim Gomringer / Tom Gomringer / Shayaa Joseph / Allen Ritter / Matthew Samuels / Johnny Stefene / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                           </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B feat, 21 Savage           </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:44 </v>
+        <v xml:space="preserve">02:36 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1396,28 +1455,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">She Bad        </v>
+        <v xml:space="preserve">Astrothunder         </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Keenon Jackson / Leslie Andre Wakefield Jr. / Dijon McFarlane                                                                                                                                                                                                        </v>
+        <v xml:space="preserve"> Stephen Bruner / Adam Feeney / John Mayer / Thomas Paxton-Beesley / Matthew Tavares / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                     </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B feat, YG                  </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:50 </v>
+        <v xml:space="preserve">02:22 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1436,28 +1495,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Thru Your Phone</v>
+        <v xml:space="preserve">Yosemite             </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Benjamin Levin / Alexandra Tamposi / Justin Tranter / Andrew Wotman                                                                                                                                                                                                  </v>
+        <v xml:space="preserve"> Chandler Durham / Navraj Goraya / June James / Sergio Kitchens / Ramiro Morales / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                         </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B                           </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:08 </v>
+        <v xml:space="preserve">02:29 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1476,28 +1535,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I Do           </v>
+        <v xml:space="preserve">Can't Say            </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Belcalis Almanzar / Nija Charles / Kevin Gomringer / Tim Gomringer / Shane Lindstrom / Solana Rowe                                                                                                                                                                                       </v>
+        <v xml:space="preserve"> James Austin Cyr / Ebony Oshunrinde / Don Toliver / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                                                       </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Cardi B feat. SZA                 </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:20 </v>
+        <v xml:space="preserve">03:18 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1509,35 +1568,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Who? What!           </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Kirshnik Ball / Adam Feeney / Samuel Gloade / Brock Korsan / Ronald LaTour / Quavious Marshall / Lamont Porter / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:56 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1549,35 +1608,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Butterfly Effect     </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Shane Lindstrom / Donald Paton / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:10 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1589,35 +1648,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Houstonfornication   </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Nima Jahanbin / Paimon Jahanbin / Matthew Samuels / Rupert Thomas / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                                       </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:37 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1629,35 +1688,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Coffee Bean          </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Mike Dean / Paul Jefferies / Tim Suby / Jacques Webster / Cydel Young                                                                                                                                                                                                                                                                                                                                                                                                                                                                     </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v>Travis Scott</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:29 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1676,21 +1735,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1716,21 +1775,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1756,21 +1815,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1796,21 +1855,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1841,9 +1900,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1872,7 +1931,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1886,10 +1945,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.18263888888888891</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1897,16 +1956,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.21666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1914,16 +1973,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.15486111111111112</v>
+        <v>0.12847222222222224</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1931,16 +1990,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.14583333333333334</v>
+        <v>0.23472222222222219</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1948,16 +2007,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19722222222222222</v>
+        <v>0.15138888888888888</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1965,16 +2024,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17569444444444446</v>
+        <v>0.10069444444444443</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1982,16 +2041,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12291666666666667</v>
+        <v>0.16041666666666668</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1999,16 +2058,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.15902777777777777</v>
+        <v>0.1361111111111111</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2016,16 +2075,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15555555555555556</v>
+        <v>0.10833333333333334</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2033,16 +2092,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.15972222222222224</v>
+        <v>9.8611111111111108E-2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2050,16 +2109,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.10347222222222223</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2067,58 +2126,114 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.13749999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.12222222222222223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.13194444444444445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.15069444444444444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="2">
-        <v>0.1388888888888889</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="5:5">
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="5:5">
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="5:5">
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.1451388888888889</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="5:5">
+    <row r="20" spans="1:5">
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="5:5">
+    <row r="21" spans="1:5">
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="5:5">
+    <row r="22" spans="1:5">
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="5:5">
+    <row r="23" spans="1:5">
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="5:5">
+    <row r="24" spans="1:5">
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="5:5">
+    <row r="25" spans="1:5">
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="5:5">
+    <row r="26" spans="1:5">
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="5:5">
+    <row r="27" spans="1:5">
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="5:5">
+    <row r="28" spans="1:5">
       <c r="E28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 06162120 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="travisscott3" localSheetId="0">Sheet1!$A$1:$E$18</definedName>
-    <definedName name="travisscott3" localSheetId="2">Sheet3!$A$1:$E$18</definedName>
+    <definedName name="playboicarti1" localSheetId="0">Sheet1!$A$1:$E$20</definedName>
+    <definedName name="playboicarti1" localSheetId="2">Sheet3!$A$1:$E$20</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/travisscott3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/playboicarti1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/travisscott3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/playboicarti1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="47">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,109 +72,127 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>Stargazing</t>
-  </si>
-  <si>
-    <t>Mike Dean / Samuel Gloade / Brandon Korn / Jamie Lepe / Lamont Porter / Sonny Corey Uwaezuoke / Jacques Webster / Brandon Whitfield / Cydel Young</t>
-  </si>
-  <si>
-    <t>Travis Scott</t>
-  </si>
-  <si>
-    <t>Carousel</t>
-  </si>
-  <si>
-    <t>Christopher Breaux / Roget Chahayed / Michael Diamond / Mike Diamond / Chauncey Hollis / Adam Horovitz / Rick Rubin / Jacques Webster / Adam Yauch</t>
-  </si>
-  <si>
-    <t>Sicko Mode</t>
-  </si>
-  <si>
-    <t>Khalif Brown / Luther Campbell / Harry Casey / Harry Wayne "K.C." Casey / Brytavious Chambers / Mike Dean / Mirsad Dervic / Keith Elam / Kamaal Fareed / Richard Finch / Kevin Gomringer / Tim Gomringer / Aubrey Graham / Osten Harvey / John Edward Hawkins / Bryan Higgins / Chauncey Hollis / James Jackson / Kirk Jones / Chris Martin / Christopher Martin / Ali Shaheed Muhammad / Chylow Parker / Fred Scruggs / Trevor Smith / Malik Taylor / Tyrone Taylor / Christopher Wallace / Jacques Webster / Ozan Yildirim / Cydel Young</t>
-  </si>
-  <si>
-    <t>R.I.P Screw</t>
-  </si>
-  <si>
-    <t>Khalif Brown / Mike Dean / Trocon Roberts / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Stop Trying to Be God</t>
-  </si>
-  <si>
-    <t>Joshua Adams / James Blake / Mike Dean / Kevin Gomringer / Tim Gomringer / James Litherland / Jacques Webster</t>
-  </si>
-  <si>
-    <t>No Bystanders</t>
-  </si>
-  <si>
-    <t>Paul Beauregard / Darnell Carlton / Mike Dean / Ricky Dunigan / Khadimou Fall / Khadimoul Fall / Bj?rk Gudmundsdottir / Bj?rk Gu?mundsd?ttir / Jarad Higgins / Jordan Houston / Lola Mitchell / Ebony Oshunrinde / Robert Phillips / Sigurjon Sigurdsson / Bryan Simmons / Jacques Webster / Cydel Young</t>
-  </si>
-  <si>
-    <t>Skeletons</t>
-  </si>
-  <si>
-    <t>Mike Dean / Reine Fiske / Kevin Parker / Abel Tesfaye / Jacques Webster / Kanye West / Pharrell Williams</t>
-  </si>
-  <si>
-    <t>Wake Up</t>
-  </si>
-  <si>
-    <t>Mike Dean / Adam Feeney / Kaan Gunesberk / Nima Jahanbin / Paimon Jahanbin / Abel Tesfaye / Rupert Thomas / Jacques Webster</t>
-  </si>
-  <si>
-    <t>5% Tint</t>
-  </si>
-  <si>
-    <t>Robert Barnett / Patrick Brown / Mike Dean / Cameron Gipp / Willie Knighton / Ray Murray / Trocon Roberts / Rico Wade / Jacques Webster</t>
-  </si>
-  <si>
-    <t>NC-17</t>
-  </si>
-  <si>
-    <t>Mike Dean / Kevin Gomringer / Tim Gomringer / Tom Gomringer / Shayaa Joseph / Allen Ritter / Matthew Samuels / Johnny Stefene / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Astrothunder</t>
-  </si>
-  <si>
-    <t>Stephen Bruner / Adam Feeney / John Mayer / Thomas Paxton-Beesley / Matthew Tavares / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Yosemite</t>
-  </si>
-  <si>
-    <t>Chandler Durham / Navraj Goraya / June James / Sergio Kitchens / Ramiro Morales / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Can't Say</t>
-  </si>
-  <si>
-    <t>James Austin Cyr / Ebony Oshunrinde / Don Toliver / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Who? What!</t>
-  </si>
-  <si>
-    <t>Kirshnik Ball / Adam Feeney / Samuel Gloade / Brock Korsan / Ronald LaTour / Quavious Marshall / Lamont Porter / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Butterfly Effect</t>
-  </si>
-  <si>
-    <t>Shane Lindstrom / Donald Paton / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Houstonfornication</t>
-  </si>
-  <si>
-    <t>Nima Jahanbin / Paimon Jahanbin / Matthew Samuels / Rupert Thomas / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Coffee Bean</t>
-  </si>
-  <si>
-    <t>Mike Dean / Paul Jefferies / Tim Suby / Jacques Webster / Cydel Young</t>
+    <t>Long Time (Intro)</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Jordan Jenks</t>
+  </si>
+  <si>
+    <t>Playboi Carti</t>
+  </si>
+  <si>
+    <t>R.I.P.</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Jordan Jenks / Donald DeGrate, Jr. / Devell Moore / Shirley Murdock / Larry Troutman / Roger Troutman</t>
+  </si>
+  <si>
+    <t>Lean 4 Real</t>
+  </si>
+  <si>
+    <t>Joseph Adenuga / Jordan Carter / Jordan Jenks / Ricky Mullings</t>
+  </si>
+  <si>
+    <t>Playboi Carti feat. Skepta</t>
+  </si>
+  <si>
+    <t>Old Money</t>
+  </si>
+  <si>
+    <t>Love Hurts</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Jordan Jenks / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Playboi Carti feat. Travis Scott</t>
+  </si>
+  <si>
+    <t>Shoota</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Jamaal Henry / Symere Woods</t>
+  </si>
+  <si>
+    <t>Playboi Carti feat. Lil Uzi Vert</t>
+  </si>
+  <si>
+    <t>Right Now</t>
+  </si>
+  <si>
+    <t>Poke It Out</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Jordan Jenks / Onika Maraj</t>
+  </si>
+  <si>
+    <t>Home (KOD)</t>
+  </si>
+  <si>
+    <t>Fell in Luv</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Isaac Gerasimou / Megan James / Jordan Jenks / Corin Roddick</t>
+  </si>
+  <si>
+    <t>Playboi Carti feat. Bryson Tiler</t>
+  </si>
+  <si>
+    <t>Foreign</t>
+  </si>
+  <si>
+    <t>Pull Up</t>
+  </si>
+  <si>
+    <t>Mileage</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Keith Cozart / Jordan Jenks</t>
+  </si>
+  <si>
+    <t>Playboi Carti feat. Cheif Keef</t>
+  </si>
+  <si>
+    <t>FlatBed Freestyle</t>
+  </si>
+  <si>
+    <t>No Time</t>
+  </si>
+  <si>
+    <t>Don Cannon / Jordan Carter / Sergio Kitchens</t>
+  </si>
+  <si>
+    <t>Playboi Carti feat. Gunna</t>
+  </si>
+  <si>
+    <t>Middle of the Summer</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Redd Coldhearted / Jordan Jenks</t>
+  </si>
+  <si>
+    <t>Playboi Carti feat. Redd Coldhearted</t>
+  </si>
+  <si>
+    <t>Choppa Won't Miss</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Jordan Jenks / Jeffery Williams</t>
+  </si>
+  <si>
+    <t>Playboi Carti, Young Thug</t>
+  </si>
+  <si>
+    <t>R.I.P. Fredo</t>
+  </si>
+  <si>
+    <t>Jordan Carter / Jordan Jenks / Quantavious Thomas</t>
+  </si>
+  <si>
+    <t>Playboi Carti feat. Young Nudy</t>
+  </si>
+  <si>
+    <t>Top</t>
   </si>
 </sst>
 </file>
@@ -269,11 +287,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="travisscott3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="playboicarti1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="travisscott3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="playboicarti1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -582,9 +600,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -613,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.1875</v>
+        <v>0.14652777777777778</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -630,7 +648,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.125</v>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -644,10 +662,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0.21666666666666667</v>
+        <v>0.12291666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -655,16 +673,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.12847222222222224</v>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -678,10 +696,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2">
-        <v>0.23472222222222219</v>
+        <v>2.0833333333333333E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -689,16 +707,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.10625</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -706,16 +724,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.10069444444444443</v>
+        <v>0.14375000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -723,16 +741,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.18680555555555556</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -740,16 +758,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.1125</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -763,10 +781,10 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2">
-        <v>0.10833333333333334</v>
+        <v>0.14305555555555557</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -774,10 +792,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -794,13 +812,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.10347222222222223</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -808,16 +826,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
       <c r="E14" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.10347222222222223</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -828,13 +846,13 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="2">
-        <v>0.12222222222222223</v>
+        <v>0.13402777777777777</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -842,16 +860,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
       <c r="E16" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.15208333333333332</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -865,10 +883,10 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E17" s="2">
-        <v>0.15069444444444444</v>
+        <v>9.5138888888888884E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -876,23 +894,51 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.15069444444444444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.11180555555555556</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="2">
-        <v>0.1451388888888889</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="E20" s="2"/>
+      <c r="E20" s="2">
+        <v>9.2361111111111116E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="E21" s="2"/>
@@ -928,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="A3:K21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K23" sqref="A3:K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -949,15 +995,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>522</v>
+        <v>117</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -977,21 +1023,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                </v>
+        <v xml:space="preserve"> Title               </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                </v>
+        <v xml:space="preserve"> Composers                                                                                                           </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer   </v>
+        <v xml:space="preserve"> Performer                           </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1016,21 +1062,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------- </v>
+        <v xml:space="preserve">-------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> --------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------ </v>
+        <v xml:space="preserve"> ------------------------------------ </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1055,28 +1101,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Stargazing           </v>
+        <v xml:space="preserve">Long Time (Intro)   </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mike Dean / Samuel Gloade / Brandon Korn / Jamie Lepe / Lamont Porter / Sonny Corey Uwaezuoke / Jacques Webster / Brandon Whitfield / Cydel Young                                                                                                                                                                                                                                                                                                                                                                                         </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:30 </v>
+        <v xml:space="preserve">03:31 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1095,28 +1141,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Carousel             </v>
+        <v xml:space="preserve">R.I.P.              </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christopher Breaux / Roget Chahayed / Michael Diamond / Mike Diamond / Chauncey Hollis / Adam Horovitz / Rick Rubin / Jacques Webster / Adam Yauch                                                                                                                                                                                                                                                                                                                                                                                        </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Donald DeGrate, Jr. / Devell Moore / Shirley Murdock / Larry Troutman / Roger Troutman</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:00 </v>
+        <v xml:space="preserve">03:12 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1135,28 +1181,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sicko Mode           </v>
+        <v xml:space="preserve">Lean 4 Real         </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Khalif Brown / Luther Campbell / Harry Casey / Harry Wayne "K.C." Casey / Brytavious Chambers / Mike Dean / Mirsad Dervic / Keith Elam / Kamaal Fareed / Richard Finch / Kevin Gomringer / Tim Gomringer / Aubrey Graham / Osten Harvey / John Edward Hawkins / Bryan Higgins / Chauncey Hollis / James Jackson / Kirk Jones / Chris Martin / Christopher Martin / Ali Shaheed Muhammad / Chylow Parker / Fred Scruggs / Trevor Smith / Malik Taylor / Tyrone Taylor / Christopher Wallace / Jacques Webster / Ozan Yildirim / Cydel Young</v>
+        <v xml:space="preserve"> Joseph Adenuga / Jordan Carter / Jordan Jenks / Ricky Mullings                                                       </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti feat. Skepta          </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:12 </v>
+        <v xml:space="preserve">02:57 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1175,28 +1221,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">R.I.P Screw          </v>
+        <v xml:space="preserve">Old Money           </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Khalif Brown / Mike Dean / Trocon Roberts / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                                                               </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:05 </v>
+        <v xml:space="preserve">02:15 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1215,28 +1261,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Stop Trying to Be God</v>
+        <v xml:space="preserve">Love Hurts          </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Joshua Adams / James Blake / Mike Dean / Kevin Gomringer / Tim Gomringer / James Litherland / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                             </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Jacques Webster                                                                       </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti feat. Travis Scott    </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:38 </v>
+        <v xml:space="preserve">00:03 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1255,28 +1301,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Bystanders        </v>
+        <v xml:space="preserve">Shoota              </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Paul Beauregard / Darnell Carlton / Mike Dean / Ricky Dunigan / Khadimou Fall / Khadimoul Fall / Bj?rk Gudmundsdottir / Bj?rk Gu?mundsd?ttir / Jarad Higgins / Jordan Houston / Lola Mitchell / Ebony Oshunrinde / Robert Phillips / Sigurjon Sigurdsson / Bryan Simmons / Jacques Webster / Cydel Young                                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve"> Jordan Carter / Jamaal Henry / Symere Woods                                                                          </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti feat. Lil Uzi Vert    </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:38 </v>
+        <v xml:space="preserve">02:33 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1295,28 +1341,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Skeletons            </v>
+        <v xml:space="preserve">Right Now           </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mike Dean / Reine Fiske / Kevin Parker / Abel Tesfaye / Jacques Webster / Kanye West / Pharrell Williams                                                                                                                                                                                                                                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:25 </v>
+        <v xml:space="preserve">03:27 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1335,28 +1381,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Wake Up              </v>
+        <v xml:space="preserve">Poke It Out         </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mike Dean / Adam Feeney / Kaan Gunesberk / Nima Jahanbin / Paimon Jahanbin / Abel Tesfaye / Rupert Thomas / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                               </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Onika Maraj                                                                           </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:51 </v>
+        <v xml:space="preserve">04:29 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1375,28 +1421,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">5% Tint              </v>
+        <v xml:space="preserve">Home (KOD)          </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Barnett / Patrick Brown / Mike Dean / Cameron Gipp / Willie Knighton / Ray Murray / Trocon Roberts / Rico Wade / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                   </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:16 </v>
+        <v xml:space="preserve">02:42 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1415,28 +1461,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">NC-17                </v>
+        <v xml:space="preserve">Fell in Luv         </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mike Dean / Kevin Gomringer / Tim Gomringer / Tom Gomringer / Shayaa Joseph / Allen Ritter / Matthew Samuels / Johnny Stefene / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                           </v>
+        <v xml:space="preserve"> Jordan Carter / Isaac Gerasimou / Megan James / Jordan Jenks / Corin Roddick                                         </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti feat. Bryson Tiler    </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:36 </v>
+        <v xml:space="preserve">03:26 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1455,21 +1501,21 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Astrothunder         </v>
+        <v xml:space="preserve">Foreign             </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Stephen Bruner / Adam Feeney / John Mayer / Thomas Paxton-Beesley / Matthew Tavares / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                     </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
@@ -1495,28 +1541,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Yosemite             </v>
+        <v xml:space="preserve">Pull Up             </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chandler Durham / Navraj Goraya / June James / Sergio Kitchens / Ramiro Morales / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                         </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:29 </v>
+        <v xml:space="preserve">03:36 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1535,28 +1581,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Can't Say            </v>
+        <v xml:space="preserve">Mileage             </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> James Austin Cyr / Ebony Oshunrinde / Don Toliver / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                                                       </v>
+        <v xml:space="preserve"> Jordan Carter / Keith Cozart / Jordan Jenks                                                                          </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti feat. Cheif Keef      </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:18 </v>
+        <v xml:space="preserve">02:29 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1575,28 +1621,28 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Who? What!           </v>
+        <v xml:space="preserve">FlatBed Freestyle   </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kirshnik Ball / Adam Feeney / Samuel Gloade / Brock Korsan / Ronald LaTour / Quavious Marshall / Lamont Porter / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:56 </v>
+        <v xml:space="preserve">03:13 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1615,28 +1661,28 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Butterfly Effect     </v>
+        <v xml:space="preserve">No Time             </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Shane Lindstrom / Donald Paton / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Don Cannon / Jordan Carter / Sergio Kitchens                                                                         </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti feat. Gunna           </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:10 </v>
+        <v xml:space="preserve">03:39 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1655,28 +1701,28 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Houstonfornication   </v>
+        <v>Middle of the Summer</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nima Jahanbin / Paimon Jahanbin / Matthew Samuels / Rupert Thomas / Jacques Webster                                                                                                                                                                                                                                                                                                                                                                                                                                                       </v>
+        <v xml:space="preserve"> Jordan Carter / Redd Coldhearted / Jordan Jenks                                                                      </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v>Playboi Carti feat. Redd Coldhearted</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:37 </v>
+        <v xml:space="preserve">02:17 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1695,28 +1741,28 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Coffee Bean          </v>
+        <v xml:space="preserve">Choppa Won't Miss   </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mike Dean / Paul Jefferies / Tim Suby / Jacques Webster / Cydel Young                                                                                                                                                                                                                                                                                                                                                                                                                                                                     </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Jeffery Williams                                                                      </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Travis Scott</v>
+        <v xml:space="preserve">Playboi Carti, Young Thug           </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:29 </v>
+        <v xml:space="preserve">03:37 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1728,35 +1774,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">R.I.P. Fredo        </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Quantavious Thomas                                                                    </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">Playboi Carti feat. Young Nudy      </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:41 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1768,35 +1814,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Top                 </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </v>
+        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">Playboi Carti                       </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:13 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -1815,21 +1861,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </v>
+        <v xml:space="preserve">                                                                                                                      </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1855,21 +1901,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                                           </v>
+        <v xml:space="preserve">                                                                                                                      </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                    </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1900,9 +1946,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1931,7 +1977,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.1875</v>
+        <v>0.14652777777777778</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1948,7 +1994,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.125</v>
+        <v>0.13333333333333333</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1962,10 +2008,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0.21666666666666667</v>
+        <v>0.12291666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1973,16 +2019,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.12847222222222224</v>
+        <v>9.375E-2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1996,10 +2042,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E6" s="2">
-        <v>0.23472222222222219</v>
+        <v>2.0833333333333333E-3</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2007,16 +2053,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.10625</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2024,16 +2070,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.10069444444444443</v>
+        <v>0.14375000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2041,16 +2087,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.18680555555555556</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2058,16 +2104,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.1125</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2081,10 +2127,10 @@
         <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2">
-        <v>0.10833333333333334</v>
+        <v>0.14305555555555557</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2092,10 +2138,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -2112,13 +2158,13 @@
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.10347222222222223</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2126,16 +2172,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
       <c r="E14" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.10347222222222223</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2146,13 +2192,13 @@
         <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="2">
-        <v>0.12222222222222223</v>
+        <v>0.13402777777777777</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2160,16 +2206,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
       <c r="E16" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.15208333333333332</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2183,10 +2229,10 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E17" s="2">
-        <v>0.15069444444444444</v>
+        <v>9.5138888888888884E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2194,23 +2240,51 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.15069444444444444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.11180555555555556</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="2">
-        <v>0.1451388888888889</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="E20" s="2"/>
+      <c r="E20" s="2">
+        <v>9.2361111111111116E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="E21" s="2"/>

</xml_diff>

<commit_message>
feat: added 2 old reviews 06182140
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="playboicarti1" localSheetId="0">Sheet1!$A$1:$E$20</definedName>
-    <definedName name="playboicarti1" localSheetId="2">Sheet3!$A$1:$E$20</definedName>
+    <definedName name="vincestaples4" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="vincestaples4" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/playboicarti1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/vincestaples4.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/playboicarti1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/vincestaples4.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="27">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,127 +72,67 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>Long Time (Intro)</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Jordan Jenks</t>
-  </si>
-  <si>
-    <t>Playboi Carti</t>
-  </si>
-  <si>
-    <t>R.I.P.</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Jordan Jenks / Donald DeGrate, Jr. / Devell Moore / Shirley Murdock / Larry Troutman / Roger Troutman</t>
-  </si>
-  <si>
-    <t>Lean 4 Real</t>
-  </si>
-  <si>
-    <t>Joseph Adenuga / Jordan Carter / Jordan Jenks / Ricky Mullings</t>
-  </si>
-  <si>
-    <t>Playboi Carti feat. Skepta</t>
-  </si>
-  <si>
-    <t>Old Money</t>
-  </si>
-  <si>
-    <t>Love Hurts</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Jordan Jenks / Jacques Webster</t>
-  </si>
-  <si>
-    <t>Playboi Carti feat. Travis Scott</t>
-  </si>
-  <si>
-    <t>Shoota</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Jamaal Henry / Symere Woods</t>
-  </si>
-  <si>
-    <t>Playboi Carti feat. Lil Uzi Vert</t>
-  </si>
-  <si>
-    <t>Right Now</t>
-  </si>
-  <si>
-    <t>Poke It Out</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Jordan Jenks / Onika Maraj</t>
-  </si>
-  <si>
-    <t>Home (KOD)</t>
-  </si>
-  <si>
-    <t>Fell in Luv</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Isaac Gerasimou / Megan James / Jordan Jenks / Corin Roddick</t>
-  </si>
-  <si>
-    <t>Playboi Carti feat. Bryson Tiler</t>
-  </si>
-  <si>
-    <t>Foreign</t>
-  </si>
-  <si>
-    <t>Pull Up</t>
-  </si>
-  <si>
-    <t>Mileage</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Keith Cozart / Jordan Jenks</t>
-  </si>
-  <si>
-    <t>Playboi Carti feat. Cheif Keef</t>
-  </si>
-  <si>
-    <t>FlatBed Freestyle</t>
-  </si>
-  <si>
-    <t>No Time</t>
-  </si>
-  <si>
-    <t>Don Cannon / Jordan Carter / Sergio Kitchens</t>
-  </si>
-  <si>
-    <t>Playboi Carti feat. Gunna</t>
-  </si>
-  <si>
-    <t>Middle of the Summer</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Redd Coldhearted / Jordan Jenks</t>
-  </si>
-  <si>
-    <t>Playboi Carti feat. Redd Coldhearted</t>
-  </si>
-  <si>
-    <t>Choppa Won't Miss</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Jordan Jenks / Jeffery Williams</t>
-  </si>
-  <si>
-    <t>Playboi Carti, Young Thug</t>
-  </si>
-  <si>
-    <t>R.I.P. Fredo</t>
-  </si>
-  <si>
-    <t>Jordan Carter / Jordan Jenks / Quantavious Thomas</t>
-  </si>
-  <si>
-    <t>Playboi Carti feat. Young Nudy</t>
-  </si>
-  <si>
-    <t>Top</t>
+    <t>Feels Like Summer</t>
+  </si>
+  <si>
+    <t>Kenneth Charles Blume III / Vincent Staples</t>
+  </si>
+  <si>
+    <t>Vince Staples</t>
+  </si>
+  <si>
+    <t>Outside!</t>
+  </si>
+  <si>
+    <t>Don't Get Chipped</t>
+  </si>
+  <si>
+    <t>Kevin Gomringer / Tim Gomringer / Kenneth Charles Blume III / Johnny McKinzie / Vincent Staples</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>Vincent Staples / Marvin Thomas</t>
+  </si>
+  <si>
+    <t>New Earlsweatshirt</t>
+  </si>
+  <si>
+    <t>Kenneth Charles Blume III / Thebe Kgositsile / Vincent Staples</t>
+  </si>
+  <si>
+    <t>Run the Bands</t>
+  </si>
+  <si>
+    <t>Fun!</t>
+  </si>
+  <si>
+    <t>Vincent Staples / Earl Stevens / Marvin Thomas</t>
+  </si>
+  <si>
+    <t>No Bleedin</t>
+  </si>
+  <si>
+    <t>Kenneth Charles Blume III / Kamaiyah Johnson / Vincent Staples</t>
+  </si>
+  <si>
+    <t>Brand New Tyga</t>
+  </si>
+  <si>
+    <t>Kenneth Charles Blume III / Michael Stevenson</t>
+  </si>
+  <si>
+    <t>[562] 453-9382</t>
+  </si>
+  <si>
+    <t>Kurt Alexander / Louie G. / Kenneth Charles Blume III / Natalie P?rez</t>
+  </si>
+  <si>
+    <t>Tweakin'</t>
+  </si>
+  <si>
+    <t>Kenneth Charles Blume III / Graham Muron / Kehlani Parrish / Vincent Staples</t>
   </si>
 </sst>
 </file>
@@ -287,11 +227,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="playboicarti1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vincestaples4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="playboicarti1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vincestaples4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,7 +531,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -600,13 +540,13 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -617,7 +557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -631,10 +571,11 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14652777777777778</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0.10347222222222223</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -642,327 +583,227 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.13333333333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.12291666666666667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.10277777777777779</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>9.375E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>9.5138888888888884E-2</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>2.0833333333333333E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.10625</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.13055555555555556</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.14375000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.11875000000000001</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.18680555555555556</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.14305555555555557</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>9.8611111111111108E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.10347222222222223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.13402777777777777</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.15208333333333332</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="2">
-        <v>9.5138888888888884E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.15069444444444444</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.11180555555555556</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2">
-        <v>9.2361111111111116E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="E28" s="2"/>
+        <v>0.12916666666666668</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="6:6">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="6:6">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="6:6">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="6:6">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="6:6">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="6:6">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="6:6">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="6:6">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="6:6">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="6:6">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="6:6">
+      <c r="F28" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -974,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K23" sqref="A3:K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="A3:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -995,15 +836,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -1023,21 +864,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title               </v>
+        <v xml:space="preserve"> Title             </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                           </v>
+        <v xml:space="preserve"> Composers                                                                                     </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                           </v>
+        <v xml:space="preserve"> Performer    </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1062,21 +903,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">-------------------- </v>
+        <v xml:space="preserve">------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> --------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------ </v>
+        <v xml:space="preserve"> ------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1101,28 +942,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Long Time (Intro)   </v>
+        <v xml:space="preserve">Feels Like Summer </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
+        <v xml:space="preserve"> Kenneth Charles Blume III / Vincent Staples                                                    </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:31 </v>
+        <v xml:space="preserve">02:29 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1141,28 +982,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">R.I.P.              </v>
+        <v xml:space="preserve">Outside!          </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Donald DeGrate, Jr. / Devell Moore / Shirley Murdock / Larry Troutman / Roger Troutman</v>
+        <v xml:space="preserve"> Kenneth Charles Blume III / Vincent Staples                                                    </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:12 </v>
+        <v xml:space="preserve">02:05 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1181,28 +1022,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lean 4 Real         </v>
+        <v xml:space="preserve">Don't Get Chipped </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Joseph Adenuga / Jordan Carter / Jordan Jenks / Ricky Mullings                                                       </v>
+        <v xml:space="preserve"> Kevin Gomringer / Tim Gomringer / Kenneth Charles Blume III / Johnny McKinzie / Vincent Staples</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti feat. Skepta          </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:57 </v>
+        <v xml:space="preserve">02:28 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1221,28 +1062,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Old Money           </v>
+        <v xml:space="preserve">Relay             </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
+        <v xml:space="preserve"> Vincent Staples / Marvin Thomas                                                                </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:15 </v>
+        <v xml:space="preserve">02:17 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1261,28 +1102,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Love Hurts          </v>
+        <v>New Earlsweatshirt</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Jacques Webster                                                                       </v>
+        <v xml:space="preserve"> Kenneth Charles Blume III / Thebe Kgositsile / Vincent Staples                                 </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti feat. Travis Scott    </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:03 </v>
+        <v xml:space="preserve">00:22 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1301,28 +1142,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Shoota              </v>
+        <v xml:space="preserve">Run the Bands     </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jamaal Henry / Symere Woods                                                                          </v>
+        <v xml:space="preserve"> Vincent Staples / Marvin Thomas                                                                </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti feat. Lil Uzi Vert    </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:33 </v>
+        <v xml:space="preserve">03:08 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1341,28 +1182,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Right Now           </v>
+        <v xml:space="preserve">Fun!              </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
+        <v xml:space="preserve"> Vincent Staples / Earl Stevens / Marvin Thomas                                                 </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:27 </v>
+        <v xml:space="preserve">02:51 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1381,28 +1222,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Poke It Out         </v>
+        <v xml:space="preserve">No Bleedin        </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Onika Maraj                                                                           </v>
+        <v xml:space="preserve"> Kenneth Charles Blume III / Kamaiyah Johnson / Vincent Staples                                 </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:29 </v>
+        <v xml:space="preserve">02:03 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1421,28 +1262,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Home (KOD)          </v>
+        <v xml:space="preserve">Brand New Tyga    </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
+        <v xml:space="preserve"> Kenneth Charles Blume III / Michael Stevenson                                                  </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:42 </v>
+        <v xml:space="preserve">00:35 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1461,28 +1302,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fell in Luv         </v>
+        <v xml:space="preserve">[562] 453-9382    </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Isaac Gerasimou / Megan James / Jordan Jenks / Corin Roddick                                         </v>
+        <v xml:space="preserve"> Kurt Alexander / Louie G. / Kenneth Charles Blume III / Natalie P?rez                          </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti feat. Bryson Tiler    </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:26 </v>
+        <v xml:space="preserve">00:52 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1501,28 +1342,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Foreign             </v>
+        <v xml:space="preserve">Tweakin'          </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
+        <v xml:space="preserve"> Kenneth Charles Blume III / Graham Muron / Kehlani Parrish / Vincent Staples                   </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v>Vince Staples</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:22 </v>
+        <v xml:space="preserve">03:06 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1534,35 +1375,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pull Up             </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:36 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1574,35 +1415,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Mileage             </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Keith Cozart / Jordan Jenks                                                                          </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti feat. Cheif Keef      </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:29 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1614,35 +1455,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">FlatBed Freestyle   </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:13 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1654,35 +1495,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Time             </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Don Cannon / Jordan Carter / Sergio Kitchens                                                                         </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti feat. Gunna           </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:39 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1694,35 +1535,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Middle of the Summer</v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Redd Coldhearted / Jordan Jenks                                                                      </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Playboi Carti feat. Redd Coldhearted</v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:17 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1734,35 +1575,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Choppa Won't Miss   </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Jeffery Williams                                                                      </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti, Young Thug           </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:37 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1774,35 +1615,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">R.I.P. Fredo        </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks / Quantavious Thomas                                                                    </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti feat. Young Nudy      </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:41 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1814,35 +1655,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Top                 </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jordan Carter / Jordan Jenks                                                                                         </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Playboi Carti                       </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:13 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -1861,21 +1702,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1901,21 +1742,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                    </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1937,7 +1778,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1946,13 +1787,13 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -1963,7 +1804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1977,10 +1818,11 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14652777777777778</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>0.10347222222222223</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1988,327 +1830,227 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.13333333333333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>8.6805555555555566E-2</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.12291666666666667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>0.10277777777777779</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>9.375E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>9.5138888888888884E-2</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>2.0833333333333333E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.10625</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>0.13055555555555556</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.14375000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>0.11875000000000001</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.18680555555555556</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.14305555555555557</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>9.8611111111111108E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.10347222222222223</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.13402777777777777</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.15208333333333332</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="2">
-        <v>9.5138888888888884E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.15069444444444444</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.11180555555555556</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="2">
-        <v>9.2361111111111116E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="E28" s="2"/>
+        <v>0.12916666666666668</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="6:6">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="6:6">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="6:6">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="6:6">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="6:6">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="6:6">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="6:6">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="6:6">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="6:6">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="6:6">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="6:6">
+      <c r="F28" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
feat:06202125 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="vincestaples4" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="vincestaples4" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="ellamai1" localSheetId="0">Sheet1!$A$1:$E$16</definedName>
+    <definedName name="ellamai1" localSheetId="2">Sheet3!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/vincestaples4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/ellamai1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/vincestaples4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/ellamai1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="37">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,67 +72,97 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>Feels Like Summer</t>
-  </si>
-  <si>
-    <t>Kenneth Charles Blume III / Vincent Staples</t>
-  </si>
-  <si>
-    <t>Vince Staples</t>
-  </si>
-  <si>
-    <t>Outside!</t>
-  </si>
-  <si>
-    <t>Don't Get Chipped</t>
-  </si>
-  <si>
-    <t>Kevin Gomringer / Tim Gomringer / Kenneth Charles Blume III / Johnny McKinzie / Vincent Staples</t>
-  </si>
-  <si>
-    <t>Relay</t>
-  </si>
-  <si>
-    <t>Vincent Staples / Marvin Thomas</t>
-  </si>
-  <si>
-    <t>New Earlsweatshirt</t>
-  </si>
-  <si>
-    <t>Kenneth Charles Blume III / Thebe Kgositsile / Vincent Staples</t>
-  </si>
-  <si>
-    <t>Run the Bands</t>
-  </si>
-  <si>
-    <t>Fun!</t>
-  </si>
-  <si>
-    <t>Vincent Staples / Earl Stevens / Marvin Thomas</t>
-  </si>
-  <si>
-    <t>No Bleedin</t>
-  </si>
-  <si>
-    <t>Kenneth Charles Blume III / Kamaiyah Johnson / Vincent Staples</t>
-  </si>
-  <si>
-    <t>Brand New Tyga</t>
-  </si>
-  <si>
-    <t>Kenneth Charles Blume III / Michael Stevenson</t>
-  </si>
-  <si>
-    <t>[562] 453-9382</t>
-  </si>
-  <si>
-    <t>Kurt Alexander / Louie G. / Kenneth Charles Blume III / Natalie P?rez</t>
-  </si>
-  <si>
-    <t>Tweakin'</t>
-  </si>
-  <si>
-    <t>Kenneth Charles Blume III / Graham Muron / Kehlani Parrish / Vincent Staples</t>
+    <t>Emotion</t>
+  </si>
+  <si>
+    <t>Ella Mai</t>
+  </si>
+  <si>
+    <t>Good Bad</t>
+  </si>
+  <si>
+    <t>Ella Mai / Nana Rogues / Nathaniel Warner</t>
+  </si>
+  <si>
+    <t>Dangerous</t>
+  </si>
+  <si>
+    <t>Prince Charles / Bryan-Michael Cox / Ella Mai</t>
+  </si>
+  <si>
+    <t>Sauce</t>
+  </si>
+  <si>
+    <t>Quintin Gulledge / Ella Mai / Dijon McFarlane / Varren Wade</t>
+  </si>
+  <si>
+    <t>Whatchamacallit</t>
+  </si>
+  <si>
+    <t>Chris Brown / Jordan Holt / Sam Hook / Ella Mai / Dijon McFarlane</t>
+  </si>
+  <si>
+    <t>Ella Mai feat. Chris Brown</t>
+  </si>
+  <si>
+    <t>Cheap Shot</t>
+  </si>
+  <si>
+    <t>Shawn Butler / Ella Mai / Harmony Samuels / Varren Wade</t>
+  </si>
+  <si>
+    <t>Shot Clock</t>
+  </si>
+  <si>
+    <t>Jahron Brathwaite / Benjamin Bush / Stephen Garrett / Aubrey Graham / Micah John / Ella Mai / Dijon McFarlane / Timothy Mosley</t>
+  </si>
+  <si>
+    <t>Boo'd Up</t>
+  </si>
+  <si>
+    <t>Larrance Dopson / Joelle James / Ella Mai / Dijon McFarlane</t>
+  </si>
+  <si>
+    <t>Everything</t>
+  </si>
+  <si>
+    <t>Dayyon Alexander / Quintin Gulledge / Ella Mai / Dijon McFarlane / Jeff Shum</t>
+  </si>
+  <si>
+    <t>Ella Ma feat. John Legendi</t>
+  </si>
+  <si>
+    <t>Own It</t>
+  </si>
+  <si>
+    <t>Lucky Dave / Jamie Foxx / Ella Mai / Billy Moss / Marcos Palacios / Miykal Snoddy</t>
+  </si>
+  <si>
+    <t>Run My Mouth</t>
+  </si>
+  <si>
+    <t>Ray Harlowe / Ella Mai / Dijon McFarlane</t>
+  </si>
+  <si>
+    <t>Gut Feeling</t>
+  </si>
+  <si>
+    <t>Caroline Ailin / Trey Campbell / Quintin Gulledge / H.E.R. / Ella Mai / Dijon McFarlane</t>
+  </si>
+  <si>
+    <t>Ella Mai feat. H.E.R.</t>
+  </si>
+  <si>
+    <t>Trip</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Richard Brown / Prince Charles / Michael Conroy / Robbie Grey / Quintin Gulledge / Peder Losneg?rd / Ella Mai / Gary McDowell / Dijon McFarlane / Stephen Walker</t>
   </si>
 </sst>
 </file>
@@ -227,11 +257,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vincestaples4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ellamai1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vincestaples4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ellamai1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,15 +564,15 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCellId="1" sqref="A1:XFD1048576 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -564,14 +594,11 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
-        <v>0.10347222222222223</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -580,16 +607,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>8.6805555555555566E-2</v>
+        <v>0.15902777777777777</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -604,10 +631,10 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.10277777777777779</v>
+        <v>0.19375000000000001</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -622,10 +649,10 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>9.5138888888888884E-2</v>
+        <v>0.1277777777777778</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -640,10 +667,10 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2">
-        <v>1.5277777777777777E-2</v>
+        <v>0.12430555555555556</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -652,16 +679,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -670,16 +697,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>0.11875000000000001</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -688,16 +715,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2">
-        <v>8.5416666666666655E-2</v>
+        <v>0.16597222222222222</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -706,16 +733,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2">
-        <v>2.4305555555555556E-2</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -724,16 +751,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2">
-        <v>3.6111111111111115E-2</v>
+        <v>0.17430555555555557</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -742,31 +769,89 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12916666666666668</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.16388888888888889</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.14861111111111111</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.17500000000000002</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.18888888888888888</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="6:6">
@@ -816,7 +901,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="A3:K15"/>
+      <selection activeCell="K19" sqref="A3:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -836,15 +921,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -864,21 +949,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title             </v>
+        <v xml:space="preserve"> Title          </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                     </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                      </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer    </v>
+        <v xml:space="preserve"> Performer                 </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -903,21 +988,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------ </v>
+        <v xml:space="preserve">--------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------- </v>
+        <v xml:space="preserve"> -------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -942,28 +1027,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Feels Like Summer </v>
+        <v xml:space="preserve">Emotion        </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kenneth Charles Blume III / Vincent Staples                                                    </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:29 </v>
+        <v xml:space="preserve">00:11 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -982,28 +1067,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Outside!          </v>
+        <v xml:space="preserve">Good Bad       </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kenneth Charles Blume III / Vincent Staples                                                    </v>
+        <v xml:space="preserve"> Ella Mai / Nana Rogues / Nathaniel Warner                                                                                                                       </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:05 </v>
+        <v xml:space="preserve">03:49 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1022,28 +1107,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Don't Get Chipped </v>
+        <v xml:space="preserve">Dangerous      </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kevin Gomringer / Tim Gomringer / Kenneth Charles Blume III / Johnny McKinzie / Vincent Staples</v>
+        <v xml:space="preserve"> Prince Charles / Bryan-Michael Cox / Ella Mai                                                                                                                   </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:28 </v>
+        <v xml:space="preserve">04:39 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1062,28 +1147,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Relay             </v>
+        <v xml:space="preserve">Sauce          </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples / Marvin Thomas                                                                </v>
+        <v xml:space="preserve"> Quintin Gulledge / Ella Mai / Dijon McFarlane / Varren Wade                                                                                                     </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:17 </v>
+        <v xml:space="preserve">03:04 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1102,28 +1187,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>New Earlsweatshirt</v>
+        <v>Whatchamacallit</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kenneth Charles Blume III / Thebe Kgositsile / Vincent Staples                                 </v>
+        <v xml:space="preserve"> Chris Brown / Jordan Holt / Sam Hook / Ella Mai / Dijon McFarlane                                                                                               </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v>Ella Mai feat. Chris Brown</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:22 </v>
+        <v xml:space="preserve">02:59 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1142,28 +1227,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Run the Bands     </v>
+        <v xml:space="preserve">Cheap Shot     </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples / Marvin Thomas                                                                </v>
+        <v xml:space="preserve"> Shawn Butler / Ella Mai / Harmony Samuels / Varren Wade                                                                                                         </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:08 </v>
+        <v xml:space="preserve">04:01 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1182,28 +1267,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fun!              </v>
+        <v xml:space="preserve">Shot Clock     </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples / Earl Stevens / Marvin Thomas                                                 </v>
+        <v xml:space="preserve"> Jahron Brathwaite / Benjamin Bush / Stephen Garrett / Aubrey Graham / Micah John / Ella Mai / Dijon McFarlane / Timothy Mosley                                  </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:51 </v>
+        <v xml:space="preserve">03:21 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1222,28 +1307,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Bleedin        </v>
+        <v xml:space="preserve">Boo'd Up       </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kenneth Charles Blume III / Kamaiyah Johnson / Vincent Staples                                 </v>
+        <v xml:space="preserve"> Larrance Dopson / Joelle James / Ella Mai / Dijon McFarlane                                                                                                     </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:03 </v>
+        <v xml:space="preserve">03:59 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1262,28 +1347,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Brand New Tyga    </v>
+        <v xml:space="preserve">Everything     </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kenneth Charles Blume III / Michael Stevenson                                                  </v>
+        <v xml:space="preserve"> Dayyon Alexander / Quintin Gulledge / Ella Mai / Dijon McFarlane / Jeff Shum                                                                                    </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v>Ella Ma feat. John Legendi</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:35 </v>
+        <v xml:space="preserve">03:01 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1302,28 +1387,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">[562] 453-9382    </v>
+        <v xml:space="preserve">Own It         </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kurt Alexander / Louie G. / Kenneth Charles Blume III / Natalie P?rez                          </v>
+        <v xml:space="preserve"> Lucky Dave / Jamie Foxx / Ella Mai / Billy Moss / Marcos Palacios / Miykal Snoddy                                                                               </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:52 </v>
+        <v xml:space="preserve">04:11 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1342,28 +1427,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Tweakin'          </v>
+        <v xml:space="preserve">Run My Mouth   </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kenneth Charles Blume III / Graham Muron / Kehlani Parrish / Vincent Staples                   </v>
+        <v xml:space="preserve"> Ray Harlowe / Ella Mai / Dijon McFarlane                                                                                                                        </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vince Staples</v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:06 </v>
+        <v xml:space="preserve">02:35 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1375,35 +1460,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Gut Feeling    </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve"> Caroline Ailin / Trey Campbell / Quintin Gulledge / H.E.R. / Ella Mai / Dijon McFarlane                                                                         </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">Ella Mai feat. H.E.R.     </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:56 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1415,35 +1500,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Trip           </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve"> Quintin Gulledge / Ella Mai / Dijon McFarlane / Varren Wade                                                                                                     </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:34 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1455,35 +1540,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Close          </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve"> Quintin Gulledge / Ella Mai / Dijon McFarlane / Varren Wade                                                                                                     </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:12 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1495,35 +1580,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">Easy           </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve"> Richard Brown / Prince Charles / Michael Conroy / Robbie Grey / Quintin Gulledge / Peder Losneg?rd / Ella Mai / Gary McDowell / Dijon McFarlane / Stephen Walker</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">Ella Mai                  </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:32 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1542,21 +1627,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1582,21 +1667,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1622,21 +1707,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1662,21 +1747,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1702,21 +1787,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1742,21 +1827,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1787,9 +1872,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1811,14 +1896,11 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
-        <v>0.10347222222222223</v>
+        <v>7.6388888888888886E-3</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1827,16 +1909,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>8.6805555555555566E-2</v>
+        <v>0.15902777777777777</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1851,10 +1933,10 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.10277777777777779</v>
+        <v>0.19375000000000001</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1869,10 +1951,10 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>9.5138888888888884E-2</v>
+        <v>0.1277777777777778</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1887,10 +1969,10 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2">
-        <v>1.5277777777777777E-2</v>
+        <v>0.12430555555555556</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1899,16 +1981,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1917,16 +1999,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>0.11875000000000001</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1935,16 +2017,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2">
-        <v>8.5416666666666655E-2</v>
+        <v>0.16597222222222222</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1953,16 +2035,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2">
-        <v>2.4305555555555556E-2</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1971,16 +2053,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2">
-        <v>3.6111111111111115E-2</v>
+        <v>0.17430555555555557</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1989,31 +2071,89 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12916666666666668</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.16388888888888889</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.14861111111111111</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.17500000000000002</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.18888888888888888</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="6:6">

</xml_diff>

<commit_message>
feat: 06211825 added a new review
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\my-carbon-site\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +12,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ellamai1" localSheetId="0">Sheet1!$A$1:$E$16</definedName>
-    <definedName name="ellamai1" localSheetId="2">Sheet3!$A$1:$E$16</definedName>
+    <definedName name="liluzivert2" localSheetId="0">Sheet1!$A$1:$E$19</definedName>
+    <definedName name="liluzivert2" localSheetId="2">Sheet3!$A$1:$E$19</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,15 +26,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/ellamai1.htm" htmlTables="1">
+  <connection id="1" name="接続" type="4" refreshedVersion="4" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/liluzivert2.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
-  <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/ellamai1.htm" htmlTables="1">
+  <connection id="2" name="接続1" type="4" refreshedVersion="4" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/liluzivert2.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,15 +44,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="50">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Performer</t>
-  </si>
-  <si>
     <t xml:space="preserve"> --- </t>
     <phoneticPr fontId="1"/>
   </si>
@@ -66,113 +58,155 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Title/Composer</t>
-  </si>
-  <si>
-    <t>Emotion</t>
-  </si>
-  <si>
-    <t>Ella Mai</t>
-  </si>
-  <si>
-    <t>Good Bad</t>
-  </si>
-  <si>
-    <t>Ella Mai / Nana Rogues / Nathaniel Warner</t>
-  </si>
-  <si>
-    <t>Dangerous</t>
-  </si>
-  <si>
-    <t>Prince Charles / Bryan-Michael Cox / Ella Mai</t>
-  </si>
-  <si>
-    <t>Sauce</t>
-  </si>
-  <si>
-    <t>Quintin Gulledge / Ella Mai / Dijon McFarlane / Varren Wade</t>
-  </si>
-  <si>
-    <t>Whatchamacallit</t>
-  </si>
-  <si>
-    <t>Chris Brown / Jordan Holt / Sam Hook / Ella Mai / Dijon McFarlane</t>
-  </si>
-  <si>
-    <t>Ella Mai feat. Chris Brown</t>
-  </si>
-  <si>
-    <t>Cheap Shot</t>
-  </si>
-  <si>
-    <t>Shawn Butler / Ella Mai / Harmony Samuels / Varren Wade</t>
-  </si>
-  <si>
-    <t>Shot Clock</t>
-  </si>
-  <si>
-    <t>Jahron Brathwaite / Benjamin Bush / Stephen Garrett / Aubrey Graham / Micah John / Ella Mai / Dijon McFarlane / Timothy Mosley</t>
-  </si>
-  <si>
-    <t>Boo'd Up</t>
-  </si>
-  <si>
-    <t>Larrance Dopson / Joelle James / Ella Mai / Dijon McFarlane</t>
-  </si>
-  <si>
-    <t>Everything</t>
-  </si>
-  <si>
-    <t>Dayyon Alexander / Quintin Gulledge / Ella Mai / Dijon McFarlane / Jeff Shum</t>
-  </si>
-  <si>
-    <t>Ella Ma feat. John Legendi</t>
-  </si>
-  <si>
-    <t>Own It</t>
-  </si>
-  <si>
-    <t>Lucky Dave / Jamie Foxx / Ella Mai / Billy Moss / Marcos Palacios / Miykal Snoddy</t>
-  </si>
-  <si>
-    <t>Run My Mouth</t>
-  </si>
-  <si>
-    <t>Ray Harlowe / Ella Mai / Dijon McFarlane</t>
-  </si>
-  <si>
-    <t>Gut Feeling</t>
-  </si>
-  <si>
-    <t>Caroline Ailin / Trey Campbell / Quintin Gulledge / H.E.R. / Ella Mai / Dijon McFarlane</t>
-  </si>
-  <si>
-    <t>Ella Mai feat. H.E.R.</t>
-  </si>
-  <si>
-    <t>Trip</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Easy</t>
-  </si>
-  <si>
-    <t>Richard Brown / Prince Charles / Michael Conroy / Robbie Grey / Quintin Gulledge / Peder Losneg?rd / Ella Mai / Gary McDowell / Dijon McFarlane / Stephen Walker</t>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Writer(s)</t>
+  </si>
+  <si>
+    <t>Producer(s)</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Baby Pluto</t>
+  </si>
+  <si>
+    <t>Symere Woods, Brandon Veal, Daniel Perez, Vincent DeLon, Ivison Smith</t>
+  </si>
+  <si>
+    <t>Brandon Finessin</t>
+  </si>
+  <si>
+    <t>Lo Mein</t>
+  </si>
+  <si>
+    <t>Symere Woods, Brandon Veal, Daniel Perez</t>
+  </si>
+  <si>
+    <t>Silly Watch</t>
+  </si>
+  <si>
+    <t>Symere Woods,, Jonathan Priester</t>
+  </si>
+  <si>
+    <t>Supah Mario</t>
+  </si>
+  <si>
+    <t>Pop</t>
+  </si>
+  <si>
+    <t>Symere Woods, Jordan Ortiz, Brandon Veal</t>
+  </si>
+  <si>
+    <t>You Better Move</t>
+  </si>
+  <si>
+    <t>Symere Woods, Brandon Veal</t>
+  </si>
+  <si>
+    <t>Homecoming</t>
+  </si>
+  <si>
+    <t>Symere Woods, Daniel Perez</t>
+  </si>
+  <si>
+    <t>Bugz Ronin</t>
+  </si>
+  <si>
+    <t>I'm Sorry</t>
+  </si>
+  <si>
+    <t>Symere Woods, Brandon Veal, Anton Mendo</t>
+  </si>
+  <si>
+    <t>Celebration Station</t>
+  </si>
+  <si>
+    <t>Symere Woods, Brandon Veal, Tobias Dekker</t>
+  </si>
+  <si>
+    <t>Bigger Than Life</t>
+  </si>
+  <si>
+    <t>Symere Woods, Jordan Ortiz, Dylan Cleary-Krell</t>
+  </si>
+  <si>
+    <t>Dez Wright</t>
+  </si>
+  <si>
+    <t>Chrome Heart Tags</t>
+  </si>
+  <si>
+    <t>Symere Woods, Keith Cozart</t>
+  </si>
+  <si>
+    <t>Chief Keef</t>
+  </si>
+  <si>
+    <t>Bust Me</t>
+  </si>
+  <si>
+    <t>Prices</t>
+  </si>
+  <si>
+    <t>Symere Woods, Harold Harper, Jacques Webster, Rog?t Chahayed, Scott Mescudi, Kasseem Dean, Magnus H?iberg, Chauncey Hollis, Jr., Brittany Hazzard, Carlton Mays, Jr.</t>
+  </si>
+  <si>
+    <t>Harper</t>
+  </si>
+  <si>
+    <t>Urgency (featuring Syd)</t>
+  </si>
+  <si>
+    <t>Symere Woods, Sydney Bennett, Nick Eaholtz, Wesley Glass, Robert Richardson</t>
+  </si>
+  <si>
+    <t>Bobby Raps</t>
+  </si>
+  <si>
+    <t>Venetia</t>
+  </si>
+  <si>
+    <t>Secure the Bag</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>Symere Woods, Bryan Simmons</t>
+  </si>
+  <si>
+    <t>TM88</t>
+  </si>
+  <si>
+    <t>Futsal Shuffle 2020 (bonus track)</t>
+  </si>
+  <si>
+    <t>Symere Woods, Anton Mendo, Brandon Veal, Cas van der Heijden, Mees van der Bruggen</t>
+  </si>
+  <si>
+    <t>That Way (bonus track)</t>
+  </si>
+  <si>
+    <t>Symere Woods, Jonathan Priester, Andres Espana, Milan Modi, Andreas Carlsson, Max Martin</t>
+  </si>
+  <si>
+    <t>Felipe Spain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -257,11 +291,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ellamai1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="liluzivert2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ellamai1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="liluzivert2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -553,7 +587,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,330 +598,385 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="A1:XFD1048576 A1"/>
+      <selection activeCellId="1" sqref="A1:XFD1048576 A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" customWidth="1"/>
+    <col min="3" max="3" width="80.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>7.6388888888888886E-3</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15902777777777777</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
-        <v>0.19375000000000001</v>
+        <v>0.1361111111111111</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>0.12430555555555556</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.14861111111111111</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13958333333333334</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16597222222222222</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2">
-        <v>0.17430555555555557</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1076388888888889</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2">
-        <v>0.16388888888888889</v>
+        <v>0.16180555555555556</v>
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2">
-        <v>0.17500000000000002</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E16" s="2">
-        <v>0.18888888888888888</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.16319444444444445</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.13819444444444443</v>
+      </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14722222222222223</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="6:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="6:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="6:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F28" s="2"/>
     </row>
   </sheetData>
@@ -901,42 +990,42 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="A3:K19"/>
+      <selection activeCell="K22" sqref="A3:K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.1796875" customWidth="1"/>
+    <col min="3" max="3" width="3.90625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.08984375" customWidth="1"/>
     <col min="5" max="5" width="4" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.21875" customWidth="1"/>
-    <col min="7" max="7" width="4.44140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" customWidth="1"/>
-    <col min="11" max="11" width="3.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.1796875" customWidth="1"/>
+    <col min="7" max="7" width="4.453125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" customWidth="1"/>
+    <col min="9" max="9" width="4.36328125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" customWidth="1"/>
+    <col min="11" max="11" width="3.453125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -949,21 +1038,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title          </v>
+        <v xml:space="preserve"> Title                            </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                      </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                          </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                 </v>
+        <v xml:space="preserve"> Performer       </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -976,45 +1065,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------- </v>
+        <v xml:space="preserve">--------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------------- </v>
+        <v xml:space="preserve"> ---------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1027,34 +1116,34 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Emotion        </v>
+        <v xml:space="preserve">Baby Pluto                       </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Symere Woods, Brandon Veal, Daniel Perez, Vincent DeLon, Ivison Smith                                                                                               </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v>Brandon Finessin</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:11 </v>
+        <v xml:space="preserve">03:30 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1067,34 +1156,34 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Good Bad       </v>
+        <v xml:space="preserve">Lo Mein                          </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ella Mai / Nana Rogues / Nathaniel Warner                                                                                                                       </v>
+        <v xml:space="preserve"> Symere Woods, Brandon Veal, Daniel Perez                                                                                                                            </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v>Brandon Finessin</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:49 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1107,34 +1196,34 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dangerous      </v>
+        <v xml:space="preserve">Silly Watch                      </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Prince Charles / Bryan-Michael Cox / Ella Mai                                                                                                                   </v>
+        <v xml:space="preserve"> Symere Woods,, Jonathan Priester                                                                                                                                    </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v xml:space="preserve">Supah Mario     </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:39 </v>
+        <v xml:space="preserve">03:16 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1147,34 +1236,34 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sauce          </v>
+        <v xml:space="preserve">Pop                              </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Quintin Gulledge / Ella Mai / Dijon McFarlane / Varren Wade                                                                                                     </v>
+        <v xml:space="preserve"> Symere Woods, Jordan Ortiz, Brandon Veal                                                                                                                            </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v>Brandon Finessin</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:04 </v>
+        <v xml:space="preserve">03:47 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1187,34 +1276,34 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Whatchamacallit</v>
+        <v xml:space="preserve">You Better Move                  </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Brown / Jordan Holt / Sam Hook / Ella Mai / Dijon McFarlane                                                                                               </v>
+        <v xml:space="preserve"> Symere Woods, Brandon Veal                                                                                                                                          </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Ella Mai feat. Chris Brown</v>
+        <v>Brandon Finessin</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:59 </v>
+        <v xml:space="preserve">03:17 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1227,34 +1316,34 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Cheap Shot     </v>
+        <v xml:space="preserve">Homecoming                       </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Shawn Butler / Ella Mai / Harmony Samuels / Varren Wade                                                                                                         </v>
+        <v xml:space="preserve"> Symere Woods, Daniel Perez                                                                                                                                          </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v xml:space="preserve">Bugz Ronin      </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:01 </v>
+        <v xml:space="preserve">03:34 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1267,34 +1356,34 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Shot Clock     </v>
+        <v xml:space="preserve">I'm Sorry                        </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jahron Brathwaite / Benjamin Bush / Stephen Garrett / Aubrey Graham / Micah John / Ella Mai / Dijon McFarlane / Timothy Mosley                                  </v>
+        <v xml:space="preserve"> Symere Woods, Brandon Veal, Anton Mendo                                                                                                                             </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v>Brandon Finessin</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:21 </v>
+        <v xml:space="preserve">03:32 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1307,34 +1396,34 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Boo'd Up       </v>
+        <v xml:space="preserve">Celebration Station              </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Larrance Dopson / Joelle James / Ella Mai / Dijon McFarlane                                                                                                     </v>
+        <v xml:space="preserve"> Symere Woods, Brandon Veal, Tobias Dekker                                                                                                                           </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v>Brandon Finessin</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:59 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1347,34 +1436,34 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Everything     </v>
+        <v xml:space="preserve">Bigger Than Life                 </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dayyon Alexander / Quintin Gulledge / Ella Mai / Dijon McFarlane / Jeff Shum                                                                                    </v>
+        <v xml:space="preserve"> Symere Woods, Jordan Ortiz, Dylan Cleary-Krell                                                                                                                      </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Ella Ma feat. John Legendi</v>
+        <v xml:space="preserve">Dez Wright      </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:01 </v>
+        <v xml:space="preserve">03:13 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1387,34 +1476,34 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Own It         </v>
+        <v xml:space="preserve">Chrome Heart Tags                </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Lucky Dave / Jamie Foxx / Ella Mai / Billy Moss / Marcos Palacios / Miykal Snoddy                                                                               </v>
+        <v xml:space="preserve"> Symere Woods, Keith Cozart                                                                                                                                          </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v xml:space="preserve">Chief Keef      </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:11 </v>
+        <v xml:space="preserve">03:33 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1427,34 +1516,34 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Run My Mouth   </v>
+        <v xml:space="preserve">Bust Me                          </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ray Harlowe / Ella Mai / Dijon McFarlane                                                                                                                        </v>
+        <v xml:space="preserve"> Symere Woods, Daniel Perez                                                                                                                                          </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v xml:space="preserve">Bugz Ronin      </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:35 </v>
+        <v xml:space="preserve">03:14 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1467,34 +1556,34 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Gut Feeling    </v>
+        <v xml:space="preserve">Prices                           </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Caroline Ailin / Trey Campbell / Quintin Gulledge / H.E.R. / Ella Mai / Dijon McFarlane                                                                         </v>
+        <v xml:space="preserve"> Symere Woods, Harold Harper, Jacques Webster, Rog?t Chahayed, Scott Mescudi, Kasseem Dean, Magnus H?iberg, Chauncey Hollis, Jr., Brittany Hazzard, Carlton Mays, Jr.</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai feat. H.E.R.     </v>
+        <v xml:space="preserve">Harper          </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:56 </v>
+        <v xml:space="preserve">03:53 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1507,34 +1596,34 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Trip           </v>
+        <v xml:space="preserve">Urgency (featuring Syd)          </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Quintin Gulledge / Ella Mai / Dijon McFarlane / Varren Wade                                                                                                     </v>
+        <v xml:space="preserve"> Symere Woods, Sydney Bennett, Nick Eaholtz, Wesley Glass, Robert Richardson                                                                                         </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v xml:space="preserve">Bobby Raps      </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:34 </v>
+        <v xml:space="preserve">03:01 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1547,34 +1636,34 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Close          </v>
+        <v xml:space="preserve">Venetia                          </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Quintin Gulledge / Ella Mai / Dijon McFarlane / Varren Wade                                                                                                     </v>
+        <v xml:space="preserve"> Symere Woods, Brandon Veal, Tobias Dekker                                                                                                                           </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v>Brandon Finessin</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:12 </v>
+        <v xml:space="preserve">03:09 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1587,154 +1676,154 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Easy           </v>
+        <v xml:space="preserve">Secure the Bag                   </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Richard Brown / Prince Charles / Michael Conroy / Robbie Grey / Quintin Gulledge / Peder Losneg?rd / Ella Mai / Gary McDowell / Dijon McFarlane / Stephen Walker</v>
+        <v xml:space="preserve"> Symere Woods, Daniel Perez                                                                                                                                          </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Ella Mai                  </v>
+        <v xml:space="preserve">Bugz Ronin      </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:32 </v>
+        <v xml:space="preserve">03:58 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">P2                               </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Symere Woods, Bryan Simmons                                                                                                                                         </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">TM88            </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:55 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v>Futsal Shuffle 2020 (bonus track)</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Symere Woods, Anton Mendo, Brandon Veal, Cas van der Heijden, Mees van der Bruggen                                                                                  </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v>Brandon Finessin</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:19 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">That Way (bonus track)           </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Symere Woods, Jonathan Priester, Andres Espana, Milan Modi, Andreas Carlsson, Max Martin                                                                            </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">Felipe Spain    </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:32 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1747,21 +1836,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                                                                                                     </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1774,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1787,21 +1876,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                                                                                                     </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1814,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1827,21 +1916,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                                                                                                     </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1869,327 +1958,382 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" customWidth="1"/>
+    <col min="2" max="2" width="31.08984375" customWidth="1"/>
+    <col min="3" max="3" width="80.7265625" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="7.1796875" customWidth="1"/>
+    <col min="6" max="6" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>7.6388888888888886E-3</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15902777777777777</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
-        <v>0.19375000000000001</v>
+        <v>0.1361111111111111</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>0.12430555555555556</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.14861111111111111</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13958333333333334</v>
+        <v>0.14722222222222223</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16597222222222222</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2">
-        <v>0.17430555555555557</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1076388888888889</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E13" s="2">
-        <v>0.16388888888888889</v>
+        <v>0.16180555555555556</v>
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="E14" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2">
-        <v>0.17500000000000002</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E16" s="2">
-        <v>0.18888888888888888</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.16319444444444445</v>
+      </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.13819444444444443</v>
+      </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14722222222222223</v>
+      </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="6:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="6:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="6:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
       <c r="F28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 06212300 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\my-carbon-site\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,10 +17,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="liluzivert2" localSheetId="0">Sheet1!$A$1:$E$19</definedName>
-    <definedName name="liluzivert2" localSheetId="2">Sheet3!$A$1:$E$19</definedName>
+    <definedName name="serpentwithfeet1" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="serpentwithfeet1" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,15 +32,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="接続" type="4" refreshedVersion="4" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/liluzivert2.htm" htmlTables="1">
+  <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/serpentwithfeet1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
-  <connection id="2" name="接続1" type="4" refreshedVersion="4" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/liluzivert2.htm" htmlTables="1">
+  <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/serpentwithfeet1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -44,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="20">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -58,155 +64,65 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>No.</t>
+    <t>Title/Composer</t>
   </si>
   <si>
-    <t>Title</t>
+    <t>Performer</t>
   </si>
   <si>
-    <t>Writer(s)</t>
+    <t>Time</t>
   </si>
   <si>
-    <t>Producer(s)</t>
+    <t>Whisper</t>
   </si>
   <si>
-    <t>Length</t>
+    <t>Katie Gately / serpentwithfeet</t>
   </si>
   <si>
-    <t>Baby Pluto</t>
+    <t>serpentwithfeet</t>
   </si>
   <si>
-    <t>Symere Woods, Brandon Veal, Daniel Perez, Vincent DeLon, Ivison Smith</t>
+    <t>Messy</t>
   </si>
   <si>
-    <t>Brandon Finessin</t>
+    <t>Wrong Tree</t>
   </si>
   <si>
-    <t>Lo Mein</t>
+    <t>Fragrant</t>
   </si>
   <si>
-    <t>Symere Woods, Brandon Veal, Daniel Perez</t>
+    <t>Mourning Song</t>
   </si>
   <si>
-    <t>Silly Watch</t>
+    <t>Cherubim</t>
   </si>
   <si>
-    <t>Symere Woods,, Jonathan Priester</t>
+    <t>Seedless</t>
   </si>
   <si>
-    <t>Supah Mario</t>
+    <t>Invoice</t>
   </si>
   <si>
-    <t>Pop</t>
+    <t>Paul Epworth / serpentwithfeet</t>
   </si>
   <si>
-    <t>Symere Woods, Jordan Ortiz, Brandon Veal</t>
+    <t>Waft</t>
   </si>
   <si>
-    <t>You Better Move</t>
+    <t>Slow Syrup</t>
   </si>
   <si>
-    <t>Symere Woods, Brandon Veal</t>
-  </si>
-  <si>
-    <t>Homecoming</t>
-  </si>
-  <si>
-    <t>Symere Woods, Daniel Perez</t>
-  </si>
-  <si>
-    <t>Bugz Ronin</t>
-  </si>
-  <si>
-    <t>I'm Sorry</t>
-  </si>
-  <si>
-    <t>Symere Woods, Brandon Veal, Anton Mendo</t>
-  </si>
-  <si>
-    <t>Celebration Station</t>
-  </si>
-  <si>
-    <t>Symere Woods, Brandon Veal, Tobias Dekker</t>
-  </si>
-  <si>
-    <t>Bigger Than Life</t>
-  </si>
-  <si>
-    <t>Symere Woods, Jordan Ortiz, Dylan Cleary-Krell</t>
-  </si>
-  <si>
-    <t>Dez Wright</t>
-  </si>
-  <si>
-    <t>Chrome Heart Tags</t>
-  </si>
-  <si>
-    <t>Symere Woods, Keith Cozart</t>
-  </si>
-  <si>
-    <t>Chief Keef</t>
-  </si>
-  <si>
-    <t>Bust Me</t>
-  </si>
-  <si>
-    <t>Prices</t>
-  </si>
-  <si>
-    <t>Symere Woods, Harold Harper, Jacques Webster, Rog?t Chahayed, Scott Mescudi, Kasseem Dean, Magnus H?iberg, Chauncey Hollis, Jr., Brittany Hazzard, Carlton Mays, Jr.</t>
-  </si>
-  <si>
-    <t>Harper</t>
-  </si>
-  <si>
-    <t>Urgency (featuring Syd)</t>
-  </si>
-  <si>
-    <t>Symere Woods, Sydney Bennett, Nick Eaholtz, Wesley Glass, Robert Richardson</t>
-  </si>
-  <si>
-    <t>Bobby Raps</t>
-  </si>
-  <si>
-    <t>Venetia</t>
-  </si>
-  <si>
-    <t>Secure the Bag</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>Symere Woods, Bryan Simmons</t>
-  </si>
-  <si>
-    <t>TM88</t>
-  </si>
-  <si>
-    <t>Futsal Shuffle 2020 (bonus track)</t>
-  </si>
-  <si>
-    <t>Symere Woods, Anton Mendo, Brandon Veal, Cas van der Heijden, Mees van der Bruggen</t>
-  </si>
-  <si>
-    <t>That Way (bonus track)</t>
-  </si>
-  <si>
-    <t>Symere Woods, Jonathan Priester, Andres Espana, Milan Modi, Andreas Carlsson, Max Martin</t>
-  </si>
-  <si>
-    <t>Felipe Spain</t>
+    <t>Bless Ur Heart</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -291,11 +207,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="liluzivert2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serpentwithfeet1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="liluzivert2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serpentwithfeet1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -601,382 +517,279 @@
       <selection activeCellId="1" sqref="A1:XFD1048576 A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" customWidth="1"/>
-    <col min="3" max="3" width="80.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14583333333333334</v>
+        <v>0.18124999999999999</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.14652777777777778</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.15486111111111112</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.15763888888888888</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.13819444444444443</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.1451388888888889</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.14791666666666667</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.18263888888888891</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.16180555555555556</v>
-      </c>
+    <row r="13" spans="1:6">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.12569444444444444</v>
-      </c>
+    <row r="14" spans="1:6">
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.13125000000000001</v>
-      </c>
+    <row r="15" spans="1:6">
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.16527777777777777</v>
-      </c>
+    <row r="16" spans="1:6">
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.16319444444444445</v>
-      </c>
+    <row r="17" spans="5:6">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.13819444444444443</v>
-      </c>
+    <row r="18" spans="5:6">
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14722222222222223</v>
-      </c>
+    <row r="19" spans="5:6">
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:6">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:6">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:6">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:6">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:6">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:6">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:6">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:6">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:6">
       <c r="F28" s="2"/>
     </row>
   </sheetData>
@@ -990,42 +803,42 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="A3:K22"/>
+      <selection activeCell="K15" sqref="A3:K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" customWidth="1"/>
-    <col min="3" max="3" width="3.90625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.08984375" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="3" max="3" width="3.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="4" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" customWidth="1"/>
-    <col min="7" max="7" width="4.453125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" customWidth="1"/>
-    <col min="9" max="9" width="4.36328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1"/>
-    <col min="11" max="11" width="3.453125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.21875" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" customWidth="1"/>
+    <col min="11" max="11" width="3.44140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>164</v>
+        <v>30</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1038,21 +851,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                            </v>
+        <v xml:space="preserve"> Title         </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                          </v>
+        <v xml:space="preserve"> Composers                    </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer       </v>
+        <v xml:space="preserve"> Performer      </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1065,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1077,21 +890,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------------------- </v>
+        <v xml:space="preserve">-------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------- </v>
+        <v xml:space="preserve"> --------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1103,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1116,34 +929,34 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Baby Pluto                       </v>
+        <v xml:space="preserve">Whisper       </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Brandon Veal, Daniel Perez, Vincent DeLon, Ivison Smith                                                                                               </v>
+        <v xml:space="preserve"> Katie Gately / serpentwithfeet</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Finessin</v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:30 </v>
+        <v xml:space="preserve">04:21 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1156,34 +969,34 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lo Mein                          </v>
+        <v xml:space="preserve">Messy         </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Brandon Veal, Daniel Perez                                                                                                                            </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Finessin</v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">03:31 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1196,34 +1009,34 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Silly Watch                      </v>
+        <v xml:space="preserve">Wrong Tree    </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods,, Jonathan Priester                                                                                                                                    </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Supah Mario     </v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:16 </v>
+        <v xml:space="preserve">03:43 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1236,34 +1049,34 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pop                              </v>
+        <v xml:space="preserve">Fragrant      </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Jordan Ortiz, Brandon Veal                                                                                                                            </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Finessin</v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:47 </v>
+        <v xml:space="preserve">03:14 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1276,34 +1089,34 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">You Better Move                  </v>
+        <v xml:space="preserve">Mourning Song </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Brandon Veal                                                                                                                                          </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Finessin</v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:17 </v>
+        <v xml:space="preserve">03:19 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1316,34 +1129,34 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Homecoming                       </v>
+        <v xml:space="preserve">Cherubim      </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Daniel Perez                                                                                                                                          </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Bugz Ronin      </v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:34 </v>
+        <v xml:space="preserve">03:38 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1356,34 +1169,34 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I'm Sorry                        </v>
+        <v xml:space="preserve">Seedless      </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Brandon Veal, Anton Mendo                                                                                                                             </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Finessin</v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:32 </v>
+        <v xml:space="preserve">03:29 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1396,34 +1209,34 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Celebration Station              </v>
+        <v xml:space="preserve">Invoice       </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Brandon Veal, Tobias Dekker                                                                                                                           </v>
+        <v xml:space="preserve"> Paul Epworth / serpentwithfeet</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Finessin</v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">04:01 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1436,34 +1249,34 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bigger Than Life                 </v>
+        <v xml:space="preserve">Waft          </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Jordan Ortiz, Dylan Cleary-Krell                                                                                                                      </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dez Wright      </v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:13 </v>
+        <v xml:space="preserve">02:48 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1476,34 +1289,34 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Chrome Heart Tags                </v>
+        <v xml:space="preserve">Slow Syrup    </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Keith Cozart                                                                                                                                          </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chief Keef      </v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:33 </v>
+        <v xml:space="preserve">03:20 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1516,314 +1329,314 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bust Me                          </v>
+        <v>Bless Ur Heart</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Daniel Perez                                                                                                                                          </v>
+        <v xml:space="preserve"> serpentwithfeet               </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Bugz Ronin      </v>
+        <v>serpentwithfeet</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:14 </v>
+        <v xml:space="preserve">04:23 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Prices                           </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Harold Harper, Jacques Webster, Rog?t Chahayed, Scott Mescudi, Kasseem Dean, Magnus H?iberg, Chauncey Hollis, Jr., Brittany Hazzard, Carlton Mays, Jr.</v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Harper          </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:53 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Urgency (featuring Syd)          </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Sydney Bennett, Nick Eaholtz, Wesley Glass, Robert Richardson                                                                                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Bobby Raps      </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:01 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Venetia                          </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Brandon Veal, Tobias Dekker                                                                                                                           </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Finessin</v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:09 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Secure the Bag                   </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Daniel Perez                                                                                                                                          </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Bugz Ronin      </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:58 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>0</v>
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">P2                               </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Bryan Simmons                                                                                                                                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">TM88            </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:55 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Futsal Shuffle 2020 (bonus track)</v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Anton Mendo, Brandon Veal, Cas van der Heijden, Mees van der Bruggen                                                                                  </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Finessin</v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:19 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>0</v>
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">That Way (bonus track)           </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Symere Woods, Jonathan Priester, Andres Espana, Milan Modi, Andreas Carlsson, Max Martin                                                                            </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Felipe Spain    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:32 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1836,21 +1649,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                     </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1863,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1876,21 +1689,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                     </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1903,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1916,21 +1729,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">              </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                     </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1958,382 +1771,279 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.08984375" customWidth="1"/>
-    <col min="2" max="2" width="31.08984375" customWidth="1"/>
-    <col min="3" max="3" width="80.7265625" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="7.1796875" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="29.21875" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14583333333333334</v>
+        <v>0.18124999999999999</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.14652777777777778</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.15486111111111112</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.15763888888888888</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.13819444444444443</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.14722222222222223</v>
+        <v>0.1451388888888889</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.14791666666666667</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.18263888888888891</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.16180555555555556</v>
-      </c>
+    <row r="13" spans="1:6">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.12569444444444444</v>
-      </c>
+    <row r="14" spans="1:6">
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.13125000000000001</v>
-      </c>
+    <row r="15" spans="1:6">
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.16527777777777777</v>
-      </c>
+    <row r="16" spans="1:6">
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.16319444444444445</v>
-      </c>
+    <row r="17" spans="5:6">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.13819444444444443</v>
-      </c>
+    <row r="18" spans="5:6">
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14722222222222223</v>
-      </c>
+    <row r="19" spans="5:6">
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:6">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:6">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:6">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:6">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:6">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:6">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:6">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:6">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:6">
       <c r="F28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 05222115 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="serpentwithfeet1" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
-    <definedName name="serpentwithfeet1" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
+    <definedName name="youngfathers2" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="youngfathers2" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/serpentwithfeet1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/youngfathers2.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/serpentwithfeet1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/youngfathers2.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="21">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,46 +73,49 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Whisper</t>
+    <t>See How</t>
   </si>
   <si>
-    <t>Katie Gately / serpentwithfeet</t>
+    <t>Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</t>
   </si>
   <si>
-    <t>serpentwithfeet</t>
+    <t>Young Fathers</t>
   </si>
   <si>
-    <t>Messy</t>
+    <t>Fee Fi</t>
   </si>
   <si>
-    <t>Wrong Tree</t>
+    <t>In My View</t>
   </si>
   <si>
-    <t>Fragrant</t>
+    <t>Turn</t>
   </si>
   <si>
-    <t>Mourning Song</t>
+    <t>Kayus Bankole / Graham Hastings / Alloysious Massaquoi / Dave Sitek</t>
   </si>
   <si>
-    <t>Cherubim</t>
+    <t>Lord</t>
   </si>
   <si>
-    <t>Seedless</t>
+    <t>Tremolo</t>
   </si>
   <si>
-    <t>Invoice</t>
+    <t>Wow</t>
   </si>
   <si>
-    <t>Paul Epworth / serpentwithfeet</t>
+    <t>Border Girl</t>
   </si>
   <si>
-    <t>Waft</t>
+    <t>Holy Ghost</t>
   </si>
   <si>
-    <t>Slow Syrup</t>
+    <t>Wire</t>
   </si>
   <si>
-    <t>Bless Ur Heart</t>
+    <t>Toy</t>
+  </si>
+  <si>
+    <t>Picking You</t>
   </si>
 </sst>
 </file>
@@ -207,11 +210,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serpentwithfeet1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="youngfathers2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="serpentwithfeet1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="youngfathers2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,8 +524,8 @@
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="3" max="3" width="70.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -551,7 +554,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.18124999999999999</v>
+        <v>8.4027777777777771E-2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -563,13 +566,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.14652777777777778</v>
+        <v>0.11180555555555556</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -581,13 +584,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15486111111111112</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -599,13 +602,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.15</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -614,16 +617,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.14861111111111111</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -632,16 +635,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -650,16 +653,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1451388888888889</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -668,10 +671,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -689,13 +692,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.11666666666666665</v>
+        <v>0.10555555555555556</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -707,13 +710,13 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1388888888888889</v>
+        <v>6.9444444444444434E-2</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -725,20 +728,32 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.18263888888888891</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.1277777777777778</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
@@ -803,7 +818,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="A3:K15"/>
+      <selection activeCell="K16" sqref="A3:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -827,11 +842,11 @@
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -858,14 +873,14 @@
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                    </v>
+        <v xml:space="preserve"> Composers                                                             </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer      </v>
+        <v xml:space="preserve"> Performer    </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -897,14 +912,14 @@
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------ </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> --------------- </v>
+        <v xml:space="preserve"> ------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -929,28 +944,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Whisper       </v>
+        <v xml:space="preserve">See How       </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Katie Gately / serpentwithfeet</v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:21 </v>
+        <v xml:space="preserve">02:01 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -969,28 +984,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Messy         </v>
+        <v xml:space="preserve">Fee Fi        </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:31 </v>
+        <v xml:space="preserve">02:41 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1009,28 +1024,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Wrong Tree    </v>
+        <v xml:space="preserve">In My View    </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:43 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1049,28 +1064,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fragrant      </v>
+        <v xml:space="preserve">Turn          </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Alloysious Massaquoi / Dave Sitek    </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:14 </v>
+        <v xml:space="preserve">03:36 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1089,28 +1104,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Mourning Song </v>
+        <v xml:space="preserve">Lord          </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:19 </v>
+        <v xml:space="preserve">03:34 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1129,28 +1144,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Cherubim      </v>
+        <v xml:space="preserve">Tremolo       </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:38 </v>
+        <v xml:space="preserve">03:08 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1169,28 +1184,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Seedless      </v>
+        <v xml:space="preserve">Wow           </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:29 </v>
+        <v xml:space="preserve">04:00 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1209,21 +1224,21 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Invoice       </v>
+        <v xml:space="preserve">Border Girl   </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Paul Epworth / serpentwithfeet</v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
@@ -1249,28 +1264,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Waft          </v>
+        <v xml:space="preserve">Holy Ghost    </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:48 </v>
+        <v xml:space="preserve">02:32 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1289,28 +1304,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Slow Syrup    </v>
+        <v xml:space="preserve">Wire          </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:20 </v>
+        <v xml:space="preserve">01:40 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1329,28 +1344,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Bless Ur Heart</v>
+        <v xml:space="preserve">Toy           </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> serpentwithfeet               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>serpentwithfeet</v>
+        <v>Young Fathers</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:23 </v>
+        <v xml:space="preserve">03:13 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1362,35 +1377,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">Picking You   </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Alloysious Massaquoi / Dave Sitek    </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v>Young Fathers</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:04 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1416,14 +1431,14 @@
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
@@ -1456,14 +1471,14 @@
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
@@ -1496,14 +1511,14 @@
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1536,14 +1551,14 @@
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1576,14 +1591,14 @@
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1616,14 +1631,14 @@
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1656,14 +1671,14 @@
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1696,14 +1711,14 @@
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1736,14 +1751,14 @@
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                                                                        </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1775,8 +1790,8 @@
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="29.21875" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="3" max="3" width="70.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1805,7 +1820,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.18124999999999999</v>
+        <v>8.4027777777777771E-2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1817,13 +1832,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.14652777777777778</v>
+        <v>0.11180555555555556</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1835,13 +1850,13 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15486111111111112</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1853,13 +1868,13 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.15</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1868,16 +1883,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.14861111111111111</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1886,16 +1901,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1904,16 +1919,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1451388888888889</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1922,10 +1937,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -1943,13 +1958,13 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.11666666666666665</v>
+        <v>0.10555555555555556</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1961,13 +1976,13 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1388888888888889</v>
+        <v>6.9444444444444434E-2</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1979,20 +1994,32 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.18263888888888891</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.1277777777777778</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">

</xml_diff>

<commit_message>
feat: 06232210 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="youngfathers2" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="youngfathers2" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="andersonpaak3" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="andersonpaak3" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/youngfathers2.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/andersonpaak3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/youngfathers2.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/andersonpaak3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="46">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -64,58 +64,133 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Title/Composer</t>
-  </si>
-  <si>
     <t>Performer</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>See How</t>
-  </si>
-  <si>
-    <t>Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</t>
-  </si>
-  <si>
-    <t>Young Fathers</t>
-  </si>
-  <si>
-    <t>Fee Fi</t>
-  </si>
-  <si>
-    <t>In My View</t>
-  </si>
-  <si>
-    <t>Turn</t>
-  </si>
-  <si>
-    <t>Kayus Bankole / Graham Hastings / Alloysious Massaquoi / Dave Sitek</t>
-  </si>
-  <si>
-    <t>Lord</t>
-  </si>
-  <si>
-    <t>Tremolo</t>
-  </si>
-  <si>
-    <t>Wow</t>
-  </si>
-  <si>
-    <t>Border Girl</t>
-  </si>
-  <si>
-    <t>Holy Ghost</t>
-  </si>
-  <si>
-    <t>Wire</t>
-  </si>
-  <si>
-    <t>Toy</t>
-  </si>
-  <si>
-    <t>Picking You</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Writer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>The Chase</t>
+  </si>
+  <si>
+    <t>Kadhja Bonet, Brandon Anderson, Jairus Mozee</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. Kadhja Bonet</t>
+  </si>
+  <si>
+    <t>Headlow</t>
+  </si>
+  <si>
+    <t>Brandon Anderson, Jose Rios, Kadhja Bonet, Michael Redict, Ron Avant</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. Norelle</t>
+  </si>
+  <si>
+    <t>Tints</t>
+  </si>
+  <si>
+    <t>Brandon Anderson, Jeff Gitelma, Sydney Bennettm Robert Lewis, Kendrick Duckworth, David Pimentel, Taylor Parks, Om'Mas Keith</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. Kendrick Lamar</t>
+  </si>
+  <si>
+    <t>Who R U?</t>
+  </si>
+  <si>
+    <t>Brandon Anderson, Dwayne Abernathy Jr, .Sylvester Jordan, Andre Young, Melvin Henderson, Andre Brissett</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak</t>
+  </si>
+  <si>
+    <t>6 Summers</t>
+  </si>
+  <si>
+    <t>Brandon Anderson, Jason Pounds, Melvin Henderson, Tia Myrie</t>
+  </si>
+  <si>
+    <t>Saviers Road</t>
+  </si>
+  <si>
+    <t>Brandon Anderson, Patrick Douthit, Tia Myrie</t>
+  </si>
+  <si>
+    <t>Smile/Petty</t>
+  </si>
+  <si>
+    <t>Brandon Anderson, Keifer Shackleford, Matthew Merisola</t>
+  </si>
+  <si>
+    <t>Mansa Musa</t>
+  </si>
+  <si>
+    <t>Andre Brissett, Andre Young, Brandon Anderson, Abernathy Jr., Eric Mercer, Melvin Henderson, Sylvester Jordan, Tia Myrie, Yannick Koffi</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. Dr. Dre &amp; Cocoa Sarai</t>
+  </si>
+  <si>
+    <t>Brother's Keepers</t>
+  </si>
+  <si>
+    <t>Brandon Anderson, Abernathy Jr., Jairus Mozee, Kadhja Bonet, Terrence Thornton</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. Pusha T</t>
+  </si>
+  <si>
+    <t>Anywhere</t>
+  </si>
+  <si>
+    <t>Alana Chenevert, Brandon Anderson, Calvin Broadus Jr., Pounds, Peter Hernandez, Reagan James</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. Snoop Dogg &amp; The Last Artful, Dodgr</t>
+  </si>
+  <si>
+    <t>Trippy</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Brandon Anderson, Chris Dave, Curt Chambers, Cleo Sample</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. J. Cole</t>
+  </si>
+  <si>
+    <t>Cheers</t>
+  </si>
+  <si>
+    <t>Andre Brissett, Andre Young, Brandon Anderson, Kamaal Fareed, Sylvester Jordan</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. Q-Tip</t>
+  </si>
+  <si>
+    <t>Sweet Chick</t>
+  </si>
+  <si>
+    <t>Brandon Anderson, Bryan Sledge, Melvin Henderson, Sylvester Jordan, Tia Myrie</t>
+  </si>
+  <si>
+    <t>Brandon Anderson .Paak feat. BJ the Chicago Kid</t>
+  </si>
+  <si>
+    <t>Left to Right</t>
+  </si>
+  <si>
+    <t>Andre Young, Brandon Anderson, Pounds, Melvin Henderson, Sylvester Jordan, Tia Myrie, Trevor Smith Jr.</t>
   </si>
 </sst>
 </file>
@@ -210,11 +285,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="youngfathers2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="andersonpaak3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="youngfathers2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="andersonpaak3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -522,22 +597,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="70.21875" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="62.21875" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -545,16 +627,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>8.4027777777777771E-2</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -563,16 +645,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>0.11180555555555556</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -581,16 +663,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.18611111111111112</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -599,16 +681,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
-        <v>0.15</v>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -617,16 +699,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.19583333333333333</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -635,16 +717,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13055555555555556</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -653,16 +735,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.19583333333333333</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -671,16 +753,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.12013888888888889</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -689,16 +771,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2">
-        <v>0.10555555555555556</v>
+        <v>0.1763888888888889</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -707,16 +789,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
-        <v>6.9444444444444434E-2</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -725,16 +807,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.22430555555555556</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -743,25 +825,53 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.23194444444444443</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.16458333333333333</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.16319444444444445</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
@@ -818,7 +928,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="A3:K16"/>
+      <selection activeCell="K18" sqref="A3:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -838,15 +948,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>71</v>
+        <v>135</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -866,21 +976,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title         </v>
+        <v xml:space="preserve"> Title            </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                             </v>
+        <v xml:space="preserve"> Composers                                                                                                                             </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer    </v>
+        <v xml:space="preserve"> Performer                                                       </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -905,21 +1015,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">-------------- </v>
+        <v xml:space="preserve">----------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> --------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -944,28 +1054,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">See How       </v>
+        <v xml:space="preserve">The Chase        </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Kadhja Bonet, Brandon Anderson, Jairus Mozee                                                                                           </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak feat. Kadhja Bonet                       </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:01 </v>
+        <v xml:space="preserve">03:23 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -984,28 +1094,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fee Fi        </v>
+        <v xml:space="preserve">Headlow          </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Brandon Anderson, Jose Rios, Kadhja Bonet, Michael Redict, Ron Avant                                                                   </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak feat. Norelle                            </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:41 </v>
+        <v xml:space="preserve">04:10 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1024,28 +1134,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">In My View    </v>
+        <v xml:space="preserve">Tints            </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Brandon Anderson, Jeff Gitelma, Sydney Bennettm Robert Lewis, Kendrick Duckworth, David Pimentel, Taylor Parks, Om'Mas Keith           </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak feat. Kendrick Lamar                     </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">04:28 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1064,28 +1174,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Turn          </v>
+        <v xml:space="preserve">Who R U?         </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Alloysious Massaquoi / Dave Sitek    </v>
+        <v xml:space="preserve"> Brandon Anderson, Dwayne Abernathy Jr, .Sylvester Jordan, Andre Young, Melvin Henderson, Andre Brissett                                </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak                                          </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:36 </v>
+        <v xml:space="preserve">02:48 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1104,28 +1214,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lord          </v>
+        <v xml:space="preserve">6 Summers        </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Brandon Anderson, Jason Pounds, Melvin Henderson, Tia Myrie                                                                            </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak                                          </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:34 </v>
+        <v xml:space="preserve">04:42 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1144,28 +1254,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Tremolo       </v>
+        <v xml:space="preserve">Saviers Road     </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Brandon Anderson, Patrick Douthit, Tia Myrie                                                                                           </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak                                          </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:08 </v>
+        <v xml:space="preserve">02:24 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1184,28 +1294,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Wow           </v>
+        <v xml:space="preserve">Smile/Petty      </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Brandon Anderson, Keifer Shackleford, Matthew Merisola                                                                                 </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak                                          </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:00 </v>
+        <v xml:space="preserve">04:42 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1224,28 +1334,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Border Girl   </v>
+        <v xml:space="preserve">Mansa Musa       </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Andre Brissett, Andre Young, Brandon Anderson, Abernathy Jr., Eric Mercer, Melvin Henderson, Sylvester Jordan, Tia Myrie, Yannick Koffi</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak feat. Dr. Dre &amp; Cocoa Sarai              </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:01 </v>
+        <v xml:space="preserve">02:53 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1264,28 +1374,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Holy Ghost    </v>
+        <v>Brother's Keepers</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Brandon Anderson, Abernathy Jr., Jairus Mozee, Kadhja Bonet, Terrence Thornton                                                         </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak feat. Pusha T                            </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:32 </v>
+        <v xml:space="preserve">04:14 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1304,28 +1414,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Wire          </v>
+        <v xml:space="preserve">Anywhere         </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Alana Chenevert, Brandon Anderson, Calvin Broadus Jr., Pounds, Peter Hernandez, Reagan James                                           </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v>Brandon Anderson .Paak feat. Snoop Dogg &amp; The Last Artful, Dodgr</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:40 </v>
+        <v xml:space="preserve">03:46 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1344,28 +1454,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Toy           </v>
+        <v xml:space="preserve">Trippy           </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Timothy London / Alloysious Massaquoi</v>
+        <v xml:space="preserve"> Jermaine Cole, Brandon Anderson, Chris Dave, Curt Chambers, Cleo Sample                                                                </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak feat. J. Cole                            </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:13 </v>
+        <v xml:space="preserve">05:23 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1384,28 +1494,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Picking You   </v>
+        <v xml:space="preserve">Cheers           </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kayus Bankole / Graham Hastings / Alloysious Massaquoi / Dave Sitek    </v>
+        <v xml:space="preserve"> Andre Brissett, Andre Young, Brandon Anderson, Kamaal Fareed, Sylvester Jordan                                                         </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Young Fathers</v>
+        <v xml:space="preserve">Brandon Anderson .Paak feat. Q-Tip                              </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:04 </v>
+        <v xml:space="preserve">05:34 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1417,35 +1527,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">Sweet Chick      </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve"> Brandon Anderson, Bryan Sledge, Melvin Henderson, Sylvester Jordan, Tia Myrie                                                          </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">Brandon Anderson .Paak feat. BJ the Chicago Kid                 </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:57 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1457,35 +1567,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">Left to Right    </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve"> Andre Young, Brandon Anderson, Pounds, Melvin Henderson, Sylvester Jordan, Tia Myrie, Trevor Smith Jr.                                 </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">Brandon Anderson .Paak                                          </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:55 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1504,21 +1614,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                        </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1544,21 +1654,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                        </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1584,21 +1694,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                        </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1624,21 +1734,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                        </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1664,21 +1774,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                        </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1704,21 +1814,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                        </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1744,21 +1854,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">              </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                        </v>
+        <v xml:space="preserve">                                                                                                                                        </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                                                </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1788,22 +1898,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="70.21875" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="62.21875" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1811,16 +1928,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
-        <v>8.4027777777777771E-2</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1829,16 +1946,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>0.11180555555555556</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1847,16 +1964,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.18611111111111112</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1865,16 +1982,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2">
-        <v>0.15</v>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1883,16 +2000,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.19583333333333333</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1901,16 +2018,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13055555555555556</v>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1919,16 +2036,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.19583333333333333</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1937,16 +2054,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.12013888888888889</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1955,16 +2072,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2">
-        <v>0.10555555555555556</v>
+        <v>0.1763888888888889</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1973,16 +2090,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E11" s="2">
-        <v>6.9444444444444434E-2</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -1991,16 +2108,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.22430555555555556</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -2009,25 +2126,53 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.23194444444444443</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.16458333333333333</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.16319444444444445</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">

</xml_diff>

<commit_message>
feat: added 2 old reviews, tag modify
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="earlsweatshirt3" localSheetId="0">Sheet1!$A$1:$E$16</definedName>
-    <definedName name="earlsweatshirt3" localSheetId="2">Sheet3!$A$1:$E$16</definedName>
+    <definedName name="kidsseeghosts1" localSheetId="0">Sheet1!$A$1:$E$8</definedName>
+    <definedName name="kidsseeghosts1" localSheetId="2">Sheet3!$A$1:$E$8</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/earlsweatshirt3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/kidsseeghosts1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/earlsweatshirt3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/kidsseeghosts1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="24">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,88 +73,58 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Shattered Dreams</t>
-  </si>
-  <si>
-    <t>John Thomas, Jr. / Thebe Kgositsile</t>
-  </si>
-  <si>
-    <t>Earl Sweatshirt</t>
-  </si>
-  <si>
-    <t>Red Water</t>
-  </si>
-  <si>
-    <t>Thebe Kgositsile</t>
-  </si>
-  <si>
-    <t>Cold Summers</t>
-  </si>
-  <si>
-    <t>Emma Baloka / Thebe Kgositsile / Willy N'For / Jimmy Stormy</t>
-  </si>
-  <si>
-    <t>Nowhere2go</t>
-  </si>
-  <si>
-    <t>Darryl Joseph / Thebe Kgositsile / Ad? Hakim Sayyad</t>
-  </si>
-  <si>
-    <t>Thebe Kgositsile / Denmark Vessey</t>
-  </si>
-  <si>
-    <t>Ontheway!</t>
-  </si>
-  <si>
-    <t>Giovanni Cortez / Thebe Kgositsile / Sherman Willis</t>
-  </si>
-  <si>
-    <t>Earl Sweatshirt feat: Standing on the Corner</t>
-  </si>
-  <si>
-    <t>The Mint</t>
-  </si>
-  <si>
-    <t>Sage Elsesser / Thebe Kgositsile / Robert Mansell</t>
-  </si>
-  <si>
-    <t>Earl Sweatshirt feat: Navy Blue</t>
-  </si>
-  <si>
-    <t>The Bends</t>
-  </si>
-  <si>
-    <t>Sage Elsesser / Thebe Kgositsile / Lowrell Simon / Richard Tufo</t>
-  </si>
-  <si>
-    <t>Loosie</t>
-  </si>
-  <si>
-    <t>Azucar</t>
-  </si>
-  <si>
-    <t>Donald Davis / Sage Elsesser / Thebe Kgositsile / Harvey Scales / Albert Vance</t>
-  </si>
-  <si>
-    <t>Eclipse</t>
-  </si>
-  <si>
-    <t>Veins</t>
-  </si>
-  <si>
-    <t>Thebe Kgositsile / Curtis Mayfield</t>
-  </si>
-  <si>
-    <t>Playing Possum</t>
-  </si>
-  <si>
-    <t>Earl Sweatshirt feat: Cheryl Harris / Keorapetse Kgositsile</t>
-  </si>
-  <si>
-    <t>Peanut</t>
-  </si>
-  <si>
-    <t>Riot!</t>
+    <t>Feel the Love</t>
+  </si>
+  <si>
+    <t>Kanye West, Mike Dean, Scott Mescudi</t>
+  </si>
+  <si>
+    <t>Kids See Ghosts</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Kanye West, Scott Mescudi</t>
+  </si>
+  <si>
+    <t>4th Dimension</t>
+  </si>
+  <si>
+    <t>Kanye West, Louis Prima, Mike Dean, Scott Mescudi</t>
+  </si>
+  <si>
+    <t>Kids See Ghosts feat. Louis Prima</t>
+  </si>
+  <si>
+    <t>Freeee (Ghost Town, Pt. 2)</t>
+  </si>
+  <si>
+    <t>Corin Littler, Jeff Bhasker, Kanye West, Mike Dean, Scott Mescudi, Tyrone Griffin Jr</t>
+  </si>
+  <si>
+    <t>Kids See Ghosts feat, Ty Dolla $ign</t>
+  </si>
+  <si>
+    <t>Reborn</t>
+  </si>
+  <si>
+    <t>Scott Mescudi</t>
+  </si>
+  <si>
+    <t>Dante Smith, Kanye West, Scott Mescudi</t>
+  </si>
+  <si>
+    <t>Kids See Ghosts feat, Yasin Bey</t>
+  </si>
+  <si>
+    <t>Cudi Montage</t>
+  </si>
+  <si>
+    <t>Kanye West, Kurt Cobain, Mike Dean, Scott Mescudi</t>
+  </si>
+  <si>
+    <t>Kids See Ghosts feat. Mr Hudson</t>
   </si>
 </sst>
 </file>
@@ -252,11 +222,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="earlsweatshirt3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kidsseeghosts1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="earlsweatshirt3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kidsseeghosts1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,10 +534,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="73.33203125" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="76.44140625" customWidth="1"/>
+    <col min="4" max="4" width="32.77734375" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -596,7 +566,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>9.7222222222222224E-2</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -614,7 +584,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>7.2222222222222229E-2</v>
+        <v>9.7916666666666666E-2</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -629,10 +599,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>4.5833333333333337E-2</v>
+        <v>0.10625</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -641,16 +611,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>7.8472222222222221E-2</v>
+        <v>0.14375000000000002</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -658,17 +628,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>44189</v>
+      <c r="B6" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>7.3611111111111113E-2</v>
+        <v>0.22569444444444445</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -677,16 +647,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
-        <v>7.013888888888889E-2</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -695,161 +665,51 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.11458333333333333</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2">
-        <v>6.5277777777777782E-2</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2">
-        <v>4.0972222222222222E-2</v>
-      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>5.9027777777777783E-2</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2">
-        <v>6.458333333333334E-2</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>8.2638888888888887E-2</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="2">
-        <v>6.5277777777777782E-2</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5.0694444444444452E-2</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>4.5833333333333337E-2</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="5:6">
@@ -902,7 +762,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="K11" sqref="A3:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -922,15 +782,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -950,21 +810,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title           </v>
+        <v xml:space="preserve"> Title                     </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                    </v>
+        <v xml:space="preserve"> Composers                                                                          </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                                  </v>
+        <v xml:space="preserve"> Performer                          </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -989,21 +849,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">---------------- </v>
+        <v xml:space="preserve">-------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1028,28 +888,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Shattered Dreams</v>
+        <v xml:space="preserve">Feel the Love             </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> John Thomas, Jr. / Thebe Kgositsile                                           </v>
+        <v xml:space="preserve"> Kanye West, Mike Dean, Scott Mescudi                                                </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">Kids See Ghosts                    </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:20 </v>
+        <v xml:space="preserve">02:45 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1068,28 +928,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Red Water       </v>
+        <v xml:space="preserve">Fire                      </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Thebe Kgositsile                                                              </v>
+        <v xml:space="preserve"> Kanye West, Scott Mescudi                                                           </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">Kids See Ghosts                    </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:44 </v>
+        <v xml:space="preserve">02:21 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1108,28 +968,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Cold Summers    </v>
+        <v xml:space="preserve">4th Dimension             </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Emma Baloka / Thebe Kgositsile / Willy N'For / Jimmy Stormy                   </v>
+        <v xml:space="preserve"> Kanye West, Louis Prima, Mike Dean, Scott Mescudi                                   </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">Kids See Ghosts feat. Louis Prima  </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:06 </v>
+        <v xml:space="preserve">02:33 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1148,28 +1008,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Nowhere2go      </v>
+        <v>Freeee (Ghost Town, Pt. 2)</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Darryl Joseph / Thebe Kgositsile / Ad? Hakim Sayyad                           </v>
+        <v xml:space="preserve"> Corin Littler, Jeff Bhasker, Kanye West, Mike Dean, Scott Mescudi, Tyrone Griffin Jr</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v>Kids See Ghosts feat, Ty Dolla $ign</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:53 </v>
+        <v xml:space="preserve">03:27 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1188,28 +1048,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">44189           </v>
+        <v xml:space="preserve">Reborn                    </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Thebe Kgositsile / Denmark Vessey                                             </v>
+        <v xml:space="preserve"> Scott Mescudi                                                                       </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">Kids See Ghosts                    </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:46 </v>
+        <v xml:space="preserve">05:25 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1228,28 +1088,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ontheway!       </v>
+        <v xml:space="preserve">Kids See Ghosts           </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Giovanni Cortez / Thebe Kgositsile / Sherman Willis                           </v>
+        <v xml:space="preserve"> Dante Smith, Kanye West, Scott Mescudi                                              </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt feat: Standing on the Corner               </v>
+        <v xml:space="preserve">Kids See Ghosts feat, Yasin Bey    </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:41 </v>
+        <v xml:space="preserve">04:05 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1268,28 +1128,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Mint        </v>
+        <v xml:space="preserve">Cudi Montage              </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Sage Elsesser / Thebe Kgositsile / Robert Mansell                             </v>
+        <v xml:space="preserve"> Kanye West, Kurt Cobain, Mike Dean, Scott Mescudi                                   </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt feat: Navy Blue                            </v>
+        <v xml:space="preserve">Kids See Ghosts feat. Mr Hudson    </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:45 </v>
+        <v xml:space="preserve">03:17 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1301,35 +1161,35 @@
       </c>
       <c r="B12">
         <f>Sheet1!A9</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Bends       </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Sage Elsesser / Thebe Kgositsile / Lowrell Simon / Richard Tufo               </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:34 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1341,35 +1201,35 @@
       </c>
       <c r="B13">
         <f>Sheet1!A10</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Loosie          </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Thebe Kgositsile                                                              </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:59 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1381,35 +1241,35 @@
       </c>
       <c r="B14">
         <f>Sheet1!A11</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Azucar          </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Donald Davis / Sage Elsesser / Thebe Kgositsile / Harvey Scales / Albert Vance</v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:25 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1421,35 +1281,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Eclipse         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Thebe Kgositsile                                                              </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:33 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1461,35 +1321,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Veins           </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Thebe Kgositsile / Curtis Mayfield                                            </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:59 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1501,35 +1361,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Playing Possum  </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Thebe Kgositsile                                                              </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Earl Sweatshirt feat: Cheryl Harris / Keorapetse Kgositsile</v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:34 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1541,35 +1401,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Peanut          </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Thebe Kgositsile                                                              </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:13 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1581,35 +1441,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Riot!           </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Thebe Kgositsile                                                              </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Earl Sweatshirt                                            </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:06 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1628,21 +1488,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                               </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1668,21 +1528,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                               </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1708,21 +1568,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                               </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1748,21 +1608,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                               </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1788,21 +1648,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                               </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1828,21 +1688,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                               </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                   </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1872,10 +1732,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="73.33203125" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="76.44140625" customWidth="1"/>
+    <col min="4" max="4" width="32.77734375" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1904,7 +1764,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>9.7222222222222224E-2</v>
+        <v>0.11458333333333333</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1922,7 +1782,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>7.2222222222222229E-2</v>
+        <v>9.7916666666666666E-2</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1937,10 +1797,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>4.5833333333333337E-2</v>
+        <v>0.10625</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1949,16 +1809,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>7.8472222222222221E-2</v>
+        <v>0.14375000000000002</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1966,17 +1826,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>44189</v>
+      <c r="B6" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>7.3611111111111113E-2</v>
+        <v>0.22569444444444445</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1985,16 +1845,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
-        <v>7.013888888888889E-2</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -2003,161 +1863,51 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.11458333333333333</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2">
-        <v>6.5277777777777782E-2</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2">
-        <v>4.0972222222222222E-2</v>
-      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>5.9027777777777783E-2</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2">
-        <v>6.458333333333334E-2</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>8.2638888888888887E-2</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="2">
-        <v>6.5277777777777782E-2</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5.0694444444444452E-2</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>4.5833333333333337E-2</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="5:6">

</xml_diff>

<commit_message>
feat: 06282150 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="kidsseeghosts1" localSheetId="0">Sheet1!$A$1:$E$8</definedName>
-    <definedName name="kidsseeghosts1" localSheetId="2">Sheet3!$A$1:$E$8</definedName>
+    <definedName name="georgiaannemuldrow" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
+    <definedName name="georgiaannemuldrow" localSheetId="2">Sheet3!$A$1:$E$14</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/kidsseeghosts1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/georgiaannemuldrow.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/kidsseeghosts1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/georgiaannemuldrow.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="29">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,58 +73,73 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Feel the Love</t>
-  </si>
-  <si>
-    <t>Kanye West, Mike Dean, Scott Mescudi</t>
-  </si>
-  <si>
-    <t>Kids See Ghosts</t>
-  </si>
-  <si>
-    <t>Fire</t>
-  </si>
-  <si>
-    <t>Kanye West, Scott Mescudi</t>
-  </si>
-  <si>
-    <t>4th Dimension</t>
-  </si>
-  <si>
-    <t>Kanye West, Louis Prima, Mike Dean, Scott Mescudi</t>
-  </si>
-  <si>
-    <t>Kids See Ghosts feat. Louis Prima</t>
-  </si>
-  <si>
-    <t>Freeee (Ghost Town, Pt. 2)</t>
-  </si>
-  <si>
-    <t>Corin Littler, Jeff Bhasker, Kanye West, Mike Dean, Scott Mescudi, Tyrone Griffin Jr</t>
-  </si>
-  <si>
-    <t>Kids See Ghosts feat, Ty Dolla $ign</t>
-  </si>
-  <si>
-    <t>Reborn</t>
-  </si>
-  <si>
-    <t>Scott Mescudi</t>
-  </si>
-  <si>
-    <t>Dante Smith, Kanye West, Scott Mescudi</t>
-  </si>
-  <si>
-    <t>Kids See Ghosts feat, Yasin Bey</t>
-  </si>
-  <si>
-    <t>Cudi Montage</t>
-  </si>
-  <si>
-    <t>Kanye West, Kurt Cobain, Mike Dean, Scott Mescudi</t>
-  </si>
-  <si>
-    <t>Kids See Ghosts feat. Mr Hudson</t>
+    <t>I.O.T.A. (Instrument of the Ancestors)</t>
+  </si>
+  <si>
+    <t>Georgia Anne Muldrow</t>
+  </si>
+  <si>
+    <t>Play It Up</t>
+  </si>
+  <si>
+    <t>John Groover / Michael Cox, Jr. / Georgia Anne Muldrow</t>
+  </si>
+  <si>
+    <t>Overload</t>
+  </si>
+  <si>
+    <t>Khalil Abdul-Rahman / John Groover / Michael Cox, Jr. / Georgia Anne Muldrow</t>
+  </si>
+  <si>
+    <t>Blam</t>
+  </si>
+  <si>
+    <t>Williehook (Skit)</t>
+  </si>
+  <si>
+    <t>Aerosol</t>
+  </si>
+  <si>
+    <t>Nick Lubberson / Georgia Anne Muldrow</t>
+  </si>
+  <si>
+    <t>Vital Transformation</t>
+  </si>
+  <si>
+    <t>Allan Dela Merced Malabanan / Georgia Anne Muldrow</t>
+  </si>
+  <si>
+    <t>You Can Always Count on Me</t>
+  </si>
+  <si>
+    <t>Buddy Jones / Charlie Wilson</t>
+  </si>
+  <si>
+    <t>Georgia Anne Muldrow feat. Shana Jenson</t>
+  </si>
+  <si>
+    <t>These Are the Things I Really Like About You</t>
+  </si>
+  <si>
+    <t>Georgia Anne Muldrow / Dudley Perkins</t>
+  </si>
+  <si>
+    <t>Georgia Anne Muldrow feat. Dudley Perkins</t>
+  </si>
+  <si>
+    <t>Canadian Hillbilly</t>
+  </si>
+  <si>
+    <t>Conmigo (Reprise)</t>
+  </si>
+  <si>
+    <t>Bobbie's Dittie</t>
+  </si>
+  <si>
+    <t>Miles Griffith / Georgia Anne Muldrow / Nokware Declaime Perkins</t>
+  </si>
+  <si>
+    <t>Ciao</t>
   </si>
 </sst>
 </file>
@@ -222,11 +237,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kidsseeghosts1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="georgiaannemuldrow" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="kidsseeghosts1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="georgiaannemuldrow" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,10 +549,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="76.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="41.5546875" customWidth="1"/>
+    <col min="3" max="3" width="72.77734375" customWidth="1"/>
+    <col min="4" max="4" width="40.21875" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -563,10 +578,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
-        <v>0.11458333333333333</v>
+        <v>4.7916666666666663E-2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -575,16 +590,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>9.7916666666666666E-2</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -593,16 +608,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.10625</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -611,16 +626,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>0.14375000000000002</v>
+        <v>0.11597222222222221</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -629,16 +644,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
-        <v>0.22569444444444445</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -647,16 +662,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
-        <v>0.17013888888888887</v>
+        <v>8.4027777777777771E-2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -665,43 +680,125 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.13680555555555554</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>9.375E-2</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="E11" s="2"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.18124999999999999</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.10902777777777778</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.18611111111111112</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4.0972222222222222E-2</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
@@ -762,7 +859,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="A3:K11"/>
+      <selection activeCell="K17" sqref="A3:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -782,15 +879,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -810,21 +907,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                     </v>
+        <v xml:space="preserve"> Title                                       </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                          </v>
+        <v xml:space="preserve"> Composers                                                                  </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                          </v>
+        <v xml:space="preserve"> Performer                                </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -849,21 +946,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">-------------------------- </v>
+        <v xml:space="preserve">-------------------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -888,28 +985,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Feel the Love             </v>
+        <v xml:space="preserve">I.O.T.A. (Instrument of the Ancestors)      </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kanye West, Mike Dean, Scott Mescudi                                                </v>
+        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Kids See Ghosts                    </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:45 </v>
+        <v xml:space="preserve">01:09 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -928,28 +1025,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fire                      </v>
+        <v xml:space="preserve">Play It Up                                  </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kanye West, Scott Mescudi                                                           </v>
+        <v xml:space="preserve"> John Groover / Michael Cox, Jr. / Georgia Anne Muldrow                      </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Kids See Ghosts                    </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:21 </v>
+        <v xml:space="preserve">03:47 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -968,28 +1065,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">4th Dimension             </v>
+        <v xml:space="preserve">Overload                                    </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kanye West, Louis Prima, Mike Dean, Scott Mescudi                                   </v>
+        <v xml:space="preserve"> Khalil Abdul-Rahman / John Groover / Michael Cox, Jr. / Georgia Anne Muldrow</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Kids See Ghosts feat. Louis Prima  </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:33 </v>
+        <v xml:space="preserve">03:58 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1008,28 +1105,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Freeee (Ghost Town, Pt. 2)</v>
+        <v xml:space="preserve">Blam                                        </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Corin Littler, Jeff Bhasker, Kanye West, Mike Dean, Scott Mescudi, Tyrone Griffin Jr</v>
+        <v xml:space="preserve"> John Groover / Michael Cox, Jr. / Georgia Anne Muldrow                      </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Kids See Ghosts feat, Ty Dolla $ign</v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:27 </v>
+        <v xml:space="preserve">02:47 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1048,28 +1145,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Reborn                    </v>
+        <v xml:space="preserve">Williehook (Skit)                           </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Scott Mescudi                                                                       </v>
+        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Kids See Ghosts                    </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:25 </v>
+        <v xml:space="preserve">00:54 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1088,28 +1185,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Kids See Ghosts           </v>
+        <v xml:space="preserve">Aerosol                                     </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Dante Smith, Kanye West, Scott Mescudi                                              </v>
+        <v xml:space="preserve"> Nick Lubberson / Georgia Anne Muldrow                                       </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Kids See Ghosts feat, Yasin Bey    </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:05 </v>
+        <v xml:space="preserve">02:01 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1128,28 +1225,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Cudi Montage              </v>
+        <v xml:space="preserve">Vital Transformation                        </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kanye West, Kurt Cobain, Mike Dean, Scott Mescudi                                   </v>
+        <v xml:space="preserve"> Allan Dela Merced Malabanan / Georgia Anne Muldrow                          </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Kids See Ghosts feat. Mr Hudson    </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:17 </v>
+        <v xml:space="preserve">04:28 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1161,35 +1258,35 @@
       </c>
       <c r="B12">
         <f>Sheet1!A9</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">You Can Always Count on Me                  </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve"> Buddy Jones / Charlie Wilson                                                </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Georgia Anne Muldrow feat. Shana Jenson  </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:05 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1201,35 +1298,35 @@
       </c>
       <c r="B13">
         <f>Sheet1!A10</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v>These Are the Things I Really Like About You</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve"> Georgia Anne Muldrow / Dudley Perkins                                       </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v>Georgia Anne Muldrow feat. Dudley Perkins</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:15 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1241,35 +1338,35 @@
       </c>
       <c r="B14">
         <f>Sheet1!A11</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">Canadian Hillbilly                          </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:21 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1281,35 +1378,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">Conmigo (Reprise)                           </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:37 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1321,35 +1418,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">Bobbie's Dittie                             </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve"> Miles Griffith / Georgia Anne Muldrow / Nokware Declaime Perkins            </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:28 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1361,35 +1458,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">Ciao                                        </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">00:59 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1408,21 +1505,21 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                            </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                             </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                         </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
@@ -1448,21 +1545,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                            </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                             </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                         </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1488,21 +1585,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                            </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                             </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                         </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1528,21 +1625,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                            </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                             </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                         </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1568,21 +1665,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                            </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                             </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                         </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1608,21 +1705,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                            </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                             </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                         </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1648,21 +1745,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                            </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                             </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                         </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1688,21 +1785,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                            </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                             </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                   </v>
+        <v xml:space="preserve">                                         </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1732,10 +1829,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="76.44140625" customWidth="1"/>
-    <col min="4" max="4" width="32.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="41.5546875" customWidth="1"/>
+    <col min="3" max="3" width="72.77734375" customWidth="1"/>
+    <col min="4" max="4" width="40.21875" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1761,10 +1858,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
-        <v>0.11458333333333333</v>
+        <v>4.7916666666666663E-2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1773,16 +1870,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>9.7916666666666666E-2</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1791,16 +1888,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.10625</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1809,16 +1906,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>0.14375000000000002</v>
+        <v>0.11597222222222221</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1827,16 +1924,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
-        <v>0.22569444444444445</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1845,16 +1942,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
-        <v>0.17013888888888887</v>
+        <v>8.4027777777777771E-2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1863,43 +1960,125 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.18611111111111112</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.12847222222222224</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.13680555555555554</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>9.375E-2</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="E11" s="2"/>
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.18124999999999999</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.10902777777777778</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.18611111111111112</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>4.0972222222222222E-2</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">

</xml_diff>

<commit_message>
feat: 06292215 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="georgiaannemuldrow" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
-    <definedName name="georgiaannemuldrow" localSheetId="2">Sheet3!$A$1:$E$14</definedName>
+    <definedName name="jcole3" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="jcole3" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/georgiaannemuldrow.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/jcole3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/georgiaannemuldrow.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/jcole3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="32">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,73 +73,82 @@
     <t>Time</t>
   </si>
   <si>
-    <t>I.O.T.A. (Instrument of the Ancestors)</t>
-  </si>
-  <si>
-    <t>Georgia Anne Muldrow</t>
-  </si>
-  <si>
-    <t>Play It Up</t>
-  </si>
-  <si>
-    <t>John Groover / Michael Cox, Jr. / Georgia Anne Muldrow</t>
-  </si>
-  <si>
-    <t>Overload</t>
-  </si>
-  <si>
-    <t>Khalil Abdul-Rahman / John Groover / Michael Cox, Jr. / Georgia Anne Muldrow</t>
-  </si>
-  <si>
-    <t>Blam</t>
-  </si>
-  <si>
-    <t>Williehook (Skit)</t>
-  </si>
-  <si>
-    <t>Aerosol</t>
-  </si>
-  <si>
-    <t>Nick Lubberson / Georgia Anne Muldrow</t>
-  </si>
-  <si>
-    <t>Vital Transformation</t>
-  </si>
-  <si>
-    <t>Allan Dela Merced Malabanan / Georgia Anne Muldrow</t>
-  </si>
-  <si>
-    <t>You Can Always Count on Me</t>
-  </si>
-  <si>
-    <t>Buddy Jones / Charlie Wilson</t>
-  </si>
-  <si>
-    <t>Georgia Anne Muldrow feat. Shana Jenson</t>
-  </si>
-  <si>
-    <t>These Are the Things I Really Like About You</t>
-  </si>
-  <si>
-    <t>Georgia Anne Muldrow / Dudley Perkins</t>
-  </si>
-  <si>
-    <t>Georgia Anne Muldrow feat. Dudley Perkins</t>
-  </si>
-  <si>
-    <t>Canadian Hillbilly</t>
-  </si>
-  <si>
-    <t>Conmigo (Reprise)</t>
-  </si>
-  <si>
-    <t>Bobbie's Dittie</t>
-  </si>
-  <si>
-    <t>Miles Griffith / Georgia Anne Muldrow / Nokware Declaime Perkins</t>
-  </si>
-  <si>
-    <t>Ciao</t>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Richard Clay, Carl Clay, Wayne Garfield</t>
+  </si>
+  <si>
+    <t>J. Cole</t>
+  </si>
+  <si>
+    <t>KOD</t>
+  </si>
+  <si>
+    <t>Jermaine Cole</t>
+  </si>
+  <si>
+    <t>Photograph</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Raymond Evans, Jay Livingston, Francis Hime</t>
+  </si>
+  <si>
+    <t>The Cut Off</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Kill Edward, Bill Withers, Takehiro Honda</t>
+  </si>
+  <si>
+    <t>J. Cole feat,. Kill Edward</t>
+  </si>
+  <si>
+    <t>ATM</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Nicholas Brodszky, ]Sammy Cahn</t>
+  </si>
+  <si>
+    <t>Motiv8</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Roy Ayers, James Bedford, Lamont Porter, Sylvia Striplin, Christopher Wallace</t>
+  </si>
+  <si>
+    <t>Kevin's Heart</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Tyler Williams, Mark Pellizzer</t>
+  </si>
+  <si>
+    <t>Brackets</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Richard Pryor, Marilyn Bergman, Alan Bergman, Quincy Jones</t>
+  </si>
+  <si>
+    <t>Once an Addict (Interlude)</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Ron Gilmore, Micha? Urbaniak</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Kill Edward, John Dankworth</t>
+  </si>
+  <si>
+    <t>Window Pain (Outro)</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Kill Edward</t>
+  </si>
+  <si>
+    <t>1985 (Intro to "The Fall Off")</t>
+  </si>
+  <si>
+    <t>Jermaine Cole, Jorge Barreiro</t>
   </si>
 </sst>
 </file>
@@ -237,11 +246,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="georgiaannemuldrow" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jcole3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="georgiaannemuldrow" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jcole3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -544,15 +553,15 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="A1:XFD1048576 A1:XFD1048576"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" customWidth="1"/>
-    <col min="3" max="3" width="72.77734375" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -578,10 +587,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>4.7916666666666663E-2</v>
+        <v>7.4305555555555555E-2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -590,16 +599,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15763888888888888</v>
+        <v>0.13263888888888889</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -608,16 +617,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.16527777777777777</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -626,16 +635,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
-        <v>0.11597222222222221</v>
+        <v>0.16458333333333333</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -644,16 +653,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>3.7499999999999999E-2</v>
+        <v>0.15</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -662,16 +671,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>8.4027777777777771E-2</v>
+        <v>9.2361111111111116E-2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -680,16 +689,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.18611111111111112</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -698,16 +707,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12847222222222224</v>
+        <v>0.21875</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -716,16 +725,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>9.375E-2</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -734,16 +743,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2">
-        <v>0.18124999999999999</v>
+        <v>0.17847222222222223</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -752,16 +761,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.10902777777777778</v>
+        <v>0.1986111111111111</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -770,35 +779,21 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.18611111111111112</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2">
-        <v>4.0972222222222222E-2</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
@@ -859,7 +854,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="A3:K17"/>
+      <selection activeCell="K16" sqref="A3:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -879,15 +874,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -907,21 +902,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                                       </v>
+        <v xml:space="preserve"> Title                         </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                  </v>
+        <v xml:space="preserve"> Composers                                                                                  </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                </v>
+        <v xml:space="preserve"> Performer                 </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -946,21 +941,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">-------------------------------------------- </v>
+        <v xml:space="preserve">------------------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> -------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------- </v>
+        <v xml:space="preserve"> -------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -985,28 +980,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I.O.T.A. (Instrument of the Ancestors)      </v>
+        <v xml:space="preserve">Intro                         </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
+        <v xml:space="preserve"> Jermaine Cole, Richard Clay, Carl Clay, Wayne Garfield                                      </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:09 </v>
+        <v xml:space="preserve">01:47 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1025,28 +1020,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Play It Up                                  </v>
+        <v xml:space="preserve">KOD                           </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> John Groover / Michael Cox, Jr. / Georgia Anne Muldrow                      </v>
+        <v xml:space="preserve"> Jermaine Cole                                                                               </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:47 </v>
+        <v xml:space="preserve">03:11 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1065,28 +1060,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Overload                                    </v>
+        <v xml:space="preserve">Photograph                    </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Khalil Abdul-Rahman / John Groover / Michael Cox, Jr. / Georgia Anne Muldrow</v>
+        <v xml:space="preserve"> Jermaine Cole, Raymond Evans, Jay Livingston, Francis Hime                                  </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:58 </v>
+        <v xml:space="preserve">03:38 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1105,28 +1100,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Blam                                        </v>
+        <v xml:space="preserve">The Cut Off                   </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> John Groover / Michael Cox, Jr. / Georgia Anne Muldrow                      </v>
+        <v xml:space="preserve"> Jermaine Cole, Kill Edward, Bill Withers, Takehiro Honda                                    </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v>J. Cole feat,. Kill Edward</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:47 </v>
+        <v xml:space="preserve">03:57 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1145,28 +1140,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Williehook (Skit)                           </v>
+        <v xml:space="preserve">ATM                           </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
+        <v xml:space="preserve"> Jermaine Cole, Nicholas Brodszky, ]Sammy Cahn                                               </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:54 </v>
+        <v xml:space="preserve">03:36 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1185,28 +1180,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Aerosol                                     </v>
+        <v xml:space="preserve">Motiv8                        </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nick Lubberson / Georgia Anne Muldrow                                       </v>
+        <v xml:space="preserve"> Jermaine Cole, Roy Ayers, James Bedford, Lamont Porter, Sylvia Striplin, Christopher Wallace</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:01 </v>
+        <v xml:space="preserve">02:13 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1225,28 +1220,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Vital Transformation                        </v>
+        <v xml:space="preserve">Kevin's Heart                 </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Allan Dela Merced Malabanan / Georgia Anne Muldrow                          </v>
+        <v xml:space="preserve"> Jermaine Cole, Tyler Williams, Mark Pellizzer                                               </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:28 </v>
+        <v xml:space="preserve">03:20 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1265,28 +1260,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">You Can Always Count on Me                  </v>
+        <v xml:space="preserve">Brackets                      </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Buddy Jones / Charlie Wilson                                                </v>
+        <v xml:space="preserve"> Jermaine Cole, Richard Pryor, Marilyn Bergman, Alan Bergman, Quincy Jones                   </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow feat. Shana Jenson  </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:05 </v>
+        <v xml:space="preserve">05:15 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1305,28 +1300,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>These Are the Things I Really Like About You</v>
+        <v xml:space="preserve">Once an Addict (Interlude)    </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Georgia Anne Muldrow / Dudley Perkins                                       </v>
+        <v xml:space="preserve"> Jermaine Cole, Ron Gilmore, Micha? Urbaniak                                                 </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Georgia Anne Muldrow feat. Dudley Perkins</v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:15 </v>
+        <v xml:space="preserve">03:17 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1345,28 +1340,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Canadian Hillbilly                          </v>
+        <v xml:space="preserve">Friends                       </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
+        <v xml:space="preserve"> Jermaine Cole, Kill Edward, John Dankworth                                                  </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v>J. Cole feat,. Kill Edward</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:21 </v>
+        <v xml:space="preserve">04:17 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1385,28 +1380,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Conmigo (Reprise)                           </v>
+        <v xml:space="preserve">Window Pain (Outro)           </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
+        <v xml:space="preserve"> Jermaine Cole, Kill Edward                                                                  </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:37 </v>
+        <v xml:space="preserve">04:46 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1425,28 +1420,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Bobbie's Dittie                             </v>
+        <v>1985 (Intro to "The Fall Off")</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Miles Griffith / Georgia Anne Muldrow / Nokware Declaime Perkins            </v>
+        <v xml:space="preserve"> Jermaine Cole, Jorge Barreiro                                                               </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">J. Cole                   </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:28 </v>
+        <v xml:space="preserve">03:10 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1458,35 +1453,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ciao                                        </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Georgia Anne Muldrow                                                        </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Georgia Anne Muldrow                     </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:59 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1505,21 +1500,21 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                            </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                             </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
@@ -1545,21 +1540,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                            </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                             </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1585,21 +1580,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                            </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                             </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1625,21 +1620,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                            </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                             </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1665,21 +1660,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                            </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                             </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1705,21 +1700,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                            </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                             </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1745,21 +1740,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                            </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                             </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1785,21 +1780,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                            </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                             </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                         </v>
+        <v xml:space="preserve">                          </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1830,9 +1825,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" customWidth="1"/>
-    <col min="3" max="3" width="72.77734375" customWidth="1"/>
-    <col min="4" max="4" width="40.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1858,10 +1853,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>4.7916666666666663E-2</v>
+        <v>7.4305555555555555E-2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1870,16 +1865,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15763888888888888</v>
+        <v>0.13263888888888889</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1888,16 +1883,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.16527777777777777</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1906,16 +1901,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2">
-        <v>0.11597222222222221</v>
+        <v>0.16458333333333333</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1924,16 +1919,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>3.7499999999999999E-2</v>
+        <v>0.15</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1942,16 +1937,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>8.4027777777777771E-2</v>
+        <v>9.2361111111111116E-2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1960,16 +1955,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.18611111111111112</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1978,16 +1973,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12847222222222224</v>
+        <v>0.21875</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1996,16 +1991,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>9.375E-2</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -2014,16 +2009,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E11" s="2">
-        <v>0.18124999999999999</v>
+        <v>0.17847222222222223</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -2032,16 +2027,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.10902777777777778</v>
+        <v>0.1986111111111111</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -2050,35 +2045,21 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.18611111111111112</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="2">
-        <v>4.0972222222222222E-2</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">

</xml_diff>

<commit_message>
feat: 06302315 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,11 +17,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="jcole3" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="jcole3" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="nipseyhustle1" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="nipseyhustle1" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/jcole3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/nipseyhustle1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/jcole3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/nipseyhustle1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="45">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,82 +72,121 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Intro</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Richard Clay, Carl Clay, Wayne Garfield</t>
-  </si>
-  <si>
-    <t>J. Cole</t>
-  </si>
-  <si>
-    <t>KOD</t>
-  </si>
-  <si>
-    <t>Jermaine Cole</t>
-  </si>
-  <si>
-    <t>Photograph</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Raymond Evans, Jay Livingston, Francis Hime</t>
-  </si>
-  <si>
-    <t>The Cut Off</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Kill Edward, Bill Withers, Takehiro Honda</t>
-  </si>
-  <si>
-    <t>J. Cole feat,. Kill Edward</t>
-  </si>
-  <si>
-    <t>ATM</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Nicholas Brodszky, ]Sammy Cahn</t>
-  </si>
-  <si>
-    <t>Motiv8</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Roy Ayers, James Bedford, Lamont Porter, Sylvia Striplin, Christopher Wallace</t>
-  </si>
-  <si>
-    <t>Kevin's Heart</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Tyler Williams, Mark Pellizzer</t>
-  </si>
-  <si>
-    <t>Brackets</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Richard Pryor, Marilyn Bergman, Alan Bergman, Quincy Jones</t>
-  </si>
-  <si>
-    <t>Once an Addict (Interlude)</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Ron Gilmore, Micha? Urbaniak</t>
-  </si>
-  <si>
-    <t>Friends</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Kill Edward, John Dankworth</t>
-  </si>
-  <si>
-    <t>Window Pain (Outro)</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Kill Edward</t>
-  </si>
-  <si>
-    <t>1985 (Intro to "The Fall Off")</t>
-  </si>
-  <si>
-    <t>Jermaine Cole, Jorge Barreiro</t>
+    <t>Victory Lap</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Stacy Barthe / Amaire Johnson / Jonathan King / Alex Turner</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. Stacey Barthe</t>
+  </si>
+  <si>
+    <t>Rap Niggas</t>
+  </si>
+  <si>
+    <t>Khalil Abdul-Rahman / Ermias Asghedom / Larrance Dopson / James Groover / Michael Cox, Jr.</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle</t>
+  </si>
+  <si>
+    <t>Last Time That I Checc'd</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Christopher "Brody" Brown / Larrance Dopson / James Groover / Keenan Jackson / Zairyus Jackson / Michael Cox, Jr.</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. YG</t>
+  </si>
+  <si>
+    <t>Young Nigga</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Sean Combs / Larrance Dopson / James Groover / Michael Cox, Jr. / Jaire Kwayera Clarence Lewis / Elgin Lumpkin / Curtis Mayfield / Axel Morgan / Timothy Mosley / PartyNextDoor / Robert Reives</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. Puff Daddy</t>
+  </si>
+  <si>
+    <t>Dedication</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Alexandria Dopson / Larrance Dopson / Kendrick Duckworth / Lamar Edwards / James Groover / Michael Cox, Jr. / Axel Morgan</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle Kendrick Lamar</t>
+  </si>
+  <si>
+    <t>Blue Laces 2</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Larrance Dopson / James Groover / Willie Hutch / Michael Cox, Jr. / Leroy Williams</t>
+  </si>
+  <si>
+    <t>Hussle &amp; Motivate</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Shawn Carter / Martin Charmin / Torrance Esmond / Askia Fountain / James Groover / Mark James / Michael Cox, Jr. / Derrick Okoth / Charles Strouse / Maurice David Wade</t>
+  </si>
+  <si>
+    <t>Status Symbol 3</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / James Groover / Michael Cox, Jr. / Simmie Sims</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. Buddy</t>
+  </si>
+  <si>
+    <t>Succa Proof</t>
+  </si>
+  <si>
+    <t>Khalil Abdul-Rahman / Ermias Asghedom / Larrance Dopson / Garnett Flynn / Jaret Griffin-Black / James Groover / Michael Cox, Jr. / Garfield Spence</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. Konshens and J.Black</t>
+  </si>
+  <si>
+    <t>Keyz 2 the City 2</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Braylin Bowman / Joshua Conerly / Jacob Dutton / James Groover / Joshua Henderson / Christian Jones / Michael Cox, Jr. / Teddy Walton</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. TeeFlii</t>
+  </si>
+  <si>
+    <t>Grinding All My Life</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Askia Fountain / Shane Lindstrom</t>
+  </si>
+  <si>
+    <t>Million While You Young</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Jacob Dutton / Lamar Edwards / James Groover / Amaire Johnson / Michael Cox, Jr. / Robert Mandell / Terius Nash</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. The-Dream</t>
+  </si>
+  <si>
+    <t>Loaded Bases</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Larrance Dopson / Jake Dutton / Cee Lo Green</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. Cee-Lo Green</t>
+  </si>
+  <si>
+    <t>Real Big</t>
+  </si>
+  <si>
+    <t>Ermias Asghedom / Alexandria Dopson / Larrance Dopson / James Groover / Michael Cox, Jr. / Rebekah Muhammad</t>
+  </si>
+  <si>
+    <t>Nipsey Hussle feat. Marsha Ambrosius</t>
   </si>
 </sst>
 </file>
@@ -246,11 +284,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jcole3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nipseyhustle1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="jcole3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nipseyhustle1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -553,16 +591,17 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -590,7 +629,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>7.4305555555555555E-2</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -605,10 +644,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.13263888888888889</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -617,16 +656,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.15625</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -635,16 +674,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16458333333333333</v>
+        <v>0.16388888888888889</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -653,16 +692,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
-        <v>0.15</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -671,16 +710,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
-        <v>9.2361111111111116E-2</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -689,16 +728,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.17916666666666667</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -707,16 +746,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>0.21875</v>
+        <v>0.21180555555555555</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -725,16 +764,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -743,16 +782,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2">
-        <v>0.17847222222222223</v>
+        <v>0.12847222222222224</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -761,16 +800,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1986111111111111</v>
+        <v>0.12152777777777778</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -779,25 +818,53 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.18333333333333335</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.13263888888888889</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.64652777777777781</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
@@ -854,7 +921,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="A3:K16"/>
+      <selection activeCell="K18" sqref="A3:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -874,15 +941,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>92</v>
+        <v>209</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -902,21 +969,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                         </v>
+        <v xml:space="preserve"> Title                   </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                  </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                                                                       </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                 </v>
+        <v xml:space="preserve"> Performer                               </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -941,21 +1008,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------------------ </v>
+        <v xml:space="preserve">------------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -980,28 +1047,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Intro                         </v>
+        <v xml:space="preserve">Victory Lap             </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Richard Clay, Carl Clay, Wayne Garfield                                      </v>
+        <v xml:space="preserve"> Ermias Asghedom / Stacy Barthe / Amaire Johnson / Jonathan King / Alex Turner                                                                                                                                    </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle feat. Stacey Barthe       </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:47 </v>
+        <v xml:space="preserve">03:58 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1020,28 +1087,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">KOD                           </v>
+        <v xml:space="preserve">Rap Niggas              </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole                                                                               </v>
+        <v xml:space="preserve"> Khalil Abdul-Rahman / Ermias Asghedom / Larrance Dopson / James Groover / Michael Cox, Jr.                                                                                                                       </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle                           </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:11 </v>
+        <v xml:space="preserve">03:46 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1060,28 +1127,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Photograph                    </v>
+        <v>Last Time That I Checc'd</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Raymond Evans, Jay Livingston, Francis Hime                                  </v>
+        <v xml:space="preserve"> Ermias Asghedom / Christopher "Brody" Brown / Larrance Dopson / James Groover / Keenan Jackson / Zairyus Jackson / Michael Cox, Jr.                                                                              </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle feat. YG                  </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:38 </v>
+        <v xml:space="preserve">03:45 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1100,28 +1167,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Cut Off                   </v>
+        <v xml:space="preserve">Young Nigga             </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Kill Edward, Bill Withers, Takehiro Honda                                    </v>
+        <v xml:space="preserve"> Ermias Asghedom / Sean Combs / Larrance Dopson / James Groover / Michael Cox, Jr. / Jaire Kwayera Clarence Lewis / Elgin Lumpkin / Curtis Mayfield / Axel Morgan / Timothy Mosley / PartyNextDoor / Robert Reives</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>J. Cole feat,. Kill Edward</v>
+        <v xml:space="preserve">Nipsey Hussle feat. Puff Daddy          </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:57 </v>
+        <v xml:space="preserve">03:56 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1140,28 +1207,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">ATM                           </v>
+        <v xml:space="preserve">Dedication              </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Nicholas Brodszky, ]Sammy Cahn                                               </v>
+        <v xml:space="preserve"> Ermias Asghedom / Alexandria Dopson / Larrance Dopson / Kendrick Duckworth / Lamar Edwards / James Groover / Michael Cox, Jr. / Axel Morgan                                                                      </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle Kendrick Lamar            </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:36 </v>
+        <v xml:space="preserve">04:05 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1180,28 +1247,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Motiv8                        </v>
+        <v xml:space="preserve">Blue Laces 2            </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Roy Ayers, James Bedford, Lamont Porter, Sylvia Striplin, Christopher Wallace</v>
+        <v xml:space="preserve"> Ermias Asghedom / Larrance Dopson / James Groover / Willie Hutch / Michael Cox, Jr. / Leroy Williams                                                                                                             </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle                           </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:13 </v>
+        <v xml:space="preserve">04:10 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1220,28 +1287,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Kevin's Heart                 </v>
+        <v xml:space="preserve">Hussle &amp; Motivate       </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Tyler Williams, Mark Pellizzer                                               </v>
+        <v xml:space="preserve"> Ermias Asghedom / Shawn Carter / Martin Charmin / Torrance Esmond / Askia Fountain / James Groover / Mark James / Michael Cox, Jr. / Derrick Okoth / Charles Strouse / Maurice David Wade                        </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle                           </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:20 </v>
+        <v xml:space="preserve">04:18 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1260,28 +1327,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Brackets                      </v>
+        <v xml:space="preserve">Status Symbol 3         </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Richard Pryor, Marilyn Bergman, Alan Bergman, Quincy Jones                   </v>
+        <v xml:space="preserve"> Ermias Asghedom / James Groover / Michael Cox, Jr. / Simmie Sims                                                                                                                                                 </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle feat. Buddy               </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:15 </v>
+        <v xml:space="preserve">05:05 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1300,28 +1367,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Once an Addict (Interlude)    </v>
+        <v xml:space="preserve">Succa Proof             </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Ron Gilmore, Micha? Urbaniak                                                 </v>
+        <v xml:space="preserve"> Khalil Abdul-Rahman / Ermias Asghedom / Larrance Dopson / Garnett Flynn / Jaret Griffin-Black / James Groover / Michael Cox, Jr. / Garfield Spence                                                               </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v>Nipsey Hussle feat. Konshens and J.Black</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:17 </v>
+        <v xml:space="preserve">03:21 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1340,28 +1407,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Friends                       </v>
+        <v xml:space="preserve">Keyz 2 the City 2       </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Kill Edward, John Dankworth                                                  </v>
+        <v xml:space="preserve"> Ermias Asghedom / Braylin Bowman / Joshua Conerly / Jacob Dutton / James Groover / Joshua Henderson / Christian Jones / Michael Cox, Jr. / Teddy Walton                                                          </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>J. Cole feat,. Kill Edward</v>
+        <v xml:space="preserve">Nipsey Hussle feat. TeeFlii             </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:17 </v>
+        <v xml:space="preserve">03:05 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1380,28 +1447,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Window Pain (Outro)           </v>
+        <v xml:space="preserve">Grinding All My Life    </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Kill Edward                                                                  </v>
+        <v xml:space="preserve"> Ermias Asghedom / Askia Fountain / Shane Lindstrom                                                                                                                                                               </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle                           </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:46 </v>
+        <v xml:space="preserve">02:55 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1420,28 +1487,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>1985 (Intro to "The Fall Off")</v>
+        <v xml:space="preserve">Million While You Young </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole, Jorge Barreiro                                                               </v>
+        <v xml:space="preserve"> Ermias Asghedom / Jacob Dutton / Lamar Edwards / James Groover / Amaire Johnson / Michael Cox, Jr. / Robert Mandell / Terius Nash                                                                                </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">J. Cole                   </v>
+        <v xml:space="preserve">Nipsey Hussle feat. The-Dream           </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:10 </v>
+        <v xml:space="preserve">04:24 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1453,35 +1520,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">Loaded Bases            </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve"> Ermias Asghedom / Larrance Dopson / Jake Dutton / Cee Lo Green                                                                                                                                                   </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">Nipsey Hussle feat. Cee-Lo Green        </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:11 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1493,35 +1560,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">Real Big                </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve"> Ermias Asghedom / Alexandria Dopson / Larrance Dopson / James Groover / Michael Cox, Jr. / Rebekah Muhammad                                                                                                      </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">Nipsey Hussle feat. Marsha Ambrosius    </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">15:31 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1540,21 +1607,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1580,21 +1647,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1620,21 +1687,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1660,21 +1727,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1700,21 +1767,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1740,21 +1807,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1780,21 +1847,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                          </v>
+        <v xml:space="preserve">                                        </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1825,10 +1892,11 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="27.109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1856,7 +1924,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>7.4305555555555555E-2</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1871,10 +1939,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.13263888888888889</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1883,16 +1951,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.15625</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1901,16 +1969,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16458333333333333</v>
+        <v>0.16388888888888889</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1919,16 +1987,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
-        <v>0.15</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1937,16 +2005,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
-        <v>9.2361111111111116E-2</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1955,16 +2023,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.17916666666666667</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1973,16 +2041,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>0.21875</v>
+        <v>0.21180555555555555</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1991,16 +2059,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -2009,16 +2077,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2">
-        <v>0.17847222222222223</v>
+        <v>0.12847222222222224</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -2027,16 +2095,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1986111111111111</v>
+        <v>0.12152777777777778</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -2045,25 +2113,53 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="E13" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.18333333333333335</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.13263888888888889</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.64652777777777781</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">

</xml_diff>

<commit_message>
feat: 07022300 added 2 old reviews.
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="nipseyhustle1" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
-    <definedName name="nipseyhustle1" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
+    <definedName name="brandoncoleman1" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="brandoncoleman1" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/nipseyhustle1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/brandoncoleman1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/nipseyhustle1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/brandoncoleman1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="31">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,121 +72,79 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Victory Lap</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Stacy Barthe / Amaire Johnson / Jonathan King / Alex Turner</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. Stacey Barthe</t>
-  </si>
-  <si>
-    <t>Rap Niggas</t>
-  </si>
-  <si>
-    <t>Khalil Abdul-Rahman / Ermias Asghedom / Larrance Dopson / James Groover / Michael Cox, Jr.</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle</t>
-  </si>
-  <si>
-    <t>Last Time That I Checc'd</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Christopher "Brody" Brown / Larrance Dopson / James Groover / Keenan Jackson / Zairyus Jackson / Michael Cox, Jr.</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. YG</t>
-  </si>
-  <si>
-    <t>Young Nigga</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Sean Combs / Larrance Dopson / James Groover / Michael Cox, Jr. / Jaire Kwayera Clarence Lewis / Elgin Lumpkin / Curtis Mayfield / Axel Morgan / Timothy Mosley / PartyNextDoor / Robert Reives</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. Puff Daddy</t>
-  </si>
-  <si>
-    <t>Dedication</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Alexandria Dopson / Larrance Dopson / Kendrick Duckworth / Lamar Edwards / James Groover / Michael Cox, Jr. / Axel Morgan</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle Kendrick Lamar</t>
-  </si>
-  <si>
-    <t>Blue Laces 2</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Larrance Dopson / James Groover / Willie Hutch / Michael Cox, Jr. / Leroy Williams</t>
-  </si>
-  <si>
-    <t>Hussle &amp; Motivate</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Shawn Carter / Martin Charmin / Torrance Esmond / Askia Fountain / James Groover / Mark James / Michael Cox, Jr. / Derrick Okoth / Charles Strouse / Maurice David Wade</t>
-  </si>
-  <si>
-    <t>Status Symbol 3</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / James Groover / Michael Cox, Jr. / Simmie Sims</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. Buddy</t>
-  </si>
-  <si>
-    <t>Succa Proof</t>
-  </si>
-  <si>
-    <t>Khalil Abdul-Rahman / Ermias Asghedom / Larrance Dopson / Garnett Flynn / Jaret Griffin-Black / James Groover / Michael Cox, Jr. / Garfield Spence</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. Konshens and J.Black</t>
-  </si>
-  <si>
-    <t>Keyz 2 the City 2</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Braylin Bowman / Joshua Conerly / Jacob Dutton / James Groover / Joshua Henderson / Christian Jones / Michael Cox, Jr. / Teddy Walton</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. TeeFlii</t>
-  </si>
-  <si>
-    <t>Grinding All My Life</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Askia Fountain / Shane Lindstrom</t>
-  </si>
-  <si>
-    <t>Million While You Young</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Jacob Dutton / Lamar Edwards / James Groover / Amaire Johnson / Michael Cox, Jr. / Robert Mandell / Terius Nash</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. The-Dream</t>
-  </si>
-  <si>
-    <t>Loaded Bases</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Larrance Dopson / Jake Dutton / Cee Lo Green</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. Cee-Lo Green</t>
-  </si>
-  <si>
-    <t>Real Big</t>
-  </si>
-  <si>
-    <t>Ermias Asghedom / Alexandria Dopson / Larrance Dopson / James Groover / Michael Cox, Jr. / Rebekah Muhammad</t>
-  </si>
-  <si>
-    <t>Nipsey Hussle feat. Marsha Ambrosius</t>
+    <t>Live for Today</t>
+  </si>
+  <si>
+    <t>Sam Brawner / Brandon Coleman</t>
+  </si>
+  <si>
+    <t>Brandon Coleman</t>
+  </si>
+  <si>
+    <t>All Around the World</t>
+  </si>
+  <si>
+    <t>Brandon Coleman / Corey Mason / Dominic Thiroux</t>
+  </si>
+  <si>
+    <t>A Letter to My Buggers</t>
+  </si>
+  <si>
+    <t>Brandon Coleman / Crystal Starr Knighton / Dominic Thiroux</t>
+  </si>
+  <si>
+    <t>Addiction</t>
+  </si>
+  <si>
+    <t>Brandon Coleman / Sheera Ehrig</t>
+  </si>
+  <si>
+    <t>Brandon Coleman feat. Sheera</t>
+  </si>
+  <si>
+    <t>Sexy</t>
+  </si>
+  <si>
+    <t>Brandon Coleman / Robert Miller</t>
+  </si>
+  <si>
+    <t>There's No Turning Back</t>
+  </si>
+  <si>
+    <t>Brandon Coleman / Jasmine Mitchell</t>
+  </si>
+  <si>
+    <t>Resistance</t>
+  </si>
+  <si>
+    <t>Sundae</t>
+  </si>
+  <si>
+    <t>Brandon Coleman / N'Dambi</t>
+  </si>
+  <si>
+    <t>Brandon Coleman feat. N'Dambi</t>
+  </si>
+  <si>
+    <t>Just Reach for the Stars</t>
+  </si>
+  <si>
+    <t>Brandon Coleman / Patrice Quinn</t>
+  </si>
+  <si>
+    <t>Love</t>
+  </si>
+  <si>
+    <t>Brandon Coleman / Richie Pena</t>
+  </si>
+  <si>
+    <t>Giant Feelings</t>
+  </si>
+  <si>
+    <t>Brandon Coleman feat. Patrice Quinn, Techdizzle</t>
+  </si>
+  <si>
+    <t>Walk Free</t>
   </si>
 </sst>
 </file>
@@ -284,11 +242,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nipseyhustle1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="brandoncoleman1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="nipseyhustle1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="brandoncoleman1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,17 +549,16 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="38.21875" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="4" max="4" width="44.88671875" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -629,7 +586,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16527777777777777</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -644,10 +601,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -656,16 +613,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15625</v>
+        <v>0.18402777777777779</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -674,16 +631,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="2">
-        <v>0.16388888888888889</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -692,16 +649,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17013888888888887</v>
+        <v>0.18888888888888888</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -710,16 +667,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.17361111111111113</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -728,16 +685,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17916666666666667</v>
+        <v>7.7083333333333337E-2</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -746,16 +703,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
-        <v>0.21180555555555555</v>
+        <v>0.15069444444444444</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -764,16 +721,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13958333333333334</v>
+        <v>8.4722222222222213E-2</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -782,16 +739,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.12847222222222224</v>
+        <v>0.17083333333333331</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -800,16 +757,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12152777777777778</v>
+        <v>0.23819444444444446</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -818,53 +775,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.18333333333333335</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.13263888888888889</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.64652777777777781</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
@@ -921,7 +850,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="A3:K18"/>
+      <selection activeCell="A3" sqref="A3:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -945,11 +874,11 @@
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>209</v>
+        <v>58</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -976,14 +905,14 @@
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                                                                       </v>
+        <v xml:space="preserve"> Composers                                                </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                               </v>
+        <v xml:space="preserve"> Performer                                      </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1015,14 +944,14 @@
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1047,28 +976,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Victory Lap             </v>
+        <v xml:space="preserve">Live for Today          </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Stacy Barthe / Amaire Johnson / Jonathan King / Alex Turner                                                                                                                                    </v>
+        <v xml:space="preserve"> Sam Brawner / Brandon Coleman                             </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle feat. Stacey Barthe       </v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:58 </v>
+        <v xml:space="preserve">04:03 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1087,28 +1016,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Rap Niggas              </v>
+        <v xml:space="preserve">All Around the World    </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Khalil Abdul-Rahman / Ermias Asghedom / Larrance Dopson / James Groover / Michael Cox, Jr.                                                                                                                       </v>
+        <v xml:space="preserve"> Brandon Coleman / Corey Mason / Dominic Thiroux           </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle                           </v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:46 </v>
+        <v xml:space="preserve">04:03 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1127,28 +1056,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Last Time That I Checc'd</v>
+        <v xml:space="preserve">A Letter to My Buggers  </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Christopher "Brody" Brown / Larrance Dopson / James Groover / Keenan Jackson / Zairyus Jackson / Michael Cox, Jr.                                                                              </v>
+        <v xml:space="preserve"> Brandon Coleman / Crystal Starr Knighton / Dominic Thiroux</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle feat. YG                  </v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:45 </v>
+        <v xml:space="preserve">04:25 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1167,28 +1096,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Young Nigga             </v>
+        <v xml:space="preserve">Addiction               </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Sean Combs / Larrance Dopson / James Groover / Michael Cox, Jr. / Jaire Kwayera Clarence Lewis / Elgin Lumpkin / Curtis Mayfield / Axel Morgan / Timothy Mosley / PartyNextDoor / Robert Reives</v>
+        <v xml:space="preserve"> Brandon Coleman / Sheera Ehrig                            </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle feat. Puff Daddy          </v>
+        <v xml:space="preserve">Brandon Coleman feat. Sheera                   </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:56 </v>
+        <v xml:space="preserve">03:33 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1207,28 +1136,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dedication              </v>
+        <v xml:space="preserve">Sexy                    </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Alexandria Dopson / Larrance Dopson / Kendrick Duckworth / Lamar Edwards / James Groover / Michael Cox, Jr. / Axel Morgan                                                                      </v>
+        <v xml:space="preserve"> Brandon Coleman / Robert Miller                           </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle Kendrick Lamar            </v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:05 </v>
+        <v xml:space="preserve">04:32 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1247,28 +1176,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Blue Laces 2            </v>
+        <v xml:space="preserve">There's No Turning Back </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Larrance Dopson / James Groover / Willie Hutch / Michael Cox, Jr. / Leroy Williams                                                                                                             </v>
+        <v xml:space="preserve"> Brandon Coleman / Jasmine Mitchell                        </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle                           </v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:10 </v>
+        <v xml:space="preserve">02:20 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1287,28 +1216,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hussle &amp; Motivate       </v>
+        <v xml:space="preserve">Resistance              </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Shawn Carter / Martin Charmin / Torrance Esmond / Askia Fountain / James Groover / Mark James / Michael Cox, Jr. / Derrick Okoth / Charles Strouse / Maurice David Wade                        </v>
+        <v xml:space="preserve"> Brandon Coleman                                           </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle                           </v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:18 </v>
+        <v xml:space="preserve">01:51 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1327,28 +1256,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Status Symbol 3         </v>
+        <v xml:space="preserve">Sundae                  </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / James Groover / Michael Cox, Jr. / Simmie Sims                                                                                                                                                 </v>
+        <v xml:space="preserve"> Brandon Coleman / N'Dambi                                 </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle feat. Buddy               </v>
+        <v xml:space="preserve">Brandon Coleman feat. N'Dambi                  </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:05 </v>
+        <v xml:space="preserve">03:37 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1367,28 +1296,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Succa Proof             </v>
+        <v>Just Reach for the Stars</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Khalil Abdul-Rahman / Ermias Asghedom / Larrance Dopson / Garnett Flynn / Jaret Griffin-Black / James Groover / Michael Cox, Jr. / Garfield Spence                                                               </v>
+        <v xml:space="preserve"> Brandon Coleman / Patrice Quinn                           </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Nipsey Hussle feat. Konshens and J.Black</v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:21 </v>
+        <v xml:space="preserve">02:02 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1407,28 +1336,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Keyz 2 the City 2       </v>
+        <v xml:space="preserve">Love                    </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Braylin Bowman / Joshua Conerly / Jacob Dutton / James Groover / Joshua Henderson / Christian Jones / Michael Cox, Jr. / Teddy Walton                                                          </v>
+        <v xml:space="preserve"> Brandon Coleman / Richie Pena                             </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle feat. TeeFlii             </v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:05 </v>
+        <v xml:space="preserve">04:06 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1447,28 +1376,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Grinding All My Life    </v>
+        <v xml:space="preserve">Giant Feelings          </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Askia Fountain / Shane Lindstrom                                                                                                                                                               </v>
+        <v xml:space="preserve"> Brandon Coleman                                           </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle                           </v>
+        <v>Brandon Coleman feat. Patrice Quinn, Techdizzle</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:55 </v>
+        <v xml:space="preserve">05:43 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1487,28 +1416,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Million While You Young </v>
+        <v xml:space="preserve">Walk Free               </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Jacob Dutton / Lamar Edwards / James Groover / Amaire Johnson / Michael Cox, Jr. / Robert Mandell / Terius Nash                                                                                </v>
+        <v xml:space="preserve"> Brandon Coleman                                           </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle feat. The-Dream           </v>
+        <v xml:space="preserve">Brandon Coleman                                </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:24 </v>
+        <v xml:space="preserve">03:55 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1520,35 +1449,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Loaded Bases            </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Larrance Dopson / Jake Dutton / Cee Lo Green                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle feat. Cee-Lo Green        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:11 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1560,35 +1489,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Real Big                </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ermias Asghedom / Alexandria Dopson / Larrance Dopson / James Groover / Michael Cox, Jr. / Rebekah Muhammad                                                                                                      </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Nipsey Hussle feat. Marsha Ambrosius    </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">15:31 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1614,14 +1543,14 @@
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1654,14 +1583,14 @@
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1694,14 +1623,14 @@
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1734,14 +1663,14 @@
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1774,14 +1703,14 @@
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1814,14 +1743,14 @@
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1854,14 +1783,14 @@
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                           </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1892,11 +1821,10 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="38.21875" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="4" max="4" width="44.88671875" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1924,7 +1852,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16527777777777777</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1939,10 +1867,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1951,16 +1879,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15625</v>
+        <v>0.18402777777777779</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1969,16 +1897,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="2">
-        <v>0.16388888888888889</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1987,16 +1915,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17013888888888887</v>
+        <v>0.18888888888888888</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -2005,16 +1933,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.17361111111111113</v>
+        <v>9.7222222222222224E-2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -2023,16 +1951,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17916666666666667</v>
+        <v>7.7083333333333337E-2</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -2041,16 +1969,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
-        <v>0.21180555555555555</v>
+        <v>0.15069444444444444</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -2059,16 +1987,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.13958333333333334</v>
+        <v>8.4722222222222213E-2</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -2077,16 +2005,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.12847222222222224</v>
+        <v>0.17083333333333331</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -2095,16 +2023,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12152777777777778</v>
+        <v>0.23819444444444446</v>
       </c>
       <c r="F12" s="2"/>
     </row>
@@ -2113,53 +2041,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.18333333333333335</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.13263888888888889</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.64652777777777781</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">

</xml_diff>

<commit_message>
feat: 07042455 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="brandoncoleman1" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="brandoncoleman1" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="weeknd5" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="weeknd5" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/brandoncoleman1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/weeknd5.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/brandoncoleman1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/weeknd5.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="21">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -63,88 +63,58 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Performer</t>
-  </si>
-  <si>
-    <t>Title/Composer</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Live for Today</t>
-  </si>
-  <si>
-    <t>Sam Brawner / Brandon Coleman</t>
-  </si>
-  <si>
-    <t>Brandon Coleman</t>
-  </si>
-  <si>
-    <t>All Around the World</t>
-  </si>
-  <si>
-    <t>Brandon Coleman / Corey Mason / Dominic Thiroux</t>
-  </si>
-  <si>
-    <t>A Letter to My Buggers</t>
-  </si>
-  <si>
-    <t>Brandon Coleman / Crystal Starr Knighton / Dominic Thiroux</t>
-  </si>
-  <si>
-    <t>Addiction</t>
-  </si>
-  <si>
-    <t>Brandon Coleman / Sheera Ehrig</t>
-  </si>
-  <si>
-    <t>Brandon Coleman feat. Sheera</t>
-  </si>
-  <si>
-    <t>Sexy</t>
-  </si>
-  <si>
-    <t>Brandon Coleman / Robert Miller</t>
-  </si>
-  <si>
-    <t>There's No Turning Back</t>
-  </si>
-  <si>
-    <t>Brandon Coleman / Jasmine Mitchell</t>
-  </si>
-  <si>
-    <t>Resistance</t>
-  </si>
-  <si>
-    <t>Sundae</t>
-  </si>
-  <si>
-    <t>Brandon Coleman / N'Dambi</t>
-  </si>
-  <si>
-    <t>Brandon Coleman feat. N'Dambi</t>
-  </si>
-  <si>
-    <t>Just Reach for the Stars</t>
-  </si>
-  <si>
-    <t>Brandon Coleman / Patrice Quinn</t>
-  </si>
-  <si>
-    <t>Love</t>
-  </si>
-  <si>
-    <t>Brandon Coleman / Richie Pena</t>
-  </si>
-  <si>
-    <t>Giant Feelings</t>
-  </si>
-  <si>
-    <t>Brandon Coleman feat. Patrice Quinn, Techdizzle</t>
-  </si>
-  <si>
-    <t>Walk Free</t>
+    <t xml:space="preserve"> Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Composer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Performer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time </t>
+  </si>
+  <si>
+    <t>Call Out My Name</t>
+  </si>
+  <si>
+    <t>Abel "The Weeknd" Tesfaye, Adam Feeney, Nicolas Jaar</t>
+  </si>
+  <si>
+    <t>The Weeknd</t>
+  </si>
+  <si>
+    <t>Try Me</t>
+  </si>
+  <si>
+    <t>Abel "The Weeknd" Tesfaye, Ahmad Balshe, Jason Quenneville, Adam Feeney, Michael Len Williams II, Marquel Middlebrooks</t>
+  </si>
+  <si>
+    <t>Wasted Times</t>
+  </si>
+  <si>
+    <t>Abel "The Weeknd" Tesfaye, Brittany "Starrah" Hazzard, Sonny Moore, Adam Feeney</t>
+  </si>
+  <si>
+    <t>I Was Never There</t>
+  </si>
+  <si>
+    <t>Abel "The Weeknd" Tesfaye, Mike L?vy, Adam Feeney</t>
+  </si>
+  <si>
+    <t>The Weeknd feat. Gesaffelstein</t>
+  </si>
+  <si>
+    <t>Hurt You</t>
+  </si>
+  <si>
+    <t>Guy-Manuel de Homem-Christo, Abel "The Weeknd" Tesfaye, Mike L?vy, Henry Russell Walter</t>
+  </si>
+  <si>
+    <t>Privilege</t>
+  </si>
+  <si>
+    <t>Abel "The Weeknd" Tesfaye, Jason Quenneville, Adam Feeney</t>
   </si>
 </sst>
 </file>
@@ -242,11 +212,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="brandoncoleman1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="weeknd5" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="brandoncoleman1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="weeknd5" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -549,27 +519,31 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -577,16 +551,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -595,16 +569,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -613,16 +587,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.18402777777777779</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -631,16 +605,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>0.14791666666666667</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -649,16 +623,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="2">
-        <v>0.18888888888888888</v>
+        <v>0.15972222222222224</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -667,125 +641,43 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>9.7222222222222224E-2</v>
+        <v>0.11805555555555557</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2">
-        <v>7.7083333333333337E-2</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.15069444444444444</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8.4722222222222213E-2</v>
-      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.17083333333333331</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.23819444444444446</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.16319444444444445</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
@@ -849,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -870,15 +762,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -898,21 +790,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                   </v>
+        <v xml:space="preserve"> Title            </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                </v>
+        <v xml:space="preserve"> Composers                                                                                                            </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                      </v>
+        <v xml:space="preserve"> Performer                     </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -937,21 +829,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------------ </v>
+        <v xml:space="preserve">----------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------ </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -976,28 +868,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Live for Today          </v>
+        <v xml:space="preserve">Call Out My Name </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Sam Brawner / Brandon Coleman                             </v>
+        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Adam Feeney, Nicolas Jaar                                                                  </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v xml:space="preserve">The Weeknd                    </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:03 </v>
+        <v xml:space="preserve">03:48 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1016,28 +908,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">All Around the World    </v>
+        <v xml:space="preserve">Try Me           </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman / Corey Mason / Dominic Thiroux           </v>
+        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Ahmad Balshe, Jason Quenneville, Adam Feeney, Michael Len Williams II, Marquel Middlebrooks</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v xml:space="preserve">The Weeknd                    </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:03 </v>
+        <v xml:space="preserve">03:41 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1056,28 +948,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">A Letter to My Buggers  </v>
+        <v xml:space="preserve">Wasted Times     </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman / Crystal Starr Knighton / Dominic Thiroux</v>
+        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Brittany "Starrah" Hazzard, Sonny Moore, Adam Feeney                                       </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v xml:space="preserve">The Weeknd                    </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:25 </v>
+        <v xml:space="preserve">03:40 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1096,28 +988,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Addiction               </v>
+        <v>I Was Never There</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman / Sheera Ehrig                            </v>
+        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Mike L?vy, Adam Feeney                                                                     </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman feat. Sheera                   </v>
+        <v>The Weeknd feat. Gesaffelstein</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:33 </v>
+        <v xml:space="preserve">04:01 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1136,28 +1028,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sexy                    </v>
+        <v xml:space="preserve">Hurt You         </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman / Robert Miller                           </v>
+        <v xml:space="preserve"> Guy-Manuel de Homem-Christo, Abel "The Weeknd" Tesfaye, Mike L?vy, Henry Russell Walter                               </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v>The Weeknd feat. Gesaffelstein</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:32 </v>
+        <v xml:space="preserve">03:50 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1176,28 +1068,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">There's No Turning Back </v>
+        <v xml:space="preserve">Privilege        </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman / Jasmine Mitchell                        </v>
+        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Jason Quenneville, Adam Feeney                                                             </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v xml:space="preserve">The Weeknd                    </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:20 </v>
+        <v xml:space="preserve">02:50 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1209,35 +1101,35 @@
       </c>
       <c r="B11">
         <f>Sheet1!A8</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Resistance              </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:51 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1249,35 +1141,35 @@
       </c>
       <c r="B12">
         <f>Sheet1!A9</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sundae                  </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman / N'Dambi                                 </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman feat. N'Dambi                  </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:37 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1289,35 +1181,35 @@
       </c>
       <c r="B13">
         <f>Sheet1!A10</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Just Reach for the Stars</v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman / Patrice Quinn                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:02 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1329,35 +1221,35 @@
       </c>
       <c r="B14">
         <f>Sheet1!A11</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Love                    </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman / Richie Pena                             </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:06 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1369,35 +1261,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Giant Feelings          </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Brandon Coleman feat. Patrice Quinn, Techdizzle</v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:43 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1409,35 +1301,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Walk Free               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Coleman                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Brandon Coleman                                </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:55 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1456,21 +1348,21 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
@@ -1496,21 +1388,21 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
@@ -1536,21 +1428,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1576,21 +1468,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1616,21 +1508,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1656,21 +1548,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1696,21 +1588,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1736,21 +1628,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1776,21 +1668,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                        </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                           </v>
+        <v xml:space="preserve">                                                                                                                       </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                              </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1820,22 +1712,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="44.88671875" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1843,16 +1739,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1861,16 +1757,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1879,16 +1775,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.18402777777777779</v>
+        <v>0.15277777777777776</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1897,16 +1793,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>0.14791666666666667</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1915,16 +1811,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="2">
-        <v>0.18888888888888888</v>
+        <v>0.15972222222222224</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1933,125 +1829,43 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>9.7222222222222224E-2</v>
+        <v>0.11805555555555557</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2">
-        <v>7.7083333333333337E-2</v>
-      </c>
+      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.15069444444444444</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8.4722222222222213E-2</v>
-      </c>
+      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.17083333333333331</v>
-      </c>
+      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.23819444444444446</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.16319444444444445</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">

</xml_diff>

<commit_message>
feat: 07051710 added new review
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\my-carbon-site\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +12,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="weeknd5" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="weeknd5" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="weeknd6" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="weeknd6" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,15 +26,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/weeknd5.htm" htmlTables="1">
+  <connection id="1" name="接続" type="4" refreshedVersion="4" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/weeknd6.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
-  <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/weeknd5.htm" htmlTables="1">
+  <connection id="2" name="接続1" type="4" refreshedVersion="4" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/weeknd6.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="34">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -63,68 +58,107 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve"> Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Composer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Performer </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time </t>
-  </si>
-  <si>
-    <t>Call Out My Name</t>
-  </si>
-  <si>
-    <t>Abel "The Weeknd" Tesfaye, Adam Feeney, Nicolas Jaar</t>
-  </si>
-  <si>
     <t>The Weeknd</t>
   </si>
   <si>
-    <t>Try Me</t>
-  </si>
-  <si>
-    <t>Abel "The Weeknd" Tesfaye, Ahmad Balshe, Jason Quenneville, Adam Feeney, Michael Len Williams II, Marquel Middlebrooks</t>
-  </si>
-  <si>
-    <t>Wasted Times</t>
-  </si>
-  <si>
-    <t>Abel "The Weeknd" Tesfaye, Brittany "Starrah" Hazzard, Sonny Moore, Adam Feeney</t>
-  </si>
-  <si>
-    <t>I Was Never There</t>
-  </si>
-  <si>
-    <t>Abel "The Weeknd" Tesfaye, Mike L?vy, Adam Feeney</t>
-  </si>
-  <si>
-    <t>The Weeknd feat. Gesaffelstein</t>
-  </si>
-  <si>
-    <t>Hurt You</t>
-  </si>
-  <si>
-    <t>Guy-Manuel de Homem-Christo, Abel "The Weeknd" Tesfaye, Mike L?vy, Henry Russell Walter</t>
-  </si>
-  <si>
-    <t>Privilege</t>
-  </si>
-  <si>
-    <t>Abel "The Weeknd" Tesfaye, Jason Quenneville, Adam Feeney</t>
+    <t>Title/Composer</t>
+  </si>
+  <si>
+    <t>Performer</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Alone Again</t>
+  </si>
+  <si>
+    <t>Adam Feeney / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Too Late</t>
+  </si>
+  <si>
+    <t>Eric Frederic / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Hardest to Love</t>
+  </si>
+  <si>
+    <t>Oscar Holter / Max Martin / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Scared to Live</t>
+  </si>
+  <si>
+    <t>Ahmad Balshe / Oscar Holter / Elton John / Daniel Lopatin / Max Martin / Bernie Taupin / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Snowchild</t>
+  </si>
+  <si>
+    <t>Ahmad Balshe / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Escape from LA</t>
+  </si>
+  <si>
+    <t>Metro Boomin / Mike McTaggart / Carlo "Illangelo" Montagnese / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Heartless</t>
+  </si>
+  <si>
+    <t>Metro Boomin / Carlo "Illangelo" Montagnese / Andre Proctor / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Faith</t>
+  </si>
+  <si>
+    <t>Ahmad Balshe / Metro Boomin / Carlo "Illangelo" Montagnese / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Blinding Lights</t>
+  </si>
+  <si>
+    <t>Ahmad Balshe / Oscar Holter / Max Martin / Jason Quenneville / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>In Your Eyes</t>
+  </si>
+  <si>
+    <t>Ahmad Balshe / Oscar Holter / Max Martin / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>Save Your Tears</t>
+  </si>
+  <si>
+    <t>Repeat After Me (Interlude)</t>
+  </si>
+  <si>
+    <t>Daniel Lopatin / Kevin Parker / Abel Tesfaye</t>
+  </si>
+  <si>
+    <t>After Hours</t>
+  </si>
+  <si>
+    <t>Ahmad Balshe / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye / Mario Winans</t>
+  </si>
+  <si>
+    <t>Until I Bleed Out</t>
+  </si>
+  <si>
+    <t>Metro Boomin / Daniel Lopatin / Notinbed / Mejdi Rhars / Abel Tesfaye</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,11 +246,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="weeknd5" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="weeknd6" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="weeknd5" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="weeknd6" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -508,7 +542,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -522,21 +556,18 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.26953125" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="3" width="80.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="5.453125" customWidth="1"/>
+    <col min="6" max="6" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
@@ -546,7 +577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -557,178 +588,288 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.16597222222222222</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.15347222222222223</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15277777777777776</v>
+        <v>0.14652777777777778</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.13263888888888889</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2">
-        <v>0.15972222222222224</v>
+        <v>0.17152777777777775</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.19652777777777777</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.11805555555555557</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="E10" s="2"/>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.14166666666666666</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
-      <c r="E11" s="2"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.16458333333333333</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6">
-      <c r="E12" s="2"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.14930555555555555</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="2"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.13541666666666666</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.25138888888888888</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.13194444444444445</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="5:6">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.5">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="5:6">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.5">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="5:6">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.5">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="5:6">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="5:6">
+    <row r="21" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="5:6">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="5:6">
+    <row r="23" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="5:6">
+    <row r="24" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="5:6">
+    <row r="25" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="5:6">
+    <row r="26" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="5:6">
+    <row r="27" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="5:6">
+    <row r="28" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F28" s="2"/>
     </row>
   </sheetData>
@@ -742,42 +883,42 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:K10"/>
+      <selection activeCell="K18" sqref="A3:K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.1796875" customWidth="1"/>
+    <col min="3" max="3" width="3.90625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.08984375" customWidth="1"/>
     <col min="5" max="5" width="4" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.21875" customWidth="1"/>
-    <col min="7" max="7" width="4.44140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" customWidth="1"/>
-    <col min="11" max="11" width="3.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.1796875" customWidth="1"/>
+    <col min="7" max="7" width="4.453125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" customWidth="1"/>
+    <col min="9" max="9" width="4.36328125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" customWidth="1"/>
+    <col min="11" max="11" width="3.453125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -790,21 +931,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title            </v>
+        <v xml:space="preserve"> Title                      </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                            </v>
+        <v xml:space="preserve"> Composers                                                                                           </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                     </v>
+        <v xml:space="preserve"> Performer </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -817,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -829,21 +970,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">----------------- </v>
+        <v xml:space="preserve">--------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------ </v>
+        <v xml:space="preserve"> ---------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -855,7 +996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -868,34 +1009,34 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Call Out My Name </v>
+        <v xml:space="preserve">Alone Again                </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Adam Feeney, Nicolas Jaar                                                                  </v>
+        <v xml:space="preserve"> Adam Feeney / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye                        </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">The Weeknd                    </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:48 </v>
+        <v xml:space="preserve">04:12 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -908,34 +1049,34 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Try Me           </v>
+        <v xml:space="preserve">Too Late                   </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Ahmad Balshe, Jason Quenneville, Adam Feeney, Michael Len Williams II, Marquel Middlebrooks</v>
+        <v xml:space="preserve"> Eric Frederic / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye                      </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">The Weeknd                    </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:41 </v>
+        <v xml:space="preserve">03:59 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -948,34 +1089,34 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Wasted Times     </v>
+        <v xml:space="preserve">Hardest to Love            </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Brittany "Starrah" Hazzard, Sonny Moore, Adam Feeney                                       </v>
+        <v xml:space="preserve"> Oscar Holter / Max Martin / Abel Tesfaye                                                             </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">The Weeknd                    </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:40 </v>
+        <v xml:space="preserve">03:31 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -988,34 +1129,34 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>I Was Never There</v>
+        <v xml:space="preserve">Scared to Live             </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Mike L?vy, Adam Feeney                                                                     </v>
+        <v xml:space="preserve"> Ahmad Balshe / Oscar Holter / Elton John / Daniel Lopatin / Max Martin / Bernie Taupin / Abel Tesfaye</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd feat. Gesaffelstein</v>
+        <v>The Weeknd</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:01 </v>
+        <v xml:space="preserve">03:11 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1028,34 +1169,34 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hurt You         </v>
+        <v xml:space="preserve">Snowchild                  </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Guy-Manuel de Homem-Christo, Abel "The Weeknd" Tesfaye, Mike L?vy, Henry Russell Walter                               </v>
+        <v xml:space="preserve"> Ahmad Balshe / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye                       </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd feat. Gesaffelstein</v>
+        <v>The Weeknd</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:50 </v>
+        <v xml:space="preserve">04:07 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1068,354 +1209,354 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Privilege        </v>
+        <v xml:space="preserve">Escape from LA             </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Abel "The Weeknd" Tesfaye, Jason Quenneville, Adam Feeney                                                             </v>
+        <v xml:space="preserve"> Metro Boomin / Mike McTaggart / Carlo "Illangelo" Montagnese / Abel Tesfaye                          </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">The Weeknd                    </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:50 </v>
+        <v xml:space="preserve">05:55 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11">
         <f>Sheet1!A8</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">Heartless                  </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve"> Metro Boomin / Carlo "Illangelo" Montagnese / Andre Proctor / Abel Tesfaye                           </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:20 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12">
         <f>Sheet1!A9</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">Faith                      </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve"> Ahmad Balshe / Metro Boomin / Carlo "Illangelo" Montagnese / Abel Tesfaye                            </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:43 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13">
         <f>Sheet1!A10</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">Blinding Lights            </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve"> Ahmad Balshe / Oscar Holter / Max Martin / Jason Quenneville / Abel Tesfaye                          </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:24 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14">
         <f>Sheet1!A11</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">In Your Eyes               </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve"> Ahmad Balshe / Oscar Holter / Max Martin / Abel Tesfaye                                              </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:57 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">Save Your Tears            </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve"> Ahmad Balshe / Oscar Holter / Max Martin / Jason Quenneville / Abel Tesfaye                          </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:35 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v>Repeat After Me (Interlude)</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve"> Daniel Lopatin / Kevin Parker / Abel Tesfaye                                                         </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">After Hours                </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve"> Ahmad Balshe / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye / Mario Winans        </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">06:02 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">Until I Bleed Out          </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve"> Metro Boomin / Daniel Lopatin / Notinbed / Mejdi Rhars / Abel Tesfaye                                </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v>The Weeknd</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:10 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1428,21 +1569,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                           </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                      </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">          </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1455,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1468,21 +1609,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                           </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                      </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">          </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1495,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1508,21 +1649,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                           </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                      </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">          </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1535,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1548,21 +1689,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                           </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                      </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">          </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1575,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1588,21 +1729,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                           </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                      </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">          </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1615,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1628,21 +1769,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                           </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                      </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">          </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1655,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1668,21 +1809,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                           </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                      </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                              </v>
+        <v xml:space="preserve">          </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1710,21 +1851,18 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.26953125" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="3" width="80.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="5.453125" customWidth="1"/>
+    <col min="6" max="6" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
@@ -1734,7 +1872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1745,178 +1883,288 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.16597222222222222</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.15347222222222223</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15277777777777776</v>
+        <v>0.14652777777777778</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.13263888888888889</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2">
-        <v>0.15972222222222224</v>
+        <v>0.17152777777777775</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.24652777777777779</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.19652777777777777</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="E7" s="2">
-        <v>0.11805555555555557</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="E10" s="2"/>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.14166666666666666</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6">
-      <c r="E11" s="2"/>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.16458333333333333</v>
+      </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6">
-      <c r="E12" s="2"/>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.14930555555555555</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="2"/>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.13541666666666666</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.25138888888888888</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.13194444444444445</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="5:6">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.5">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="5:6">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.5">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="5:6">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.5">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="5:6">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="5:6">
+    <row r="21" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="5:6">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="5:6">
+    <row r="23" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="5:6">
+    <row r="24" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="5:6">
+    <row r="25" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="5:6">
+    <row r="26" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="5:6">
+    <row r="27" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="5:6">
+    <row r="28" spans="5:6" x14ac:dyDescent="0.5">
       <c r="F28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 07052210 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\my-carbon-site\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,10 +17,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="weeknd6" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
-    <definedName name="weeknd6" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
+    <definedName name="rplusrequalnow1" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="rplusrequalnow1" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,15 +31,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="接続" type="4" refreshedVersion="4" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/weeknd6.htm" htmlTables="1">
+  <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/rplusrequalnow1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
-  <connection id="2" name="接続1" type="4" refreshedVersion="4" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/weeknd6.htm" htmlTables="1">
+  <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/rplusrequalnow1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -44,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="33">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -58,9 +63,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>The Weeknd</t>
-  </si>
-  <si>
     <t>Title/Composer</t>
   </si>
   <si>
@@ -70,95 +72,95 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Alone Again</t>
-  </si>
-  <si>
-    <t>Adam Feeney / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Too Late</t>
-  </si>
-  <si>
-    <t>Eric Frederic / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Hardest to Love</t>
-  </si>
-  <si>
-    <t>Oscar Holter / Max Martin / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Scared to Live</t>
-  </si>
-  <si>
-    <t>Ahmad Balshe / Oscar Holter / Elton John / Daniel Lopatin / Max Martin / Bernie Taupin / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Snowchild</t>
-  </si>
-  <si>
-    <t>Ahmad Balshe / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Escape from LA</t>
-  </si>
-  <si>
-    <t>Metro Boomin / Mike McTaggart / Carlo "Illangelo" Montagnese / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Heartless</t>
-  </si>
-  <si>
-    <t>Metro Boomin / Carlo "Illangelo" Montagnese / Andre Proctor / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Faith</t>
-  </si>
-  <si>
-    <t>Ahmad Balshe / Metro Boomin / Carlo "Illangelo" Montagnese / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Blinding Lights</t>
-  </si>
-  <si>
-    <t>Ahmad Balshe / Oscar Holter / Max Martin / Jason Quenneville / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>In Your Eyes</t>
-  </si>
-  <si>
-    <t>Ahmad Balshe / Oscar Holter / Max Martin / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>Save Your Tears</t>
-  </si>
-  <si>
-    <t>Repeat After Me (Interlude)</t>
-  </si>
-  <si>
-    <t>Daniel Lopatin / Kevin Parker / Abel Tesfaye</t>
-  </si>
-  <si>
-    <t>After Hours</t>
-  </si>
-  <si>
-    <t>Ahmad Balshe / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye / Mario Winans</t>
-  </si>
-  <si>
-    <t>Until I Bleed Out</t>
-  </si>
-  <si>
-    <t>Metro Boomin / Daniel Lopatin / Notinbed / Mejdi Rhars / Abel Tesfaye</t>
+    <t>Change of Tone</t>
+  </si>
+  <si>
+    <t>Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson</t>
+  </si>
+  <si>
+    <t>R+R=Now</t>
+  </si>
+  <si>
+    <t>Awake to You</t>
+  </si>
+  <si>
+    <t>By Design</t>
+  </si>
+  <si>
+    <t>Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Jahi Lake / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson</t>
+  </si>
+  <si>
+    <t>Resting Warrior</t>
+  </si>
+  <si>
+    <t>Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Rose McKinney / Justin Tyson</t>
+  </si>
+  <si>
+    <t>Needed You Still</t>
+  </si>
+  <si>
+    <t>Christian Scott aTunde Adjuah / Robert Glasper / Omari Hardwick / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Michael Neil / Justin Tyson</t>
+  </si>
+  <si>
+    <t>R+R=Now feat. Omari Hardwick</t>
+  </si>
+  <si>
+    <t>Colors in the Dark</t>
+  </si>
+  <si>
+    <t>Robert Glasper / Derrick Hodge / Terrace Martin / Rose McKinney / Arin Ray / Justin Tyson</t>
+  </si>
+  <si>
+    <t>The Night in Question</t>
+  </si>
+  <si>
+    <t>Christian Scott aTunde Adjuah / Terry Crews / Robert Glasper / Derrick Hodge / Taylor McFerrin / Justin Tyson</t>
+  </si>
+  <si>
+    <t>R+R=Now feat. Terry Crews</t>
+  </si>
+  <si>
+    <t>Reflect (Reprise)</t>
+  </si>
+  <si>
+    <t>Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Kyle Myricks / Justin Tyson</t>
+  </si>
+  <si>
+    <t>R+R=Now feat. Stally</t>
+  </si>
+  <si>
+    <t>Her=Now</t>
+  </si>
+  <si>
+    <t>Derrick Hodge / Taylor McFerrin / Amanda Seales</t>
+  </si>
+  <si>
+    <t>R+R=Now feat. Amanda Seales</t>
+  </si>
+  <si>
+    <t>Respond</t>
+  </si>
+  <si>
+    <t>Christian Scott aTunde Adjuah / Derrick Hodge / Taylor McFerrin / Justin Tyson</t>
+  </si>
+  <si>
+    <t>Been on My Mind</t>
+  </si>
+  <si>
+    <t>Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Jahi Lake / Taylor McFerrin / Amber Navran / Dante Smith</t>
+  </si>
+  <si>
+    <t>R+R=Now feat. Amber Navran</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,11 +248,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="weeknd6" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rplusrequalnow1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="weeknd6" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rplusrequalnow1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,7 +544,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,46 +558,45 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" customWidth="1"/>
-    <col min="3" max="3" width="80.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.17500000000000002</v>
+        <v>0.31388888888888888</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -603,71 +604,71 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16597222222222222</v>
+        <v>0.3430555555555555</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.14652777777777778</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13263888888888889</v>
+        <v>0.41041666666666665</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
       <c r="E6" s="2">
-        <v>0.17152777777777775</v>
+        <v>0.25625000000000003</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -678,14 +679,14 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.24652777777777779</v>
+        <v>0.19999999999999998</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -696,180 +697,140 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.32013888888888892</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2">
-        <v>0.19652777777777777</v>
+        <v>0.27916666666666667</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2">
-        <v>0.14166666666666666</v>
+        <v>0.28055555555555556</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.16458333333333333</v>
+        <v>0.22291666666666665</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2">
-        <v>0.14930555555555555</v>
+        <v>0.20069444444444443</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.13541666666666666</v>
-      </c>
+    <row r="13" spans="1:6">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.25138888888888888</v>
-      </c>
+    <row r="14" spans="1:6">
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.13194444444444445</v>
-      </c>
+    <row r="15" spans="1:6">
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:6">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:6">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:6">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:6">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:6">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:6">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:6">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:6">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:6">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:6">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:6">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:6">
       <c r="F28" s="2"/>
     </row>
   </sheetData>
@@ -883,42 +844,42 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K18" sqref="A3:K18"/>
+      <selection activeCell="K15" sqref="A3:K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" customWidth="1"/>
-    <col min="3" max="3" width="3.90625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.08984375" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="3" max="3" width="3.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="4" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" customWidth="1"/>
-    <col min="7" max="7" width="4.453125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" customWidth="1"/>
-    <col min="9" max="9" width="4.36328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1"/>
-    <col min="11" max="11" width="3.453125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.21875" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" customWidth="1"/>
+    <col min="11" max="11" width="3.44140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -931,21 +892,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                      </v>
+        <v xml:space="preserve"> Title                </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                           </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                      </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer </v>
+        <v xml:space="preserve"> Performer                   </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -958,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -970,21 +931,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------------- </v>
+        <v xml:space="preserve">--------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------- </v>
+        <v xml:space="preserve"> ---------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -996,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1009,34 +970,34 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Alone Again                </v>
+        <v xml:space="preserve">Change of Tone       </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Adam Feeney / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye                        </v>
+        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson                                </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now                     </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:12 </v>
+        <v xml:space="preserve">07:32 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1049,34 +1010,34 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Too Late                   </v>
+        <v xml:space="preserve">Awake to You         </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Eric Frederic / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye                      </v>
+        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson                                </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now                     </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:59 </v>
+        <v xml:space="preserve">08:14 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1089,34 +1050,34 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hardest to Love            </v>
+        <v xml:space="preserve">By Design            </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Oscar Holter / Max Martin / Abel Tesfaye                                                             </v>
+        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Jahi Lake / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson                    </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now                     </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:31 </v>
+        <v xml:space="preserve">05:27 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1129,34 +1090,34 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Scared to Live             </v>
+        <v xml:space="preserve">Resting Warrior      </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ahmad Balshe / Oscar Holter / Elton John / Daniel Lopatin / Max Martin / Bernie Taupin / Abel Tesfaye</v>
+        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Rose McKinney / Justin Tyson                                                  </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now                     </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:11 </v>
+        <v xml:space="preserve">09:51 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1169,34 +1130,34 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Snowchild                  </v>
+        <v xml:space="preserve">Needed You Still     </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ahmad Balshe / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye                       </v>
+        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Omari Hardwick / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Michael Neil / Justin Tyson</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v>R+R=Now feat. Omari Hardwick</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:07 </v>
+        <v xml:space="preserve">06:09 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1209,34 +1170,34 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Escape from LA             </v>
+        <v xml:space="preserve">Colors in the Dark   </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Metro Boomin / Mike McTaggart / Carlo "Illangelo" Montagnese / Abel Tesfaye                          </v>
+        <v xml:space="preserve"> Robert Glasper / Derrick Hodge / Terrace Martin / Rose McKinney / Arin Ray / Justin Tyson                                                                       </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now                     </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:55 </v>
+        <v xml:space="preserve">04:48 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1249,34 +1210,34 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Heartless                  </v>
+        <v>The Night in Question</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Metro Boomin / Carlo "Illangelo" Montagnese / Andre Proctor / Abel Tesfaye                           </v>
+        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Terry Crews / Robert Glasper / Derrick Hodge / Taylor McFerrin / Justin Tyson                                                   </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now feat. Terry Crews   </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:20 </v>
+        <v xml:space="preserve">07:41 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1289,34 +1250,34 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Faith                      </v>
+        <v xml:space="preserve">Reflect (Reprise)    </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ahmad Balshe / Metro Boomin / Carlo "Illangelo" Montagnese / Abel Tesfaye                            </v>
+        <v xml:space="preserve"> Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Kyle Myricks / Justin Tyson                                                 </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now feat. Stally        </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:43 </v>
+        <v xml:space="preserve">06:42 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1329,34 +1290,34 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Blinding Lights            </v>
+        <v xml:space="preserve">Her=Now              </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ahmad Balshe / Oscar Holter / Max Martin / Jason Quenneville / Abel Tesfaye                          </v>
+        <v xml:space="preserve"> Derrick Hodge / Taylor McFerrin / Amanda Seales                                                                                                                 </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now feat. Amanda Seales </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:24 </v>
+        <v xml:space="preserve">06:44 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1369,34 +1330,34 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">In Your Eyes               </v>
+        <v xml:space="preserve">Respond              </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ahmad Balshe / Oscar Holter / Max Martin / Abel Tesfaye                                              </v>
+        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Derrick Hodge / Taylor McFerrin / Justin Tyson                                                                                  </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now                     </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:57 </v>
+        <v xml:space="preserve">05:21 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1409,154 +1370,154 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Save Your Tears            </v>
+        <v xml:space="preserve">Been on My Mind      </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ahmad Balshe / Oscar Holter / Max Martin / Jason Quenneville / Abel Tesfaye                          </v>
+        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Jahi Lake / Taylor McFerrin / Amber Navran / Dante Smith                                       </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">R+R=Now feat. Amber Navran  </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:35 </v>
+        <v xml:space="preserve">04:49 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Repeat After Me (Interlude)</v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Daniel Lopatin / Kevin Parker / Abel Tesfaye                                                         </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">After Hours                </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ahmad Balshe / Carlo "Illangelo" Montagnese / Jason Quenneville / Abel Tesfaye / Mario Winans        </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:02 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Until I Bleed Out          </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Metro Boomin / Daniel Lopatin / Notinbed / Mejdi Rhars / Abel Tesfaye                                </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>The Weeknd</v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:10 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1569,21 +1530,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                           </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1596,7 +1557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1609,21 +1570,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                           </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1636,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1649,21 +1610,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                           </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1676,7 +1637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1689,21 +1650,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                           </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1716,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1729,21 +1690,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                           </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1756,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1769,21 +1730,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                           </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1796,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1809,21 +1770,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                           </v>
+        <v xml:space="preserve">                     </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                      </v>
+        <v xml:space="preserve">                                                                                                                                                                 </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">          </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1851,46 +1812,45 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" customWidth="1"/>
-    <col min="2" max="2" width="25.7265625" customWidth="1"/>
-    <col min="3" max="3" width="80.7265625" customWidth="1"/>
-    <col min="4" max="4" width="12.1796875" customWidth="1"/>
-    <col min="5" max="5" width="5.453125" customWidth="1"/>
-    <col min="6" max="6" width="5.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.17500000000000002</v>
+        <v>0.31388888888888888</v>
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1898,71 +1858,71 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16597222222222222</v>
+        <v>0.3430555555555555</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.14652777777777778</v>
+        <v>0.22708333333333333</v>
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13263888888888889</v>
+        <v>0.41041666666666665</v>
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
       <c r="E6" s="2">
-        <v>0.17152777777777775</v>
+        <v>0.25625000000000003</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1973,14 +1933,14 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.24652777777777779</v>
+        <v>0.19999999999999998</v>
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1991,180 +1951,140 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.32013888888888892</v>
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2">
-        <v>0.19652777777777777</v>
+        <v>0.27916666666666667</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2">
-        <v>0.14166666666666666</v>
+        <v>0.28055555555555556</v>
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.16458333333333333</v>
+        <v>0.22291666666666665</v>
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2">
-        <v>0.14930555555555555</v>
+        <v>0.20069444444444443</v>
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.13541666666666666</v>
-      </c>
+    <row r="13" spans="1:6">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.25138888888888888</v>
-      </c>
+    <row r="14" spans="1:6">
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.13194444444444445</v>
-      </c>
+    <row r="15" spans="1:6">
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:6">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:6">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:6">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:6">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:6">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:6">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:6">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:6">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:6">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:6">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:6">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:6">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:6">
       <c r="F28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 07062130 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="rplusrequalnow1" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
-    <definedName name="rplusrequalnow1" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
+    <definedName name="chrisdave1" localSheetId="0">Sheet1!$A$1:$E$16</definedName>
+    <definedName name="chrisdave1" localSheetId="2">Sheet3!$A$1:$E$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/rplusrequalnow1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/chrisdave1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/rplusrequalnow1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/chrisdave1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="46">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,85 +72,124 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Change of Tone</t>
-  </si>
-  <si>
-    <t>Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson</t>
-  </si>
-  <si>
-    <t>R+R=Now</t>
-  </si>
-  <si>
-    <t>Awake to You</t>
-  </si>
-  <si>
-    <t>By Design</t>
-  </si>
-  <si>
-    <t>Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Jahi Lake / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson</t>
-  </si>
-  <si>
-    <t>Resting Warrior</t>
-  </si>
-  <si>
-    <t>Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Rose McKinney / Justin Tyson</t>
-  </si>
-  <si>
-    <t>Needed You Still</t>
-  </si>
-  <si>
-    <t>Christian Scott aTunde Adjuah / Robert Glasper / Omari Hardwick / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Michael Neil / Justin Tyson</t>
-  </si>
-  <si>
-    <t>R+R=Now feat. Omari Hardwick</t>
-  </si>
-  <si>
-    <t>Colors in the Dark</t>
-  </si>
-  <si>
-    <t>Robert Glasper / Derrick Hodge / Terrace Martin / Rose McKinney / Arin Ray / Justin Tyson</t>
-  </si>
-  <si>
-    <t>The Night in Question</t>
-  </si>
-  <si>
-    <t>Christian Scott aTunde Adjuah / Terry Crews / Robert Glasper / Derrick Hodge / Taylor McFerrin / Justin Tyson</t>
-  </si>
-  <si>
-    <t>R+R=Now feat. Terry Crews</t>
-  </si>
-  <si>
-    <t>Reflect (Reprise)</t>
-  </si>
-  <si>
-    <t>Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Kyle Myricks / Justin Tyson</t>
-  </si>
-  <si>
-    <t>R+R=Now feat. Stally</t>
-  </si>
-  <si>
-    <t>Her=Now</t>
-  </si>
-  <si>
-    <t>Derrick Hodge / Taylor McFerrin / Amanda Seales</t>
-  </si>
-  <si>
-    <t>R+R=Now feat. Amanda Seales</t>
-  </si>
-  <si>
-    <t>Respond</t>
-  </si>
-  <si>
-    <t>Christian Scott aTunde Adjuah / Derrick Hodge / Taylor McFerrin / Justin Tyson</t>
-  </si>
-  <si>
-    <t>Been on My Mind</t>
-  </si>
-  <si>
-    <t>Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Jahi Lake / Taylor McFerrin / Amber Navran / Dante Smith</t>
-  </si>
-  <si>
-    <t>R+R=Now feat. Amber Navran</t>
+    <t>Rocks Crying</t>
+  </si>
+  <si>
+    <t>Chris Dave / Cleo Sample</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz</t>
+  </si>
+  <si>
+    <t>Universal Language</t>
+  </si>
+  <si>
+    <t>Chris Dave / Robert Glasper / Shafiq Husayn / Leolin Dockins III / Donald Rose / Sy Smith</t>
+  </si>
+  <si>
+    <t>Dat Feelin'</t>
+  </si>
+  <si>
+    <t>Chris Dave / Keyon Harrold</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz feat. Sir</t>
+  </si>
+  <si>
+    <t>Black Hole</t>
+  </si>
+  <si>
+    <t>Brandon Anderson / Chris Dave / Keyon Harrold</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz feat. Anderson.Paak</t>
+  </si>
+  <si>
+    <t>2N1</t>
+  </si>
+  <si>
+    <t>Chris Dave / Andre Harris / Pino Palladino / Isaiah Sharkey</t>
+  </si>
+  <si>
+    <t>Spread Her Wings</t>
+  </si>
+  <si>
+    <t>Charmelle Cofield / Chris Dave / Darryl Farris / Charlene Keys / Bilal Oliver / James Poyser</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz feat. Bilal, Tweet</t>
+  </si>
+  <si>
+    <t>Whatever</t>
+  </si>
+  <si>
+    <t>Chris Dave / Shafiq Husayn / Tim Stewart</t>
+  </si>
+  <si>
+    <t>Sensitive Granite</t>
+  </si>
+  <si>
+    <t>Chris Dave / Pino Palladino</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz feat. Kendra Foster</t>
+  </si>
+  <si>
+    <t>Cosmic Intercourse</t>
+  </si>
+  <si>
+    <t>Casey Benjamin / Chris Dave / Stokley Williams</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz feat. Stokely Williams</t>
+  </si>
+  <si>
+    <t>Atlanta, Texas</t>
+  </si>
+  <si>
+    <t>Chris Dave / Shafiq Husayn / Goapele Mohlabane / Kebbi Williams</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz deat. Goapele, Shafiq Husayn</t>
+  </si>
+  <si>
+    <t>Destiny N Stereo</t>
+  </si>
+  <si>
+    <t>Phonte Coleman / Chris Dave / Jason Powers / Eric Roberson / Cleo Sample</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz feat. Elzhi, Phonete Coleman, Eric Roberson</t>
+  </si>
+  <si>
+    <t>Clear View</t>
+  </si>
+  <si>
+    <t>Brandon Anderson / Chris Dave / Darryl Farris / Fin Greenall / Pino Palladino</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz feat. Anderson.Paak, SiR</t>
+  </si>
+  <si>
+    <t>Job Well Done</t>
+  </si>
+  <si>
+    <t>Chris Dave / Darryl Farris / Michael Feingold / Anna Wise</t>
+  </si>
+  <si>
+    <t>Chris Dave and the Drumhedz feat. Anna Wise, Sir</t>
+  </si>
+  <si>
+    <t>Lady Jane</t>
+  </si>
+  <si>
+    <t>Alan Pasqua</t>
+  </si>
+  <si>
+    <t>Trippy Tipsy</t>
+  </si>
+  <si>
+    <t>Chris Dave / Pino Palladino / Isaiah Sharkey</t>
   </si>
 </sst>
 </file>
@@ -248,11 +287,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rplusrequalnow1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="chrisdave1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rplusrequalnow1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="chrisdave1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -554,16 +593,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="68.109375" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -592,7 +631,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.31388888888888888</v>
+        <v>9.7916666666666666E-2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -604,13 +643,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.3430555555555555</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -619,16 +658,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0.22708333333333333</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -637,16 +676,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>0.41041666666666665</v>
+        <v>0.18958333333333333</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -655,16 +694,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.25625000000000003</v>
+        <v>4.3055555555555562E-2</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -673,16 +712,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19999999999999998</v>
+        <v>0.22430555555555556</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -691,16 +730,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.32013888888888892</v>
+        <v>9.5138888888888884E-2</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -709,16 +748,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>0.27916666666666667</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -727,16 +766,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>0.28055555555555556</v>
+        <v>0.23819444444444446</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -745,16 +784,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2">
-        <v>0.22291666666666665</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -763,35 +802,89 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2">
-        <v>0.20069444444444443</v>
+        <v>0.15902777777777777</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.26805555555555555</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.19166666666666665</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.23472222222222219</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.1013888888888889</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="5:6">
@@ -843,8 +936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K15" sqref="A3:K15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K22" sqref="A3:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -864,15 +957,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>160</v>
+        <v>92</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -892,21 +985,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                </v>
+        <v xml:space="preserve"> Title             </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                      </v>
+        <v xml:space="preserve"> Composers                                                                                  </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                   </v>
+        <v xml:space="preserve"> Performer                                                              </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -931,21 +1024,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------- </v>
+        <v xml:space="preserve">------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> -------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -970,28 +1063,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Change of Tone       </v>
+        <v xml:space="preserve">Rocks Crying      </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson                                </v>
+        <v xml:space="preserve"> Chris Dave / Cleo Sample                                                                    </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now                     </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">07:32 </v>
+        <v xml:space="preserve">02:21 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1010,28 +1103,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Awake to You         </v>
+        <v>Universal Language</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson                                </v>
+        <v xml:space="preserve"> Chris Dave / Robert Glasper / Shafiq Husayn / Leolin Dockins III / Donald Rose / Sy Smith   </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now                     </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">08:14 </v>
+        <v xml:space="preserve">03:39 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1050,28 +1143,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">By Design            </v>
+        <v xml:space="preserve">Dat Feelin'       </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Jahi Lake / Terrace Martin / Taylor McFerrin / Rose McKinney / Justin Tyson                    </v>
+        <v xml:space="preserve"> Chris Dave / Keyon Harrold                                                                  </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now                     </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Sir                                  </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:27 </v>
+        <v xml:space="preserve">03:38 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1090,28 +1183,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Resting Warrior      </v>
+        <v xml:space="preserve">Black Hole        </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Terrace Martin / Rose McKinney / Justin Tyson                                                  </v>
+        <v xml:space="preserve"> Brandon Anderson / Chris Dave / Keyon Harrold                                               </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now                     </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Anderson.Paak                        </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">09:51 </v>
+        <v xml:space="preserve">04:33 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1130,28 +1223,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Needed You Still     </v>
+        <v xml:space="preserve">2N1               </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Omari Hardwick / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Michael Neil / Justin Tyson</v>
+        <v xml:space="preserve"> Chris Dave / Andre Harris / Pino Palladino / Isaiah Sharkey                                 </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>R+R=Now feat. Omari Hardwick</v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:09 </v>
+        <v xml:space="preserve">01:02 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1170,28 +1263,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Colors in the Dark   </v>
+        <v xml:space="preserve">Spread Her Wings  </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Glasper / Derrick Hodge / Terrace Martin / Rose McKinney / Arin Ray / Justin Tyson                                                                       </v>
+        <v xml:space="preserve"> Charmelle Cofield / Chris Dave / Darryl Farris / Charlene Keys / Bilal Oliver / James Poyser</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now                     </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Bilal, Tweet                         </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:48 </v>
+        <v xml:space="preserve">05:23 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1210,28 +1303,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>The Night in Question</v>
+        <v xml:space="preserve">Whatever          </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Terry Crews / Robert Glasper / Derrick Hodge / Taylor McFerrin / Justin Tyson                                                   </v>
+        <v xml:space="preserve"> Chris Dave / Shafiq Husayn / Tim Stewart                                                    </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now feat. Terry Crews   </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">07:41 </v>
+        <v xml:space="preserve">02:17 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1250,28 +1343,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Reflect (Reprise)    </v>
+        <v xml:space="preserve">Sensitive Granite </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Glasper / Derrick Hodge / Terrace Martin / Taylor McFerrin / Rose McKinney / Kyle Myricks / Justin Tyson                                                 </v>
+        <v xml:space="preserve"> Chris Dave / Pino Palladino                                                                 </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now feat. Stally        </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Kendra Foster                        </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:42 </v>
+        <v xml:space="preserve">03:41 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1290,28 +1383,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Her=Now              </v>
+        <v>Cosmic Intercourse</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Derrick Hodge / Taylor McFerrin / Amanda Seales                                                                                                                 </v>
+        <v xml:space="preserve"> Casey Benjamin / Chris Dave / Stokley Williams                                              </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now feat. Amanda Seales </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Stokely Williams                     </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:44 </v>
+        <v xml:space="preserve">05:43 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1330,28 +1423,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Respond              </v>
+        <v xml:space="preserve">Atlanta, Texas    </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Derrick Hodge / Taylor McFerrin / Justin Tyson                                                                                  </v>
+        <v xml:space="preserve"> Chris Dave / Shafiq Husayn / Goapele Mohlabane / Kebbi Williams                             </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now                     </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz deat. Goapele, Shafiq Husayn               </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:21 </v>
+        <v xml:space="preserve">03:44 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1370,28 +1463,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Been on My Mind      </v>
+        <v xml:space="preserve">Destiny N Stereo  </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Christian Scott aTunde Adjuah / Robert Glasper / Derrick Hodge / Jahi Lake / Taylor McFerrin / Amber Navran / Dante Smith                                       </v>
+        <v xml:space="preserve"> Phonte Coleman / Chris Dave / Jason Powers / Eric Roberson / Cleo Sample                    </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">R+R=Now feat. Amber Navran  </v>
+        <v>Chris Dave and the Drumhedz feat. Elzhi, Phonete Coleman, Eric Roberson</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:49 </v>
+        <v xml:space="preserve">03:49 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1403,35 +1496,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Clear View        </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Brandon Anderson / Chris Dave / Darryl Farris / Fin Greenall / Pino Palladino               </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Anderson.Paak, SiR                   </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">06:26 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1443,35 +1536,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Job Well Done     </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Chris Dave / Darryl Farris / Michael Feingold / Anna Wise                                   </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Anna Wise, Sir                       </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:36 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1483,35 +1576,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Lady Jane         </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Alan Pasqua                                                                                 </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">05:38 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1523,35 +1616,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">Trippy Tipsy      </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Chris Dave / Pino Palladino / Isaiah Sharkey                                                </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:26 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1570,21 +1663,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                       </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1610,21 +1703,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                       </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1650,21 +1743,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                       </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1690,21 +1783,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                       </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1730,21 +1823,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                       </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1770,21 +1863,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                     </v>
+        <v xml:space="preserve">                  </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                 </v>
+        <v xml:space="preserve">                                                                                             </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                       </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1815,9 +1908,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="68.109375" customWidth="1"/>
     <col min="5" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1846,7 +1939,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.31388888888888888</v>
+        <v>9.7916666666666666E-2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -1858,13 +1951,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.3430555555555555</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -1873,16 +1966,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0.22708333333333333</v>
+        <v>0.15138888888888888</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -1891,16 +1984,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>0.41041666666666665</v>
+        <v>0.18958333333333333</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1909,16 +2002,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.25625000000000003</v>
+        <v>4.3055555555555562E-2</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -1927,16 +2020,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19999999999999998</v>
+        <v>0.22430555555555556</v>
       </c>
       <c r="F7" s="2"/>
     </row>
@@ -1945,16 +2038,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.32013888888888892</v>
+        <v>9.5138888888888884E-2</v>
       </c>
       <c r="F8" s="2"/>
     </row>
@@ -1963,16 +2056,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>0.27916666666666667</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F9" s="2"/>
     </row>
@@ -1981,16 +2074,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>0.28055555555555556</v>
+        <v>0.23819444444444446</v>
       </c>
       <c r="F10" s="2"/>
     </row>
@@ -1999,16 +2092,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2">
-        <v>0.22291666666666665</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="F11" s="2"/>
     </row>
@@ -2017,35 +2110,89 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2">
-        <v>0.20069444444444443</v>
+        <v>0.15902777777777777</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.26805555555555555</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.19166666666666665</v>
+      </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.23472222222222219</v>
+      </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.1013888888888889</v>
+      </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="5:6">

</xml_diff>

<commit_message>
feat: 07072155 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="chrisdave1" localSheetId="0">Sheet1!$A$1:$E$16</definedName>
-    <definedName name="chrisdave1" localSheetId="2">Sheet3!$A$1:$E$16</definedName>
+    <definedName name="tinashe2" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
+    <definedName name="tinashe2" localSheetId="2">Sheet3!$A$1:$E$14</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/chrisdave1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/tinashe2.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/chrisdave1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/tinashe2.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="35">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,124 +72,91 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Rocks Crying</t>
-  </si>
-  <si>
-    <t>Chris Dave / Cleo Sample</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz</t>
-  </si>
-  <si>
-    <t>Universal Language</t>
-  </si>
-  <si>
-    <t>Chris Dave / Robert Glasper / Shafiq Husayn / Leolin Dockins III / Donald Rose / Sy Smith</t>
-  </si>
-  <si>
-    <t>Dat Feelin'</t>
-  </si>
-  <si>
-    <t>Chris Dave / Keyon Harrold</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz feat. Sir</t>
-  </si>
-  <si>
-    <t>Black Hole</t>
-  </si>
-  <si>
-    <t>Brandon Anderson / Chris Dave / Keyon Harrold</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz feat. Anderson.Paak</t>
-  </si>
-  <si>
-    <t>2N1</t>
-  </si>
-  <si>
-    <t>Chris Dave / Andre Harris / Pino Palladino / Isaiah Sharkey</t>
-  </si>
-  <si>
-    <t>Spread Her Wings</t>
-  </si>
-  <si>
-    <t>Charmelle Cofield / Chris Dave / Darryl Farris / Charlene Keys / Bilal Oliver / James Poyser</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz feat. Bilal, Tweet</t>
-  </si>
-  <si>
-    <t>Whatever</t>
-  </si>
-  <si>
-    <t>Chris Dave / Shafiq Husayn / Tim Stewart</t>
-  </si>
-  <si>
-    <t>Sensitive Granite</t>
-  </si>
-  <si>
-    <t>Chris Dave / Pino Palladino</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz feat. Kendra Foster</t>
-  </si>
-  <si>
-    <t>Cosmic Intercourse</t>
-  </si>
-  <si>
-    <t>Casey Benjamin / Chris Dave / Stokley Williams</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz feat. Stokely Williams</t>
-  </si>
-  <si>
-    <t>Atlanta, Texas</t>
-  </si>
-  <si>
-    <t>Chris Dave / Shafiq Husayn / Goapele Mohlabane / Kebbi Williams</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz deat. Goapele, Shafiq Husayn</t>
-  </si>
-  <si>
-    <t>Destiny N Stereo</t>
-  </si>
-  <si>
-    <t>Phonte Coleman / Chris Dave / Jason Powers / Eric Roberson / Cleo Sample</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz feat. Elzhi, Phonete Coleman, Eric Roberson</t>
-  </si>
-  <si>
-    <t>Clear View</t>
-  </si>
-  <si>
-    <t>Brandon Anderson / Chris Dave / Darryl Farris / Fin Greenall / Pino Palladino</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz feat. Anderson.Paak, SiR</t>
-  </si>
-  <si>
-    <t>Job Well Done</t>
-  </si>
-  <si>
-    <t>Chris Dave / Darryl Farris / Michael Feingold / Anna Wise</t>
-  </si>
-  <si>
-    <t>Chris Dave and the Drumhedz feat. Anna Wise, Sir</t>
-  </si>
-  <si>
-    <t>Lady Jane</t>
-  </si>
-  <si>
-    <t>Alan Pasqua</t>
-  </si>
-  <si>
-    <t>Trippy Tipsy</t>
-  </si>
-  <si>
-    <t>Chris Dave / Pino Palladino / Isaiah Sharkey</t>
+    <t>Keep Your Eyes on the Road (Intro)</t>
+  </si>
+  <si>
+    <t>Tinashe</t>
+  </si>
+  <si>
+    <t>Joyride</t>
+  </si>
+  <si>
+    <t>Chauncey Hollis / Tinashe Kachingwe / Allen Ritter / Jacques Webster</t>
+  </si>
+  <si>
+    <t>No Drama</t>
+  </si>
+  <si>
+    <t>Kiari Cephus / Mikkel Storleer Eriksen / Tinashe Kachingwe / Youth Wilde</t>
+  </si>
+  <si>
+    <t>Tinashe feat. Offset</t>
+  </si>
+  <si>
+    <t>He Don't Want It</t>
+  </si>
+  <si>
+    <t>Tinashe Kachingwe / Tyler Williams</t>
+  </si>
+  <si>
+    <t>Ooh La La</t>
+  </si>
+  <si>
+    <t>Denisia Andrews / Brittany Coney / Jocelyn a. Donald / Tinashe Kachingwe / Klenord Raphael / Anthony G. White</t>
+  </si>
+  <si>
+    <t>Me So Bad</t>
+  </si>
+  <si>
+    <t>Floyd Bentley / Christopher Dotson / Tyrone Griffin / Mayila Caieme Marie Jones / Tinashe Kachingwe / Karim Kharbouch / Montrell "Wavy" Martinez / Mele Moore / Andre Proctor / Simon "Blwyrmnd" Schranz / Christian Ward</t>
+  </si>
+  <si>
+    <t>Tinashe feat. Ty Dolla $ign, French Montana</t>
+  </si>
+  <si>
+    <t>Ain't Good for Ya (Interlude)</t>
+  </si>
+  <si>
+    <t>Bobby Brackins / Tinashe Kachingwe / Mario Lucciano / Sidnie Tipton</t>
+  </si>
+  <si>
+    <t>Stuck With Me</t>
+  </si>
+  <si>
+    <t>Chelsea Davenport / Tinashe Kachingwe / Marcus Moore / Yukimi Nagano / David Singer-Vine / William Vanderheyden</t>
+  </si>
+  <si>
+    <t>Tinashe feat. Little Dragon</t>
+  </si>
+  <si>
+    <t>Go Easy on Me (Interlude)</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Kenneth Coby / Sarah Hudson / Clarence Coffee, Jr. / Tinashe Kachingwe / Kieran Lasker</t>
+  </si>
+  <si>
+    <t>Faded Love</t>
+  </si>
+  <si>
+    <t>Noonie Bao / Tor Erik Hermansen / Tinashe Kachingwe / Sasha Sloan / Nayvadius Wilburn</t>
+  </si>
+  <si>
+    <t>Tinashe feat. Future</t>
+  </si>
+  <si>
+    <t>No Contest</t>
+  </si>
+  <si>
+    <t>Kenneth Coby / Jeremih Felton / Ray Holton / Tinashe Kachingwe / Sayyid McDonald</t>
+  </si>
+  <si>
+    <t>Fires and Flames</t>
+  </si>
+  <si>
+    <t>Joel Compass / Amanda Ghost / Tinashe Kachingwe / K Stewart</t>
   </si>
 </sst>
 </file>
@@ -287,11 +254,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="chrisdave1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tinashe2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="chrisdave1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tinashe2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,22 +558,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="68.109375" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -617,314 +584,294 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="2">
-        <v>9.7916666666666666E-2</v>
+        <v>4.7916666666666663E-2</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.13819444444444443</v>
       </c>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>0.18958333333333333</v>
+        <v>0.11944444444444445</v>
       </c>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
-        <v>4.3055555555555562E-2</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
       <c r="E7" s="2">
-        <v>0.22430555555555556</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>9.5138888888888884E-2</v>
+        <v>4.3750000000000004E-2</v>
       </c>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
       <c r="E9" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
-        <v>0.23819444444444446</v>
+        <v>2.1527777777777781E-2</v>
       </c>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15555555555555556</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2">
-        <v>0.15902777777777777</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E13" s="2">
-        <v>0.26805555555555555</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2">
-        <v>0.19166666666666665</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.23472222222222219</v>
-      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.1013888888888889</v>
-      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="5:6">
-      <c r="E17" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="6:7">
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="5:6">
-      <c r="E18" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="6:7">
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="5:6">
-      <c r="E19" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="6:7">
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="5:6">
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="5:6">
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="5:6">
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="5:6">
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="5:6">
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="5:6">
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="5:6">
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="5:6">
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="5:6">
-      <c r="F28" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="6:7">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="6:7">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="6:7">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="6:7">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="6:7">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="6:7">
+      <c r="G28" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -936,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K22" sqref="A3:K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="A3:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -957,15 +904,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>92</v>
+        <v>217</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -985,21 +932,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title             </v>
+        <v xml:space="preserve"> Title                             </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                  </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                                                                               </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                                              </v>
+        <v xml:space="preserve"> Performer                                  </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1024,21 +971,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------ </v>
+        <v xml:space="preserve">---------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1063,28 +1010,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Rocks Crying      </v>
+        <v>Keep Your Eyes on the Road (Intro)</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Cleo Sample                                                                    </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:21 </v>
+        <v xml:space="preserve">01:09 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1103,28 +1050,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Universal Language</v>
+        <v xml:space="preserve">Joyride                           </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Robert Glasper / Shafiq Husayn / Leolin Dockins III / Donald Rose / Sy Smith   </v>
+        <v xml:space="preserve"> Chauncey Hollis / Tinashe Kachingwe / Allen Ritter / Jacques Webster                                                                                                                                                     </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:39 </v>
+        <v xml:space="preserve">03:25 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1143,28 +1090,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Dat Feelin'       </v>
+        <v xml:space="preserve">No Drama                          </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Keyon Harrold                                                                  </v>
+        <v xml:space="preserve"> Kiari Cephus / Mikkel Storleer Eriksen / Tinashe Kachingwe / Youth Wilde                                                                                                                                                 </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Sir                                  </v>
+        <v xml:space="preserve">Tinashe feat. Offset                       </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:38 </v>
+        <v xml:space="preserve">03:19 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1183,28 +1130,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Black Hole        </v>
+        <v xml:space="preserve">He Don't Want It                  </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Anderson / Chris Dave / Keyon Harrold                                               </v>
+        <v xml:space="preserve"> Tinashe Kachingwe / Tyler Williams                                                                                                                                                                                       </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Anderson.Paak                        </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:33 </v>
+        <v xml:space="preserve">02:52 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1223,28 +1170,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">2N1               </v>
+        <v xml:space="preserve">Ooh La La                         </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Andre Harris / Pino Palladino / Isaiah Sharkey                                 </v>
+        <v xml:space="preserve"> Denisia Andrews / Brittany Coney / Jocelyn a. Donald / Tinashe Kachingwe / Klenord Raphael / Anthony G. White                                                                                                            </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:02 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1263,28 +1210,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Spread Her Wings  </v>
+        <v xml:space="preserve">Me So Bad                         </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Charmelle Cofield / Chris Dave / Darryl Farris / Charlene Keys / Bilal Oliver / James Poyser</v>
+        <v xml:space="preserve"> Floyd Bentley / Christopher Dotson / Tyrone Griffin / Mayila Caieme Marie Jones / Tinashe Kachingwe / Karim Kharbouch / Montrell "Wavy" Martinez / Mele Moore / Andre Proctor / Simon "Blwyrmnd" Schranz / Christian Ward</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Bilal, Tweet                         </v>
+        <v>Tinashe feat. Ty Dolla $ign, French Montana</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:23 </v>
+        <v xml:space="preserve">03:08 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1303,28 +1250,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Whatever          </v>
+        <v xml:space="preserve">Ain't Good for Ya (Interlude)     </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Shafiq Husayn / Tim Stewart                                                    </v>
+        <v xml:space="preserve"> Bobby Brackins / Tinashe Kachingwe / Mario Lucciano / Sidnie Tipton                                                                                                                                                      </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:17 </v>
+        <v xml:space="preserve">01:03 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1343,28 +1290,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sensitive Granite </v>
+        <v xml:space="preserve">Stuck With Me                     </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Pino Palladino                                                                 </v>
+        <v xml:space="preserve"> Chelsea Davenport / Tinashe Kachingwe / Marcus Moore / Yukimi Nagano / David Singer-Vine / William Vanderheyden                                                                                                          </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Kendra Foster                        </v>
+        <v xml:space="preserve">Tinashe feat. Little Dragon                </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:41 </v>
+        <v xml:space="preserve">03:25 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1383,28 +1330,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Cosmic Intercourse</v>
+        <v xml:space="preserve">Go Easy on Me (Interlude)         </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Casey Benjamin / Chris Dave / Stokley Williams                                              </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Stokely Williams                     </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:43 </v>
+        <v xml:space="preserve">00:31 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1423,28 +1370,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Atlanta, Texas    </v>
+        <v xml:space="preserve">Salt                              </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Shafiq Husayn / Goapele Mohlabane / Kebbi Williams                             </v>
+        <v xml:space="preserve"> Kenneth Coby / Sarah Hudson / Clarence Coffee, Jr. / Tinashe Kachingwe / Kieran Lasker                                                                                                                                   </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz deat. Goapele, Shafiq Husayn               </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:44 </v>
+        <v xml:space="preserve">03:48 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1463,28 +1410,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Destiny N Stereo  </v>
+        <v xml:space="preserve">Faded Love                        </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Phonte Coleman / Chris Dave / Jason Powers / Eric Roberson / Cleo Sample                    </v>
+        <v xml:space="preserve"> Noonie Bao / Tor Erik Hermansen / Tinashe Kachingwe / Sasha Sloan / Nayvadius Wilburn                                                                                                                                    </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Chris Dave and the Drumhedz feat. Elzhi, Phonete Coleman, Eric Roberson</v>
+        <v xml:space="preserve">Tinashe feat. Future                       </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:49 </v>
+        <v xml:space="preserve">03:23 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1503,28 +1450,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Clear View        </v>
+        <v xml:space="preserve">No Contest                        </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Brandon Anderson / Chris Dave / Darryl Farris / Fin Greenall / Pino Palladino               </v>
+        <v xml:space="preserve"> Kenneth Coby / Jeremih Felton / Ray Holton / Tinashe Kachingwe / Sayyid McDonald                                                                                                                                         </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Anderson.Paak, SiR                   </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:26 </v>
+        <v xml:space="preserve">03:47 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1543,28 +1490,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Job Well Done     </v>
+        <v xml:space="preserve">Fires and Flames                  </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Darryl Farris / Michael Feingold / Anna Wise                                   </v>
+        <v xml:space="preserve"> Joel Compass / Amanda Ghost / Tinashe Kachingwe / K Stewart                                                                                                                                                              </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz feat. Anna Wise, Sir                       </v>
+        <v xml:space="preserve">Tinashe                                    </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:36 </v>
+        <v xml:space="preserve">03:46 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1576,35 +1523,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lady Jane         </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Alan Pasqua                                                                                 </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:38 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1616,35 +1563,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Trippy Tipsy      </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chris Dave / Pino Palladino / Isaiah Sharkey                                                </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Chris Dave and the Drumhedz                                            </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:26 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1663,21 +1610,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                                       </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1703,21 +1650,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                                       </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1743,21 +1690,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                                       </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1783,21 +1730,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                                       </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1823,21 +1770,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                                       </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1863,21 +1810,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                  </v>
+        <v xml:space="preserve">                                  </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                             </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                                       </v>
+        <v xml:space="preserve">                                           </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1899,7 +1846,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1908,13 +1855,13 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="68.109375" customWidth="1"/>
-    <col min="5" max="6" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -1925,314 +1872,294 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="2">
-        <v>9.7916666666666666E-2</v>
+        <v>4.7916666666666663E-2</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>0.15208333333333332</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="2">
-        <v>0.15138888888888888</v>
+        <v>0.13819444444444443</v>
       </c>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>0.18958333333333333</v>
+        <v>0.11944444444444445</v>
       </c>
       <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
-        <v>4.3055555555555562E-2</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
       <c r="E7" s="2">
-        <v>0.22430555555555556</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>9.5138888888888884E-2</v>
+        <v>4.3750000000000004E-2</v>
       </c>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
       <c r="E9" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
-        <v>0.23819444444444446</v>
+        <v>2.1527777777777781E-2</v>
       </c>
       <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15555555555555556</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E12" s="2">
-        <v>0.15902777777777777</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="E13" s="2">
-        <v>0.26805555555555555</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2">
-        <v>0.19166666666666665</v>
+        <v>0.15694444444444444</v>
       </c>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.23472222222222219</v>
-      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.1013888888888889</v>
-      </c>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="5:6">
-      <c r="E17" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="6:7">
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="5:6">
-      <c r="E18" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="6:7">
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="5:6">
-      <c r="E19" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="6:7">
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="5:6">
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="5:6">
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="5:6">
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="5:6">
-      <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="5:6">
-      <c r="F24" s="2"/>
-    </row>
-    <row r="25" spans="5:6">
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="5:6">
-      <c r="F26" s="2"/>
-    </row>
-    <row r="27" spans="5:6">
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="5:6">
-      <c r="F28" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="6:7">
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="6:7">
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="6:7">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="6:7">
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="6:7">
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="6:7">
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="6:7">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="6:7">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="6:7">
+      <c r="G28" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
feat: 07102115 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="tinashe2" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
-    <definedName name="tinashe2" localSheetId="2">Sheet3!$A$1:$E$14</definedName>
+    <definedName name="justin4" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
+    <definedName name="justin4" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/tinashe2.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/justin4.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/tinashe2.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/justin4.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="31">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,91 +72,79 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Keep Your Eyes on the Road (Intro)</t>
-  </si>
-  <si>
-    <t>Tinashe</t>
-  </si>
-  <si>
-    <t>Joyride</t>
-  </si>
-  <si>
-    <t>Chauncey Hollis / Tinashe Kachingwe / Allen Ritter / Jacques Webster</t>
-  </si>
-  <si>
-    <t>No Drama</t>
-  </si>
-  <si>
-    <t>Kiari Cephus / Mikkel Storleer Eriksen / Tinashe Kachingwe / Youth Wilde</t>
-  </si>
-  <si>
-    <t>Tinashe feat. Offset</t>
-  </si>
-  <si>
-    <t>He Don't Want It</t>
-  </si>
-  <si>
-    <t>Tinashe Kachingwe / Tyler Williams</t>
-  </si>
-  <si>
-    <t>Ooh La La</t>
-  </si>
-  <si>
-    <t>Denisia Andrews / Brittany Coney / Jocelyn a. Donald / Tinashe Kachingwe / Klenord Raphael / Anthony G. White</t>
-  </si>
-  <si>
-    <t>Me So Bad</t>
-  </si>
-  <si>
-    <t>Floyd Bentley / Christopher Dotson / Tyrone Griffin / Mayila Caieme Marie Jones / Tinashe Kachingwe / Karim Kharbouch / Montrell "Wavy" Martinez / Mele Moore / Andre Proctor / Simon "Blwyrmnd" Schranz / Christian Ward</t>
-  </si>
-  <si>
-    <t>Tinashe feat. Ty Dolla $ign, French Montana</t>
-  </si>
-  <si>
-    <t>Ain't Good for Ya (Interlude)</t>
-  </si>
-  <si>
-    <t>Bobby Brackins / Tinashe Kachingwe / Mario Lucciano / Sidnie Tipton</t>
-  </si>
-  <si>
-    <t>Stuck With Me</t>
-  </si>
-  <si>
-    <t>Chelsea Davenport / Tinashe Kachingwe / Marcus Moore / Yukimi Nagano / David Singer-Vine / William Vanderheyden</t>
-  </si>
-  <si>
-    <t>Tinashe feat. Little Dragon</t>
-  </si>
-  <si>
-    <t>Go Easy on Me (Interlude)</t>
-  </si>
-  <si>
-    <t>Salt</t>
-  </si>
-  <si>
-    <t>Kenneth Coby / Sarah Hudson / Clarence Coffee, Jr. / Tinashe Kachingwe / Kieran Lasker</t>
-  </si>
-  <si>
-    <t>Faded Love</t>
-  </si>
-  <si>
-    <t>Noonie Bao / Tor Erik Hermansen / Tinashe Kachingwe / Sasha Sloan / Nayvadius Wilburn</t>
-  </si>
-  <si>
-    <t>Tinashe feat. Future</t>
-  </si>
-  <si>
-    <t>No Contest</t>
-  </si>
-  <si>
-    <t>Kenneth Coby / Jeremih Felton / Ray Holton / Tinashe Kachingwe / Sayyid McDonald</t>
-  </si>
-  <si>
-    <t>Fires and Flames</t>
-  </si>
-  <si>
-    <t>Joel Compass / Amanda Ghost / Tinashe Kachingwe / K Stewart</t>
+    <t>Filthy</t>
+  </si>
+  <si>
+    <t>Larrance Dopson / James Fauntleroy / Nate Hills / Timothy Mosley / Justin Timberlake</t>
+  </si>
+  <si>
+    <t>Justin Timberlake</t>
+  </si>
+  <si>
+    <t>Midnight Summer Jam</t>
+  </si>
+  <si>
+    <t>Chad Hugo / Justin Timberlake / Pharrell Williams</t>
+  </si>
+  <si>
+    <t>Sauce</t>
+  </si>
+  <si>
+    <t>Nate Hills / Elliott Ives / Timothy Mosley / Justin Timberlake</t>
+  </si>
+  <si>
+    <t>Man of the Woods</t>
+  </si>
+  <si>
+    <t>Higher Higher</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>Supplies</t>
+  </si>
+  <si>
+    <t>Morning Light</t>
+  </si>
+  <si>
+    <t>Eric Hudson / Elliott Ives / Chris Stapleton / Robin Tadross / Justin Timberlake</t>
+  </si>
+  <si>
+    <t>Justin Timberlake ft. Alicia Keys</t>
+  </si>
+  <si>
+    <t>Say Something</t>
+  </si>
+  <si>
+    <t>Larrance Dopson / Nate Hills / Timothy Mosley / Chris Stapleton / Justin Timberlake</t>
+  </si>
+  <si>
+    <t>Justin Timberlake ft. Chris Stapleton</t>
+  </si>
+  <si>
+    <t>Hers (Interlude)</t>
+  </si>
+  <si>
+    <t>Flannel</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Breeze Off the Pond</t>
+  </si>
+  <si>
+    <t>Livin' Off the Land</t>
+  </si>
+  <si>
+    <t>The Hard Stuff</t>
+  </si>
+  <si>
+    <t>Young Man</t>
+  </si>
+  <si>
+    <t>James Fauntleroy / Jerome Harmon / Timothy Mosley / Justin Timberlake</t>
   </si>
 </sst>
 </file>
@@ -254,11 +242,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tinashe2" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="justin4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tinashe2" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="justin4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,15 +549,15 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="79.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
     <col min="5" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -591,11 +579,14 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>4.7916666666666663E-2</v>
+        <v>0.20347222222222219</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -605,16 +596,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1423611111111111</v>
+        <v>0.21666666666666667</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -624,16 +615,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -646,13 +637,13 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.11944444444444445</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -662,16 +653,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.17916666666666667</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -681,16 +672,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.18333333333333335</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -700,16 +691,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>4.3750000000000004E-2</v>
+        <v>0.15625</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -719,16 +710,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2">
-        <v>0.1423611111111111</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -738,13 +729,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2">
-        <v>2.1527777777777781E-2</v>
+        <v>0.19305555555555554</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -754,16 +748,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15833333333333333</v>
+        <v>4.2361111111111106E-2</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -773,16 +767,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.14097222222222222</v>
+        <v>0.20069444444444443</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -792,16 +786,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.15763888888888888</v>
+        <v>0.19375000000000001</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -811,66 +805,110 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.17430555555555557</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.20347222222222219</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.13541666666666666</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="6:7">
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.15625</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="6:7">
+    <row r="18" spans="1:7">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="6:7">
+    <row r="19" spans="1:7">
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="6:7">
+    <row r="20" spans="1:7">
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="6:7">
+    <row r="21" spans="1:7">
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="6:7">
+    <row r="22" spans="1:7">
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="6:7">
+    <row r="23" spans="1:7">
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="6:7">
+    <row r="24" spans="1:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="6:7">
+    <row r="25" spans="1:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="6:7">
+    <row r="26" spans="1:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="6:7">
+    <row r="27" spans="1:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="6:7">
+    <row r="28" spans="1:7">
       <c r="G28" s="2"/>
     </row>
   </sheetData>
@@ -884,7 +922,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="A3:K17"/>
+      <selection activeCell="K20" sqref="A3:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -904,15 +942,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>217</v>
+        <v>84</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -932,21 +970,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                             </v>
+        <v xml:space="preserve"> Title              </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                                                                               </v>
+        <v xml:space="preserve"> Composers                                                                          </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                  </v>
+        <v xml:space="preserve"> Performer                            </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -971,21 +1009,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">---------------------------------- </v>
+        <v xml:space="preserve">------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1010,28 +1048,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Keep Your Eyes on the Road (Intro)</v>
+        <v xml:space="preserve">Filthy             </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Larrance Dopson / James Fauntleroy / Nate Hills / Timothy Mosley / Justin Timberlake</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:09 </v>
+        <v xml:space="preserve">04:53 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1050,28 +1088,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Joyride                           </v>
+        <v>Midnight Summer Jam</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chauncey Hollis / Tinashe Kachingwe / Allen Ritter / Jacques Webster                                                                                                                                                     </v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:25 </v>
+        <v xml:space="preserve">05:12 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1090,28 +1128,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Drama                          </v>
+        <v xml:space="preserve">Sauce              </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kiari Cephus / Mikkel Storleer Eriksen / Tinashe Kachingwe / Youth Wilde                                                                                                                                                 </v>
+        <v xml:space="preserve"> Nate Hills / Elliott Ives / Timothy Mosley / Justin Timberlake                      </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe feat. Offset                       </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:19 </v>
+        <v xml:space="preserve">04:05 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1130,28 +1168,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">He Don't Want It                  </v>
+        <v xml:space="preserve">Man of the Woods   </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Tinashe Kachingwe / Tyler Williams                                                                                                                                                                                       </v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:52 </v>
+        <v xml:space="preserve">04:03 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1170,28 +1208,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ooh La La                         </v>
+        <v xml:space="preserve">Higher Higher      </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Denisia Andrews / Brittany Coney / Jocelyn a. Donald / Tinashe Kachingwe / Klenord Raphael / Anthony G. White                                                                                                            </v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">04:18 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1210,28 +1248,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Me So Bad                         </v>
+        <v xml:space="preserve">Wave               </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Floyd Bentley / Christopher Dotson / Tyrone Griffin / Mayila Caieme Marie Jones / Tinashe Kachingwe / Karim Kharbouch / Montrell "Wavy" Martinez / Mele Moore / Andre Proctor / Simon "Blwyrmnd" Schranz / Christian Ward</v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Tinashe feat. Ty Dolla $ign, French Montana</v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:08 </v>
+        <v xml:space="preserve">04:24 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1250,28 +1288,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ain't Good for Ya (Interlude)     </v>
+        <v xml:space="preserve">Supplies           </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Bobby Brackins / Tinashe Kachingwe / Mario Lucciano / Sidnie Tipton                                                                                                                                                      </v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:03 </v>
+        <v xml:space="preserve">03:45 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1290,28 +1328,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Stuck With Me                     </v>
+        <v xml:space="preserve">Morning Light      </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chelsea Davenport / Tinashe Kachingwe / Marcus Moore / Yukimi Nagano / David Singer-Vine / William Vanderheyden                                                                                                          </v>
+        <v xml:space="preserve"> Eric Hudson / Elliott Ives / Chris Stapleton / Robin Tadross / Justin Timberlake    </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe feat. Little Dragon                </v>
+        <v xml:space="preserve">Justin Timberlake ft. Alicia Keys    </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:25 </v>
+        <v xml:space="preserve">04:03 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1330,28 +1368,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Go Easy on Me (Interlude)         </v>
+        <v xml:space="preserve">Say Something      </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Larrance Dopson / Nate Hills / Timothy Mosley / Chris Stapleton / Justin Timberlake </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v>Justin Timberlake ft. Chris Stapleton</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:31 </v>
+        <v xml:space="preserve">04:38 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1370,28 +1408,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Salt                              </v>
+        <v xml:space="preserve">Hers (Interlude)   </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kenneth Coby / Sarah Hudson / Clarence Coffee, Jr. / Tinashe Kachingwe / Kieran Lasker                                                                                                                                   </v>
+        <v xml:space="preserve"> Justin Timberlake                                                                   </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:48 </v>
+        <v xml:space="preserve">01:01 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1410,28 +1448,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Faded Love                        </v>
+        <v xml:space="preserve">Flannel            </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Noonie Bao / Tor Erik Hermansen / Tinashe Kachingwe / Sasha Sloan / Nayvadius Wilburn                                                                                                                                    </v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe feat. Future                       </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:23 </v>
+        <v xml:space="preserve">04:49 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1450,28 +1488,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Contest                        </v>
+        <v xml:space="preserve">Montana            </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Kenneth Coby / Jeremih Felton / Ray Holton / Tinashe Kachingwe / Sayyid McDonald                                                                                                                                         </v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:47 </v>
+        <v xml:space="preserve">04:39 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1490,28 +1528,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fires and Flames                  </v>
+        <v>Breeze Off the Pond</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Joel Compass / Amanda Ghost / Tinashe Kachingwe / K Stewart                                                                                                                                                              </v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Tinashe                                    </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:46 </v>
+        <v xml:space="preserve">04:11 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1523,35 +1561,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v>Livin' Off the Land</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:53 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1563,35 +1601,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">The Hard Stuff     </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> Eric Hudson / Elliott Ives / Chris Stapleton / Robin Tadross / Justin Timberlake    </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1603,35 +1641,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">Young Man          </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve"> James Fauntleroy / Jerome Harmon / Timothy Mosley / Justin Timberlake               </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">Justin Timberlake                    </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:45 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1650,21 +1688,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                   </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1690,21 +1728,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                   </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1730,21 +1768,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                   </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1770,21 +1808,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                   </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1810,21 +1848,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                  </v>
+        <v xml:space="preserve">                   </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                          </v>
+        <v xml:space="preserve">                                                                                     </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                           </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1855,9 +1893,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="79.88671875" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
     <col min="5" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1879,11 +1917,14 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>4.7916666666666663E-2</v>
+        <v>0.20347222222222219</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1893,16 +1934,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1423611111111111</v>
+        <v>0.21666666666666667</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1912,16 +1953,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.13819444444444443</v>
+        <v>0.17013888888888887</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1934,13 +1975,13 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.11944444444444445</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1950,16 +1991,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.17916666666666667</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1969,16 +2010,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.18333333333333335</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1988,16 +2029,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>4.3750000000000004E-2</v>
+        <v>0.15625</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2007,16 +2048,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2">
-        <v>0.1423611111111111</v>
+        <v>0.16874999999999998</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2026,13 +2067,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2">
-        <v>2.1527777777777781E-2</v>
+        <v>0.19305555555555554</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2042,16 +2086,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15833333333333333</v>
+        <v>4.2361111111111106E-2</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2061,16 +2105,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.14097222222222222</v>
+        <v>0.20069444444444443</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2080,16 +2124,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0.15763888888888888</v>
+        <v>0.19375000000000001</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -2099,66 +2143,110 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2">
-        <v>0.15694444444444444</v>
+        <v>0.17430555555555557</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.20347222222222219</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.13541666666666666</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="6:7">
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.15625</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="6:7">
+    <row r="18" spans="1:7">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="6:7">
+    <row r="19" spans="1:7">
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="6:7">
+    <row r="20" spans="1:7">
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="6:7">
+    <row r="21" spans="1:7">
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="6:7">
+    <row r="22" spans="1:7">
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="6:7">
+    <row r="23" spans="1:7">
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="6:7">
+    <row r="24" spans="1:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="6:7">
+    <row r="25" spans="1:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="6:7">
+    <row r="26" spans="1:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="6:7">
+    <row r="27" spans="1:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="6:7">
+    <row r="28" spans="1:7">
       <c r="G28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 07142155 started 2017 review
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="justin4" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
-    <definedName name="justin4" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
+    <definedName name="vincestaples3" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="vincestaples3" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/justin4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/vincestaples3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/justin4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/vincestaples3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="30">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -63,88 +63,85 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Title/Composer</t>
-  </si>
-  <si>
-    <t>Performer</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Filthy</t>
-  </si>
-  <si>
-    <t>Larrance Dopson / James Fauntleroy / Nate Hills / Timothy Mosley / Justin Timberlake</t>
-  </si>
-  <si>
-    <t>Justin Timberlake</t>
-  </si>
-  <si>
-    <t>Midnight Summer Jam</t>
-  </si>
-  <si>
-    <t>Chad Hugo / Justin Timberlake / Pharrell Williams</t>
-  </si>
-  <si>
-    <t>Sauce</t>
-  </si>
-  <si>
-    <t>Nate Hills / Elliott Ives / Timothy Mosley / Justin Timberlake</t>
-  </si>
-  <si>
-    <t>Man of the Woods</t>
-  </si>
-  <si>
-    <t>Higher Higher</t>
-  </si>
-  <si>
-    <t>Wave</t>
-  </si>
-  <si>
-    <t>Supplies</t>
-  </si>
-  <si>
-    <t>Morning Light</t>
-  </si>
-  <si>
-    <t>Eric Hudson / Elliott Ives / Chris Stapleton / Robin Tadross / Justin Timberlake</t>
-  </si>
-  <si>
-    <t>Justin Timberlake ft. Alicia Keys</t>
-  </si>
-  <si>
-    <t>Say Something</t>
-  </si>
-  <si>
-    <t>Larrance Dopson / Nate Hills / Timothy Mosley / Chris Stapleton / Justin Timberlake</t>
-  </si>
-  <si>
-    <t>Justin Timberlake ft. Chris Stapleton</t>
-  </si>
-  <si>
-    <t>Hers (Interlude)</t>
-  </si>
-  <si>
-    <t>Flannel</t>
-  </si>
-  <si>
-    <t>Montana</t>
-  </si>
-  <si>
-    <t>Breeze Off the Pond</t>
-  </si>
-  <si>
-    <t>Livin' Off the Land</t>
-  </si>
-  <si>
-    <t>The Hard Stuff</t>
-  </si>
-  <si>
-    <t>Young Man</t>
-  </si>
-  <si>
-    <t>James Fauntleroy / Jerome Harmon / Timothy Mosley / Justin Timberlake</t>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Writer(s)</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Crabs in a Bucket</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Zack Sekoff, Justin Vernon, Lakisha Robinson</t>
+  </si>
+  <si>
+    <t>Vincent Staples</t>
+  </si>
+  <si>
+    <t>Big Fish</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Taiwo Hassan, Kehinde Hassan, Jordan Houston</t>
+  </si>
+  <si>
+    <t>Alyssa Interlude</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Zack Sekoff, Rodger Penzabene, Barrett Strong, Norman Whitfield</t>
+  </si>
+  <si>
+    <t>Love Can Be...</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Matthew Toth, Julio Mejia, Damon Albarn, Lakisha Robinson, Alonzo Mathis, Dana Ramey, Christopher Hussery, William Ray Norwood, Jr.</t>
+  </si>
+  <si>
+    <t>Vincent Staples, James Michael Edgar</t>
+  </si>
+  <si>
+    <t>Ramona Park Is Yankee Stadium</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Ray Brady</t>
+  </si>
+  <si>
+    <t>Yeah Right</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Samuel Long, Harley Streten, Kendrick Duckworth, Laura Jane Lowther</t>
+  </si>
+  <si>
+    <t>Homage</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Zack Sekoff, Lakisha Robinson, Joshua Murphy, Julius Preston, William Roberts</t>
+  </si>
+  <si>
+    <t>Samo</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Samuel Long, Rakim Mayers</t>
+  </si>
+  <si>
+    <t>Party People</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Zack Sekoff</t>
+  </si>
+  <si>
+    <t>BagBak</t>
+  </si>
+  <si>
+    <t>Rain Come Down</t>
+  </si>
+  <si>
+    <t>Vincent Staples, Tyrone Griffin, Jr, Zack Sekoff</t>
   </si>
 </sst>
 </file>
@@ -242,11 +239,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="justin4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vincestaples3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="justin4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vincestaples3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -549,27 +546,31 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="79.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="5" max="7" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -577,16 +578,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.20347222222222219</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -596,16 +597,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.21666666666666667</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -615,16 +616,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17013888888888887</v>
+        <v>0.10972222222222222</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -634,16 +635,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -652,17 +653,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
+      <c r="B6" s="7">
+        <v>745</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17916666666666667</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -672,16 +673,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.18333333333333335</v>
+        <v>3.5416666666666666E-2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -691,16 +692,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15625</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -710,16 +711,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.12013888888888889</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -729,16 +730,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.19305555555555554</v>
+        <v>0.12083333333333333</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -748,16 +749,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>4.2361111111111106E-2</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -767,16 +768,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.20069444444444443</v>
+        <v>0.11180555555555556</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -786,129 +787,73 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2">
-        <v>0.19375000000000001</v>
+        <v>0.19513888888888889</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.17430555555555557</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.20347222222222219</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.13541666666666666</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.15625</v>
-      </c>
+    <row r="17" spans="5:7">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="5:7">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="5:7">
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="5:7">
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="5:7">
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="5:7">
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="5:7">
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="5:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="5:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="5:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="5:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="5:7">
       <c r="G28" s="2"/>
     </row>
   </sheetData>
@@ -922,7 +867,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="A3:K20"/>
+      <selection activeCell="K16" sqref="A3:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -942,15 +887,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>84</v>
+        <v>148</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -970,21 +915,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title              </v>
+        <v xml:space="preserve"> Title                        </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                          </v>
+        <v xml:space="preserve"> Composers                                                                                                                                          </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                            </v>
+        <v xml:space="preserve"> Performer      </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1009,21 +954,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------- </v>
+        <v xml:space="preserve">----------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------- </v>
+        <v xml:space="preserve"> --------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1048,28 +993,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Filthy             </v>
+        <v xml:space="preserve">Crabs in a Bucket            </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Larrance Dopson / James Fauntleroy / Nate Hills / Timothy Mosley / Justin Timberlake</v>
+        <v xml:space="preserve"> Vincent Staples, Zack Sekoff, Justin Vernon, Lakisha Robinson                                                                                       </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:53 </v>
+        <v xml:space="preserve">03:17 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1088,28 +1033,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Midnight Summer Jam</v>
+        <v xml:space="preserve">Big Fish                     </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve"> Vincent Staples, Taiwo Hassan, Kehinde Hassan, Jordan Houston                                                                                       </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:12 </v>
+        <v xml:space="preserve">03:18 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1128,28 +1073,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sauce              </v>
+        <v xml:space="preserve">Alyssa Interlude             </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nate Hills / Elliott Ives / Timothy Mosley / Justin Timberlake                      </v>
+        <v xml:space="preserve"> Vincent Staples, Zack Sekoff, Rodger Penzabene, Barrett Strong, Norman Whitfield                                                                    </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:05 </v>
+        <v xml:space="preserve">02:38 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1168,28 +1113,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Man of the Woods   </v>
+        <v xml:space="preserve">Love Can Be...               </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve"> Vincent Staples, Matthew Toth, Julio Mejia, Damon Albarn, Lakisha Robinson, Alonzo Mathis, Dana Ramey, Christopher Hussery, William Ray Norwood, Jr.</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:03 </v>
+        <v xml:space="preserve">02:58 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1208,28 +1153,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Higher Higher      </v>
+        <v xml:space="preserve">745                          </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve"> Vincent Staples, James Michael Edgar                                                                                                                </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:18 </v>
+        <v xml:space="preserve">03:47 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1248,28 +1193,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Wave               </v>
+        <v>Ramona Park Is Yankee Stadium</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve"> Vincent Staples, Ray Brady                                                                                                                          </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:24 </v>
+        <v xml:space="preserve">00:51 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1288,28 +1233,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Supplies           </v>
+        <v xml:space="preserve">Yeah Right                   </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve"> Vincent Staples, Samuel Long, Harley Streten, Kendrick Duckworth, Laura Jane Lowther                                                                </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:45 </v>
+        <v xml:space="preserve">03:08 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1328,28 +1273,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Morning Light      </v>
+        <v xml:space="preserve">Homage                       </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Eric Hudson / Elliott Ives / Chris Stapleton / Robin Tadross / Justin Timberlake    </v>
+        <v xml:space="preserve"> Vincent Staples, Zack Sekoff, Lakisha Robinson, Joshua Murphy, Julius Preston, William Roberts                                                      </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake ft. Alicia Keys    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:03 </v>
+        <v xml:space="preserve">02:53 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1368,28 +1313,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Say Something      </v>
+        <v xml:space="preserve">Samo                         </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Larrance Dopson / Nate Hills / Timothy Mosley / Chris Stapleton / Justin Timberlake </v>
+        <v xml:space="preserve"> Vincent Staples, Samuel Long, Rakim Mayers                                                                                                          </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Justin Timberlake ft. Chris Stapleton</v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:38 </v>
+        <v xml:space="preserve">02:54 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1408,28 +1353,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hers (Interlude)   </v>
+        <v xml:space="preserve">Party People                 </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Justin Timberlake                                                                   </v>
+        <v xml:space="preserve"> Vincent Staples, Zack Sekoff                                                                                                                        </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:01 </v>
+        <v xml:space="preserve">02:58 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1448,28 +1393,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Flannel            </v>
+        <v xml:space="preserve">BagBak                       </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve"> Vincent Staples, Ray Brady                                                                                                                          </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:49 </v>
+        <v xml:space="preserve">02:41 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1488,28 +1433,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Montana            </v>
+        <v xml:space="preserve">Rain Come Down               </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve"> Vincent Staples, Tyrone Griffin, Jr, Zack Sekoff                                                                                                    </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v>Vincent Staples</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:39 </v>
+        <v xml:space="preserve">04:41 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1521,35 +1466,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Breeze Off the Pond</v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:11 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1561,35 +1506,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Livin' Off the Land</v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Chad Hugo / Justin Timberlake / Pharrell Williams                                   </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:53 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1601,35 +1546,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Hard Stuff     </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Eric Hudson / Elliott Ives / Chris Stapleton / Robin Tadross / Justin Timberlake    </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1641,35 +1586,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Young Man          </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> James Fauntleroy / Jerome Harmon / Timothy Mosley / Justin Timberlake               </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Justin Timberlake                    </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:45 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1688,21 +1633,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1728,21 +1673,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1768,21 +1713,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1808,21 +1753,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1848,21 +1793,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                   </v>
+        <v xml:space="preserve">                             </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                     </v>
+        <v xml:space="preserve">                                                                                                                                                     </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">               </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1892,22 +1837,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="79.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="5" max="7" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1915,16 +1864,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.20347222222222219</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1934,16 +1883,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>0.21666666666666667</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1953,16 +1902,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17013888888888887</v>
+        <v>0.10972222222222222</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1972,16 +1921,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1990,17 +1939,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
+      <c r="B6" s="7">
+        <v>745</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17916666666666667</v>
+        <v>0.15763888888888888</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2010,16 +1959,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.18333333333333335</v>
+        <v>3.5416666666666666E-2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2029,16 +1978,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15625</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2048,16 +1997,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16874999999999998</v>
+        <v>0.12013888888888889</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2067,16 +2016,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>0.19305555555555554</v>
+        <v>0.12083333333333333</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2086,16 +2035,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>4.2361111111111106E-2</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2105,16 +2054,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.20069444444444443</v>
+        <v>0.11180555555555556</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2124,129 +2073,73 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2">
-        <v>0.19375000000000001</v>
+        <v>0.19513888888888889</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.17430555555555557</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.20347222222222219</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.13541666666666666</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.15625</v>
-      </c>
+    <row r="17" spans="5:7">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="5:7">
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="5:7">
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="5:7">
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="5:7">
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="5:7">
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="5:7">
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="5:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="5:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="5:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="5:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="5:7">
       <c r="G28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 07152055 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="vincestaples3" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="vincestaples3" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="drake7" localSheetId="0">Sheet1!$A$1:$E$23</definedName>
+    <definedName name="drake7" localSheetId="2">Sheet3!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/vincestaples3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/drake7.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/vincestaples3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/drake7.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="58">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -63,85 +63,169 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>No.</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Writer(s)</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Crabs in a Bucket</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Zack Sekoff, Justin Vernon, Lakisha Robinson</t>
-  </si>
-  <si>
-    <t>Vincent Staples</t>
-  </si>
-  <si>
-    <t>Big Fish</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Taiwo Hassan, Kehinde Hassan, Jordan Houston</t>
-  </si>
-  <si>
-    <t>Alyssa Interlude</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Zack Sekoff, Rodger Penzabene, Barrett Strong, Norman Whitfield</t>
-  </si>
-  <si>
-    <t>Love Can Be...</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Matthew Toth, Julio Mejia, Damon Albarn, Lakisha Robinson, Alonzo Mathis, Dana Ramey, Christopher Hussery, William Ray Norwood, Jr.</t>
-  </si>
-  <si>
-    <t>Vincent Staples, James Michael Edgar</t>
-  </si>
-  <si>
-    <t>Ramona Park Is Yankee Stadium</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Ray Brady</t>
-  </si>
-  <si>
-    <t>Yeah Right</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Samuel Long, Harley Streten, Kendrick Duckworth, Laura Jane Lowther</t>
-  </si>
-  <si>
-    <t>Homage</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Zack Sekoff, Lakisha Robinson, Joshua Murphy, Julius Preston, William Roberts</t>
-  </si>
-  <si>
-    <t>Samo</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Samuel Long, Rakim Mayers</t>
-  </si>
-  <si>
-    <t>Party People</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Zack Sekoff</t>
-  </si>
-  <si>
-    <t>BagBak</t>
-  </si>
-  <si>
-    <t>Rain Come Down</t>
-  </si>
-  <si>
-    <t>Vincent Staples, Tyrone Griffin, Jr, Zack Sekoff</t>
+    <t>Performer</t>
+  </si>
+  <si>
+    <t>Title/Composer</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Free Smoke</t>
+  </si>
+  <si>
+    <t>Bryan Antoine / Paul Bender / Marvin Bernard / Aubrey Graham / Simon Mavin / Perrin Moss / Allen Ritter / Naomi Saalfield / Matthew Samuels / Daniel Sewell</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>No Long Talk</t>
+  </si>
+  <si>
+    <t>Kevin Gomringer / Tim Gomringer / Aubrey Graham / Shane Lindstrom / Nathaniel Thompson</t>
+  </si>
+  <si>
+    <t>Drake ft. Giggs</t>
+  </si>
+  <si>
+    <t>Passionfruit</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Nana Rogues</t>
+  </si>
+  <si>
+    <t>Jorja (Interlude)</t>
+  </si>
+  <si>
+    <t>Adrian Eccleston / Aubrey Graham / Jorja Smith / Don McLean / Noah Shebib</t>
+  </si>
+  <si>
+    <t>Get It Together</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Paul Jefferies / Nkosinathi Maphumulo / Bucie Nqwiliso / Noah Shebib</t>
+  </si>
+  <si>
+    <t>Drake ft. Black Cofee, Jorja Smith</t>
+  </si>
+  <si>
+    <t>Madiba Riddim</t>
+  </si>
+  <si>
+    <t>Frank Dukes / Adam Feeney / Aubrey Graham / Charlie Handsome / Paul Jefferies</t>
+  </si>
+  <si>
+    <t>Blem</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Lionel Richie / Tyler Williams</t>
+  </si>
+  <si>
+    <t>Sampha Sisay / Francis Ngyun Tran</t>
+  </si>
+  <si>
+    <t>Drake ft. Sampha</t>
+  </si>
+  <si>
+    <t>Gyalchester</t>
+  </si>
+  <si>
+    <t>Rico Brooks / Aubrey Graham / Istv?n Megyimorecz</t>
+  </si>
+  <si>
+    <t>Skepta (Interlude)</t>
+  </si>
+  <si>
+    <t>Nana Rogues / Skepta</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Kevin Gomringer / Tim Gomringer / Aubrey Graham / Shane Lindstrom / Quavious Marshall / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Drake ft. Quabo, Travi$ Scott</t>
+  </si>
+  <si>
+    <t>Sacrifices</t>
+  </si>
+  <si>
+    <t>Tauheed Epps / Aubrey Graham / Daniel Johnson / Jeffery Williams / Tyler Williams</t>
+  </si>
+  <si>
+    <t>Drake ft. 2 Chainz, Young Thug</t>
+  </si>
+  <si>
+    <t>Nothings into Somethings</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Paimon Jahanbin / Ryan Martinez / Edgar Nabeyin Panford</t>
+  </si>
+  <si>
+    <t>Teenage Fever</t>
+  </si>
+  <si>
+    <t>LaShawn Daniels / Aubrey Graham / Fred "Uncle Freddie" Jerkins III / Rodney Jerkins / Jennifer Lopez / Cory Rooney / Marvin Thomas</t>
+  </si>
+  <si>
+    <t>KMT</t>
+  </si>
+  <si>
+    <t>Courtney Clayburn / Aubrey Graham / Cameron Shaikh / Nathaniel Thompson</t>
+  </si>
+  <si>
+    <t>Lose You</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Noah Shebib / Steven Vidal</t>
+  </si>
+  <si>
+    <t>Can't Have Everything</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Steve Samson / Jaswinder Singh</t>
+  </si>
+  <si>
+    <t>Glow</t>
+  </si>
+  <si>
+    <t>Phillip Bailey / Gabriel Garz?n-Montano / Noah Goldstein / Aubrey Graham / Anthony Jeffries / Louis King Johnson Jr. / Ilsey Juber / King Louie / Majid Al Maskati / Carlo "Illangelo" Montagnese / Kenza Samir / Sakiya Sandifer / Noah Shebib / Jordan Ullman / Kanye West / Maurice White / Cydel Young / Malik Yusef</t>
+  </si>
+  <si>
+    <t>Drake ft. Kanye West</t>
+  </si>
+  <si>
+    <t>Since Way Back</t>
+  </si>
+  <si>
+    <t>Jahron Brathwaite / Warryn Campbell / Aubrey Graham / R. Kelly / Ryan Martinez / Noah Shebib</t>
+  </si>
+  <si>
+    <t>Drake ft. PARTYNEXTDOOR</t>
+  </si>
+  <si>
+    <t>Fake Love</t>
+  </si>
+  <si>
+    <t>Adam Feeney / Aubrey Graham / Brittany Hazzard / Anderson Hernandez / Leon Huff / Gene McFadden / John Whitehead</t>
+  </si>
+  <si>
+    <t>Ice Melts</t>
+  </si>
+  <si>
+    <t>Aubrey Graham / Larry Griffin, Jr. / Jonathan D. Priester / Jeffery Williams</t>
+  </si>
+  <si>
+    <t>Drake ft. Young Thug</t>
+  </si>
+  <si>
+    <t>Do Not Disturb</t>
+  </si>
+  <si>
+    <t>Snoh Aalegra / Aubrey Graham / Leven Kali / Allen Ritter / Matthew Samuels / Noah Shebib</t>
   </si>
 </sst>
 </file>
@@ -239,11 +323,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vincestaples3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="drake7" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="vincestaples3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="drake7" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -551,26 +635,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="7" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -578,16 +658,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -597,16 +677,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -622,10 +702,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.10972222222222222</v>
+        <v>0.2076388888888889</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -641,10 +721,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.12361111111111112</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -653,17 +733,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>745</v>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>0.15763888888888888</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -673,16 +753,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>3.5416666666666666E-2</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -692,16 +772,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.15069444444444444</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -710,17 +790,17 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
+      <c r="B9">
+        <v>4422</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12013888888888889</v>
+        <v>0.12916666666666668</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -730,16 +810,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12083333333333333</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -749,16 +829,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.12361111111111112</v>
+        <v>9.930555555555555E-2</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -768,16 +848,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2">
-        <v>0.11180555555555556</v>
+        <v>0.16458333333333333</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -787,73 +867,219 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2">
-        <v>0.19513888888888889</v>
+        <v>0.21388888888888891</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.10694444444444444</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.15277777777777776</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.11319444444444444</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:7">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.21180555555555555</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="5:7">
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.15833333333333333</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="5:7">
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14305555555555557</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7">
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.25555555555555559</v>
+      </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7">
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.14652777777777778</v>
+      </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="5:7">
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.17430555555555557</v>
+      </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="5:7">
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.19722222222222222</v>
+      </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="5:7">
+    <row r="24" spans="1:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="5:7">
+    <row r="25" spans="1:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="5:7">
+    <row r="26" spans="1:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="5:7">
+    <row r="27" spans="1:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="5:7">
+    <row r="28" spans="1:7">
       <c r="G28" s="2"/>
     </row>
   </sheetData>
@@ -867,7 +1093,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="A3:K16"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -887,15 +1113,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>148</v>
+        <v>312</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -915,21 +1141,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                        </v>
+        <v xml:space="preserve"> Title                   </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                          </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                                                                                                                                                                              </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer      </v>
+        <v xml:space="preserve"> Performer                         </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -954,21 +1180,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">----------------------------- </v>
+        <v xml:space="preserve">------------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> --------------- </v>
+        <v xml:space="preserve"> ---------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -993,28 +1219,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Crabs in a Bucket            </v>
+        <v xml:space="preserve">Free Smoke              </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Zack Sekoff, Justin Vernon, Lakisha Robinson                                                                                       </v>
+        <v xml:space="preserve"> Bryan Antoine / Paul Bender / Marvin Bernard / Aubrey Graham / Simon Mavin / Perrin Moss / Allen Ritter / Naomi Saalfield / Matthew Samuels / Daniel Sewell                                                                                                                                                             </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:17 </v>
+        <v xml:space="preserve">03:39 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1033,28 +1259,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Big Fish                     </v>
+        <v xml:space="preserve">No Long Talk            </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Taiwo Hassan, Kehinde Hassan, Jordan Houston                                                                                       </v>
+        <v xml:space="preserve"> Kevin Gomringer / Tim Gomringer / Aubrey Graham / Shane Lindstrom / Nathaniel Thompson                                                                                                                                                                                                                                  </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake ft. Giggs                   </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:18 </v>
+        <v xml:space="preserve">02:30 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1073,28 +1299,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Alyssa Interlude             </v>
+        <v xml:space="preserve">Passionfruit            </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Zack Sekoff, Rodger Penzabene, Barrett Strong, Norman Whitfield                                                                    </v>
+        <v xml:space="preserve"> Aubrey Graham / Nana Rogues                                                                                                                                                                                                                                                                                             </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:38 </v>
+        <v xml:space="preserve">04:59 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1113,28 +1339,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Love Can Be...               </v>
+        <v xml:space="preserve">Jorja (Interlude)       </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Matthew Toth, Julio Mejia, Damon Albarn, Lakisha Robinson, Alonzo Mathis, Dana Ramey, Christopher Hussery, William Ray Norwood, Jr.</v>
+        <v xml:space="preserve"> Adrian Eccleston / Aubrey Graham / Jorja Smith / Don McLean / Noah Shebib                                                                                                                                                                                                                                               </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:58 </v>
+        <v xml:space="preserve">01:48 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1153,28 +1379,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">745                          </v>
+        <v xml:space="preserve">Get It Together         </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, James Michael Edgar                                                                                                                </v>
+        <v xml:space="preserve"> Aubrey Graham / Paul Jefferies / Nkosinathi Maphumulo / Bucie Nqwiliso / Noah Shebib                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v>Drake ft. Black Cofee, Jorja Smith</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:47 </v>
+        <v xml:space="preserve">04:10 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1193,28 +1419,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Ramona Park Is Yankee Stadium</v>
+        <v xml:space="preserve">Madiba Riddim           </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Ray Brady                                                                                                                          </v>
+        <v xml:space="preserve"> Frank Dukes / Adam Feeney / Aubrey Graham / Charlie Handsome / Paul Jefferies                                                                                                                                                                                                                                           </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:51 </v>
+        <v xml:space="preserve">03:25 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1233,28 +1459,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Yeah Right                   </v>
+        <v xml:space="preserve">Blem                    </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Samuel Long, Harley Streten, Kendrick Duckworth, Laura Jane Lowther                                                                </v>
+        <v xml:space="preserve"> Aubrey Graham / Lionel Richie / Tyler Williams                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:08 </v>
+        <v xml:space="preserve">03:37 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1273,28 +1499,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Homage                       </v>
+        <v xml:space="preserve">4422                    </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Zack Sekoff, Lakisha Robinson, Joshua Murphy, Julius Preston, William Roberts                                                      </v>
+        <v xml:space="preserve"> Sampha Sisay / Francis Ngyun Tran                                                                                                                                                                                                                                                                                       </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake ft. Sampha                  </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:53 </v>
+        <v xml:space="preserve">03:06 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1313,28 +1539,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Samo                         </v>
+        <v xml:space="preserve">Gyalchester             </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Samuel Long, Rakim Mayers                                                                                                          </v>
+        <v xml:space="preserve"> Rico Brooks / Aubrey Graham / Istv?n Megyimorecz                                                                                                                                                                                                                                                                        </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:54 </v>
+        <v xml:space="preserve">03:09 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1353,28 +1579,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Party People                 </v>
+        <v xml:space="preserve">Skepta (Interlude)      </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Zack Sekoff                                                                                                                        </v>
+        <v xml:space="preserve"> Nana Rogues / Skepta                                                                                                                                                                                                                                                                                                    </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:58 </v>
+        <v xml:space="preserve">02:23 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1393,28 +1619,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">BagBak                       </v>
+        <v xml:space="preserve">Portland                </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Ray Brady                                                                                                                          </v>
+        <v xml:space="preserve"> Kevin Gomringer / Tim Gomringer / Aubrey Graham / Shane Lindstrom / Quavious Marshall / Jacques Webster                                                                                                                                                                                                                 </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake ft. Quabo, Travi$ Scott     </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:41 </v>
+        <v xml:space="preserve">03:57 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1433,28 +1659,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Rain Come Down               </v>
+        <v xml:space="preserve">Sacrifices              </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Vincent Staples, Tyrone Griffin, Jr, Zack Sekoff                                                                                                    </v>
+        <v xml:space="preserve"> Tauheed Epps / Aubrey Graham / Daniel Johnson / Jeffery Williams / Tyler Williams                                                                                                                                                                                                                                       </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Vincent Staples</v>
+        <v xml:space="preserve">Drake ft. 2 Chainz, Young Thug    </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:41 </v>
+        <v xml:space="preserve">05:08 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1466,35 +1692,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v>Nothings into Somethings</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> Aubrey Graham / Paimon Jahanbin / Ryan Martinez / Edgar Nabeyin Panford                                                                                                                                                                                                                                                 </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:34 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1506,35 +1732,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">Teenage Fever           </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> LaShawn Daniels / Aubrey Graham / Fred "Uncle Freddie" Jerkins III / Rodney Jerkins / Jennifer Lopez / Cory Rooney / Marvin Thomas                                                                                                                                                                                      </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:40 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1546,35 +1772,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">KMT                     </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> Courtney Clayburn / Aubrey Graham / Cameron Shaikh / Nathaniel Thompson                                                                                                                                                                                                                                                 </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake ft. Giggs                   </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">02:43 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1586,35 +1812,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">Lose You                </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> Aubrey Graham / Noah Shebib / Steven Vidal                                                                                                                                                                                                                                                                              </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">05:05 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1626,35 +1852,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">Can't Have Everything   </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> Aubrey Graham / Steve Samson / Jaswinder Singh                                                                                                                                                                                                                                                                          </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:48 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1666,35 +1892,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">Glow                    </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> Phillip Bailey / Gabriel Garz?n-Montano / Noah Goldstein / Aubrey Graham / Anthony Jeffries / Louis King Johnson Jr. / Ilsey Juber / King Louie / Majid Al Maskati / Carlo "Illangelo" Montagnese / Kenza Samir / Sakiya Sandifer / Noah Shebib / Jordan Ullman / Kanye West / Maurice White / Cydel Young / Malik Yusef</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake ft. Kanye West              </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:26 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1706,35 +1932,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">Since Way Back          </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> Jahron Brathwaite / Warryn Campbell / Aubrey Graham / R. Kelly / Ryan Martinez / Noah Shebib                                                                                                                                                                                                                            </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake ft. PARTYNEXTDOOR           </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">06:08 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -1746,35 +1972,35 @@
       </c>
       <c r="B24">
         <f>Sheet1!A21</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">Fake Love               </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> Adam Feeney / Aubrey Graham / Brittany Hazzard / Anderson Hernandez / Leon Huff / Gene McFadden / John Whitehead                                                                                                                                                                                                        </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake                             </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J24" s="3" t="str">
         <f>TEXT(Sheet1!E21,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:31 </v>
       </c>
       <c r="K24" s="4" t="s">
         <v>0</v>
@@ -1786,35 +2012,35 @@
       </c>
       <c r="B25">
         <f>Sheet1!A22</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                             </v>
+        <v xml:space="preserve">Ice Melts               </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                     </v>
+        <v xml:space="preserve"> Aubrey Graham / Larry Griffin, Jr. / Jonathan D. Priester / Jeffery Williams                                                                                                                                                                                                                                            </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">               </v>
+        <v xml:space="preserve">Drake ft. Young Thug              </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J25" s="3" t="str">
         <f>TEXT(Sheet1!E22,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:11 </v>
       </c>
       <c r="K25" s="4" t="s">
         <v>0</v>
@@ -1837,26 +2063,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="7" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1864,16 +2086,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13680555555555554</v>
+        <v>0.15208333333333332</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1883,16 +2105,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1908,10 +2130,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.10972222222222222</v>
+        <v>0.2076388888888889</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1927,10 +2149,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.12361111111111112</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1939,17 +2161,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
-        <v>745</v>
+      <c r="B6" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>0.15763888888888888</v>
+        <v>0.17361111111111113</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1959,16 +2181,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>3.5416666666666666E-2</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1978,16 +2200,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.15069444444444444</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1996,17 +2218,17 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
+      <c r="B9">
+        <v>4422</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2">
-        <v>0.12013888888888889</v>
+        <v>0.12916666666666668</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2016,16 +2238,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.12083333333333333</v>
+        <v>0.13125000000000001</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2035,16 +2257,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.12361111111111112</v>
+        <v>9.930555555555555E-2</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2054,16 +2276,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2">
-        <v>0.11180555555555556</v>
+        <v>0.16458333333333333</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2073,73 +2295,219 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2">
-        <v>0.19513888888888889</v>
+        <v>0.21388888888888891</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.10694444444444444</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.15277777777777776</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="E16" s="2"/>
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.11319444444444444</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:7">
-      <c r="E17" s="2"/>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.21180555555555555</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="5:7">
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.15833333333333333</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="5:7">
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.14305555555555557</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7">
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.25555555555555559</v>
+      </c>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7">
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.14652777777777778</v>
+      </c>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="5:7">
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.17430555555555557</v>
+      </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="5:7">
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.19722222222222222</v>
+      </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="5:7">
+    <row r="24" spans="1:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="5:7">
+    <row r="25" spans="1:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="5:7">
+    <row r="26" spans="1:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="5:7">
+    <row r="27" spans="1:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="5:7">
+    <row r="28" spans="1:7">
       <c r="G28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: 07172255 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="future4" localSheetId="0">Sheet1!$A$1:$E$20</definedName>
-    <definedName name="future4" localSheetId="2">Sheet3!$A$1:$E$20</definedName>
+    <definedName name="loylecarner1" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="loylecarner1" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/future4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/loylecarner1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/future4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/loylecarner1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="33">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -66,142 +66,91 @@
     <t>Performer</t>
   </si>
   <si>
-    <t>No.</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Writer(s)</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>My Collection</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Leland Wayne, Kevin Gomringer, Tim Gomringer</t>
-  </si>
-  <si>
-    <t>Future</t>
-  </si>
-  <si>
-    <t>Comin Out Strong (featuring The Weeknd)</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Kevin Vincent, Noel Fisher, Henry Walter, Abel Tesfaye, Ahmad Balshe</t>
-  </si>
-  <si>
-    <t>Future ft. The Weeknd</t>
-  </si>
-  <si>
-    <t>Lookin Exotic</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Joshua Luellen, Jacob Dutton, Kendricke Brown, Andrew Mayer Cohen</t>
-  </si>
-  <si>
-    <t>Damage</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Dijon McFarlane, Te Whiti Warbrick, Nick Audino, Lewis Hughes, Khaled Rohaim, Noel Fisher, Gene Griffin, Teddy Riley, Aaron Robin Hall, William Gaitling</t>
-  </si>
-  <si>
-    <t>Use Me</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Noel Fisher, Sidney Swift, Justin Bradley, Ruben Raymond, Justin Rodriguez</t>
-  </si>
-  <si>
-    <t>Incredible</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Andre Proctor, William Moore, Ngandu Andy Kabamba</t>
-  </si>
-  <si>
-    <t>Testify</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Joshua Luellen</t>
-  </si>
-  <si>
-    <t>Fresh Air</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Omar Walker, Noel Fisher, Evan Smith, Benjahmin Singh-Reynolds</t>
-  </si>
-  <si>
-    <t>Neva Missa Lost</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Noel Fisher, Omar Walker, Xeryus Gittens, Donald DeGrate, Cedric Hailey</t>
-  </si>
-  <si>
-    <t>Keep Quiet</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Gary Hill, Kendricke Brown</t>
-  </si>
-  <si>
-    <t>Hallucinating</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Andre Proctor</t>
-  </si>
-  <si>
-    <t>I Thank U</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Wesley Glass</t>
-  </si>
-  <si>
-    <t>New Illuminati</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Dwan Avery, Shawn Kyles</t>
-  </si>
-  <si>
-    <t>Turn On Me</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Kelvin Brown, Joshua Luellen</t>
-  </si>
-  <si>
-    <t>Selfish (featuring Rihanna)</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Noel Fisher, Omar Walker, Evan Smith, Robyn Fenty</t>
-  </si>
-  <si>
-    <t>Future ft. Rihanna</t>
-  </si>
-  <si>
-    <t>Solo</t>
-  </si>
-  <si>
-    <t>Sorry</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Leland Wayne, K. Gomringer, T. Gomringer</t>
-  </si>
-  <si>
-    <t>Pie (featuring Chris Brown)</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Noel Fisher, David Doman, Christopher Brown, Justin Thomas, Jim Stewart, Thomas Klotz</t>
-  </si>
-  <si>
-    <t>Future ft. Chris Brown</t>
-  </si>
-  <si>
-    <t>You da Baddest (featuring Nicki Minaj)</t>
-  </si>
-  <si>
-    <t>Nayvadius Wilburn, Onika Maraj, Noel Fisher, Andre Price</t>
-  </si>
-  <si>
-    <t>Future ft. Nicki Minaj</t>
+    <t>Title/Composer</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>The Isle of Arran</t>
+  </si>
+  <si>
+    <t>Ben Coyle Larner, Lawrence Lord</t>
+  </si>
+  <si>
+    <t>Loyle Carner</t>
+  </si>
+  <si>
+    <t>Mean It in the Morning</t>
+  </si>
+  <si>
+    <t>Ben Coyle Larner</t>
+  </si>
+  <si>
+    <t>Damselfly</t>
+  </si>
+  <si>
+    <t>Ben Coyle Larner, Tom Misch</t>
+  </si>
+  <si>
+    <t>Loyle Carner feat. Tom Misch</t>
+  </si>
+  <si>
+    <t>Ain't Nothing Changed</t>
+  </si>
+  <si>
+    <t>Piero Umiliani</t>
+  </si>
+  <si>
+    <t>Swear</t>
+  </si>
+  <si>
+    <t>Florence</t>
+  </si>
+  <si>
+    <t>Ben Coyle Larner, Kwes</t>
+  </si>
+  <si>
+    <t>Loyle Carner feat. Kwes</t>
+  </si>
+  <si>
+    <t>The Seamstress (Tooting Masala)</t>
+  </si>
+  <si>
+    <t>Ben Coyle Larner, Saul Mayne</t>
+  </si>
+  <si>
+    <t>Stars &amp; Shards</t>
+  </si>
+  <si>
+    <t>No Worries</t>
+  </si>
+  <si>
+    <t>Ben Coyle Larner, Krisitian Revelle, Zach Gill, Otis Jackson Jr., Romeo Jiminez, Jack Brown, William Shileds</t>
+  </si>
+  <si>
+    <t>Loyle Carner feat, Rebel Kleff, Jehst</t>
+  </si>
+  <si>
+    <t>Rebel 101</t>
+  </si>
+  <si>
+    <t>No CD</t>
+  </si>
+  <si>
+    <t>Loyle Carner feat. Rebel Kleff</t>
+  </si>
+  <si>
+    <t>Mrs. C</t>
+  </si>
+  <si>
+    <t>Sun of Jean</t>
+  </si>
+  <si>
+    <t>Ben Coyle Larner, Kwes, Steven Vengeance, John Coyle Larner</t>
+  </si>
+  <si>
+    <t>Loyle Carner feat. Mum and Dad</t>
   </si>
 </sst>
 </file>
@@ -299,11 +248,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="future4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="loylecarner1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="future4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="loylecarner1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -611,29 +560,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="7" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
+    <col min="5" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -641,16 +583,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.17708333333333334</v>
+        <v>0.14861111111111111</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -660,16 +602,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1763888888888889</v>
+        <v>0.11041666666666666</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -678,17 +620,17 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
+      <c r="B4">
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15694444444444444</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -698,16 +640,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16458333333333333</v>
+        <v>0.11944444444444445</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -717,16 +659,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17777777777777778</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -736,16 +678,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.17222222222222225</v>
+        <v>2.361111111111111E-2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -755,16 +694,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2">
-        <v>0.12361111111111112</v>
+        <v>0.1277777777777778</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -774,16 +713,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.1875</v>
+        <v>0.10486111111111111</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -793,16 +732,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.16527777777777777</v>
+        <v>0.1277777777777778</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -812,16 +751,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E11" s="2">
-        <v>0.14027777777777778</v>
+        <v>0.1875</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -831,16 +770,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.15347222222222223</v>
+        <v>1.9444444444444445E-2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -850,16 +786,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E13" s="2">
-        <v>9.7916666666666666E-2</v>
+        <v>0.17777777777777778</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -869,16 +805,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.14027777777777778</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -888,146 +824,73 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2">
-        <v>0.18333333333333335</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.17430555555555557</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.18472222222222223</v>
-      </c>
+    <row r="17" spans="5:7">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.31319444444444444</v>
-      </c>
+    <row r="18" spans="5:7">
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14652777777777778</v>
-      </c>
+    <row r="19" spans="5:7">
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.1673611111111111</v>
-      </c>
+    <row r="20" spans="5:7">
+      <c r="E20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="5:7">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="5:7">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="5:7">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="5:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="5:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="5:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="5:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="5:7">
       <c r="G28" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="http://bm.planetky.com/future4.htm"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1037,7 +900,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="A3:K23"/>
+      <selection activeCell="K18" sqref="A3:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -1057,15 +920,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -1085,21 +948,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                                  </v>
+        <v xml:space="preserve"> Title                          </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                                 </v>
+        <v xml:space="preserve"> Composers                                                                                                  </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer             </v>
+        <v xml:space="preserve"> Performer                            </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1124,21 +987,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">--------------------------------------- </v>
+        <v xml:space="preserve">------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> --------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------ </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------- </v>
+        <v xml:space="preserve"> ------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1163,28 +1026,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">My Collection                          </v>
+        <v xml:space="preserve">The Isle of Arran              </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Leland Wayne, Kevin Gomringer, Tim Gomringer                                                                                                            </v>
+        <v xml:space="preserve"> Ben Coyle Larner, Lawrence Lord                                                                             </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:15 </v>
+        <v xml:space="preserve">03:34 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1203,28 +1066,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Comin Out Strong (featuring The Weeknd)</v>
+        <v xml:space="preserve">Mean It in the Morning         </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Kevin Vincent, Noel Fisher, Henry Walter, Abel Tesfaye, Ahmad Balshe                                                                                    </v>
+        <v xml:space="preserve"> Ben Coyle Larner                                                                                            </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future ft. The Weeknd </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:14 </v>
+        <v xml:space="preserve">02:39 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1243,28 +1106,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lookin Exotic                          </v>
+        <v xml:space="preserve">44                             </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Joshua Luellen, Jacob Dutton, Kendricke Brown, Andrew Mayer Cohen                                                                                       </v>
+        <v xml:space="preserve"> Ben Coyle Larner                                                                                            </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:46 </v>
+        <v xml:space="preserve">00:48 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1283,28 +1146,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Damage                                 </v>
+        <v xml:space="preserve">Damselfly                      </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Dijon McFarlane, Te Whiti Warbrick, Nick Audino, Lewis Hughes, Khaled Rohaim, Noel Fisher, Gene Griffin, Teddy Riley, Aaron Robin Hall, William Gaitling</v>
+        <v xml:space="preserve"> Ben Coyle Larner, Tom Misch                                                                                 </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner feat. Tom Misch         </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:57 </v>
+        <v xml:space="preserve">02:52 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1323,28 +1186,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Use Me                                 </v>
+        <v xml:space="preserve">Ain't Nothing Changed          </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Noel Fisher, Sidney Swift, Justin Bradley, Ruben Raymond, Justin Rodriguez                                                                              </v>
+        <v xml:space="preserve"> Piero Umiliani                                                                                              </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:16 </v>
+        <v xml:space="preserve">03:10 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1363,28 +1226,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Incredible                             </v>
+        <v xml:space="preserve">Swear                          </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Andre Proctor, William Moore, Ngandu Andy Kabamba                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:08 </v>
+        <v xml:space="preserve">00:34 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1403,28 +1266,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Testify                                </v>
+        <v xml:space="preserve">Florence                       </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Joshua Luellen                                                                                                                                          </v>
+        <v xml:space="preserve"> Ben Coyle Larner, Kwes                                                                                      </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner feat. Kwes              </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:58 </v>
+        <v xml:space="preserve">03:04 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1443,28 +1306,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Fresh Air                              </v>
+        <v>The Seamstress (Tooting Masala)</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Omar Walker, Noel Fisher, Evan Smith, Benjahmin Singh-Reynolds                                                                                          </v>
+        <v xml:space="preserve"> Ben Coyle Larner, Saul Mayne                                                                                </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:30 </v>
+        <v xml:space="preserve">02:31 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1483,28 +1346,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Neva Missa Lost                        </v>
+        <v xml:space="preserve">Stars &amp; Shards                 </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Noel Fisher, Omar Walker, Xeryus Gittens, Donald DeGrate, Cedric Hailey                                                                                 </v>
+        <v xml:space="preserve"> Ben Coyle Larner                                                                                            </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:58 </v>
+        <v xml:space="preserve">03:04 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1523,28 +1386,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Keep Quiet                             </v>
+        <v xml:space="preserve">No Worries                     </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Gary Hill, Kendricke Brown                                                                                                                              </v>
+        <v xml:space="preserve"> Ben Coyle Larner, Krisitian Revelle, Zach Gill, Otis Jackson Jr., Romeo Jiminez, Jack Brown, William Shileds</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v>Loyle Carner feat, Rebel Kleff, Jehst</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:22 </v>
+        <v xml:space="preserve">04:30 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1563,28 +1426,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hallucinating                          </v>
+        <v xml:space="preserve">Rebel 101                      </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Andre Proctor                                                                                                                                           </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:41 </v>
+        <v xml:space="preserve">00:28 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1603,28 +1466,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">I Thank U                              </v>
+        <v xml:space="preserve">No CD                          </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Wesley Glass                                                                                                                                            </v>
+        <v xml:space="preserve"> Ben Coyle Larner                                                                                            </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner feat. Rebel Kleff       </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:21 </v>
+        <v xml:space="preserve">04:16 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1643,28 +1506,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">New Illuminati                         </v>
+        <v xml:space="preserve">Mrs. C                         </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Dwan Avery, Shawn Kyles                                                                                                                                 </v>
+        <v xml:space="preserve"> Ben Coyle Larner, Kwes                                                                                      </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner                         </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:01 </v>
+        <v xml:space="preserve">03:22 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1683,28 +1546,28 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Turn On Me                             </v>
+        <v xml:space="preserve">Sun of Jean                    </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Kelvin Brown, Joshua Luellen                                                                                                                            </v>
+        <v xml:space="preserve"> Ben Coyle Larner, Kwes, Steven Vengeance, John Coyle Larner                                                 </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">Loyle Carner feat. Mum and Dad       </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:24 </v>
+        <v xml:space="preserve">08:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1716,35 +1579,35 @@
       </c>
       <c r="B19">
         <f>Sheet1!A16</f>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Selfish (featuring Rihanna)            </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Noel Fisher, Omar Walker, Evan Smith, Robyn Fenty                                                                                                       </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future ft. Rihanna    </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J19" s="3" t="str">
         <f>TEXT(Sheet1!E16,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:11 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K19" s="4" t="s">
         <v>0</v>
@@ -1756,35 +1619,35 @@
       </c>
       <c r="B20">
         <f>Sheet1!A17</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Solo                                   </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Andre Proctor                                                                                                                                           </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J20" s="3" t="str">
         <f>TEXT(Sheet1!E17,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:26 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K20" s="4" t="s">
         <v>0</v>
@@ -1796,35 +1659,35 @@
       </c>
       <c r="B21">
         <f>Sheet1!A18</f>
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sorry                                  </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Leland Wayne, K. Gomringer, T. Gomringer                                                                                                                </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Future                </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J21" s="3" t="str">
         <f>TEXT(Sheet1!E18,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">07:31 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K21" s="4" t="s">
         <v>0</v>
@@ -1836,35 +1699,35 @@
       </c>
       <c r="B22">
         <f>Sheet1!A19</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pie (featuring Chris Brown)            </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Noel Fisher, David Doman, Christopher Brown, Justin Thomas, Jim Stewart, Thomas Klotz                                                                   </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Future ft. Chris Brown</v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J22" s="3" t="str">
         <f>TEXT(Sheet1!E19,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:31 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K22" s="4" t="s">
         <v>0</v>
@@ -1876,35 +1739,35 @@
       </c>
       <c r="B23">
         <f>Sheet1!A20</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">You da Baddest (featuring Nicki Minaj) </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nayvadius Wilburn, Onika Maraj, Noel Fisher, Andre Price                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Future ft. Nicki Minaj</v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J23" s="3" t="str">
         <f>TEXT(Sheet1!E20,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:01 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K23" s="4" t="s">
         <v>0</v>
@@ -1923,21 +1786,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                       </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1963,21 +1826,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                       </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                            </v>
+        <v xml:space="preserve">                                                                                                             </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                                     </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -2007,29 +1870,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="7" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
+    <col min="5" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2037,16 +1893,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.17708333333333334</v>
+        <v>0.14861111111111111</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -2056,16 +1912,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.1763888888888889</v>
+        <v>0.11041666666666666</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -2074,17 +1930,17 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
+      <c r="B4">
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15694444444444444</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -2094,16 +1950,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
-        <v>0.16458333333333333</v>
+        <v>0.11944444444444445</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2113,16 +1969,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.17777777777777778</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2132,16 +1988,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.17222222222222225</v>
+        <v>2.361111111111111E-2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2151,16 +2004,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2">
-        <v>0.12361111111111112</v>
+        <v>0.1277777777777778</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2170,16 +2023,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.1875</v>
+        <v>0.10486111111111111</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2189,16 +2042,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.16527777777777777</v>
+        <v>0.1277777777777778</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2208,16 +2061,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E11" s="2">
-        <v>0.14027777777777778</v>
+        <v>0.1875</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2227,16 +2080,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" s="2">
-        <v>0.15347222222222223</v>
+        <v>1.9444444444444445E-2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2246,16 +2096,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="E13" s="2">
-        <v>9.7916666666666666E-2</v>
+        <v>0.17777777777777778</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -2265,16 +2115,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.14027777777777778</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2284,139 +2134,69 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2">
-        <v>0.18333333333333335</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.17430555555555557</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.18472222222222223</v>
-      </c>
+    <row r="17" spans="5:7">
+      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.31319444444444444</v>
-      </c>
+    <row r="18" spans="5:7">
+      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.14652777777777778</v>
-      </c>
+    <row r="19" spans="5:7">
+      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.1673611111111111</v>
-      </c>
+    <row r="20" spans="5:7">
+      <c r="E20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="5:7">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="5:7">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="5:7">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="5:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="5:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="5:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="5:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="5:7">
       <c r="G28" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
07182050 added 2oldr eviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="loylecarner1" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
-    <definedName name="loylecarner1" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
+    <definedName name="mavisstaples4" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="mavisstaples4" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/loylecarner1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/mavisstaples4.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/loylecarner1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/mavisstaples4.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="19">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,85 +72,43 @@
     <t>Time</t>
   </si>
   <si>
-    <t>The Isle of Arran</t>
+    <t>Little Bit</t>
   </si>
   <si>
-    <t>Ben Coyle Larner, Lawrence Lord</t>
+    <t>Jeff Tweedy</t>
   </si>
   <si>
-    <t>Loyle Carner</t>
+    <t>Mavis Staples</t>
   </si>
   <si>
-    <t>Mean It in the Morning</t>
+    <t>If All I Was Was Black</t>
   </si>
   <si>
-    <t>Ben Coyle Larner</t>
+    <t>Mavis Staples / Jeff Tweedy</t>
   </si>
   <si>
-    <t>Damselfly</t>
+    <t>Who Told You That</t>
   </si>
   <si>
-    <t>Ben Coyle Larner, Tom Misch</t>
+    <t>Ain't No Doubt About It</t>
   </si>
   <si>
-    <t>Loyle Carner feat. Tom Misch</t>
+    <t>Peaceful Dream</t>
   </si>
   <si>
-    <t>Ain't Nothing Changed</t>
+    <t>No Time for Crying</t>
   </si>
   <si>
-    <t>Piero Umiliani</t>
+    <t>Build a Bridge</t>
   </si>
   <si>
-    <t>Swear</t>
+    <t>We Go High</t>
   </si>
   <si>
-    <t>Florence</t>
+    <t>Try Harder</t>
   </si>
   <si>
-    <t>Ben Coyle Larner, Kwes</t>
-  </si>
-  <si>
-    <t>Loyle Carner feat. Kwes</t>
-  </si>
-  <si>
-    <t>The Seamstress (Tooting Masala)</t>
-  </si>
-  <si>
-    <t>Ben Coyle Larner, Saul Mayne</t>
-  </si>
-  <si>
-    <t>Stars &amp; Shards</t>
-  </si>
-  <si>
-    <t>No Worries</t>
-  </si>
-  <si>
-    <t>Ben Coyle Larner, Krisitian Revelle, Zach Gill, Otis Jackson Jr., Romeo Jiminez, Jack Brown, William Shileds</t>
-  </si>
-  <si>
-    <t>Loyle Carner feat, Rebel Kleff, Jehst</t>
-  </si>
-  <si>
-    <t>Rebel 101</t>
-  </si>
-  <si>
-    <t>No CD</t>
-  </si>
-  <si>
-    <t>Loyle Carner feat. Rebel Kleff</t>
-  </si>
-  <si>
-    <t>Mrs. C</t>
-  </si>
-  <si>
-    <t>Sun of Jean</t>
-  </si>
-  <si>
-    <t>Ben Coyle Larner, Kwes, Steven Vengeance, John Coyle Larner</t>
-  </si>
-  <si>
-    <t>Loyle Carner feat. Mum and Dad</t>
+    <t>All Over Again</t>
   </si>
 </sst>
 </file>
@@ -248,11 +206,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="loylecarner1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mavisstaples4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="loylecarner1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mavisstaples4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,7 +510,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -561,10 +519,12 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="5" max="7" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -592,7 +552,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.16041666666666668</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -611,7 +571,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.11041666666666666</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -620,17 +580,17 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>44</v>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>3.3333333333333333E-2</v>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -640,16 +600,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.11944444444444445</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -659,16 +619,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -678,13 +638,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>2.361111111111111E-2</v>
+        <v>0.19166666666666665</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -694,16 +657,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.15069444444444444</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -713,16 +676,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.10486111111111111</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -732,16 +695,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.16041666666666668</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -751,90 +714,40 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1875</v>
+        <v>7.9166666666666663E-2</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.9444444444444445E-2</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.17777777777777778</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.14027777777777778</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
@@ -888,6 +801,21 @@
     </row>
     <row r="28" spans="5:7">
       <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="5:7">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="5:7">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="5:7">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="5:7">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -900,7 +828,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="A3:K18"/>
+      <selection activeCell="K14" sqref="A3:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -920,15 +848,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -948,21 +876,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                          </v>
+        <v xml:space="preserve"> Title                  </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                  </v>
+        <v xml:space="preserve"> Composers                 </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                            </v>
+        <v xml:space="preserve"> Performer    </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -987,21 +915,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------------------- </v>
+        <v xml:space="preserve">----------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------------------------------------------------------------ </v>
+        <v xml:space="preserve"> --------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------- </v>
+        <v xml:space="preserve"> ------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1026,28 +954,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Isle of Arran              </v>
+        <v xml:space="preserve">Little Bit             </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner, Lawrence Lord                                                                             </v>
+        <v xml:space="preserve"> Jeff Tweedy                </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:34 </v>
+        <v xml:space="preserve">03:51 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1066,28 +994,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Mean It in the Morning         </v>
+        <v xml:space="preserve">If All I Was Was Black </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner                                                                                            </v>
+        <v xml:space="preserve"> Mavis Staples / Jeff Tweedy</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:39 </v>
+        <v xml:space="preserve">03:55 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1106,28 +1034,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">44                             </v>
+        <v xml:space="preserve">Who Told You That      </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner                                                                                            </v>
+        <v xml:space="preserve"> Jeff Tweedy                </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:48 </v>
+        <v xml:space="preserve">02:48 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1146,28 +1074,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Damselfly                      </v>
+        <v>Ain't No Doubt About It</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner, Tom Misch                                                                                 </v>
+        <v xml:space="preserve"> Jeff Tweedy                </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner feat. Tom Misch         </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:52 </v>
+        <v xml:space="preserve">03:18 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1186,28 +1114,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ain't Nothing Changed          </v>
+        <v xml:space="preserve">Peaceful Dream         </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Piero Umiliani                                                                                              </v>
+        <v xml:space="preserve"> Jeff Tweedy                </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:10 </v>
+        <v xml:space="preserve">03:20 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1226,28 +1154,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Swear                          </v>
+        <v xml:space="preserve">No Time for Crying     </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve"> Mavis Staples / Jeff Tweedy</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:34 </v>
+        <v xml:space="preserve">04:36 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1266,28 +1194,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Florence                       </v>
+        <v xml:space="preserve">Build a Bridge         </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner, Kwes                                                                                      </v>
+        <v xml:space="preserve"> Jeff Tweedy                </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner feat. Kwes              </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:04 </v>
+        <v xml:space="preserve">03:37 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1306,28 +1234,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>The Seamstress (Tooting Masala)</v>
+        <v xml:space="preserve">We Go High             </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner, Saul Mayne                                                                                </v>
+        <v xml:space="preserve"> Mavis Staples / Jeff Tweedy</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:31 </v>
+        <v xml:space="preserve">03:26 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1346,28 +1274,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Stars &amp; Shards                 </v>
+        <v xml:space="preserve">Try Harder             </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner                                                                                            </v>
+        <v xml:space="preserve"> Jeff Tweedy                </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:04 </v>
+        <v xml:space="preserve">03:51 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1386,28 +1314,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Worries                     </v>
+        <v xml:space="preserve">All Over Again         </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner, Krisitian Revelle, Zach Gill, Otis Jackson Jr., Romeo Jiminez, Jack Brown, William Shileds</v>
+        <v xml:space="preserve"> Jeff Tweedy                </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Loyle Carner feat, Rebel Kleff, Jehst</v>
+        <v>Mavis Staples</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:30 </v>
+        <v xml:space="preserve">01:54 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1419,35 +1347,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Rebel 101                      </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:28 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1459,35 +1387,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No CD                          </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner                                                                                            </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner feat. Rebel Kleff       </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:16 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1499,35 +1427,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Mrs. C                         </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner, Kwes                                                                                      </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner                         </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:22 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1539,35 +1467,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sun of Jean                    </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ben Coyle Larner, Kwes, Steven Vengeance, John Coyle Larner                                                 </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Loyle Carner feat. Mum and Dad       </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">08:00 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1586,21 +1514,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1626,21 +1554,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1666,21 +1594,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1706,21 +1634,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1746,21 +1674,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1786,21 +1714,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1826,21 +1754,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                       </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                             </v>
+        <v xml:space="preserve">                            </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                     </v>
+        <v xml:space="preserve">             </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1862,7 +1790,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1871,10 +1799,12 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="33.5546875" customWidth="1"/>
-    <col min="5" max="7" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1902,7 +1832,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.14861111111111111</v>
+        <v>0.16041666666666668</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1921,7 +1851,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="2">
-        <v>0.11041666666666666</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1930,17 +1860,17 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>44</v>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>3.3333333333333333E-2</v>
+        <v>0.11666666666666665</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1950,16 +1880,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.11944444444444445</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1969,16 +1899,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1988,13 +1918,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>2.361111111111111E-2</v>
+        <v>0.19166666666666665</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2004,16 +1937,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.15069444444444444</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2023,16 +1956,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2">
-        <v>0.10486111111111111</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2042,16 +1975,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1277777777777778</v>
+        <v>0.16041666666666668</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2061,90 +1994,40 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1875</v>
+        <v>7.9166666666666663E-2</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.9444444444444445E-2</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.17777777777777778</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.14027777777777778</v>
-      </c>
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.33333333333333331</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
@@ -2198,6 +2081,21 @@
     </row>
     <row r="28" spans="5:7">
       <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="5:7">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="5:7">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="5:7">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="5:7">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="7:7">
+      <c r="G33" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
07192125 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,10 +17,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="mavisstaples4" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
-    <definedName name="mavisstaples4" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
+    <definedName name="miguel3" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="miguel3" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/mavisstaples4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/miguel3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/mavisstaples4.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/miguel3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="34">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,43 +73,88 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Little Bit</t>
-  </si>
-  <si>
-    <t>Jeff Tweedy</t>
-  </si>
-  <si>
-    <t>Mavis Staples</t>
-  </si>
-  <si>
-    <t>If All I Was Was Black</t>
-  </si>
-  <si>
-    <t>Mavis Staples / Jeff Tweedy</t>
-  </si>
-  <si>
-    <t>Who Told You That</t>
-  </si>
-  <si>
-    <t>Ain't No Doubt About It</t>
-  </si>
-  <si>
-    <t>Peaceful Dream</t>
-  </si>
-  <si>
-    <t>No Time for Crying</t>
-  </si>
-  <si>
-    <t>Build a Bridge</t>
-  </si>
-  <si>
-    <t>We Go High</t>
-  </si>
-  <si>
-    <t>Try Harder</t>
-  </si>
-  <si>
-    <t>All Over Again</t>
+    <t>Criminal</t>
+  </si>
+  <si>
+    <t>Miguel Pimentel / William Roberts / David Andrew Sitek</t>
+  </si>
+  <si>
+    <t>Miguel feat. Rick Ross</t>
+  </si>
+  <si>
+    <t>Pineapple Skies</t>
+  </si>
+  <si>
+    <t>Eyal Federman / Noel Fisher / Marvin Gaye / Odell Brown Jr. / Miguel Pimentel / Salaam Remi / David Ritz / Sidney Swift</t>
+  </si>
+  <si>
+    <t>Miguel feat, Travis Scott</t>
+  </si>
+  <si>
+    <t>Sky Walker</t>
+  </si>
+  <si>
+    <t>Roget Chahayed / Nathan Perez / Miguel Pimentel / Jacques Webster</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Banana Clip</t>
+  </si>
+  <si>
+    <t>Steve Mostyn / Miguel Pimentel</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>Miguel Pimentel / Raphael Saadiq / Dylan Wiggins</t>
+  </si>
+  <si>
+    <t>Miguel feat. Quin</t>
+  </si>
+  <si>
+    <t>Harem</t>
+  </si>
+  <si>
+    <t>Nathan Perez / Miguel Pimentel</t>
+  </si>
+  <si>
+    <t>Told You So</t>
+  </si>
+  <si>
+    <t>Jeff Bhasker / Nathan Perez / Miguel Pimentel</t>
+  </si>
+  <si>
+    <t>City of Angels</t>
+  </si>
+  <si>
+    <t>Caramelo Duro</t>
+  </si>
+  <si>
+    <t>Miguel feat/ Kali Uchis</t>
+  </si>
+  <si>
+    <t>Come Through and Chill</t>
+  </si>
+  <si>
+    <t>Jermaine Cole / Miguel Pimentel / Salaam Remi / James Yancey</t>
+  </si>
+  <si>
+    <t>Miguel feat. J. Cole, Salaam Remi</t>
+  </si>
+  <si>
+    <t>Anointed</t>
+  </si>
+  <si>
+    <t>Arden Altino / Jerry "Wonda" Duplessis / Bernard Grobman / Miguel Pimentel</t>
+  </si>
+  <si>
+    <t>Now</t>
+  </si>
+  <si>
+    <t>Nathan Perez / Miguel Pimentel / Charles Thompson</t>
   </si>
 </sst>
 </file>
@@ -206,11 +252,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mavisstaples4" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="miguel3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mavisstaples4" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="miguel3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -513,15 +559,15 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCellId="1" sqref="A1:XFD1048576 A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -552,7 +598,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.19027777777777777</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -568,10 +614,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16319444444444445</v>
+        <v>0.19513888888888889</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -581,16 +627,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.11666666666666665</v>
+        <v>0.17986111111111111</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -600,16 +646,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -619,16 +665,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.1451388888888889</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -638,16 +684,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
       <c r="E7" s="2">
-        <v>0.19166666666666665</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -657,16 +703,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15069444444444444</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -676,16 +722,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14305555555555557</v>
+        <v>0.17916666666666667</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -695,16 +741,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -714,30 +760,55 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2">
-        <v>7.9166666666666663E-2</v>
+        <v>0.22291666666666665</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.16180555555555556</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.17291666666666669</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
@@ -828,7 +899,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="A3:K14"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -848,15 +919,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -876,21 +947,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                  </v>
+        <v xml:space="preserve"> Title                 </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                 </v>
+        <v xml:space="preserve"> Composers                                                                                                             </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer    </v>
+        <v xml:space="preserve"> Performer                        </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -915,21 +986,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">----------------------- </v>
+        <v xml:space="preserve">---------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> --------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------- </v>
+        <v xml:space="preserve"> --------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -954,28 +1025,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Little Bit             </v>
+        <v xml:space="preserve">Criminal              </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jeff Tweedy                </v>
+        <v xml:space="preserve"> Miguel Pimentel / William Roberts / David Andrew Sitek                                                                 </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel feat. Rick Ross           </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:51 </v>
+        <v xml:space="preserve">04:34 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -994,28 +1065,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">If All I Was Was Black </v>
+        <v xml:space="preserve">Pineapple Skies       </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mavis Staples / Jeff Tweedy</v>
+        <v xml:space="preserve"> Eyal Federman / Noel Fisher / Marvin Gaye / Odell Brown Jr. / Miguel Pimentel / Salaam Remi / David Ritz / Sidney Swift</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel feat, Travis Scott        </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:55 </v>
+        <v xml:space="preserve">04:41 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1034,28 +1105,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Who Told You That      </v>
+        <v xml:space="preserve">Sky Walker            </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jeff Tweedy                </v>
+        <v xml:space="preserve"> Roget Chahayed / Nathan Perez / Miguel Pimentel / Jacques Webster                                                      </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel                           </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:48 </v>
+        <v xml:space="preserve">04:19 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1074,28 +1145,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Ain't No Doubt About It</v>
+        <v xml:space="preserve">Banana Clip           </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jeff Tweedy                </v>
+        <v xml:space="preserve"> Steve Mostyn / Miguel Pimentel                                                                                         </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel                           </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:18 </v>
+        <v xml:space="preserve">03:21 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1114,28 +1185,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Peaceful Dream         </v>
+        <v xml:space="preserve">Wolf                  </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jeff Tweedy                </v>
+        <v xml:space="preserve"> Miguel Pimentel / Raphael Saadiq / Dylan Wiggins                                                                       </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel feat. Quin                </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:20 </v>
+        <v xml:space="preserve">03:29 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1154,28 +1225,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">No Time for Crying     </v>
+        <v xml:space="preserve">Harem                 </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mavis Staples / Jeff Tweedy</v>
+        <v xml:space="preserve"> Nathan Perez / Miguel Pimentel                                                                                         </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel                           </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:36 </v>
+        <v xml:space="preserve">03:13 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1194,28 +1265,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Build a Bridge         </v>
+        <v xml:space="preserve">Told You So           </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jeff Tweedy                </v>
+        <v xml:space="preserve"> Jeff Bhasker / Nathan Perez / Miguel Pimentel                                                                          </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel                           </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:37 </v>
+        <v xml:space="preserve">03:10 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1234,28 +1305,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">We Go High             </v>
+        <v xml:space="preserve">City of Angels        </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Mavis Staples / Jeff Tweedy</v>
+        <v xml:space="preserve"> Nathan Perez / Miguel Pimentel                                                                                         </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel                           </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:26 </v>
+        <v xml:space="preserve">04:18 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1274,28 +1345,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Try Harder             </v>
+        <v xml:space="preserve">Caramelo Duro         </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jeff Tweedy                </v>
+        <v xml:space="preserve"> Steve Mostyn / Miguel Pimentel                                                                                         </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v xml:space="preserve">Miguel feat/ Kali Uchis          </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:51 </v>
+        <v xml:space="preserve">03:33 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1314,28 +1385,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">All Over Again         </v>
+        <v>Come Through and Chill</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jeff Tweedy                </v>
+        <v xml:space="preserve"> Jermaine Cole / Miguel Pimentel / Salaam Remi / James Yancey                                                           </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Mavis Staples</v>
+        <v>Miguel feat. J. Cole, Salaam Remi</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:54 </v>
+        <v xml:space="preserve">05:21 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1347,35 +1418,35 @@
       </c>
       <c r="B15">
         <f>Sheet1!A12</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">Anointed              </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve"> Arden Altino / Jerry "Wonda" Duplessis / Bernard Grobman / Miguel Pimentel                                             </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">Miguel                           </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:53 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1387,35 +1458,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">Now                   </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve"> Nathan Perez / Miguel Pimentel / Charles Thompson                                                                      </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">Miguel                           </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:09 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1434,21 +1505,21 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
@@ -1474,21 +1545,21 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
@@ -1514,21 +1585,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1554,21 +1625,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1594,21 +1665,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1634,21 +1705,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1674,21 +1745,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1714,21 +1785,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1754,21 +1825,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                       </v>
+        <v xml:space="preserve">                      </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                            </v>
+        <v xml:space="preserve">                                                                                                                        </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">             </v>
+        <v xml:space="preserve">                                 </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1799,9 +1870,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.109375" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -1832,7 +1903,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.19027777777777777</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1848,10 +1919,10 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16319444444444445</v>
+        <v>0.19513888888888889</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1861,16 +1932,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.11666666666666665</v>
+        <v>0.17986111111111111</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1880,16 +1951,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.13958333333333334</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1899,16 +1970,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
-        <v>0.1388888888888889</v>
+        <v>0.1451388888888889</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1918,16 +1989,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
       <c r="E7" s="2">
-        <v>0.19166666666666665</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1937,16 +2008,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15069444444444444</v>
+        <v>0.13194444444444445</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1956,16 +2027,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14305555555555557</v>
+        <v>0.17916666666666667</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1975,16 +2046,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
-        <v>0.16041666666666668</v>
+        <v>0.14791666666666667</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1994,30 +2065,55 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2">
-        <v>7.9166666666666663E-2</v>
+        <v>0.22291666666666665</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="2"/>
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.16180555555555556</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.17291666666666669</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>

</xml_diff>

<commit_message>
07202140 added 2 old review
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="miguel3" localSheetId="0">Sheet1!$A$1:$E$13</definedName>
-    <definedName name="miguel3" localSheetId="2">Sheet3!$A$1:$E$13</definedName>
+    <definedName name="mosessumney1" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="mosessumney1" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -33,14 +33,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/miguel3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/mosessumney1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/miguel3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/mosessumney1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="21">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,88 +73,49 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Criminal</t>
+    <t>Man on the Moon (Reprise)</t>
   </si>
   <si>
-    <t>Miguel Pimentel / William Roberts / David Andrew Sitek</t>
+    <t>Moses Sumney</t>
   </si>
   <si>
-    <t>Miguel feat. Rick Ross</t>
+    <t>Don't Bother Calling</t>
   </si>
   <si>
-    <t>Pineapple Skies</t>
+    <t>Plastic</t>
   </si>
   <si>
-    <t>Eyal Federman / Noel Fisher / Marvin Gaye / Odell Brown Jr. / Miguel Pimentel / Salaam Remi / David Ritz / Sidney Swift</t>
+    <t>Quarrel</t>
   </si>
   <si>
-    <t>Miguel feat, Travis Scott</t>
+    <t>Cameron Osteen / Paris Strother / Moses Sumney</t>
   </si>
   <si>
-    <t>Sky Walker</t>
+    <t>Stoicism</t>
   </si>
   <si>
-    <t>Roget Chahayed / Nathan Perez / Miguel Pimentel / Jacques Webster</t>
+    <t>Lonely World</t>
   </si>
   <si>
-    <t>Miguel</t>
+    <t>Make Out in My Car</t>
   </si>
   <si>
-    <t>Banana Clip</t>
+    <t>The Cocoon-Eyed Baby</t>
   </si>
   <si>
-    <t>Steve Mostyn / Miguel Pimentel</t>
+    <t>Doomed</t>
   </si>
   <si>
-    <t>Wolf</t>
+    <t>Matt Otto / Moses Sumney</t>
   </si>
   <si>
-    <t>Miguel Pimentel / Raphael Saadiq / Dylan Wiggins</t>
+    <t>Indulge Me</t>
   </si>
   <si>
-    <t>Miguel feat. Quin</t>
+    <t>Self-Help Tape</t>
   </si>
   <si>
-    <t>Harem</t>
-  </si>
-  <si>
-    <t>Nathan Perez / Miguel Pimentel</t>
-  </si>
-  <si>
-    <t>Told You So</t>
-  </si>
-  <si>
-    <t>Jeff Bhasker / Nathan Perez / Miguel Pimentel</t>
-  </si>
-  <si>
-    <t>City of Angels</t>
-  </si>
-  <si>
-    <t>Caramelo Duro</t>
-  </si>
-  <si>
-    <t>Miguel feat/ Kali Uchis</t>
-  </si>
-  <si>
-    <t>Come Through and Chill</t>
-  </si>
-  <si>
-    <t>Jermaine Cole / Miguel Pimentel / Salaam Remi / James Yancey</t>
-  </si>
-  <si>
-    <t>Miguel feat. J. Cole, Salaam Remi</t>
-  </si>
-  <si>
-    <t>Anointed</t>
-  </si>
-  <si>
-    <t>Arden Altino / Jerry "Wonda" Duplessis / Bernard Grobman / Miguel Pimentel</t>
-  </si>
-  <si>
-    <t>Now</t>
-  </si>
-  <si>
-    <t>Nathan Perez / Miguel Pimentel / Charles Thompson</t>
+    <t>Ludwig Goransson / Moses Sumney</t>
   </si>
 </sst>
 </file>
@@ -252,11 +213,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="miguel3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mosessumney1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="miguel3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mosessumney1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,15 +520,15 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCellId="1" sqref="A1:XFD1048576 A1:XFD1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="46.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -595,10 +556,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
-        <v>0.19027777777777777</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -608,16 +569,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>0.19513888888888889</v>
+        <v>0.16597222222222222</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -627,16 +588,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17986111111111111</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -646,16 +607,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13958333333333334</v>
+        <v>0.28125</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -665,16 +626,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
-        <v>0.1451388888888889</v>
+        <v>4.3055555555555562E-2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -684,16 +645,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.19999999999999998</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -703,16 +664,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -722,16 +683,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17916666666666667</v>
+        <v>4.7916666666666663E-2</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -741,16 +702,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
-        <v>0.14791666666666667</v>
+        <v>0.18541666666666667</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -760,16 +721,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2">
-        <v>0.22291666666666665</v>
+        <v>0.1361111111111111</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -779,36 +740,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2">
-        <v>0.16180555555555556</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.17291666666666669</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
@@ -899,7 +849,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="K15" sqref="A3:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -919,15 +869,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -947,21 +897,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                 </v>
+        <v xml:space="preserve"> Title                    </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                             </v>
+        <v xml:space="preserve"> Composers                                    </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                        </v>
+        <v xml:space="preserve"> Performer   </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -986,21 +936,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">---------------------- </v>
+        <v xml:space="preserve">------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> --------------------------------- </v>
+        <v xml:space="preserve"> ------------ </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1025,28 +975,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Criminal              </v>
+        <v>Man on the Moon (Reprise)</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Miguel Pimentel / William Roberts / David Andrew Sitek                                                                 </v>
+        <v xml:space="preserve"> Moses Sumney                                  </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel feat. Rick Ross           </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:34 </v>
+        <v xml:space="preserve">00:36 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1065,28 +1015,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pineapple Skies       </v>
+        <v xml:space="preserve">Don't Bother Calling     </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Eyal Federman / Noel Fisher / Marvin Gaye / Odell Brown Jr. / Miguel Pimentel / Salaam Remi / David Ritz / Sidney Swift</v>
+        <v xml:space="preserve"> Moses Sumney                                  </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel feat, Travis Scott        </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:41 </v>
+        <v xml:space="preserve">03:59 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1105,28 +1055,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sky Walker            </v>
+        <v xml:space="preserve">Plastic                  </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Roget Chahayed / Nathan Perez / Miguel Pimentel / Jacques Webster                                                      </v>
+        <v xml:space="preserve"> Moses Sumney                                  </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel                           </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:19 </v>
+        <v xml:space="preserve">03:08 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1145,28 +1095,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Banana Clip           </v>
+        <v xml:space="preserve">Quarrel                  </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Steve Mostyn / Miguel Pimentel                                                                                         </v>
+        <v xml:space="preserve"> Cameron Osteen / Paris Strother / Moses Sumney</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel                           </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:21 </v>
+        <v xml:space="preserve">06:45 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1185,28 +1135,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Wolf                  </v>
+        <v xml:space="preserve">Stoicism                 </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Miguel Pimentel / Raphael Saadiq / Dylan Wiggins                                                                       </v>
+        <v xml:space="preserve"> Moses Sumney                                  </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel feat. Quin                </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:29 </v>
+        <v xml:space="preserve">01:02 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1225,28 +1175,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Harem                 </v>
+        <v xml:space="preserve">Lonely World             </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nathan Perez / Miguel Pimentel                                                                                         </v>
+        <v xml:space="preserve"> Moses Sumney                                  </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel                           </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:13 </v>
+        <v xml:space="preserve">04:48 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1265,28 +1215,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Told You So           </v>
+        <v xml:space="preserve">Make Out in My Car       </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jeff Bhasker / Nathan Perez / Miguel Pimentel                                                                          </v>
+        <v xml:space="preserve"> Moses Sumney                                  </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel                           </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:10 </v>
+        <v xml:space="preserve">02:35 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1305,28 +1255,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">City of Angels        </v>
+        <v xml:space="preserve">The Cocoon-Eyed Baby     </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nathan Perez / Miguel Pimentel                                                                                         </v>
+        <v xml:space="preserve"> Moses Sumney                                  </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel                           </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:18 </v>
+        <v xml:space="preserve">01:09 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1345,28 +1295,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Caramelo Duro         </v>
+        <v xml:space="preserve">Doomed                   </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Steve Mostyn / Miguel Pimentel                                                                                         </v>
+        <v xml:space="preserve"> Matt Otto / Moses Sumney                      </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel feat/ Kali Uchis          </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:33 </v>
+        <v xml:space="preserve">04:27 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1385,28 +1335,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Come Through and Chill</v>
+        <v xml:space="preserve">Indulge Me               </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jermaine Cole / Miguel Pimentel / Salaam Remi / James Yancey                                                           </v>
+        <v xml:space="preserve"> Moses Sumney                                  </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Miguel feat. J. Cole, Salaam Remi</v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:21 </v>
+        <v xml:space="preserve">03:16 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1425,28 +1375,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Anointed              </v>
+        <v xml:space="preserve">Self-Help Tape           </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Arden Altino / Jerry "Wonda" Duplessis / Bernard Grobman / Miguel Pimentel                                             </v>
+        <v xml:space="preserve"> Ludwig Goransson / Moses Sumney               </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel                           </v>
+        <v>Moses Sumney</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:53 </v>
+        <v xml:space="preserve">03:01 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1458,35 +1408,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Now                   </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Nathan Perez / Miguel Pimentel / Charles Thompson                                                                      </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Miguel                           </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:09 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1505,21 +1455,21 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
@@ -1545,21 +1495,21 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
@@ -1585,21 +1535,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1625,21 +1575,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1665,21 +1615,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1705,21 +1655,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1745,21 +1695,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1785,21 +1735,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1825,21 +1775,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                      </v>
+        <v xml:space="preserve">                         </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                        </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                 </v>
+        <v xml:space="preserve">            </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1870,9 +1820,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="46.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -1900,10 +1850,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2">
-        <v>0.19027777777777777</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1913,16 +1863,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2">
-        <v>0.19513888888888889</v>
+        <v>0.16597222222222222</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1932,16 +1882,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
-        <v>0.17986111111111111</v>
+        <v>0.13055555555555556</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1951,16 +1901,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13958333333333334</v>
+        <v>0.28125</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1970,16 +1920,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2">
-        <v>0.1451388888888889</v>
+        <v>4.3055555555555562E-2</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1989,16 +1939,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.19999999999999998</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2008,16 +1958,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13194444444444445</v>
+        <v>0.1076388888888889</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2027,16 +1977,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17916666666666667</v>
+        <v>4.7916666666666663E-2</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2046,16 +1996,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2">
-        <v>0.14791666666666667</v>
+        <v>0.18541666666666667</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2065,16 +2015,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2">
-        <v>0.22291666666666665</v>
+        <v>0.1361111111111111</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2084,36 +2034,25 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2">
-        <v>0.16180555555555556</v>
+        <v>0.12569444444444444</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.17291666666666669</v>
-      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>

</xml_diff>

<commit_message>
07212245 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,11 +17,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="mosessumney1" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
-    <definedName name="mosessumney1" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
+    <definedName name="rapsody1" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="rapsody1" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/mosessumney1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/rapsody1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/mosessumney1.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/rapsody1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="44">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -73,49 +72,118 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Man on the Moon (Reprise)</t>
-  </si>
-  <si>
-    <t>Moses Sumney</t>
-  </si>
-  <si>
-    <t>Don't Bother Calling</t>
-  </si>
-  <si>
-    <t>Plastic</t>
-  </si>
-  <si>
-    <t>Quarrel</t>
-  </si>
-  <si>
-    <t>Cameron Osteen / Paris Strother / Moses Sumney</t>
-  </si>
-  <si>
-    <t>Stoicism</t>
-  </si>
-  <si>
-    <t>Lonely World</t>
-  </si>
-  <si>
-    <t>Make Out in My Car</t>
-  </si>
-  <si>
-    <t>The Cocoon-Eyed Baby</t>
-  </si>
-  <si>
-    <t>Doomed</t>
-  </si>
-  <si>
-    <t>Matt Otto / Moses Sumney</t>
-  </si>
-  <si>
-    <t>Indulge Me</t>
-  </si>
-  <si>
-    <t>Self-Help Tape</t>
-  </si>
-  <si>
-    <t>Ludwig Goransson / Moses Sumney</t>
+    <t>Laila's Wisdom</t>
+  </si>
+  <si>
+    <t>Marlanna Evans / Weldon Irvine / Dominick Lamb / Neil Simone</t>
+  </si>
+  <si>
+    <t>Rapsody</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>George Clinton / Bootsy Collins / William Collins / Gary Cooper / Patrick Douthit / Kendrick Duckworth / Marlanna Evans / Lance Howard / Chuck Jackson</t>
+  </si>
+  <si>
+    <t>Rapsody feat. Kendrick Lamar &amp; Lance Skiiiwalker</t>
+  </si>
+  <si>
+    <t>Chrome (Like Ooh)</t>
+  </si>
+  <si>
+    <t>Patrick Douthit / Marlanna Evans</t>
+  </si>
+  <si>
+    <t>Pay Up</t>
+  </si>
+  <si>
+    <t>Marlanna Evans / Kashif "Kash" Norville / Cicely Louise Tyson</t>
+  </si>
+  <si>
+    <t>Ridin'</t>
+  </si>
+  <si>
+    <t>Patrick Douthit / Marlanna Evans / Eric Gabouer / John Hammink / Andre Solomko / Quay Thomas</t>
+  </si>
+  <si>
+    <t>Rapsody feat. GQ</t>
+  </si>
+  <si>
+    <t>Sassy</t>
+  </si>
+  <si>
+    <t>Marlanna Evans / Eric Gabouer</t>
+  </si>
+  <si>
+    <t>Nobody</t>
+  </si>
+  <si>
+    <t>Max Bryk / Patrick Douthit / Rauli Eskolin / Marlanna Evans / Alex Franck / George Porter, Jr. / Andris Mattson / Ziggy Modeliste / Amber Navran / Naomi Neville / Leo Nocentelli / Anderson Paak / Tariq Trotter</t>
+  </si>
+  <si>
+    <t>Rapsody feat. Anderson .Paak, Black Thought &amp; Moonchild</t>
+  </si>
+  <si>
+    <t>Black &amp; Ugly</t>
+  </si>
+  <si>
+    <t>Charlie Bereal / Patrick Douthit / Marlanna Evans / Charlene Keys / Bryan Sledge</t>
+  </si>
+  <si>
+    <t>Rapsody feat. BJ the Chicago Kid</t>
+  </si>
+  <si>
+    <t>You Should Know</t>
+  </si>
+  <si>
+    <t>Robert Barnett / Merna Bishouty / Patrick Brown / Thomas Callaway / Patrick Douthit / Marlanna Evans / Eric Gabouer / Cameron Gipp / Willie Knighton / Ray Murray / Rico Wade</t>
+  </si>
+  <si>
+    <t>Rapsody feat. Busta Rhymes</t>
+  </si>
+  <si>
+    <t>A Rollercoaster Jam Called Love</t>
+  </si>
+  <si>
+    <t>Gwen Bunn / Patrick Douthit / Marlanna Evans / Michelle Hailey / Taalib Johnson / Raphael Saadiq / Carl Wheeler / D'Wayne Wiggins</t>
+  </si>
+  <si>
+    <t>Rapsody feat. Musiq Soulchild &amp; Gwen Bunn</t>
+  </si>
+  <si>
+    <t>U Used 2 Love Me</t>
+  </si>
+  <si>
+    <t>Patrick Douthit / Marlanna Evans / Terrace Martin</t>
+  </si>
+  <si>
+    <t>Rapsody feat. Terrace Martin</t>
+  </si>
+  <si>
+    <t>Knock on My Door</t>
+  </si>
+  <si>
+    <t>Piero Ciampi / Patrick Douthit / Marlanna Evans / Gianni Marchetti / Giuseppe Pavone / Bryan Sledge</t>
+  </si>
+  <si>
+    <t>OooWee</t>
+  </si>
+  <si>
+    <t>Marlanna Evans / Anderson Paak / Cicely Louise Tyson</t>
+  </si>
+  <si>
+    <t>Rapsody feat. Anderson .Paak</t>
+  </si>
+  <si>
+    <t>Jesus Coming</t>
+  </si>
+  <si>
+    <t>Patrick Douthit / Marlanna Evans / Otis Johnson / Amber Navran</t>
+  </si>
+  <si>
+    <t>Rapsody feat. Amber Navran</t>
   </si>
 </sst>
 </file>
@@ -213,11 +281,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mosessumney1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rapsody1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="mosessumney1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rapsody1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,9 +594,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="46.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="53.77734375" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -556,10 +624,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>2.4999999999999998E-2</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -569,16 +637,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16597222222222222</v>
+        <v>0.23263888888888887</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -588,16 +656,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.14444444444444446</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -607,16 +675,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.28125</v>
+        <v>0.1361111111111111</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -626,16 +694,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>4.3055555555555562E-2</v>
+        <v>0.20277777777777781</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -645,16 +713,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19999999999999998</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -664,16 +732,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1076388888888889</v>
+        <v>0.31041666666666667</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -683,16 +751,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>4.7916666666666663E-2</v>
+        <v>0.17291666666666669</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -702,16 +770,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>0.18541666666666667</v>
+        <v>0.26180555555555557</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -721,16 +789,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.22152777777777777</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -740,35 +808,74 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.1125</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.19583333333333333</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.1673611111111111</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.2638888888888889</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
@@ -849,7 +956,7 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="A3:K15"/>
+      <selection activeCell="K18" sqref="A3:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
@@ -869,15 +976,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>46</v>
+        <v>209</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -897,21 +1004,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                    </v>
+        <v xml:space="preserve"> Title                          </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                    </v>
+        <v xml:space="preserve"> Composers                                                                                                                                                                                                       </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer   </v>
+        <v xml:space="preserve"> Performer                                              </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -936,21 +1043,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------------- </v>
+        <v xml:space="preserve">------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------- </v>
+        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------ </v>
+        <v xml:space="preserve"> ------------------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -975,28 +1082,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Man on the Moon (Reprise)</v>
+        <v xml:space="preserve">Laila's Wisdom                 </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Moses Sumney                                  </v>
+        <v xml:space="preserve"> Marlanna Evans / Weldon Irvine / Dominick Lamb / Neil Simone                                                                                                                                                     </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody                                                </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:36 </v>
+        <v xml:space="preserve">03:15 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1015,28 +1122,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Don't Bother Calling     </v>
+        <v xml:space="preserve">Power                          </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Moses Sumney                                  </v>
+        <v xml:space="preserve"> George Clinton / Bootsy Collins / William Collins / Gary Cooper / Patrick Douthit / Kendrick Duckworth / Marlanna Evans / Lance Howard / Chuck Jackson                                                           </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody feat. Kendrick Lamar &amp; Lance Skiiiwalker       </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:59 </v>
+        <v xml:space="preserve">05:35 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1055,28 +1162,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Plastic                  </v>
+        <v xml:space="preserve">Chrome (Like Ooh)              </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Moses Sumney                                  </v>
+        <v xml:space="preserve"> Patrick Douthit / Marlanna Evans                                                                                                                                                                                 </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody                                                </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:08 </v>
+        <v xml:space="preserve">03:28 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1095,28 +1202,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Quarrel                  </v>
+        <v xml:space="preserve">Pay Up                         </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Cameron Osteen / Paris Strother / Moses Sumney</v>
+        <v xml:space="preserve"> Marlanna Evans / Kashif "Kash" Norville / Cicely Louise Tyson                                                                                                                                                    </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody                                                </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:45 </v>
+        <v xml:space="preserve">03:16 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1135,28 +1242,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Stoicism                 </v>
+        <v xml:space="preserve">Ridin'                         </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Moses Sumney                                  </v>
+        <v xml:space="preserve"> Patrick Douthit / Marlanna Evans / Eric Gabouer / John Hammink / Andre Solomko / Quay Thomas                                                                                                                     </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody feat. GQ                                       </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:02 </v>
+        <v xml:space="preserve">04:52 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1175,28 +1282,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lonely World             </v>
+        <v xml:space="preserve">Sassy                          </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Moses Sumney                                  </v>
+        <v xml:space="preserve"> Marlanna Evans / Eric Gabouer                                                                                                                                                                                    </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody                                                </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:48 </v>
+        <v xml:space="preserve">03:13 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1215,28 +1322,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Make Out in My Car       </v>
+        <v xml:space="preserve">Nobody                         </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Moses Sumney                                  </v>
+        <v xml:space="preserve"> Max Bryk / Patrick Douthit / Rauli Eskolin / Marlanna Evans / Alex Franck / George Porter, Jr. / Andris Mattson / Ziggy Modeliste / Amber Navran / Naomi Neville / Leo Nocentelli / Anderson Paak / Tariq Trotter</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v>Rapsody feat. Anderson .Paak, Black Thought &amp; Moonchild</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:35 </v>
+        <v xml:space="preserve">07:27 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1255,28 +1362,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">The Cocoon-Eyed Baby     </v>
+        <v xml:space="preserve">Black &amp; Ugly                   </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Moses Sumney                                  </v>
+        <v xml:space="preserve"> Charlie Bereal / Patrick Douthit / Marlanna Evans / Charlene Keys / Bryan Sledge                                                                                                                                 </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody feat. BJ the Chicago Kid                       </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">01:09 </v>
+        <v xml:space="preserve">04:09 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1295,28 +1402,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Doomed                   </v>
+        <v xml:space="preserve">You Should Know                </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Matt Otto / Moses Sumney                      </v>
+        <v xml:space="preserve"> Robert Barnett / Merna Bishouty / Patrick Brown / Thomas Callaway / Patrick Douthit / Marlanna Evans / Eric Gabouer / Cameron Gipp / Willie Knighton / Ray Murray / Rico Wade                                    </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody feat. Busta Rhymes                             </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:27 </v>
+        <v xml:space="preserve">06:17 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1335,28 +1442,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Indulge Me               </v>
+        <v>A Rollercoaster Jam Called Love</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Moses Sumney                                  </v>
+        <v xml:space="preserve"> Gwen Bunn / Patrick Douthit / Marlanna Evans / Michelle Hailey / Taalib Johnson / Raphael Saadiq / Carl Wheeler / D'Wayne Wiggins                                                                                </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody feat. Musiq Soulchild &amp; Gwen Bunn              </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:16 </v>
+        <v xml:space="preserve">05:19 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1375,28 +1482,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Self-Help Tape           </v>
+        <v xml:space="preserve">U Used 2 Love Me               </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Ludwig Goransson / Moses Sumney               </v>
+        <v xml:space="preserve"> Patrick Douthit / Marlanna Evans / Terrace Martin                                                                                                                                                                </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Moses Sumney</v>
+        <v xml:space="preserve">Rapsody feat. Terrace Martin                           </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:01 </v>
+        <v xml:space="preserve">02:42 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1408,35 +1515,35 @@
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">Knock on My Door               </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve"> Piero Ciampi / Patrick Douthit / Marlanna Evans / Gianni Marchetti / Giuseppe Pavone / Bryan Sledge                                                                                                              </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">Rapsody feat. BJ the Chicago Kid                       </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:42 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1448,35 +1555,35 @@
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">OooWee                         </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve"> Marlanna Evans / Anderson Paak / Cicely Louise Tyson                                                                                                                                                             </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">Rapsody feat. Anderson .Paak                           </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:01 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1488,35 +1595,35 @@
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">Jesus Coming                   </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve"> Patrick Douthit / Marlanna Evans / Otis Johnson / Amber Navran                                                                                                                                                   </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">Rapsody feat. Amber Navran                             </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">06:20 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1535,21 +1642,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                                       </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1575,21 +1682,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                                       </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1615,21 +1722,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                                       </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1655,21 +1762,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                                       </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1695,21 +1802,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                                       </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1735,21 +1842,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                                       </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1775,21 +1882,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                         </v>
+        <v xml:space="preserve">                               </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">            </v>
+        <v xml:space="preserve">                                                       </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1820,9 +1927,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="46.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="53.77734375" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -1850,10 +1957,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>2.4999999999999998E-2</v>
+        <v>0.13541666666666666</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1863,16 +1970,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.16597222222222222</v>
+        <v>0.23263888888888887</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1882,16 +1989,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>0.13055555555555556</v>
+        <v>0.14444444444444446</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1901,16 +2008,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.28125</v>
+        <v>0.1361111111111111</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1920,16 +2027,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>4.3055555555555562E-2</v>
+        <v>0.20277777777777781</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1939,16 +2046,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.19999999999999998</v>
+        <v>0.13402777777777777</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1958,16 +2065,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.1076388888888889</v>
+        <v>0.31041666666666667</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1977,16 +2084,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2">
-        <v>4.7916666666666663E-2</v>
+        <v>0.17291666666666669</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1996,16 +2103,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2">
-        <v>0.18541666666666667</v>
+        <v>0.26180555555555557</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2015,16 +2122,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.22152777777777777</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2034,35 +2141,74 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12569444444444444</v>
+        <v>0.1125</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.19583333333333333</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="2"/>
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.1673611111111111</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="2"/>
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.2638888888888889</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>

</xml_diff>

<commit_message>
07241730 added 1 reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\my-carbon-site\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +12,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="rapsody1" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
-    <definedName name="rapsody1" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
+    <definedName name="dave1" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="dave1" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,15 +26,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/rapsody1.htm" htmlTables="1">
+  <connection id="1" name="接続" type="4" refreshedVersion="4" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/dave1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
-  <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/rapsody1.htm" htmlTables="1">
+  <connection id="2" name="接続1" type="4" refreshedVersion="4" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/dave1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="32">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -66,134 +61,98 @@
     <t>Performer</t>
   </si>
   <si>
-    <t>Title/Composer</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
-    <t>Laila's Wisdom</t>
-  </si>
-  <si>
-    <t>Marlanna Evans / Weldon Irvine / Dominick Lamb / Neil Simone</t>
-  </si>
-  <si>
-    <t>Rapsody</t>
-  </si>
-  <si>
-    <t>Power</t>
-  </si>
-  <si>
-    <t>George Clinton / Bootsy Collins / William Collins / Gary Cooper / Patrick Douthit / Kendrick Duckworth / Marlanna Evans / Lance Howard / Chuck Jackson</t>
-  </si>
-  <si>
-    <t>Rapsody feat. Kendrick Lamar &amp; Lance Skiiiwalker</t>
-  </si>
-  <si>
-    <t>Chrome (Like Ooh)</t>
-  </si>
-  <si>
-    <t>Patrick Douthit / Marlanna Evans</t>
-  </si>
-  <si>
-    <t>Pay Up</t>
-  </si>
-  <si>
-    <t>Marlanna Evans / Kashif "Kash" Norville / Cicely Louise Tyson</t>
-  </si>
-  <si>
-    <t>Ridin'</t>
-  </si>
-  <si>
-    <t>Patrick Douthit / Marlanna Evans / Eric Gabouer / John Hammink / Andre Solomko / Quay Thomas</t>
-  </si>
-  <si>
-    <t>Rapsody feat. GQ</t>
-  </si>
-  <si>
-    <t>Sassy</t>
-  </si>
-  <si>
-    <t>Marlanna Evans / Eric Gabouer</t>
-  </si>
-  <si>
-    <t>Nobody</t>
-  </si>
-  <si>
-    <t>Max Bryk / Patrick Douthit / Rauli Eskolin / Marlanna Evans / Alex Franck / George Porter, Jr. / Andris Mattson / Ziggy Modeliste / Amber Navran / Naomi Neville / Leo Nocentelli / Anderson Paak / Tariq Trotter</t>
-  </si>
-  <si>
-    <t>Rapsody feat. Anderson .Paak, Black Thought &amp; Moonchild</t>
-  </si>
-  <si>
-    <t>Black &amp; Ugly</t>
-  </si>
-  <si>
-    <t>Charlie Bereal / Patrick Douthit / Marlanna Evans / Charlene Keys / Bryan Sledge</t>
-  </si>
-  <si>
-    <t>Rapsody feat. BJ the Chicago Kid</t>
-  </si>
-  <si>
-    <t>You Should Know</t>
-  </si>
-  <si>
-    <t>Robert Barnett / Merna Bishouty / Patrick Brown / Thomas Callaway / Patrick Douthit / Marlanna Evans / Eric Gabouer / Cameron Gipp / Willie Knighton / Ray Murray / Rico Wade</t>
-  </si>
-  <si>
-    <t>Rapsody feat. Busta Rhymes</t>
-  </si>
-  <si>
-    <t>A Rollercoaster Jam Called Love</t>
-  </si>
-  <si>
-    <t>Gwen Bunn / Patrick Douthit / Marlanna Evans / Michelle Hailey / Taalib Johnson / Raphael Saadiq / Carl Wheeler / D'Wayne Wiggins</t>
-  </si>
-  <si>
-    <t>Rapsody feat. Musiq Soulchild &amp; Gwen Bunn</t>
-  </si>
-  <si>
-    <t>U Used 2 Love Me</t>
-  </si>
-  <si>
-    <t>Patrick Douthit / Marlanna Evans / Terrace Martin</t>
-  </si>
-  <si>
-    <t>Rapsody feat. Terrace Martin</t>
-  </si>
-  <si>
-    <t>Knock on My Door</t>
-  </si>
-  <si>
-    <t>Piero Ciampi / Patrick Douthit / Marlanna Evans / Gianni Marchetti / Giuseppe Pavone / Bryan Sledge</t>
-  </si>
-  <si>
-    <t>OooWee</t>
-  </si>
-  <si>
-    <t>Marlanna Evans / Anderson Paak / Cicely Louise Tyson</t>
-  </si>
-  <si>
-    <t>Rapsody feat. Anderson .Paak</t>
-  </si>
-  <si>
-    <t>Jesus Coming</t>
-  </si>
-  <si>
-    <t>Patrick Douthit / Marlanna Evans / Otis Johnson / Amber Navran</t>
-  </si>
-  <si>
-    <t>Rapsody feat. Amber Navran</t>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Composer</t>
+  </si>
+  <si>
+    <t>Psycho</t>
+  </si>
+  <si>
+    <t>Maggie Eckford / Kyle Evans / Alexi von Guggenburg / David Omoregie / Josh Bruce Williams</t>
+  </si>
+  <si>
+    <t>Dave</t>
+  </si>
+  <si>
+    <t>Streatham</t>
+  </si>
+  <si>
+    <t>David Omoregie / Nana Rogues</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>David Omoregie / Fraser T. Smith</t>
+  </si>
+  <si>
+    <t>Purple Heart</t>
+  </si>
+  <si>
+    <t>Marsha Ambrosius / Kyle Evans / Lonnie Lynn / David Omoregie / Natalie Stewart / Scott Storch</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Jonathan Mensah / Damini Ebunoluwa Ogulu / David Omoregie</t>
+  </si>
+  <si>
+    <t>Dave feat. Burna Boy</t>
+  </si>
+  <si>
+    <t>Disaster</t>
+  </si>
+  <si>
+    <t>Momodou Jallow / Ikeoluwa Oladigbolu / David Omoregie</t>
+  </si>
+  <si>
+    <t>Screwface Capital</t>
+  </si>
+  <si>
+    <t>David Omoregie / Tyrrell Paul / Fraser T. Smith / Setlam Woldehaimanot</t>
+  </si>
+  <si>
+    <t>Dave feat J Hus</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Lesley</t>
+  </si>
+  <si>
+    <t>Maggie Eckford / James Napier / David Omoregie / Fraser T. Smith</t>
+  </si>
+  <si>
+    <t>Dave feat. Ruelle</t>
+  </si>
+  <si>
+    <t>Voices</t>
+  </si>
+  <si>
+    <t>Keith Askey / David Omoregie / Jacob Reske / Fraser T. Smith / McCulloch Reid Sutphin</t>
+  </si>
+  <si>
+    <t>Drama</t>
+  </si>
+  <si>
+    <t>Maggie Eckford / Alexi von Guggenburg / David Omoregie / Fraser T. Smith / Josh Bruce Williams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -281,11 +240,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rapsody1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dave1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="rapsody1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dave1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -577,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,67 +550,73 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.26953125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="80.7265625" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1">
+        <v>1</v>
+      </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.17291666666666669</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.23263888888888887</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -662,15 +627,15 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.14444444444444446</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -681,15 +646,15 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.11388888888888889</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -703,12 +668,12 @@
         <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>0.20277777777777781</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -719,15 +684,15 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -741,12 +706,12 @@
         <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.31041666666666667</v>
+        <v>0.17569444444444446</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -754,195 +719,156 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17291666666666669</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" s="2">
-        <v>0.26180555555555557</v>
+        <v>0.46388888888888885</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.22152777777777777</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1125</v>
+        <v>0.29444444444444445</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.19583333333333333</v>
-      </c>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.1673611111111111</v>
-      </c>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.2638888888888889</v>
-      </c>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:7">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="5:7">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="5:7">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="5:7">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="5:7">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="5:7">
+    <row r="24" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="5:7">
+    <row r="25" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="5:7">
+    <row r="26" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="5:7">
+    <row r="27" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="5:7">
+    <row r="28" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="5:7">
+    <row r="29" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="5:7">
+    <row r="30" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="5:7">
+    <row r="31" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="5:7">
+    <row r="32" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="7:7">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.5">
       <c r="G33" s="2"/>
     </row>
   </sheetData>
@@ -956,42 +882,42 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="A3:K18"/>
+      <selection activeCell="K15" sqref="A3:K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.21875" customWidth="1"/>
-    <col min="3" max="3" width="3.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="4.1796875" customWidth="1"/>
+    <col min="3" max="3" width="3.90625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.08984375" customWidth="1"/>
     <col min="5" max="5" width="4" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.21875" customWidth="1"/>
-    <col min="7" max="7" width="4.44140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" customWidth="1"/>
-    <col min="9" max="9" width="4.33203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" customWidth="1"/>
-    <col min="11" max="11" width="3.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.1796875" customWidth="1"/>
+    <col min="7" max="7" width="4.453125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" customWidth="1"/>
+    <col min="9" max="9" width="4.36328125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.453125" customWidth="1"/>
+    <col min="11" max="11" width="3.453125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>209</v>
+        <v>94</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1004,21 +930,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                          </v>
+        <v xml:space="preserve"> Title            </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                                                                                                                                       </v>
+        <v xml:space="preserve"> Composers                                                                                    </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                                              </v>
+        <v xml:space="preserve"> Performer           </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1031,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1043,21 +969,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">------------------------------- </v>
+        <v xml:space="preserve">----------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------------------------- </v>
+        <v xml:space="preserve"> -------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1069,7 +995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1082,34 +1008,34 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Laila's Wisdom                 </v>
+        <v xml:space="preserve">Psycho           </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Marlanna Evans / Weldon Irvine / Dominick Lamb / Neil Simone                                                                                                                                                     </v>
+        <v xml:space="preserve"> Maggie Eckford / Kyle Evans / Alexi von Guggenburg / David Omoregie / Josh Bruce Williams     </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody                                                </v>
+        <v xml:space="preserve">Dave                </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:15 </v>
+        <v xml:space="preserve">04:09 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1122,34 +1048,34 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Power                          </v>
+        <v xml:space="preserve">Streatham        </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> George Clinton / Bootsy Collins / William Collins / Gary Cooper / Patrick Douthit / Kendrick Duckworth / Marlanna Evans / Lance Howard / Chuck Jackson                                                           </v>
+        <v xml:space="preserve"> David Omoregie / Nana Rogues                                                                  </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. Kendrick Lamar &amp; Lance Skiiiwalker       </v>
+        <v xml:space="preserve">Dave                </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:35 </v>
+        <v xml:space="preserve">03:26 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1162,34 +1088,34 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Chrome (Like Ooh)              </v>
+        <v xml:space="preserve">Black            </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Patrick Douthit / Marlanna Evans                                                                                                                                                                                 </v>
+        <v xml:space="preserve"> David Omoregie / Fraser T. Smith                                                              </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody                                                </v>
+        <v xml:space="preserve">Dave                </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:28 </v>
+        <v xml:space="preserve">03:48 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1202,34 +1128,34 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Pay Up                         </v>
+        <v xml:space="preserve">Purple Heart     </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Marlanna Evans / Kashif "Kash" Norville / Cicely Louise Tyson                                                                                                                                                    </v>
+        <v xml:space="preserve"> Marsha Ambrosius / Kyle Evans / Lonnie Lynn / David Omoregie / Natalie Stewart / Scott Storch </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody                                                </v>
+        <v xml:space="preserve">Dave                </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:16 </v>
+        <v xml:space="preserve">02:44 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1242,34 +1168,34 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Ridin'                         </v>
+        <v xml:space="preserve">Location         </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Patrick Douthit / Marlanna Evans / Eric Gabouer / John Hammink / Andre Solomko / Quay Thomas                                                                                                                     </v>
+        <v xml:space="preserve"> Jonathan Mensah / Damini Ebunoluwa Ogulu / David Omoregie                                     </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. GQ                                       </v>
+        <v>Dave feat. Burna Boy</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:52 </v>
+        <v xml:space="preserve">04:01 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1282,34 +1208,34 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Sassy                          </v>
+        <v xml:space="preserve">Disaster         </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Marlanna Evans / Eric Gabouer                                                                                                                                                                                    </v>
+        <v xml:space="preserve"> Momodou Jallow / Ikeoluwa Oladigbolu / David Omoregie                                         </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody                                                </v>
+        <v xml:space="preserve">Dave                </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:13 </v>
+        <v xml:space="preserve">04:00 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1322,34 +1248,34 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Nobody                         </v>
+        <v>Screwface Capital</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Max Bryk / Patrick Douthit / Rauli Eskolin / Marlanna Evans / Alex Franck / George Porter, Jr. / Andris Mattson / Ziggy Modeliste / Amber Navran / Naomi Neville / Leo Nocentelli / Anderson Paak / Tariq Trotter</v>
+        <v xml:space="preserve"> David Omoregie / Tyrrell Paul / Fraser T. Smith / Setlam Woldehaimanot                        </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Rapsody feat. Anderson .Paak, Black Thought &amp; Moonchild</v>
+        <v xml:space="preserve">Dave feat J Hus     </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">07:27 </v>
+        <v xml:space="preserve">04:13 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1362,34 +1288,34 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Black &amp; Ugly                   </v>
+        <v xml:space="preserve">Environment      </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Charlie Bereal / Patrick Douthit / Marlanna Evans / Charlene Keys / Bryan Sledge                                                                                                                                 </v>
+        <v xml:space="preserve"> David Omoregie / Fraser T. Smith                                                              </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. BJ the Chicago Kid                       </v>
+        <v xml:space="preserve">Dave                </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:09 </v>
+        <v xml:space="preserve">03:23 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1402,34 +1328,34 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">You Should Know                </v>
+        <v xml:space="preserve">Lesley           </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Robert Barnett / Merna Bishouty / Patrick Brown / Thomas Callaway / Patrick Douthit / Marlanna Evans / Eric Gabouer / Cameron Gipp / Willie Knighton / Ray Murray / Rico Wade                                    </v>
+        <v xml:space="preserve"> Maggie Eckford / James Napier / David Omoregie / Fraser T. Smith                              </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. Busta Rhymes                             </v>
+        <v xml:space="preserve">Dave feat. Ruelle   </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:17 </v>
+        <v xml:space="preserve">11:08 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1442,34 +1368,34 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>A Rollercoaster Jam Called Love</v>
+        <v xml:space="preserve">Voices           </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Gwen Bunn / Patrick Douthit / Marlanna Evans / Michelle Hailey / Taalib Johnson / Raphael Saadiq / Carl Wheeler / D'Wayne Wiggins                                                                                </v>
+        <v xml:space="preserve"> Keith Askey / David Omoregie / Jacob Reske / Fraser T. Smith / McCulloch Reid Sutphin         </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. Musiq Soulchild &amp; Gwen Bunn              </v>
+        <v xml:space="preserve">Dave                </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">05:19 </v>
+        <v xml:space="preserve">03:18 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1482,154 +1408,154 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">U Used 2 Love Me               </v>
+        <v xml:space="preserve">Drama            </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Patrick Douthit / Marlanna Evans / Terrace Martin                                                                                                                                                                </v>
+        <v xml:space="preserve"> Maggie Eckford / Alexi von Guggenburg / David Omoregie / Fraser T. Smith / Josh Bruce Williams</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. Terrace Martin                           </v>
+        <v xml:space="preserve">Dave                </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:42 </v>
+        <v xml:space="preserve">07:04 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Knock on My Door               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Piero Ciampi / Patrick Douthit / Marlanna Evans / Gianni Marchetti / Giuseppe Pavone / Bryan Sledge                                                                                                              </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. BJ the Chicago Kid                       </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:42 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">OooWee                         </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Marlanna Evans / Anderson Paak / Cicely Louise Tyson                                                                                                                                                             </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. Anderson .Paak                           </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:01 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Jesus Coming                   </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Patrick Douthit / Marlanna Evans / Otis Johnson / Amber Navran                                                                                                                                                   </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Rapsody feat. Amber Navran                             </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:20 </v>
+        <v xml:space="preserve">00:00 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1642,21 +1568,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                       </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1669,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1682,21 +1608,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                       </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1709,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1722,21 +1648,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                       </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1749,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1762,21 +1688,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                       </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1789,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1802,21 +1728,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                       </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1829,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1842,21 +1768,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                       </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1869,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1882,21 +1808,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                               </v>
+        <v xml:space="preserve">                 </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                                                                                                                                                  </v>
+        <v xml:space="preserve">                                                                                               </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                                       </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1924,67 +1850,73 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="53.77734375" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.26953125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="80.7265625" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" customWidth="1"/>
+    <col min="5" max="5" width="5.81640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A1">
+        <v>1</v>
+      </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13541666666666666</v>
+        <v>0.17291666666666669</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.23263888888888887</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1995,15 +1927,15 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>0.14444444444444446</v>
+        <v>0.15833333333333333</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2014,15 +1946,15 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>0.1361111111111111</v>
+        <v>0.11388888888888889</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2036,12 +1968,12 @@
         <v>18</v>
       </c>
       <c r="E6" s="2">
-        <v>0.20277777777777781</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2052,15 +1984,15 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0.13402777777777777</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2074,12 +2006,12 @@
         <v>23</v>
       </c>
       <c r="E8" s="2">
-        <v>0.31041666666666667</v>
+        <v>0.17569444444444446</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2087,195 +2019,156 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>0.17291666666666669</v>
+        <v>0.14097222222222222</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
       <c r="E10" s="2">
-        <v>0.26180555555555557</v>
+        <v>0.46388888888888885</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>0.22152777777777777</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
-        <v>0.1125</v>
+        <v>0.29444444444444445</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.19583333333333333</v>
-      </c>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.1673611111111111</v>
-      </c>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.2638888888888889</v>
-      </c>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:7">
+    <row r="17" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="5:7">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="5:7">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="5:7">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="5:7">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.5">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="5:7">
+    <row r="24" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="5:7">
+    <row r="25" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="5:7">
+    <row r="26" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="5:7">
+    <row r="27" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="5:7">
+    <row r="28" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="5:7">
+    <row r="29" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="5:7">
+    <row r="30" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="5:7">
+    <row r="31" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="5:7">
+    <row r="32" spans="5:7" x14ac:dyDescent="0.5">
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="7:7">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.5">
       <c r="G33" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
07242120 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\carbon\my-carbon-site\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7968" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,10 +17,10 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="dave1" localSheetId="0">Sheet1!$A$1:$E$12</definedName>
-    <definedName name="dave1" localSheetId="2">Sheet3!$A$1:$E$12</definedName>
+    <definedName name="runthejewels3" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="runthejewels3" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,15 +31,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="接続" type="4" refreshedVersion="4" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/dave1.htm" htmlTables="1">
+  <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/runthejewels3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
-  <connection id="2" name="接続1" type="4" refreshedVersion="4" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://planetky.com/dave1.htm" htmlTables="1">
+  <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/runthejewels3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -44,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="30">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -64,95 +69,89 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Composer</t>
-  </si>
-  <si>
-    <t>Psycho</t>
-  </si>
-  <si>
-    <t>Maggie Eckford / Kyle Evans / Alexi von Guggenburg / David Omoregie / Josh Bruce Williams</t>
-  </si>
-  <si>
-    <t>Dave</t>
-  </si>
-  <si>
-    <t>Streatham</t>
-  </si>
-  <si>
-    <t>David Omoregie / Nana Rogues</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>David Omoregie / Fraser T. Smith</t>
-  </si>
-  <si>
-    <t>Purple Heart</t>
-  </si>
-  <si>
-    <t>Marsha Ambrosius / Kyle Evans / Lonnie Lynn / David Omoregie / Natalie Stewart / Scott Storch</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Jonathan Mensah / Damini Ebunoluwa Ogulu / David Omoregie</t>
-  </si>
-  <si>
-    <t>Dave feat. Burna Boy</t>
-  </si>
-  <si>
-    <t>Disaster</t>
-  </si>
-  <si>
-    <t>Momodou Jallow / Ikeoluwa Oladigbolu / David Omoregie</t>
-  </si>
-  <si>
-    <t>Screwface Capital</t>
-  </si>
-  <si>
-    <t>David Omoregie / Tyrrell Paul / Fraser T. Smith / Setlam Woldehaimanot</t>
-  </si>
-  <si>
-    <t>Dave feat J Hus</t>
-  </si>
-  <si>
-    <t>Environment</t>
-  </si>
-  <si>
-    <t>Lesley</t>
-  </si>
-  <si>
-    <t>Maggie Eckford / James Napier / David Omoregie / Fraser T. Smith</t>
-  </si>
-  <si>
-    <t>Dave feat. Ruelle</t>
-  </si>
-  <si>
-    <t>Voices</t>
-  </si>
-  <si>
-    <t>Keith Askey / David Omoregie / Jacob Reske / Fraser T. Smith / McCulloch Reid Sutphin</t>
-  </si>
-  <si>
-    <t>Drama</t>
-  </si>
-  <si>
-    <t>Maggie Eckford / Alexi von Guggenburg / David Omoregie / Fraser T. Smith / Josh Bruce Williams</t>
+    <t>Title/Composer</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>El-P / Killer Mike</t>
+  </si>
+  <si>
+    <t>Run the Jewels feat. Joi</t>
+  </si>
+  <si>
+    <t>Talk to Me</t>
+  </si>
+  <si>
+    <t>Run the Jewels</t>
+  </si>
+  <si>
+    <t>Legend Has It</t>
+  </si>
+  <si>
+    <t>Call Ticketron</t>
+  </si>
+  <si>
+    <t>Hey Kids</t>
+  </si>
+  <si>
+    <t>Danny Brown / El-P / Killer Mike</t>
+  </si>
+  <si>
+    <t>Run the Jewels feat. Danny Brown</t>
+  </si>
+  <si>
+    <t>Stay Gold</t>
+  </si>
+  <si>
+    <t>Don't Get Captured</t>
+  </si>
+  <si>
+    <t>Thieves! (Screamed the Ghost)</t>
+  </si>
+  <si>
+    <t>Boots / El-P / Killer Mike</t>
+  </si>
+  <si>
+    <t>Run the Jewels feat. Tande Adebimpe</t>
+  </si>
+  <si>
+    <t>Run the Jewels feat. Boots</t>
+  </si>
+  <si>
+    <t>Panther Like a Panther [Miracle Mix]</t>
+  </si>
+  <si>
+    <t>Run the Jewels feat. Trina</t>
+  </si>
+  <si>
+    <t>Everybody Stay Calm</t>
+  </si>
+  <si>
+    <t>Oh Mama</t>
+  </si>
+  <si>
+    <t>Thursday in the Danger Room</t>
+  </si>
+  <si>
+    <t>Run the Jewels feat: Kamasi Washington</t>
+  </si>
+  <si>
+    <t>A Report to Your Shareholders/Kill Your Masters</t>
+  </si>
+  <si>
+    <t>El-P / Killer Mike / Zack de la Rocha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -240,11 +239,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dave1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="runthejewels3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dave1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="runthejewels3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,7 +535,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -547,30 +546,24 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E15" sqref="A1:E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="80.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" customWidth="1"/>
-    <col min="5" max="5" width="5.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A1">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
@@ -578,297 +571,336 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.17291666666666669</v>
+        <v>0.1451388888888889</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.14305555555555557</v>
+        <v>0.10486111111111111</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>0.11388888888888889</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.13263888888888889</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.14375000000000002</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17569444444444446</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14097222222222222</v>
+        <v>0.16805555555555554</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
+      <c r="B10">
+        <v>2100</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2">
-        <v>0.46388888888888885</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>0.29444444444444445</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.15</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E14" s="2"/>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.18194444444444444</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E15" s="2"/>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.25972222222222224</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:7">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:7">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:7">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:7">
       <c r="E20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:7">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:7">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:7">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:7">
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="5:7">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="5:7">
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="5:7">
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="5:7">
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="7:7">
       <c r="G33" s="2"/>
     </row>
   </sheetData>
@@ -882,42 +914,42 @@
   <dimension ref="A2:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="A3:K15"/>
+      <selection activeCell="K18" sqref="A3:K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="4.1796875" customWidth="1"/>
-    <col min="3" max="3" width="3.90625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.08984375" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" customWidth="1"/>
+    <col min="3" max="3" width="3.88671875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
     <col min="5" max="5" width="4" style="4" customWidth="1"/>
-    <col min="6" max="6" width="38.1796875" customWidth="1"/>
-    <col min="7" max="7" width="4.453125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" customWidth="1"/>
-    <col min="9" max="9" width="4.36328125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="8.453125" customWidth="1"/>
-    <col min="11" max="11" width="3.453125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="38.21875" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.77734375" customWidth="1"/>
+    <col min="9" max="9" width="4.33203125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" customWidth="1"/>
+    <col min="11" max="11" width="3.44140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -930,21 +962,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title            </v>
+        <v xml:space="preserve"> Title                                          </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                                                                                    </v>
+        <v xml:space="preserve"> Composers                           </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer           </v>
+        <v xml:space="preserve"> Performer                             </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -957,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -969,21 +1001,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">----------------- </v>
+        <v xml:space="preserve">----------------------------------------------- </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ---------------------------------------------------------------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------- </v>
+        <v xml:space="preserve"> -------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -995,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1008,34 +1040,34 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Psycho           </v>
+        <v xml:space="preserve">Down                                           </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Maggie Eckford / Kyle Evans / Alexi von Guggenburg / David Omoregie / Josh Bruce Williams     </v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave                </v>
+        <v xml:space="preserve">Run the Jewels feat. Joi              </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:09 </v>
+        <v xml:space="preserve">03:29 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1048,34 +1080,34 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Streatham        </v>
+        <v xml:space="preserve">Talk to Me                                     </v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> David Omoregie / Nana Rogues                                                                  </v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave                </v>
+        <v xml:space="preserve">Run the Jewels                        </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:26 </v>
+        <v xml:space="preserve">02:31 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1088,34 +1120,34 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Black            </v>
+        <v xml:space="preserve">Legend Has It                                  </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> David Omoregie / Fraser T. Smith                                                              </v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave                </v>
+        <v xml:space="preserve">Run the Jewels                        </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:48 </v>
+        <v xml:space="preserve">03:25 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1128,34 +1160,34 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Purple Heart     </v>
+        <v xml:space="preserve">Call Ticketron                                 </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Marsha Ambrosius / Kyle Evans / Lonnie Lynn / David Omoregie / Natalie Stewart / Scott Storch </v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave                </v>
+        <v xml:space="preserve">Run the Jewels                        </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:44 </v>
+        <v xml:space="preserve">03:18 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1168,34 +1200,34 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Location         </v>
+        <v xml:space="preserve">Hey Kids                                       </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Jonathan Mensah / Damini Ebunoluwa Ogulu / David Omoregie                                     </v>
+        <v xml:space="preserve"> Danny Brown / El-P / Killer Mike     </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Dave feat. Burna Boy</v>
+        <v xml:space="preserve">Run the Jewels feat. Danny Brown      </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:01 </v>
+        <v xml:space="preserve">03:11 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1208,34 +1240,34 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Disaster         </v>
+        <v xml:space="preserve">Stay Gold                                      </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Momodou Jallow / Ikeoluwa Oladigbolu / David Omoregie                                         </v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave                </v>
+        <v xml:space="preserve">Run the Jewels                        </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:00 </v>
+        <v xml:space="preserve">03:27 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1248,34 +1280,34 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>Screwface Capital</v>
+        <v xml:space="preserve">Don't Get Captured                             </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> David Omoregie / Tyrrell Paul / Fraser T. Smith / Setlam Woldehaimanot                        </v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave feat J Hus     </v>
+        <v xml:space="preserve">Run the Jewels                        </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:13 </v>
+        <v xml:space="preserve">03:12 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1288,34 +1320,34 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Environment      </v>
+        <v xml:space="preserve">Thieves! (Screamed the Ghost)                  </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> David Omoregie / Fraser T. Smith                                                              </v>
+        <v xml:space="preserve"> Boots / El-P / Killer Mike           </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave                </v>
+        <v xml:space="preserve">Run the Jewels feat. Tande Adebimpe   </v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:23 </v>
+        <v xml:space="preserve">04:02 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1328,34 +1360,34 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Lesley           </v>
+        <v xml:space="preserve">2100                                           </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Maggie Eckford / James Napier / David Omoregie / Fraser T. Smith                              </v>
+        <v xml:space="preserve"> Boots / El-P / Killer Mike           </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave feat. Ruelle   </v>
+        <v xml:space="preserve">Run the Jewels feat. Boots            </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">11:08 </v>
+        <v xml:space="preserve">04:01 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1368,34 +1400,34 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Voices           </v>
+        <v xml:space="preserve">Panther Like a Panther [Miracle Mix]           </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Keith Askey / David Omoregie / Jacob Reske / Fraser T. Smith / McCulloch Reid Sutphin         </v>
+        <v xml:space="preserve"> Boots / El-P / Killer Mike           </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave                </v>
+        <v xml:space="preserve">Run the Jewels feat. Trina            </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:18 </v>
+        <v xml:space="preserve">03:41 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1408,154 +1440,154 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Drama            </v>
+        <v xml:space="preserve">Everybody Stay Calm                            </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Maggie Eckford / Alexi von Guggenburg / David Omoregie / Fraser T. Smith / Josh Bruce Williams</v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Dave                </v>
+        <v xml:space="preserve">Run the Jewels                        </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">07:04 </v>
+        <v xml:space="preserve">02:58 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16">
         <f>Sheet1!A13</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">Oh Mama                                        </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">Run the Jewels                        </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">03:36 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>0</v>
       </c>
       <c r="B17">
         <f>Sheet1!A14</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">Thursday in the Danger Room                    </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve"> El-P / Killer Mike                   </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v>Run the Jewels feat: Kamasi Washington</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">04:22 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>0</v>
       </c>
       <c r="B18">
         <f>Sheet1!A15</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v>A Report to Your Shareholders/Kill Your Masters</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve"> El-P / Killer Mike / Zack de la Rocha</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">Run the Jewels                        </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">00:00 </v>
+        <v xml:space="preserve">06:14 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1568,21 +1600,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1595,7 +1627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1608,21 +1640,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1635,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1648,21 +1680,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1675,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1688,21 +1720,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1715,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1728,21 +1760,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1755,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1768,21 +1800,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1795,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1808,21 +1840,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                 </v>
+        <v xml:space="preserve">                                               </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                                                                               </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">                                      </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1850,27 +1882,21 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.8" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="80.7265625" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" customWidth="1"/>
-    <col min="5" max="5" width="5.81640625" customWidth="1"/>
-    <col min="6" max="6" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6328125" customWidth="1"/>
+    <col min="1" max="1" width="3.5546875" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A1">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
@@ -1878,297 +1904,336 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="2">
-        <v>0.17291666666666669</v>
+        <v>0.1451388888888889</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="2">
-        <v>0.14305555555555557</v>
+        <v>0.10486111111111111</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>0.15833333333333333</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>0.11388888888888889</v>
+        <v>0.13749999999999998</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.13263888888888889</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>0.16666666666666666</v>
+        <v>0.14375000000000002</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>0.17569444444444446</v>
+        <v>0.13333333333333333</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E9" s="2">
-        <v>0.14097222222222222</v>
+        <v>0.16805555555555554</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
+      <c r="B10">
+        <v>2100</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2">
-        <v>0.46388888888888885</v>
+        <v>0.1673611111111111</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.15347222222222223</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>0.29444444444444445</v>
+        <v>0.12361111111111112</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.15</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E14" s="2"/>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.18194444444444444</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="E15" s="2"/>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.25972222222222224</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:7">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="17" spans="5:7">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="18" spans="5:7">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="5:7">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="20" spans="5:7">
       <c r="E20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="21" spans="5:7">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="22" spans="5:7">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="23" spans="5:7">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="24" spans="5:7">
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="25" spans="5:7">
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="26" spans="5:7">
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="27" spans="5:7">
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="28" spans="5:7">
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="29" spans="5:7">
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="30" spans="5:7">
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="31" spans="5:7">
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="5:7" x14ac:dyDescent="0.5">
+    <row r="32" spans="5:7">
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.5">
+    <row r="33" spans="7:7">
       <c r="G33" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
07262140 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="runthejewels3" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
-    <definedName name="runthejewels3" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
+    <definedName name="tyler3" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="tyler3" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/runthejewels3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/tyler3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/runthejewels3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/tyler3.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="38">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,76 +72,100 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>Down</t>
-  </si>
-  <si>
-    <t>El-P / Killer Mike</t>
-  </si>
-  <si>
-    <t>Run the Jewels feat. Joi</t>
-  </si>
-  <si>
-    <t>Talk to Me</t>
-  </si>
-  <si>
-    <t>Run the Jewels</t>
-  </si>
-  <si>
-    <t>Legend Has It</t>
-  </si>
-  <si>
-    <t>Call Ticketron</t>
-  </si>
-  <si>
-    <t>Hey Kids</t>
-  </si>
-  <si>
-    <t>Danny Brown / El-P / Killer Mike</t>
-  </si>
-  <si>
-    <t>Run the Jewels feat. Danny Brown</t>
-  </si>
-  <si>
-    <t>Stay Gold</t>
-  </si>
-  <si>
-    <t>Don't Get Captured</t>
-  </si>
-  <si>
-    <t>Thieves! (Screamed the Ghost)</t>
-  </si>
-  <si>
-    <t>Boots / El-P / Killer Mike</t>
-  </si>
-  <si>
-    <t>Run the Jewels feat. Tande Adebimpe</t>
-  </si>
-  <si>
-    <t>Run the Jewels feat. Boots</t>
-  </si>
-  <si>
-    <t>Panther Like a Panther [Miracle Mix]</t>
-  </si>
-  <si>
-    <t>Run the Jewels feat. Trina</t>
-  </si>
-  <si>
-    <t>Everybody Stay Calm</t>
-  </si>
-  <si>
-    <t>Oh Mama</t>
-  </si>
-  <si>
-    <t>Thursday in the Danger Room</t>
-  </si>
-  <si>
-    <t>Run the Jewels feat: Kamasi Washington</t>
-  </si>
-  <si>
-    <t>A Report to Your Shareholders/Kill Your Masters</t>
-  </si>
-  <si>
-    <t>El-P / Killer Mike / Zack de la Rocha</t>
+    <t>Foreword</t>
+  </si>
+  <si>
+    <t>Michael Karoli / Jaki Liebezeit / Alex OConnor / Tyler Okonma / Irmin Schmidt / Holger Schuering / Damo Suzuki</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. Rex Orange County</t>
+  </si>
+  <si>
+    <t>Where This Flower Blooms</t>
+  </si>
+  <si>
+    <t>Frank Ocean / Tyler Okonma</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. Frank ocean</t>
+  </si>
+  <si>
+    <t>Sometimes...</t>
+  </si>
+  <si>
+    <t>Tyler Okonma</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator</t>
+  </si>
+  <si>
+    <t>See You Again</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. Kali Uchis</t>
+  </si>
+  <si>
+    <t>Who Dat Boy</t>
+  </si>
+  <si>
+    <t>Rakim Mayers / Tyler Okonma</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. A.$.A.P Rockey</t>
+  </si>
+  <si>
+    <t>Pothole</t>
+  </si>
+  <si>
+    <t>Roy Ayers / Tyler Okonma</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. Jaden Smith</t>
+  </si>
+  <si>
+    <t>Garden Shed</t>
+  </si>
+  <si>
+    <t>Tyler Okonma / Estelle Swaray</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. Estelle</t>
+  </si>
+  <si>
+    <t>Boredom</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. Rex Orange County, Anna Of the North</t>
+  </si>
+  <si>
+    <t>I Ain't Got Time!</t>
+  </si>
+  <si>
+    <t>911/Mr. Lonely</t>
+  </si>
+  <si>
+    <t>Raymond Calhoun / Frank Ocean / Tyler Okonma</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. Frank Ocean, Steve Lacy</t>
+  </si>
+  <si>
+    <t>Droppin' Seeds</t>
+  </si>
+  <si>
+    <t>Dwayne Carter / Tyler Okonma</t>
+  </si>
+  <si>
+    <t>Tyler, The Creator feat. Lil Wayne</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>Glitter</t>
+  </si>
+  <si>
+    <t>Enjoy Right Now Today</t>
   </si>
 </sst>
 </file>
@@ -239,11 +263,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="runthejewels3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tyler3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="runthejewels3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tyler3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -552,9 +576,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="44.88671875" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="57.77734375" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -585,7 +609,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.1451388888888889</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -598,13 +622,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.10486111111111111</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -614,16 +638,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1423611111111111</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -633,16 +657,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.125</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -652,16 +676,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13263888888888889</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -671,16 +695,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2">
-        <v>0.14375000000000002</v>
+        <v>0.16388888888888889</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -690,16 +714,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13333333333333333</v>
+        <v>0.15486111111111112</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -709,16 +733,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16805555555555554</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -727,17 +751,17 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>2100</v>
+      <c r="B10" t="s">
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -747,16 +771,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.17708333333333334</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -766,16 +790,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12361111111111112</v>
+        <v>4.0972222222222222E-2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -785,16 +809,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2">
-        <v>0.15</v>
+        <v>0.15625</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -804,16 +828,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2">
-        <v>0.18194444444444444</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -823,16 +847,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2">
-        <v>0.25972222222222224</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -934,15 +958,15 @@
     <row r="2" spans="1:11">
       <c r="D2" s="1">
         <f t="array" ref="D2">MAX(LENB(Sheet1!B1:'Sheet1'!B30))</f>
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1">
         <f t="array" ref="F2">MAX(LENB(Sheet1!C1:'Sheet1'!C30))</f>
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="H2" s="1">
         <f t="array" ref="H2">MAX(LENB(Sheet1!D1:'Sheet1'!D30))</f>
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="J2" s="1">
         <f>7</f>
@@ -962,21 +986,21 @@
       </c>
       <c r="D3" t="str">
         <f>" "&amp;LEFTB("Title"&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve"> Title                                          </v>
+        <v xml:space="preserve"> Title                   </v>
       </c>
       <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="str">
         <f>" "&amp;LEFTB("Composers"&amp;REPT(" ",$F$2-1),$F$2-1)</f>
-        <v xml:space="preserve"> Composers                           </v>
+        <v xml:space="preserve"> Composers                                                                                                    </v>
       </c>
       <c r="G3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H3" t="str">
         <f>" "&amp;LEFTB("Performer"&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve"> Performer                             </v>
+        <v xml:space="preserve"> Performer                                                    </v>
       </c>
       <c r="I3" s="4" t="s">
         <v>0</v>
@@ -1001,21 +1025,21 @@
       </c>
       <c r="D4" t="str">
         <f>REPT("-",$D$2)&amp;" "</f>
-        <v xml:space="preserve">----------------------------------------------- </v>
+        <v xml:space="preserve">------------------------ </v>
       </c>
       <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F4" t="str">
         <f>" "&amp;REPT("-",$F$2)&amp;" "</f>
-        <v xml:space="preserve"> ------------------------------------- </v>
+        <v xml:space="preserve"> -------------------------------------------------------------------------------------------------------------- </v>
       </c>
       <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="str">
         <f>" "&amp;REPT("-",$H$2)&amp;" "</f>
-        <v xml:space="preserve"> -------------------------------------- </v>
+        <v xml:space="preserve"> ------------------------------------------------------------- </v>
       </c>
       <c r="I4" s="4" t="s">
         <v>0</v>
@@ -1040,28 +1064,28 @@
       </c>
       <c r="D5" s="6" t="str">
         <f>LEFTB(Sheet1!B2&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Down                                           </v>
+        <v xml:space="preserve">Foreword                </v>
       </c>
       <c r="E5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F5" t="str">
         <f>" "&amp;LEFTB(Sheet1!C2&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Michael Karoli / Jaki Liebezeit / Alex OConnor / Tyler Okonma / Irmin Schmidt / Holger Schuering / Damo Suzuki</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H5" t="str">
         <f>LEFTB(Sheet1!D2&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels feat. Joi              </v>
+        <v xml:space="preserve">Tyler, The Creator feat. Rex Orange County                   </v>
       </c>
       <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J5" s="3" t="str">
         <f>TEXT(Sheet1!E2,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:29 </v>
+        <v xml:space="preserve">03:14 </v>
       </c>
       <c r="K5" s="4" t="s">
         <v>0</v>
@@ -1080,28 +1104,28 @@
       </c>
       <c r="D6" s="6" t="str">
         <f>LEFTB(Sheet1!B3&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Talk to Me                                     </v>
+        <v>Where This Flower Blooms</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="str">
         <f>" "&amp;LEFTB(Sheet1!C3&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Frank Ocean / Tyler Okonma                                                                                    </v>
       </c>
       <c r="G6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LEFTB(Sheet1!D3&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels                        </v>
+        <v xml:space="preserve">Tyler, The Creator feat. Frank ocean                         </v>
       </c>
       <c r="I6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="3" t="str">
         <f>TEXT(Sheet1!E3,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:31 </v>
+        <v xml:space="preserve">03:14 </v>
       </c>
       <c r="K6" s="4" t="s">
         <v>0</v>
@@ -1120,28 +1144,28 @@
       </c>
       <c r="D7" s="6" t="str">
         <f>LEFTB(Sheet1!B4&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Legend Has It                                  </v>
+        <v xml:space="preserve">Sometimes...            </v>
       </c>
       <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F7" t="str">
         <f>" "&amp;LEFTB(Sheet1!C4&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Tyler Okonma                                                                                                  </v>
       </c>
       <c r="G7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LEFTB(Sheet1!D4&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels                        </v>
+        <v xml:space="preserve">Tyler, The Creator                                           </v>
       </c>
       <c r="I7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J7" s="3" t="str">
         <f>TEXT(Sheet1!E4,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:25 </v>
+        <v xml:space="preserve">00:36 </v>
       </c>
       <c r="K7" s="4" t="s">
         <v>0</v>
@@ -1160,28 +1184,28 @@
       </c>
       <c r="D8" s="6" t="str">
         <f>LEFTB(Sheet1!B5&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Call Ticketron                                 </v>
+        <v xml:space="preserve">See You Again           </v>
       </c>
       <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F8" t="str">
         <f>" "&amp;LEFTB(Sheet1!C5&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Tyler Okonma                                                                                                  </v>
       </c>
       <c r="G8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LEFTB(Sheet1!D5&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels                        </v>
+        <v xml:space="preserve">Tyler, The Creator feat. Kali Uchis                          </v>
       </c>
       <c r="I8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J8" s="3" t="str">
         <f>TEXT(Sheet1!E5,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:18 </v>
+        <v xml:space="preserve">03:00 </v>
       </c>
       <c r="K8" s="4" t="s">
         <v>0</v>
@@ -1200,28 +1224,28 @@
       </c>
       <c r="D9" s="6" t="str">
         <f>LEFTB(Sheet1!B6&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Hey Kids                                       </v>
+        <v xml:space="preserve">Who Dat Boy             </v>
       </c>
       <c r="E9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F9" t="str">
         <f>" "&amp;LEFTB(Sheet1!C6&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Danny Brown / El-P / Killer Mike     </v>
+        <v xml:space="preserve"> Rakim Mayers / Tyler Okonma                                                                                   </v>
       </c>
       <c r="G9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LEFTB(Sheet1!D6&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels feat. Danny Brown      </v>
+        <v xml:space="preserve">Tyler, The Creator feat. A.$.A.P Rockey                      </v>
       </c>
       <c r="I9" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="3" t="str">
         <f>TEXT(Sheet1!E6,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:11 </v>
+        <v xml:space="preserve">03:25 </v>
       </c>
       <c r="K9" s="4" t="s">
         <v>0</v>
@@ -1240,28 +1264,28 @@
       </c>
       <c r="D10" s="6" t="str">
         <f>LEFTB(Sheet1!B7&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Stay Gold                                      </v>
+        <v xml:space="preserve">Pothole                 </v>
       </c>
       <c r="E10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F10" t="str">
         <f>" "&amp;LEFTB(Sheet1!C7&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Roy Ayers / Tyler Okonma                                                                                      </v>
       </c>
       <c r="G10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H10" t="str">
         <f>LEFTB(Sheet1!D7&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels                        </v>
+        <v xml:space="preserve">Tyler, The Creator feat. Jaden Smith                         </v>
       </c>
       <c r="I10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="3" t="str">
         <f>TEXT(Sheet1!E7,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:27 </v>
+        <v xml:space="preserve">03:56 </v>
       </c>
       <c r="K10" s="4" t="s">
         <v>0</v>
@@ -1280,28 +1304,28 @@
       </c>
       <c r="D11" s="6" t="str">
         <f>LEFTB(Sheet1!B8&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Don't Get Captured                             </v>
+        <v xml:space="preserve">Garden Shed             </v>
       </c>
       <c r="E11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="str">
         <f>" "&amp;LEFTB(Sheet1!C8&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Tyler Okonma / Estelle Swaray                                                                                 </v>
       </c>
       <c r="G11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H11" t="str">
         <f>LEFTB(Sheet1!D8&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels                        </v>
+        <v xml:space="preserve">Tyler, The Creator feat. Estelle                             </v>
       </c>
       <c r="I11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J11" s="3" t="str">
         <f>TEXT(Sheet1!E8,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:12 </v>
+        <v xml:space="preserve">03:43 </v>
       </c>
       <c r="K11" s="4" t="s">
         <v>0</v>
@@ -1320,28 +1344,28 @@
       </c>
       <c r="D12" s="6" t="str">
         <f>LEFTB(Sheet1!B9&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Thieves! (Screamed the Ghost)                  </v>
+        <v xml:space="preserve">Boredom                 </v>
       </c>
       <c r="E12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="str">
         <f>" "&amp;LEFTB(Sheet1!C9&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Boots / El-P / Killer Mike           </v>
+        <v xml:space="preserve"> Tyler Okonma                                                                                                  </v>
       </c>
       <c r="G12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H12" t="str">
         <f>LEFTB(Sheet1!D9&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels feat. Tande Adebimpe   </v>
+        <v>Tyler, The Creator feat. Rex Orange County, Anna Of the North</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="3" t="str">
         <f>TEXT(Sheet1!E9,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:02 </v>
+        <v xml:space="preserve">05:20 </v>
       </c>
       <c r="K12" s="4" t="s">
         <v>0</v>
@@ -1360,28 +1384,28 @@
       </c>
       <c r="D13" s="6" t="str">
         <f>LEFTB(Sheet1!B10&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">2100                                           </v>
+        <v xml:space="preserve">I Ain't Got Time!       </v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F13" t="str">
         <f>" "&amp;LEFTB(Sheet1!C10&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Boots / El-P / Killer Mike           </v>
+        <v xml:space="preserve"> Tyler Okonma                                                                                                  </v>
       </c>
       <c r="G13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H13" t="str">
         <f>LEFTB(Sheet1!D10&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels feat. Boots            </v>
+        <v xml:space="preserve">Tyler, The Creator                                           </v>
       </c>
       <c r="I13" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J13" s="3" t="str">
         <f>TEXT(Sheet1!E10,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:01 </v>
+        <v xml:space="preserve">03:26 </v>
       </c>
       <c r="K13" s="4" t="s">
         <v>0</v>
@@ -1400,28 +1424,28 @@
       </c>
       <c r="D14" s="6" t="str">
         <f>LEFTB(Sheet1!B11&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Panther Like a Panther [Miracle Mix]           </v>
+        <v xml:space="preserve">911/Mr. Lonely          </v>
       </c>
       <c r="E14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F14" t="str">
         <f>" "&amp;LEFTB(Sheet1!C11&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> Boots / El-P / Killer Mike           </v>
+        <v xml:space="preserve"> Raymond Calhoun / Frank Ocean / Tyler Okonma                                                                  </v>
       </c>
       <c r="G14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H14" t="str">
         <f>LEFTB(Sheet1!D11&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels feat. Trina            </v>
+        <v xml:space="preserve">Tyler, The Creator feat. Frank Ocean, Steve Lacy             </v>
       </c>
       <c r="I14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J14" s="3" t="str">
         <f>TEXT(Sheet1!E11,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:41 </v>
+        <v xml:space="preserve">04:15 </v>
       </c>
       <c r="K14" s="4" t="s">
         <v>0</v>
@@ -1440,28 +1464,28 @@
       </c>
       <c r="D15" s="6" t="str">
         <f>LEFTB(Sheet1!B12&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Everybody Stay Calm                            </v>
+        <v xml:space="preserve">Droppin' Seeds          </v>
       </c>
       <c r="E15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F15" t="str">
         <f>" "&amp;LEFTB(Sheet1!C12&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Dwayne Carter / Tyler Okonma                                                                                  </v>
       </c>
       <c r="G15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H15" t="str">
         <f>LEFTB(Sheet1!D12&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels                        </v>
+        <v xml:space="preserve">Tyler, The Creator feat. Lil Wayne                           </v>
       </c>
       <c r="I15" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="3" t="str">
         <f>TEXT(Sheet1!E12,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">02:58 </v>
+        <v xml:space="preserve">00:59 </v>
       </c>
       <c r="K15" s="4" t="s">
         <v>0</v>
@@ -1480,28 +1504,28 @@
       </c>
       <c r="D16" s="6" t="str">
         <f>LEFTB(Sheet1!B13&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Oh Mama                                        </v>
+        <v xml:space="preserve">November                </v>
       </c>
       <c r="E16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F16" t="str">
         <f>" "&amp;LEFTB(Sheet1!C13&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Tyler Okonma                                                                                                  </v>
       </c>
       <c r="G16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H16" t="str">
         <f>LEFTB(Sheet1!D13&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels                        </v>
+        <v xml:space="preserve">Tyler, The Creator                                           </v>
       </c>
       <c r="I16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J16" s="3" t="str">
         <f>TEXT(Sheet1!E13,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">03:36 </v>
+        <v xml:space="preserve">03:45 </v>
       </c>
       <c r="K16" s="4" t="s">
         <v>0</v>
@@ -1520,28 +1544,28 @@
       </c>
       <c r="D17" s="6" t="str">
         <f>LEFTB(Sheet1!B14&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">Thursday in the Danger Room                    </v>
+        <v xml:space="preserve">Glitter                 </v>
       </c>
       <c r="E17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F17" t="str">
         <f>" "&amp;LEFTB(Sheet1!C14&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike                   </v>
+        <v xml:space="preserve"> Tyler Okonma                                                                                                  </v>
       </c>
       <c r="G17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H17" t="str">
         <f>LEFTB(Sheet1!D14&amp;REPT(" ",$H$2),$H$2)</f>
-        <v>Run the Jewels feat: Kamasi Washington</v>
+        <v xml:space="preserve">Tyler, The Creator                                           </v>
       </c>
       <c r="I17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J17" s="3" t="str">
         <f>TEXT(Sheet1!E14,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">04:22 </v>
+        <v xml:space="preserve">03:44 </v>
       </c>
       <c r="K17" s="4" t="s">
         <v>0</v>
@@ -1560,28 +1584,28 @@
       </c>
       <c r="D18" t="str">
         <f>LEFTB(Sheet1!B15&amp;REPT(" ",$D$2),$D$2)</f>
-        <v>A Report to Your Shareholders/Kill Your Masters</v>
+        <v xml:space="preserve">Enjoy Right Now Today   </v>
       </c>
       <c r="E18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F18" t="str">
         <f>" "&amp;LEFTB(Sheet1!C15&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve"> El-P / Killer Mike / Zack de la Rocha</v>
+        <v xml:space="preserve"> Tyler Okonma                                                                                                  </v>
       </c>
       <c r="G18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H18" t="str">
         <f>LEFTB(Sheet1!D15&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">Run the Jewels                        </v>
+        <v xml:space="preserve">Tyler, The Creator                                           </v>
       </c>
       <c r="I18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="J18" s="3" t="str">
         <f>TEXT(Sheet1!E15,"HH:MM")&amp;" "</f>
-        <v xml:space="preserve">06:14 </v>
+        <v xml:space="preserve">03:55 </v>
       </c>
       <c r="K18" s="4" t="s">
         <v>0</v>
@@ -1600,21 +1624,21 @@
       </c>
       <c r="D19" t="str">
         <f>LEFTB(Sheet1!B16&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F19" t="str">
         <f>" "&amp;LEFTB(Sheet1!C16&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H19" t="str">
         <f>LEFTB(Sheet1!D16&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                             </v>
       </c>
       <c r="I19" s="4" t="s">
         <v>0</v>
@@ -1640,21 +1664,21 @@
       </c>
       <c r="D20" t="str">
         <f>LEFTB(Sheet1!B17&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F20" t="str">
         <f>" "&amp;LEFTB(Sheet1!C17&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H20" t="str">
         <f>LEFTB(Sheet1!D17&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                             </v>
       </c>
       <c r="I20" s="4" t="s">
         <v>0</v>
@@ -1680,21 +1704,21 @@
       </c>
       <c r="D21" t="str">
         <f>LEFTB(Sheet1!B18&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F21" t="str">
         <f>" "&amp;LEFTB(Sheet1!C18&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G21" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H21" t="str">
         <f>LEFTB(Sheet1!D18&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                             </v>
       </c>
       <c r="I21" s="4" t="s">
         <v>0</v>
@@ -1720,21 +1744,21 @@
       </c>
       <c r="D22" t="str">
         <f>LEFTB(Sheet1!B19&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F22" t="str">
         <f>" "&amp;LEFTB(Sheet1!C19&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G22" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H22" t="str">
         <f>LEFTB(Sheet1!D19&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                             </v>
       </c>
       <c r="I22" s="4" t="s">
         <v>0</v>
@@ -1760,21 +1784,21 @@
       </c>
       <c r="D23" t="str">
         <f>LEFTB(Sheet1!B20&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F23" t="str">
         <f>" "&amp;LEFTB(Sheet1!C20&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H23" t="str">
         <f>LEFTB(Sheet1!D20&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                             </v>
       </c>
       <c r="I23" s="4" t="s">
         <v>0</v>
@@ -1800,21 +1824,21 @@
       </c>
       <c r="D24" t="str">
         <f>LEFTB(Sheet1!B21&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F24" t="str">
         <f>" "&amp;LEFTB(Sheet1!C21&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H24" t="str">
         <f>LEFTB(Sheet1!D21&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                             </v>
       </c>
       <c r="I24" s="4" t="s">
         <v>0</v>
@@ -1840,21 +1864,21 @@
       </c>
       <c r="D25" t="str">
         <f>LEFTB(Sheet1!B22&amp;REPT(" ",$D$2),$D$2)</f>
-        <v xml:space="preserve">                                               </v>
+        <v xml:space="preserve">                        </v>
       </c>
       <c r="E25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="F25" t="str">
         <f>" "&amp;LEFTB(Sheet1!C22&amp;REPT(" ",$F$2),$F$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                                                                               </v>
       </c>
       <c r="G25" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H25" t="str">
         <f>LEFTB(Sheet1!D22&amp;REPT(" ",$H$2),$H$2)</f>
-        <v xml:space="preserve">                                      </v>
+        <v xml:space="preserve">                                                             </v>
       </c>
       <c r="I25" s="4" t="s">
         <v>0</v>
@@ -1885,9 +1909,9 @@
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="44.88671875" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="80.88671875" customWidth="1"/>
+    <col min="4" max="4" width="57.77734375" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -1918,7 +1942,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.1451388888888889</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1931,13 +1955,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.10486111111111111</v>
+        <v>0.13472222222222222</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1947,16 +1971,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
-        <v>0.1423611111111111</v>
+        <v>2.4999999999999998E-2</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1966,16 +1990,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
-        <v>0.13749999999999998</v>
+        <v>0.125</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1985,16 +2009,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
-        <v>0.13263888888888889</v>
+        <v>0.1423611111111111</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -2004,16 +2028,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E7" s="2">
-        <v>0.14375000000000002</v>
+        <v>0.16388888888888889</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -2023,16 +2047,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2">
-        <v>0.13333333333333333</v>
+        <v>0.15486111111111112</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -2042,16 +2066,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2">
-        <v>0.16805555555555554</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -2060,17 +2084,17 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>2100</v>
+      <c r="B10" t="s">
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E10" s="2">
-        <v>0.1673611111111111</v>
+        <v>0.14305555555555557</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -2080,16 +2104,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
-        <v>0.15347222222222223</v>
+        <v>0.17708333333333334</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -2099,16 +2123,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E12" s="2">
-        <v>0.12361111111111112</v>
+        <v>4.0972222222222222E-2</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -2118,16 +2142,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2">
-        <v>0.15</v>
+        <v>0.15625</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -2137,16 +2161,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2">
-        <v>0.18194444444444444</v>
+        <v>0.15555555555555556</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -2156,16 +2180,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2">
-        <v>0.25972222222222224</v>
+        <v>0.16319444444444445</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>

</xml_diff>

<commit_message>
07272200 added 2 old reviews
</commit_message>
<xml_diff>
--- a/tracklist.xlsx
+++ b/tracklist.xlsx
@@ -17,8 +17,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="tyler3" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
-    <definedName name="tyler3" localSheetId="2">Sheet3!$A$1:$E$15</definedName>
+    <definedName name="stormzy1" localSheetId="0">Sheet1!$A$1:$E$17</definedName>
+    <definedName name="stormzy1" localSheetId="2">Sheet3!$A$1:$E$17</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,14 +32,14 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="接続" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/tyler3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/stormzy1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
     </webPr>
   </connection>
   <connection id="2" name="接続1" type="4" refreshedVersion="6" background="1" saveData="1">
-    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/tyler3.htm" htmlTables="1">
+    <webPr sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="http://bm.planetky.com/stormzy1.htm" htmlTables="1">
       <tables count="1">
         <x v="4"/>
       </tables>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="44">
   <si>
     <t>|</t>
     <phoneticPr fontId="1"/>
@@ -72,100 +72,118 @@
     <t>Title/Composer</t>
   </si>
   <si>
-    <t>Foreword</t>
-  </si>
-  <si>
-    <t>Michael Karoli / Jaki Liebezeit / Alex OConnor / Tyler Okonma / Irmin Schmidt / Holger Schuering / Damo Suzuki</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. Rex Orange County</t>
-  </si>
-  <si>
-    <t>Where This Flower Blooms</t>
-  </si>
-  <si>
-    <t>Frank Ocean / Tyler Okonma</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. Frank ocean</t>
-  </si>
-  <si>
-    <t>Sometimes...</t>
-  </si>
-  <si>
-    <t>Tyler Okonma</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator</t>
-  </si>
-  <si>
-    <t>See You Again</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. Kali Uchis</t>
-  </si>
-  <si>
-    <t>Who Dat Boy</t>
-  </si>
-  <si>
-    <t>Rakim Mayers / Tyler Okonma</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. A.$.A.P Rockey</t>
-  </si>
-  <si>
-    <t>Pothole</t>
-  </si>
-  <si>
-    <t>Roy Ayers / Tyler Okonma</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. Jaden Smith</t>
-  </si>
-  <si>
-    <t>Garden Shed</t>
-  </si>
-  <si>
-    <t>Tyler Okonma / Estelle Swaray</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. Estelle</t>
-  </si>
-  <si>
-    <t>Boredom</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. Rex Orange County, Anna Of the North</t>
-  </si>
-  <si>
-    <t>I Ain't Got Time!</t>
-  </si>
-  <si>
-    <t>911/Mr. Lonely</t>
-  </si>
-  <si>
-    <t>Raymond Calhoun / Frank Ocean / Tyler Okonma</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. Frank Ocean, Steve Lacy</t>
-  </si>
-  <si>
-    <t>Droppin' Seeds</t>
-  </si>
-  <si>
-    <t>Dwayne Carter / Tyler Okonma</t>
-  </si>
-  <si>
-    <t>Tyler, The Creator feat. Lil Wayne</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>Glitter</t>
-  </si>
-  <si>
-    <t>Enjoy Right Now Today</t>
+    <t>First Things First</t>
+  </si>
+  <si>
+    <t>Mura Masa / Michael Omari</t>
+  </si>
+  <si>
+    <t>Stormzy</t>
+  </si>
+  <si>
+    <t>Cold</t>
+  </si>
+  <si>
+    <t>Swifta Beater / Michael Omari</t>
+  </si>
+  <si>
+    <t>Stormzy feat. Ghetts, J Hus</t>
+  </si>
+  <si>
+    <t>Bad Boys</t>
+  </si>
+  <si>
+    <t>Ghetts / J Hus / Momodou Jallow / Michael Omari</t>
+  </si>
+  <si>
+    <t>Blinded by Your Grace, Pt. 1</t>
+  </si>
+  <si>
+    <t>Michael Omari / Fraser T. Smith / Varren Wade / Dion Wardle</t>
+  </si>
+  <si>
+    <t>Big for Your Boots</t>
+  </si>
+  <si>
+    <t>Nozomi Cohen / Karl Joseph</t>
+  </si>
+  <si>
+    <t>Velvet/Jenny Francis (Interlude)</t>
+  </si>
+  <si>
+    <t>Mikey Akin / Nao / Michael Omari / Moses Samuels</t>
+  </si>
+  <si>
+    <t>Mr. Skeng</t>
+  </si>
+  <si>
+    <t>Karl Joseph / Michael Omari</t>
+  </si>
+  <si>
+    <t>Cigarettes &amp; Cush</t>
+  </si>
+  <si>
+    <t>Kehlani / Michael Omari / Fraser T. Smith / Dion Wardle</t>
+  </si>
+  <si>
+    <t>Stormzy feat. Kehlani</t>
+  </si>
+  <si>
+    <t>21 Gun Salute (Interlude)</t>
+  </si>
+  <si>
+    <t>Mikey Akin / Michael Omari / Moses Samuels / Jermaine Scott</t>
+  </si>
+  <si>
+    <t>Stormzy feat. Wretch 32</t>
+  </si>
+  <si>
+    <t>Blinded by Your Grace, Pt. 2</t>
+  </si>
+  <si>
+    <t>Uzoechi Emenike / Michael Omari / Fraser T. Smith</t>
+  </si>
+  <si>
+    <t>Stormzy feat. Mnek</t>
+  </si>
+  <si>
+    <t>Return of the Rucksack</t>
+  </si>
+  <si>
+    <t>Karl Joseph / Michael Omari / Dizzee Rascal</t>
+  </si>
+  <si>
+    <t>100 Bags</t>
+  </si>
+  <si>
+    <t>Sunny Kale / Michael Omari</t>
+  </si>
+  <si>
+    <t>Don't Cry for Me</t>
+  </si>
+  <si>
+    <t>Jacob Anderson / Prince Galalie / Isra Lohata / Michael Omari / Varren Wade / Wizzy Wow</t>
+  </si>
+  <si>
+    <t>Stormzy fat. Raleigh Ritchie</t>
+  </si>
+  <si>
+    <t>Crazy Titch (Interlude)</t>
+  </si>
+  <si>
+    <t>Crazy Titch</t>
+  </si>
+  <si>
+    <t>Shut Up</t>
+  </si>
+  <si>
+    <t>Michael Omari / XTC</t>
+  </si>
+  <si>
+    <t>Lay Me Bare</t>
+  </si>
+  <si>
+    <t>Kwabs / Michael Omari / Fraser T. Smith</t>
   </si>
 </sst>
 </file>
@@ -263,11 +281,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tyler3" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="stormzy1" connectionId="2" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tyler3" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="stormzy1" connectionId="1" autoFormatId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -570,15 +588,15 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="A1:E15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5"/>
   <cols>
     <col min="1" max="1" width="3.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
     <col min="3" max="3" width="80.88671875" customWidth="1"/>
-    <col min="4" max="4" width="57.77734375" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
     <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.6640625" customWidth="1"/>
@@ -609,7 +627,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.14375000000000002</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -628,7 +646,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="2">
-        <v>0.13472222222222222</v>
+        <v>0.10833333333333334</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -644,10 +662,10 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2">
-        <v>2.4999999999999998E-2</v>
+        <v>0.17083333333333331</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -657,16 +675,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E5" s="2">
-        <v>0.125</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -676,16 +694,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>18</v>
-      </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E6" s="2">
-        <v>0.1423611111111111</v>
+        <v>0.16527777777777777</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -695,16 +713,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2">
-        <v>0.16388888888888889</v>
+        <v>0.23541666666666669</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -714,16 +732,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2">
-        <v>0.15486111111111112</v>
+        <v>0.13680555555555554</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -733,16 +751,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E9" s="2">
-        <v>0.22222222222222221</v>
+        <v>0.24236111111111111</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -752,16 +770,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
    